<commit_message>
Updated Final Requirements Sheet Group 10
</commit_message>
<xml_diff>
--- a/FinalRequirements.xlsx
+++ b/FinalRequirements.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28813"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10413"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7D5FC9DF-D770-4083-83A8-0CCEE3BAA020}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meomeomeo/Desktop/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{17091DDB-1535-394A-8CB4-DC13C7BA4D06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="100">
   <si>
     <t>Tested By</t>
   </si>
@@ -90,28 +95,418 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t xml:space="preserve"> The page shall show all
-available players in as a list
-on the Join Game page.</t>
-  </si>
-  <si>
-    <t>displayPlayers()</t>
-  </si>
-  <si>
-    <t>UI001</t>
-  </si>
-  <si>
-    <t>test 1, steps 10-20</t>
-  </si>
-  <si>
     <t>cut and paste the screenshot of each page in this part of the spreadsheet, please. use as much space is needed.</t>
+  </si>
+  <si>
+    <t>The page will show the user their username and which game they are in.</t>
+  </si>
+  <si>
+    <t>requestPlayersUserName(), handleUsernames()</t>
+  </si>
+  <si>
+    <t>The page will show the user the other players user name when they have joined.</t>
+  </si>
+  <si>
+    <t>displayPlayers(), requestAllUsername()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The page will show the user the two bots in their lobby. </t>
+  </si>
+  <si>
+    <t>addPlayerToLobby(), toggleEntitySelection()</t>
+  </si>
+  <si>
+    <t>The page will show 10 lobbies that the user can join which every lobby they want, but can only be in one.</t>
+  </si>
+  <si>
+    <t>displayLobbies(), refreshLobbies(), joinLobby()</t>
+  </si>
+  <si>
+    <t>The page will show a go back button for the user to go back to the new account/login page.</t>
+  </si>
+  <si>
+    <t>handleBackButton() (if implemented)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The page shall gather the information of the user’s username from the page manager in order to show it in the lobby. </t>
+  </si>
+  <si>
+    <t>The page shall show all available players in as a list on the Join Game page.</t>
+  </si>
+  <si>
+    <t>displayPlayers(), selectPlayer()</t>
+  </si>
+  <si>
+    <t>The page shall show a list of available lobbies that users can join.</t>
+  </si>
+  <si>
+    <r>
+      <t>displayLobbies()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>refreshLobbies()</t>
+    </r>
+  </si>
+  <si>
+    <t>The user shall be able to select a lobby to join.</t>
+  </si>
+  <si>
+    <t>joinLobby()</t>
+  </si>
+  <si>
+    <t>The page shall show the current status of each lobby (e.g., full, open).</t>
+  </si>
+  <si>
+    <r>
+      <t>getLobbyStatus()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>updateLobbyStatus()</t>
+    </r>
+  </si>
+  <si>
+    <t>The user shall be able to see the number of players currently in each lobby.</t>
+  </si>
+  <si>
+    <t>displayLobbyPlayerCount()</t>
+  </si>
+  <si>
+    <t>The user shall be able to leave a lobby if they wish to join a different one.</t>
+  </si>
+  <si>
+    <r>
+      <t>leaveLobby()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>updateLobbyList()</t>
+    </r>
+  </si>
+  <si>
+    <t>The page shall display a "Start Game" button once the user has joined a lobby.</t>
+  </si>
+  <si>
+    <r>
+      <t>displayStartButton()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>startGame()</t>
+    </r>
+  </si>
+  <si>
+    <t>The page shall show an error message if the user tries to join a full lobby.</t>
+  </si>
+  <si>
+    <r>
+      <t>displayErrorMessage()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>checkLobbyAvailability()</t>
+    </r>
+  </si>
+  <si>
+    <t>The user shall be able to view the usernames of all players in the lobby.</t>
+  </si>
+  <si>
+    <t>displayPlayersInLobby()</t>
+    <phoneticPr fontId="0"/>
+  </si>
+  <si>
+    <t>The user shall be able to send a message to other players in the lobby.</t>
+  </si>
+  <si>
+    <r>
+      <t>sendMessage()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>receiveMessages()</t>
+    </r>
+  </si>
+  <si>
+    <t>The page shall refresh automatically to update the list of players and lobbies every few seconds.</t>
+  </si>
+  <si>
+    <t>refreshPage()</t>
+  </si>
+  <si>
+    <t>The user shall be able to select a bot to add to their game, if available.</t>
+  </si>
+  <si>
+    <r>
+      <t>addBot()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>toggleEntitySelection()</t>
+    </r>
+  </si>
+  <si>
+    <t>The page shall allow the user to toggle between viewing available lobbies and their current lobby.</t>
+  </si>
+  <si>
+    <t>toggleLobbyView()</t>
+  </si>
+  <si>
+    <t>The page shall display a "waiting for players" message if the user is in a lobby but the game hasn’t started yet.</t>
+  </si>
+  <si>
+    <t>displayWaitingMessage()</t>
+  </si>
+  <si>
+    <t>The user shall be able to see which lobby they are currently in.</t>
+  </si>
+  <si>
+    <t>displayCurrentLobby()</t>
+  </si>
+  <si>
+    <t>The user shall be able to leave the current game and return to the lobby selection page.</t>
+  </si>
+  <si>
+    <r>
+      <t>leaveGame()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>returnToLobbySelection()</t>
+    </r>
+  </si>
+  <si>
+    <t>The page shall indicate when the game has started.</t>
+    <phoneticPr fontId="0"/>
+  </si>
+  <si>
+    <t>startGameIndicator()</t>
+  </si>
+  <si>
+    <t>The page shall provide a visual indicator of the user’s current progress in the lobby (e.g., loading bar).</t>
+    <phoneticPr fontId="0"/>
+  </si>
+  <si>
+    <t>displayProgress()</t>
+  </si>
+  <si>
+    <t>The page shall display the users in the particular game session they have choosen to be in.</t>
+  </si>
+  <si>
+    <t>displayUsers()</t>
+  </si>
+  <si>
+    <t>The page shall register when a button is being pressed and send the message in order to accept the receving message.</t>
+  </si>
+  <si>
+    <t>msg()</t>
+  </si>
+  <si>
+    <t>The page shall show the user when players have been selected and enables the Join Game button when both players have been selected.</t>
+  </si>
+  <si>
+    <t>updateSelectionDisplay()</t>
+  </si>
+  <si>
+    <t>R001</t>
+    <phoneticPr fontId="0"/>
+  </si>
+  <si>
+    <t>R002</t>
+  </si>
+  <si>
+    <t>R003</t>
+  </si>
+  <si>
+    <t>R004</t>
+  </si>
+  <si>
+    <t>R005</t>
+  </si>
+  <si>
+    <t>R006</t>
+  </si>
+  <si>
+    <t>R007</t>
+  </si>
+  <si>
+    <t>R008</t>
+  </si>
+  <si>
+    <t>R009</t>
+  </si>
+  <si>
+    <t>R010</t>
+  </si>
+  <si>
+    <t>R011</t>
+  </si>
+  <si>
+    <t>R012</t>
+  </si>
+  <si>
+    <t>R013</t>
+  </si>
+  <si>
+    <t>R014</t>
+  </si>
+  <si>
+    <t>R015</t>
+  </si>
+  <si>
+    <t>R016</t>
+  </si>
+  <si>
+    <t>R017</t>
+  </si>
+  <si>
+    <t>R018</t>
+  </si>
+  <si>
+    <t>R019</t>
+  </si>
+  <si>
+    <t>R020</t>
+  </si>
+  <si>
+    <t>R021</t>
+  </si>
+  <si>
+    <t>R022</t>
+  </si>
+  <si>
+    <t>R023</t>
+  </si>
+  <si>
+    <t>R024</t>
+  </si>
+  <si>
+    <t>R025</t>
+  </si>
+  <si>
+    <t>R026</t>
+  </si>
+  <si>
+    <t>R027</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -122,8 +517,20 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -134,7 +541,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -142,21 +549,58 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -491,28 +935,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S9"/>
+  <dimension ref="A1:S33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="36.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="46.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="24" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="36.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="41.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="29.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="36.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="K1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="F2" t="s">
         <v>1</v>
       </c>
@@ -550,7 +994,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -570,58 +1014,477 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="43.5">
-      <c r="A4">
-        <v>1</v>
+    <row r="4" spans="1:19" ht="48" x14ac:dyDescent="0.2">
+      <c r="A4" s="11" t="s">
+        <v>73</v>
       </c>
       <c r="B4" s="1">
         <v>10</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="S4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="1" t="s">
+    </row>
+    <row r="5" spans="1:19" ht="31" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" s="1">
+        <v>10</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="3"/>
+    </row>
+    <row r="6" spans="1:19" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="B6" s="1">
+        <v>10</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="3"/>
+    </row>
+    <row r="7" spans="1:19" ht="34" x14ac:dyDescent="0.2">
+      <c r="A7" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="B7" s="1">
+        <v>10</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="5"/>
+    </row>
+    <row r="8" spans="1:19" ht="34" x14ac:dyDescent="0.2">
+      <c r="A8" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="B8" s="1">
+        <v>10</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" spans="1:19" ht="51" x14ac:dyDescent="0.2">
+      <c r="A9" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="B9" s="1">
+        <v>10</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F4" t="s">
-        <v>22</v>
-      </c>
-      <c r="S4" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19">
-      <c r="A5">
-        <v>2</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19">
-      <c r="A6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19">
-      <c r="A7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19">
-      <c r="A8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19">
-      <c r="A9">
-        <v>6</v>
-      </c>
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="1:19" ht="31" x14ac:dyDescent="0.2">
+      <c r="A10" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="B10" s="1">
+        <v>10</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="3"/>
+    </row>
+    <row r="11" spans="1:19" ht="34" x14ac:dyDescent="0.2">
+      <c r="A11" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="B11" s="1">
+        <v>10</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="6"/>
+    </row>
+    <row r="12" spans="1:19" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="B12" s="1">
+        <v>10</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" s="3"/>
+    </row>
+    <row r="13" spans="1:19" ht="34" x14ac:dyDescent="0.2">
+      <c r="A13" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="B13" s="1">
+        <v>10</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="6"/>
+    </row>
+    <row r="14" spans="1:19" ht="31" x14ac:dyDescent="0.2">
+      <c r="A14" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="B14" s="1">
+        <v>10</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14" s="3"/>
+    </row>
+    <row r="15" spans="1:19" ht="34" x14ac:dyDescent="0.2">
+      <c r="A15" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="B15" s="1">
+        <v>10</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" s="6"/>
+    </row>
+    <row r="16" spans="1:19" ht="31" x14ac:dyDescent="0.2">
+      <c r="A16" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="B16" s="1">
+        <v>10</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E16" s="6"/>
+    </row>
+    <row r="17" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A17" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="B17" s="1">
+        <v>10</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E17" s="6"/>
+    </row>
+    <row r="18" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A18" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="B18" s="1">
+        <v>10</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E18" s="3"/>
+    </row>
+    <row r="19" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A19" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="B19" s="1">
+        <v>10</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E19" s="6"/>
+    </row>
+    <row r="20" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A20" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="B20" s="1">
+        <v>10</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E20" s="3"/>
+    </row>
+    <row r="21" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A21" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="B21" s="1">
+        <v>10</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E21" s="6"/>
+    </row>
+    <row r="22" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A22" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="B22" s="1">
+        <v>10</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E22" s="3"/>
+    </row>
+    <row r="23" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A23" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="B23" s="1">
+        <v>10</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E23" s="3"/>
+    </row>
+    <row r="24" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A24" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="B24" s="1">
+        <v>10</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E24" s="3"/>
+    </row>
+    <row r="25" spans="1:5" ht="31" x14ac:dyDescent="0.2">
+      <c r="A25" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="B25" s="1">
+        <v>10</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E25" s="6"/>
+    </row>
+    <row r="26" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A26" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="B26" s="1">
+        <v>10</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E26" s="3"/>
+    </row>
+    <row r="27" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A27" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="B27" s="1">
+        <v>10</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E27" s="3"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B28" s="1">
+        <v>10</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="E28" s="9"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="3"/>
+      <c r="B29" s="1">
+        <v>10</v>
+      </c>
+      <c r="C29" s="8"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B30" s="1">
+        <v>10</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E30" s="3"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="3"/>
+      <c r="B31" s="1">
+        <v>10</v>
+      </c>
+      <c r="C31" s="10"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B32" s="1">
+        <v>10</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E32" s="3"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" s="3"/>
+      <c r="B33" s="1">
+        <v>10</v>
+      </c>
+      <c r="C33" s="10"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
     </row>
   </sheetData>
+  <mergeCells count="33">
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="D28:E29"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="D30:E31"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="D32:E33"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added the database requirements
</commit_message>
<xml_diff>
--- a/FinalRequirements.xlsx
+++ b/FinalRequirements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brant/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ibrah\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C49519C7-29EB-CD44-A5CA-42C1D9C19782}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB0B801E-33E3-4E8E-8630-19E23E1E6953}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="860" yWindow="560" windowWidth="50260" windowHeight="28140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="183">
   <si>
     <t>Tested By</t>
   </si>
@@ -482,6 +482,114 @@
   </si>
   <si>
     <t>If Bot I has capture move(s) available, these shall hold first priority when choosing a move to make.</t>
+  </si>
+  <si>
+    <t>DB.java</t>
+  </si>
+  <si>
+    <t>Be able to Save and Load Games that may have lost connection</t>
+  </si>
+  <si>
+    <t>Store the Current Position and turn history</t>
+  </si>
+  <si>
+    <t>allow user to retrieve username, password, and email</t>
+  </si>
+  <si>
+    <t>allow user to set username, password and email</t>
+  </si>
+  <si>
+    <t>The results of every game played will be stored into a database, and shall be used for building the contents of the leaderboard.</t>
+  </si>
+  <si>
+    <t>The database will use SQLITE</t>
+  </si>
+  <si>
+    <t>The database shall record when the game starts or ends</t>
+  </si>
+  <si>
+    <t>The Leaderboard will be based on rating system/ELO</t>
+  </si>
+  <si>
+    <t>R049</t>
+  </si>
+  <si>
+    <t>R050</t>
+  </si>
+  <si>
+    <t>R051</t>
+  </si>
+  <si>
+    <t>R052</t>
+  </si>
+  <si>
+    <t>R053</t>
+  </si>
+  <si>
+    <t>R054</t>
+  </si>
+  <si>
+    <t>R055</t>
+  </si>
+  <si>
+    <t>R056</t>
+  </si>
+  <si>
+    <t>R057</t>
+  </si>
+  <si>
+    <t>R058</t>
+  </si>
+  <si>
+    <t>R059</t>
+  </si>
+  <si>
+    <t>R060</t>
+  </si>
+  <si>
+    <t>R061</t>
+  </si>
+  <si>
+    <t>R062</t>
+  </si>
+  <si>
+    <t>R063</t>
+  </si>
+  <si>
+    <t>The database shall Not have any duplicate emails or usernames</t>
+  </si>
+  <si>
+    <t>The Database shall give the current leaderboard positions</t>
+  </si>
+  <si>
+    <t>The Database shall give the Time elapsed</t>
+  </si>
+  <si>
+    <t>The Database shall give the Provide User Id</t>
+  </si>
+  <si>
+    <t>The Database shall calculate a player's ELO score using win/loss data</t>
+  </si>
+  <si>
+    <t>The Database shall allow setting and retrieving the game's board state</t>
+  </si>
+  <si>
+    <t>The Database shall track the number of wins and losses per player</t>
+  </si>
+  <si>
+    <t>setBoardstate() , getBoardstate()</t>
+  </si>
+  <si>
+    <t>setUsername() , setPassword() , setEmail()</t>
+  </si>
+  <si>
+    <t>getUsername() , getPassword() , getEmail()</t>
+  </si>
+  <si>
+    <t>calculateElo()</t>
+  </si>
+  <si>
+    <t>getUserID()</t>
   </si>
 </sst>
 </file>
@@ -536,7 +644,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -559,11 +667,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -602,6 +723,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -787,8 +917,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BE40BDEB-2F06-144D-B216-1B597D73F842}" name="Table1" displayName="Table1" ref="A3:E49" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A3:E49" xr:uid="{BE40BDEB-2F06-144D-B216-1B597D73F842}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BE40BDEB-2F06-144D-B216-1B597D73F842}" name="Table1" displayName="Table1" ref="A3:E64" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A3:E64" xr:uid="{BE40BDEB-2F06-144D-B216-1B597D73F842}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{B21B0785-0173-D145-A443-FA0BA41EF992}" name="ID" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{F4BBF6E4-4A05-FE42-95C4-FED1ADB2E7EC}" name="Group" dataDxfId="3"/>
@@ -1117,28 +1247,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S49"/>
+  <dimension ref="A1:S64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="N64" sqref="N64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="8" customWidth="1"/>
-    <col min="3" max="3" width="144.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="45.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="22.1640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="36.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="144.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.6328125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="22.1796875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="36.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
       <c r="K1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
       <c r="F2" t="s">
         <v>1</v>
       </c>
@@ -1176,7 +1306,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -1196,7 +1326,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="48" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19" ht="44" x14ac:dyDescent="0.4">
       <c r="A4" s="9" t="s">
         <v>65</v>
       </c>
@@ -1214,7 +1344,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19" ht="16" x14ac:dyDescent="0.4">
       <c r="A5" s="9" t="s">
         <v>66</v>
       </c>
@@ -1229,7 +1359,7 @@
       </c>
       <c r="E5" s="3"/>
     </row>
-    <row r="6" spans="1:19" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19" ht="16" x14ac:dyDescent="0.4">
       <c r="A6" s="9" t="s">
         <v>67</v>
       </c>
@@ -1244,7 +1374,7 @@
       </c>
       <c r="E6" s="3"/>
     </row>
-    <row r="7" spans="1:19" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19" ht="16" x14ac:dyDescent="0.4">
       <c r="A7" s="9" t="s">
         <v>68</v>
       </c>
@@ -1259,7 +1389,7 @@
       </c>
       <c r="E7" s="4"/>
     </row>
-    <row r="8" spans="1:19" ht="17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:19" ht="16" x14ac:dyDescent="0.4">
       <c r="A8" s="9" t="s">
         <v>69</v>
       </c>
@@ -1274,7 +1404,7 @@
       </c>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:19" ht="17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:19" ht="16" x14ac:dyDescent="0.4">
       <c r="A9" s="9" t="s">
         <v>70</v>
       </c>
@@ -1289,7 +1419,7 @@
       </c>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="1:19" ht="17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:19" ht="16" x14ac:dyDescent="0.4">
       <c r="A10" s="9" t="s">
         <v>71</v>
       </c>
@@ -1304,7 +1434,7 @@
       </c>
       <c r="E10" s="3"/>
     </row>
-    <row r="11" spans="1:19" ht="17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:19" ht="16" x14ac:dyDescent="0.4">
       <c r="A11" s="9" t="s">
         <v>72</v>
       </c>
@@ -1319,7 +1449,7 @@
       </c>
       <c r="E11" s="5"/>
     </row>
-    <row r="12" spans="1:19" ht="17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:19" ht="16" x14ac:dyDescent="0.4">
       <c r="A12" s="9" t="s">
         <v>73</v>
       </c>
@@ -1334,7 +1464,7 @@
       </c>
       <c r="E12" s="3"/>
     </row>
-    <row r="13" spans="1:19" ht="17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:19" ht="16" x14ac:dyDescent="0.4">
       <c r="A13" s="9" t="s">
         <v>74</v>
       </c>
@@ -1349,7 +1479,7 @@
       </c>
       <c r="E13" s="5"/>
     </row>
-    <row r="14" spans="1:19" ht="17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:19" ht="16" x14ac:dyDescent="0.4">
       <c r="A14" s="9" t="s">
         <v>75</v>
       </c>
@@ -1364,7 +1494,7 @@
       </c>
       <c r="E14" s="3"/>
     </row>
-    <row r="15" spans="1:19" ht="17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:19" ht="16" x14ac:dyDescent="0.4">
       <c r="A15" s="9" t="s">
         <v>76</v>
       </c>
@@ -1379,7 +1509,7 @@
       </c>
       <c r="E15" s="5"/>
     </row>
-    <row r="16" spans="1:19" ht="17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:19" ht="16" x14ac:dyDescent="0.4">
       <c r="A16" s="9" t="s">
         <v>77</v>
       </c>
@@ -1394,7 +1524,7 @@
       </c>
       <c r="E16" s="5"/>
     </row>
-    <row r="17" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" ht="16" x14ac:dyDescent="0.4">
       <c r="A17" s="9" t="s">
         <v>78</v>
       </c>
@@ -1409,7 +1539,7 @@
       </c>
       <c r="E17" s="5"/>
     </row>
-    <row r="18" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" ht="16" x14ac:dyDescent="0.4">
       <c r="A18" s="9" t="s">
         <v>79</v>
       </c>
@@ -1424,7 +1554,7 @@
       </c>
       <c r="E18" s="3"/>
     </row>
-    <row r="19" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" ht="16" x14ac:dyDescent="0.4">
       <c r="A19" s="9" t="s">
         <v>80</v>
       </c>
@@ -1439,7 +1569,7 @@
       </c>
       <c r="E19" s="5"/>
     </row>
-    <row r="20" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" ht="16" x14ac:dyDescent="0.4">
       <c r="A20" s="9" t="s">
         <v>81</v>
       </c>
@@ -1454,7 +1584,7 @@
       </c>
       <c r="E20" s="3"/>
     </row>
-    <row r="21" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" ht="16" x14ac:dyDescent="0.4">
       <c r="A21" s="9" t="s">
         <v>82</v>
       </c>
@@ -1469,7 +1599,7 @@
       </c>
       <c r="E21" s="5"/>
     </row>
-    <row r="22" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" ht="16" x14ac:dyDescent="0.4">
       <c r="A22" s="9" t="s">
         <v>83</v>
       </c>
@@ -1484,7 +1614,7 @@
       </c>
       <c r="E22" s="3"/>
     </row>
-    <row r="23" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" ht="16" x14ac:dyDescent="0.4">
       <c r="A23" s="9" t="s">
         <v>84</v>
       </c>
@@ -1499,7 +1629,7 @@
       </c>
       <c r="E23" s="3"/>
     </row>
-    <row r="24" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" ht="16" x14ac:dyDescent="0.4">
       <c r="A24" s="9" t="s">
         <v>85</v>
       </c>
@@ -1514,7 +1644,7 @@
       </c>
       <c r="E24" s="3"/>
     </row>
-    <row r="25" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" ht="16" x14ac:dyDescent="0.4">
       <c r="A25" s="9" t="s">
         <v>86</v>
       </c>
@@ -1529,7 +1659,7 @@
       </c>
       <c r="E25" s="5"/>
     </row>
-    <row r="26" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" ht="16" x14ac:dyDescent="0.4">
       <c r="A26" s="9" t="s">
         <v>87</v>
       </c>
@@ -1544,7 +1674,7 @@
       </c>
       <c r="E26" s="3"/>
     </row>
-    <row r="27" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" ht="16" x14ac:dyDescent="0.4">
       <c r="A27" s="9" t="s">
         <v>88</v>
       </c>
@@ -1559,7 +1689,7 @@
       </c>
       <c r="E27" s="3"/>
     </row>
-    <row r="28" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" ht="16" x14ac:dyDescent="0.4">
       <c r="A28" s="3" t="s">
         <v>89</v>
       </c>
@@ -1574,7 +1704,7 @@
       </c>
       <c r="E28" s="7"/>
     </row>
-    <row r="29" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" ht="16" x14ac:dyDescent="0.4">
       <c r="A29" s="3" t="s">
         <v>90</v>
       </c>
@@ -1589,7 +1719,7 @@
       </c>
       <c r="E29" s="3"/>
     </row>
-    <row r="30" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" ht="16" x14ac:dyDescent="0.4">
       <c r="A30" s="3" t="s">
         <v>91</v>
       </c>
@@ -1604,7 +1734,7 @@
       </c>
       <c r="E30" s="3"/>
     </row>
-    <row r="31" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" ht="16" x14ac:dyDescent="0.4">
       <c r="A31" s="3" t="s">
         <v>115</v>
       </c>
@@ -1619,7 +1749,7 @@
       </c>
       <c r="E31" s="3"/>
     </row>
-    <row r="32" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" ht="16" x14ac:dyDescent="0.4">
       <c r="A32" s="3" t="s">
         <v>116</v>
       </c>
@@ -1634,7 +1764,7 @@
       </c>
       <c r="E32" s="3"/>
     </row>
-    <row r="33" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" ht="16" x14ac:dyDescent="0.4">
       <c r="A33" s="3" t="s">
         <v>117</v>
       </c>
@@ -1649,7 +1779,7 @@
       </c>
       <c r="E33" s="3"/>
     </row>
-    <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A34" s="3" t="s">
         <v>118</v>
       </c>
@@ -1664,7 +1794,7 @@
       </c>
       <c r="E34" s="3"/>
     </row>
-    <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A35" s="3" t="s">
         <v>119</v>
       </c>
@@ -1679,7 +1809,7 @@
       </c>
       <c r="E35" s="3"/>
     </row>
-    <row r="36" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" ht="16" x14ac:dyDescent="0.4">
       <c r="A36" s="3" t="s">
         <v>120</v>
       </c>
@@ -1694,7 +1824,7 @@
       </c>
       <c r="E36" s="3"/>
     </row>
-    <row r="37" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" ht="16" x14ac:dyDescent="0.4">
       <c r="A37" s="3" t="s">
         <v>121</v>
       </c>
@@ -1709,7 +1839,7 @@
       </c>
       <c r="E37" s="3"/>
     </row>
-    <row r="38" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" ht="16" x14ac:dyDescent="0.4">
       <c r="A38" s="3" t="s">
         <v>122</v>
       </c>
@@ -1724,7 +1854,7 @@
       </c>
       <c r="E38" s="3"/>
     </row>
-    <row r="39" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A39" s="3" t="s">
         <v>123</v>
       </c>
@@ -1739,7 +1869,7 @@
       </c>
       <c r="E39" s="3"/>
     </row>
-    <row r="40" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A40" s="3" t="s">
         <v>124</v>
       </c>
@@ -1754,7 +1884,7 @@
       </c>
       <c r="E40" s="3"/>
     </row>
-    <row r="41" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A41" s="3" t="s">
         <v>125</v>
       </c>
@@ -1769,7 +1899,7 @@
       </c>
       <c r="E41" s="3"/>
     </row>
-    <row r="42" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A42" s="3" t="s">
         <v>126</v>
       </c>
@@ -1784,7 +1914,7 @@
       </c>
       <c r="E42" s="3"/>
     </row>
-    <row r="43" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A43" s="3" t="s">
         <v>127</v>
       </c>
@@ -1799,7 +1929,7 @@
       </c>
       <c r="E43" s="3"/>
     </row>
-    <row r="44" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A44" s="3" t="s">
         <v>128</v>
       </c>
@@ -1814,7 +1944,7 @@
       </c>
       <c r="E44" s="3"/>
     </row>
-    <row r="45" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A45" s="3" t="s">
         <v>129</v>
       </c>
@@ -1829,7 +1959,7 @@
       </c>
       <c r="E45" s="3"/>
     </row>
-    <row r="46" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A46" s="3" t="s">
         <v>130</v>
       </c>
@@ -1844,7 +1974,7 @@
       </c>
       <c r="E46" s="3"/>
     </row>
-    <row r="47" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A47" s="3" t="s">
         <v>131</v>
       </c>
@@ -1859,7 +1989,7 @@
       </c>
       <c r="E47" s="3"/>
     </row>
-    <row r="48" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A48" s="3" t="s">
         <v>132</v>
       </c>
@@ -1874,7 +2004,7 @@
       </c>
       <c r="E48" s="3"/>
     </row>
-    <row r="49" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" ht="31" x14ac:dyDescent="0.35">
       <c r="A49" s="3" t="s">
         <v>133</v>
       </c>
@@ -1888,6 +2018,223 @@
         <v>93</v>
       </c>
       <c r="E49" s="3"/>
+    </row>
+    <row r="50" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A50" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B50" s="1">
+        <v>14</v>
+      </c>
+      <c r="C50" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="E50" s="3"/>
+    </row>
+    <row r="51" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A51" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B51" s="1">
+        <v>14</v>
+      </c>
+      <c r="C51" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="E51" s="3"/>
+    </row>
+    <row r="52" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A52" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B52" s="1">
+        <v>14</v>
+      </c>
+      <c r="C52" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3"/>
+    </row>
+    <row r="53" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A53" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B53" s="1">
+        <v>14</v>
+      </c>
+      <c r="C53" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="D53" s="3"/>
+      <c r="E53" s="3"/>
+    </row>
+    <row r="54" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A54" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B54" s="1">
+        <v>14</v>
+      </c>
+      <c r="C54" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="E54" s="3"/>
+    </row>
+    <row r="55" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A55" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="B55" s="1">
+        <v>14</v>
+      </c>
+      <c r="C55" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="E55" s="3"/>
+    </row>
+    <row r="56" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A56" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="B56" s="1">
+        <v>14</v>
+      </c>
+      <c r="C56" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="E56" s="3"/>
+    </row>
+    <row r="57" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A57" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B57" s="1">
+        <v>14</v>
+      </c>
+      <c r="C57" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="E57" s="3"/>
+    </row>
+    <row r="58" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A58" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="B58" s="1">
+        <v>14</v>
+      </c>
+      <c r="C58" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="E58" s="3"/>
+    </row>
+    <row r="59" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A59" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="B59" s="1">
+        <v>14</v>
+      </c>
+      <c r="C59" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="E59" s="3"/>
+    </row>
+    <row r="60" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A60" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="B60" s="1">
+        <v>14</v>
+      </c>
+      <c r="C60" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="E60" s="3"/>
+    </row>
+    <row r="61" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A61" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="B61" s="1">
+        <v>14</v>
+      </c>
+      <c r="C61" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="E61" s="3"/>
+    </row>
+    <row r="62" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A62" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="B62" s="1">
+        <v>14</v>
+      </c>
+      <c r="C62" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="D62" s="3"/>
+      <c r="E62" s="3"/>
+    </row>
+    <row r="63" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A63" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="B63" s="1">
+        <v>14</v>
+      </c>
+      <c r="C63" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="D63" s="3"/>
+      <c r="E63" s="3"/>
+    </row>
+    <row r="64" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A64" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="B64" s="16">
+        <v>14</v>
+      </c>
+      <c r="C64" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="D64" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="E64" s="15"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>

<commit_message>
Add Group 11 Requirements
</commit_message>
<xml_diff>
--- a/FinalRequirements.xlsx
+++ b/FinalRequirements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10116"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ibrah\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raisatasnim/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB0B801E-33E3-4E8E-8630-19E23E1E6953}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F108DAD8-348D-9842-BB6C-E59B2D17790B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="294">
   <si>
     <t>Tested By</t>
   </si>
@@ -590,13 +590,346 @@
   </si>
   <si>
     <t>getUserID()</t>
+  </si>
+  <si>
+    <t>R064</t>
+  </si>
+  <si>
+    <t>R065</t>
+  </si>
+  <si>
+    <t>R066</t>
+  </si>
+  <si>
+    <t>R067</t>
+  </si>
+  <si>
+    <t>R068</t>
+  </si>
+  <si>
+    <t>R069</t>
+  </si>
+  <si>
+    <t>R070</t>
+  </si>
+  <si>
+    <t>R071</t>
+  </si>
+  <si>
+    <t>R072</t>
+  </si>
+  <si>
+    <t>R073</t>
+  </si>
+  <si>
+    <t>R074</t>
+  </si>
+  <si>
+    <t>R075</t>
+  </si>
+  <si>
+    <t>R076</t>
+  </si>
+  <si>
+    <t>R077</t>
+  </si>
+  <si>
+    <t>R078</t>
+  </si>
+  <si>
+    <t>R079</t>
+  </si>
+  <si>
+    <t>R080</t>
+  </si>
+  <si>
+    <t>R081</t>
+  </si>
+  <si>
+    <t>R082</t>
+  </si>
+  <si>
+    <t>R083</t>
+  </si>
+  <si>
+    <t>R084</t>
+  </si>
+  <si>
+    <t>R085</t>
+  </si>
+  <si>
+    <t>R086</t>
+  </si>
+  <si>
+    <t>R087</t>
+  </si>
+  <si>
+    <t>R088</t>
+  </si>
+  <si>
+    <t>R089</t>
+  </si>
+  <si>
+    <t>R090</t>
+  </si>
+  <si>
+    <t>R091</t>
+  </si>
+  <si>
+    <t>R092</t>
+  </si>
+  <si>
+    <t>R093</t>
+  </si>
+  <si>
+    <t>R094</t>
+  </si>
+  <si>
+    <t>R095</t>
+  </si>
+  <si>
+    <t>R096</t>
+  </si>
+  <si>
+    <t>R097</t>
+  </si>
+  <si>
+    <t>R098</t>
+  </si>
+  <si>
+    <t>R099</t>
+  </si>
+  <si>
+    <t>R100</t>
+  </si>
+  <si>
+    <t>R101</t>
+  </si>
+  <si>
+    <t>R102</t>
+  </si>
+  <si>
+    <t>R103</t>
+  </si>
+  <si>
+    <t>R104</t>
+  </si>
+  <si>
+    <t>R105</t>
+  </si>
+  <si>
+    <t>R106</t>
+  </si>
+  <si>
+    <t>R107</t>
+  </si>
+  <si>
+    <t>R108</t>
+  </si>
+  <si>
+    <t>R109</t>
+  </si>
+  <si>
+    <t>The Game should have 8 x 8 array checkers board.</t>
+  </si>
+  <si>
+    <t>The board should display 24 checkers (12 red and 12 black) at the start of the game.</t>
+  </si>
+  <si>
+    <t>Pieces should be clearly distinguishable by color for two players.</t>
+  </si>
+  <si>
+    <t>The board should support different themes that players can choose from.</t>
+  </si>
+  <si>
+    <t>When a piece reaches the last row, it should become a King and be visually distinct.</t>
+  </si>
+  <si>
+    <t>Players should be able to move pieces by dragging and dropping.</t>
+  </si>
+  <si>
+    <t>The game should validate whether a move is legal, and prevent invalid moves.</t>
+  </si>
+  <si>
+    <t>The game should highlight valid moves when a piece is selected.</t>
+  </si>
+  <si>
+    <t>When it is not the player’s turn, their own pieces should be faded or unclickable, while the opponent's pieces are highlighted, and vice versa.</t>
+  </si>
+  <si>
+    <t>The game should track and display the number of pieces captured.</t>
+  </si>
+  <si>
+    <t>The game should indicate whose turn it is at all times.</t>
+  </si>
+  <si>
+    <t>The game should provide clear win/loss/draw notifications at the end of a match.</t>
+  </si>
+  <si>
+    <t>A move history should be maintained, allowing players to view previous game states.</t>
+  </si>
+  <si>
+    <t>The board should display a timer to track the duration of the game.</t>
+  </si>
+  <si>
+    <t>Players should have the option to restart the game after it ends.</t>
+  </si>
+  <si>
+    <t>The game should support username input and display for both players.</t>
+  </si>
+  <si>
+    <t>A sound effect should play when a piece is moved.</t>
+  </si>
+  <si>
+    <t>A distinct sound effect should play when a piece is kinged.</t>
+  </si>
+  <si>
+    <t>A different sound effect should play when a piece is captured.</t>
+  </si>
+  <si>
+    <t>Players should be able to toggle sound effects on or off.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diagonally placement for the checkers. </t>
+  </si>
+  <si>
+    <t>A sound effect should play at the beginning of a game</t>
+  </si>
+  <si>
+    <t>A sound effect should play when a game is won</t>
+  </si>
+  <si>
+    <t>A sound effect should play when a game is lost</t>
+  </si>
+  <si>
+    <t>A sound effect should play when a game is drawn</t>
+  </si>
+  <si>
+    <t>A sound effect should play when a player recieves a draw proposal</t>
+  </si>
+  <si>
+    <t>Players should be able to adjust the volume of sound effects.</t>
+  </si>
+  <si>
+    <t>A sound effect should play when a piece is captured</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The move history of the active game in play should in store in a linked list on the html alongside the turn order. On the main page there should be two buttons, one to go move backwards in the game history and another to go a move forward in the game history. </t>
+  </si>
+  <si>
+    <t>The move history of the game in play should be displayed in checkers notation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A move that is made by the player (Whether it would be dragged or clicked), will be sent to the page manager system for checking if the valid move is legal or not. </t>
+  </si>
+  <si>
+    <t>The usernames for each player (or bot) shall be recieved by the pagemanager</t>
+  </si>
+  <si>
+    <t>If a bot is in game, a unique tag shall be displayed for them, replacing where the ranking would normally be displayed.</t>
+  </si>
+  <si>
+    <t>For the themes, a hashmap shall be used for storage of themes</t>
+  </si>
+  <si>
+    <t>The ranking of each player shall be displayed by their username, this data will be recived from the page manager system</t>
+  </si>
+  <si>
+    <t>Once a move has been verified that it is legal or not via data from the page manager. The gameboard will update with the new positions, if the move was illegal the, the attempted to be moved piece will return to its previous position</t>
+  </si>
+  <si>
+    <t>There shall be a resignation button for when a player wishes to resign</t>
+  </si>
+  <si>
+    <t>Clicking the resignation button will require a second conformation click.</t>
+  </si>
+  <si>
+    <t>When a piece moves multiple times in a single turn, there shall be a small visual update delay between each move the moving piece captures during that turn.</t>
+  </si>
+  <si>
+    <t>Both proposing and accepting a draw will require a second conformation click when clicked.</t>
+  </si>
+  <si>
+    <t>When a player clicks the draw button, on or off their turn, the opposing player will be notified that they are being proposed a draw.</t>
+  </si>
+  <si>
+    <t>There shall be a draw button for when a player wishes to propose a draw</t>
+  </si>
+  <si>
+    <t>The game should automatically restart when a player resigns.</t>
+  </si>
+  <si>
+    <t>The game should automatically restart when a player ACCEPTS a proposed draw.</t>
+  </si>
+  <si>
+    <t>When a draw is proposed there will be a 10 second timer for the draw to be either confirmed or declined.</t>
+  </si>
+  <si>
+    <t>The recently moved piece should be highlighted briefly.</t>
+  </si>
+  <si>
+    <t>createBoard()</t>
+  </si>
+  <si>
+    <t>.red .blue</t>
+  </si>
+  <si>
+    <t>toggleTheme</t>
+  </si>
+  <si>
+    <t>executeValidMove(), .king</t>
+  </si>
+  <si>
+    <t>createPiece()</t>
+  </si>
+  <si>
+    <t>socket.send()</t>
+  </si>
+  <si>
+    <t>displayPlayerTurn()</t>
+  </si>
+  <si>
+    <t>displayEndState(endOfGameState), alert()</t>
+  </si>
+  <si>
+    <t>drawTimer()</t>
+  </si>
+  <si>
+    <t>location.reload()</t>
+  </si>
+  <si>
+    <t>getPlayerdata()</t>
+  </si>
+  <si>
+    <t>soundManager.playsound()</t>
+  </si>
+  <si>
+    <t>soundToggle()</t>
+  </si>
+  <si>
+    <t>soundManager.init()</t>
+  </si>
+  <si>
+    <t>soundsManager.playSound()</t>
+  </si>
+  <si>
+    <t>cell.addEventListener()</t>
+  </si>
+  <si>
+    <t>executeValidMove()</t>
+  </si>
+  <si>
+    <t>resignbtn</t>
+  </si>
+  <si>
+    <t>drawBtn</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -634,6 +967,12 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -684,7 +1023,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -727,11 +1066,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -917,8 +1260,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BE40BDEB-2F06-144D-B216-1B597D73F842}" name="Table1" displayName="Table1" ref="A3:E64" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A3:E64" xr:uid="{BE40BDEB-2F06-144D-B216-1B597D73F842}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BE40BDEB-2F06-144D-B216-1B597D73F842}" name="Table1" displayName="Table1" ref="A3:E110" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A3:E110" xr:uid="{BE40BDEB-2F06-144D-B216-1B597D73F842}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{B21B0785-0173-D145-A443-FA0BA41EF992}" name="ID" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{F4BBF6E4-4A05-FE42-95C4-FED1ADB2E7EC}" name="Group" dataDxfId="3"/>
@@ -1247,28 +1590,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S64"/>
+  <dimension ref="A1:S110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="N64" sqref="N64"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="C72" sqref="C72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="8" customWidth="1"/>
-    <col min="3" max="3" width="144.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="45.6328125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="22.1796875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="36.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="144.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="22.1640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="36.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="K1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="F2" t="s">
         <v>1</v>
       </c>
@@ -1306,7 +1649,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -1326,7 +1669,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="44" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:19" ht="48" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>65</v>
       </c>
@@ -1344,7 +1687,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="16" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>66</v>
       </c>
@@ -1359,7 +1702,7 @@
       </c>
       <c r="E5" s="3"/>
     </row>
-    <row r="6" spans="1:19" ht="16" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
         <v>67</v>
       </c>
@@ -1374,7 +1717,7 @@
       </c>
       <c r="E6" s="3"/>
     </row>
-    <row r="7" spans="1:19" ht="16" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
         <v>68</v>
       </c>
@@ -1389,7 +1732,7 @@
       </c>
       <c r="E7" s="4"/>
     </row>
-    <row r="8" spans="1:19" ht="16" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
         <v>69</v>
       </c>
@@ -1404,7 +1747,7 @@
       </c>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:19" ht="16" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
         <v>70</v>
       </c>
@@ -1419,7 +1762,7 @@
       </c>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="1:19" ht="16" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
         <v>71</v>
       </c>
@@ -1434,7 +1777,7 @@
       </c>
       <c r="E10" s="3"/>
     </row>
-    <row r="11" spans="1:19" ht="16" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
         <v>72</v>
       </c>
@@ -1449,7 +1792,7 @@
       </c>
       <c r="E11" s="5"/>
     </row>
-    <row r="12" spans="1:19" ht="16" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
         <v>73</v>
       </c>
@@ -1464,7 +1807,7 @@
       </c>
       <c r="E12" s="3"/>
     </row>
-    <row r="13" spans="1:19" ht="16" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
         <v>74</v>
       </c>
@@ -1479,7 +1822,7 @@
       </c>
       <c r="E13" s="5"/>
     </row>
-    <row r="14" spans="1:19" ht="16" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
         <v>75</v>
       </c>
@@ -1494,7 +1837,7 @@
       </c>
       <c r="E14" s="3"/>
     </row>
-    <row r="15" spans="1:19" ht="16" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
         <v>76</v>
       </c>
@@ -1509,7 +1852,7 @@
       </c>
       <c r="E15" s="5"/>
     </row>
-    <row r="16" spans="1:19" ht="16" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
         <v>77</v>
       </c>
@@ -1524,7 +1867,7 @@
       </c>
       <c r="E16" s="5"/>
     </row>
-    <row r="17" spans="1:5" ht="16" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
         <v>78</v>
       </c>
@@ -1539,7 +1882,7 @@
       </c>
       <c r="E17" s="5"/>
     </row>
-    <row r="18" spans="1:5" ht="16" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
         <v>79</v>
       </c>
@@ -1554,7 +1897,7 @@
       </c>
       <c r="E18" s="3"/>
     </row>
-    <row r="19" spans="1:5" ht="16" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="9" t="s">
         <v>80</v>
       </c>
@@ -1569,7 +1912,7 @@
       </c>
       <c r="E19" s="5"/>
     </row>
-    <row r="20" spans="1:5" ht="16" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="9" t="s">
         <v>81</v>
       </c>
@@ -1584,7 +1927,7 @@
       </c>
       <c r="E20" s="3"/>
     </row>
-    <row r="21" spans="1:5" ht="16" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="9" t="s">
         <v>82</v>
       </c>
@@ -1599,7 +1942,7 @@
       </c>
       <c r="E21" s="5"/>
     </row>
-    <row r="22" spans="1:5" ht="16" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="9" t="s">
         <v>83</v>
       </c>
@@ -1614,7 +1957,7 @@
       </c>
       <c r="E22" s="3"/>
     </row>
-    <row r="23" spans="1:5" ht="16" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="9" t="s">
         <v>84</v>
       </c>
@@ -1629,7 +1972,7 @@
       </c>
       <c r="E23" s="3"/>
     </row>
-    <row r="24" spans="1:5" ht="16" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="9" t="s">
         <v>85</v>
       </c>
@@ -1644,7 +1987,7 @@
       </c>
       <c r="E24" s="3"/>
     </row>
-    <row r="25" spans="1:5" ht="16" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="9" t="s">
         <v>86</v>
       </c>
@@ -1659,7 +2002,7 @@
       </c>
       <c r="E25" s="5"/>
     </row>
-    <row r="26" spans="1:5" ht="16" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="9" t="s">
         <v>87</v>
       </c>
@@ -1674,7 +2017,7 @@
       </c>
       <c r="E26" s="3"/>
     </row>
-    <row r="27" spans="1:5" ht="16" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="9" t="s">
         <v>88</v>
       </c>
@@ -1689,7 +2032,7 @@
       </c>
       <c r="E27" s="3"/>
     </row>
-    <row r="28" spans="1:5" ht="16" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>89</v>
       </c>
@@ -1704,7 +2047,7 @@
       </c>
       <c r="E28" s="7"/>
     </row>
-    <row r="29" spans="1:5" ht="16" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>90</v>
       </c>
@@ -1719,7 +2062,7 @@
       </c>
       <c r="E29" s="3"/>
     </row>
-    <row r="30" spans="1:5" ht="16" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>91</v>
       </c>
@@ -1734,7 +2077,7 @@
       </c>
       <c r="E30" s="3"/>
     </row>
-    <row r="31" spans="1:5" ht="16" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>115</v>
       </c>
@@ -1749,7 +2092,7 @@
       </c>
       <c r="E31" s="3"/>
     </row>
-    <row r="32" spans="1:5" ht="16" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>116</v>
       </c>
@@ -1764,7 +2107,7 @@
       </c>
       <c r="E32" s="3"/>
     </row>
-    <row r="33" spans="1:5" ht="16" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>117</v>
       </c>
@@ -1779,7 +2122,7 @@
       </c>
       <c r="E33" s="3"/>
     </row>
-    <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>118</v>
       </c>
@@ -1794,7 +2137,7 @@
       </c>
       <c r="E34" s="3"/>
     </row>
-    <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>119</v>
       </c>
@@ -1809,7 +2152,7 @@
       </c>
       <c r="E35" s="3"/>
     </row>
-    <row r="36" spans="1:5" ht="16" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>120</v>
       </c>
@@ -1824,7 +2167,7 @@
       </c>
       <c r="E36" s="3"/>
     </row>
-    <row r="37" spans="1:5" ht="16" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>121</v>
       </c>
@@ -1839,7 +2182,7 @@
       </c>
       <c r="E37" s="3"/>
     </row>
-    <row r="38" spans="1:5" ht="16" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>122</v>
       </c>
@@ -1854,7 +2197,7 @@
       </c>
       <c r="E38" s="3"/>
     </row>
-    <row r="39" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>123</v>
       </c>
@@ -1869,7 +2212,7 @@
       </c>
       <c r="E39" s="3"/>
     </row>
-    <row r="40" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>124</v>
       </c>
@@ -1884,7 +2227,7 @@
       </c>
       <c r="E40" s="3"/>
     </row>
-    <row r="41" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>125</v>
       </c>
@@ -1899,7 +2242,7 @@
       </c>
       <c r="E41" s="3"/>
     </row>
-    <row r="42" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>126</v>
       </c>
@@ -1914,7 +2257,7 @@
       </c>
       <c r="E42" s="3"/>
     </row>
-    <row r="43" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>127</v>
       </c>
@@ -1929,7 +2272,7 @@
       </c>
       <c r="E43" s="3"/>
     </row>
-    <row r="44" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>128</v>
       </c>
@@ -1944,7 +2287,7 @@
       </c>
       <c r="E44" s="3"/>
     </row>
-    <row r="45" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>129</v>
       </c>
@@ -1959,7 +2302,7 @@
       </c>
       <c r="E45" s="3"/>
     </row>
-    <row r="46" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>130</v>
       </c>
@@ -1974,7 +2317,7 @@
       </c>
       <c r="E46" s="3"/>
     </row>
-    <row r="47" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
         <v>131</v>
       </c>
@@ -1989,7 +2332,7 @@
       </c>
       <c r="E47" s="3"/>
     </row>
-    <row r="48" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
         <v>132</v>
       </c>
@@ -2004,7 +2347,7 @@
       </c>
       <c r="E48" s="3"/>
     </row>
-    <row r="49" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
         <v>133</v>
       </c>
@@ -2019,7 +2362,7 @@
       </c>
       <c r="E49" s="3"/>
     </row>
-    <row r="50" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>156</v>
       </c>
@@ -2034,7 +2377,7 @@
       </c>
       <c r="E50" s="3"/>
     </row>
-    <row r="51" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
         <v>157</v>
       </c>
@@ -2049,7 +2392,7 @@
       </c>
       <c r="E51" s="3"/>
     </row>
-    <row r="52" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
         <v>158</v>
       </c>
@@ -2062,7 +2405,7 @@
       <c r="D52" s="3"/>
       <c r="E52" s="3"/>
     </row>
-    <row r="53" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
         <v>159</v>
       </c>
@@ -2075,7 +2418,7 @@
       <c r="D53" s="3"/>
       <c r="E53" s="3"/>
     </row>
-    <row r="54" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
         <v>160</v>
       </c>
@@ -2090,7 +2433,7 @@
       </c>
       <c r="E54" s="3"/>
     </row>
-    <row r="55" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
         <v>161</v>
       </c>
@@ -2105,7 +2448,7 @@
       </c>
       <c r="E55" s="3"/>
     </row>
-    <row r="56" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
         <v>162</v>
       </c>
@@ -2120,7 +2463,7 @@
       </c>
       <c r="E56" s="3"/>
     </row>
-    <row r="57" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
         <v>163</v>
       </c>
@@ -2135,7 +2478,7 @@
       </c>
       <c r="E57" s="3"/>
     </row>
-    <row r="58" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
         <v>164</v>
       </c>
@@ -2150,7 +2493,7 @@
       </c>
       <c r="E58" s="3"/>
     </row>
-    <row r="59" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
         <v>165</v>
       </c>
@@ -2165,7 +2508,7 @@
       </c>
       <c r="E59" s="3"/>
     </row>
-    <row r="60" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
         <v>166</v>
       </c>
@@ -2180,7 +2523,7 @@
       </c>
       <c r="E60" s="3"/>
     </row>
-    <row r="61" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
         <v>167</v>
       </c>
@@ -2195,7 +2538,7 @@
       </c>
       <c r="E61" s="3"/>
     </row>
-    <row r="62" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
         <v>168</v>
       </c>
@@ -2208,7 +2551,7 @@
       <c r="D62" s="3"/>
       <c r="E62" s="3"/>
     </row>
-    <row r="63" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
         <v>169</v>
       </c>
@@ -2221,20 +2564,694 @@
       <c r="D63" s="3"/>
       <c r="E63" s="3"/>
     </row>
-    <row r="64" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="B64" s="16">
+      <c r="B64" s="1">
         <v>14</v>
       </c>
-      <c r="C64" s="17" t="s">
+      <c r="C64" s="16" t="s">
         <v>171</v>
       </c>
       <c r="D64" s="15" t="s">
         <v>147</v>
       </c>
       <c r="E64" s="15"/>
+    </row>
+    <row r="65" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A65" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="B65" s="1">
+        <v>11</v>
+      </c>
+      <c r="C65" s="14" t="s">
+        <v>229</v>
+      </c>
+      <c r="D65" s="14" t="s">
+        <v>275</v>
+      </c>
+      <c r="E65" s="3"/>
+    </row>
+    <row r="66" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A66" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="B66" s="1">
+        <v>11</v>
+      </c>
+      <c r="C66" s="19" t="s">
+        <v>230</v>
+      </c>
+      <c r="D66" s="14" t="s">
+        <v>275</v>
+      </c>
+      <c r="E66" s="3"/>
+    </row>
+    <row r="67" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A67" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="B67" s="1">
+        <v>11</v>
+      </c>
+      <c r="C67" s="19" t="s">
+        <v>231</v>
+      </c>
+      <c r="D67" s="14" t="s">
+        <v>276</v>
+      </c>
+      <c r="E67" s="3"/>
+    </row>
+    <row r="68" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A68" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="B68" s="1">
+        <v>11</v>
+      </c>
+      <c r="C68" s="17" t="s">
+        <v>232</v>
+      </c>
+      <c r="D68" s="14" t="s">
+        <v>277</v>
+      </c>
+      <c r="E68" s="3"/>
+    </row>
+    <row r="69" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A69" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="B69" s="1">
+        <v>11</v>
+      </c>
+      <c r="C69" s="17" t="s">
+        <v>233</v>
+      </c>
+      <c r="D69" s="14" t="s">
+        <v>278</v>
+      </c>
+      <c r="E69" s="3"/>
+    </row>
+    <row r="70" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A70" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="B70" s="1">
+        <v>11</v>
+      </c>
+      <c r="C70" s="17" t="s">
+        <v>234</v>
+      </c>
+      <c r="D70" s="14" t="s">
+        <v>279</v>
+      </c>
+      <c r="E70" s="3"/>
+    </row>
+    <row r="71" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A71" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="B71" s="1">
+        <v>11</v>
+      </c>
+      <c r="C71" s="17" t="s">
+        <v>235</v>
+      </c>
+      <c r="D71" s="14" t="s">
+        <v>280</v>
+      </c>
+      <c r="E71" s="3"/>
+    </row>
+    <row r="72" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A72" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="B72" s="1">
+        <v>11</v>
+      </c>
+      <c r="C72" s="17" t="s">
+        <v>236</v>
+      </c>
+      <c r="D72" s="14"/>
+      <c r="E72" s="3"/>
+    </row>
+    <row r="73" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A73" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B73" s="1">
+        <v>11</v>
+      </c>
+      <c r="C73" s="18" t="s">
+        <v>237</v>
+      </c>
+      <c r="D73" s="14"/>
+      <c r="E73" s="3"/>
+    </row>
+    <row r="74" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A74" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="B74" s="1">
+        <v>11</v>
+      </c>
+      <c r="C74" s="17" t="s">
+        <v>238</v>
+      </c>
+      <c r="D74" s="14"/>
+      <c r="E74" s="3"/>
+    </row>
+    <row r="75" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A75" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="B75" s="1">
+        <v>11</v>
+      </c>
+      <c r="C75" s="17" t="s">
+        <v>239</v>
+      </c>
+      <c r="D75" s="14" t="s">
+        <v>281</v>
+      </c>
+      <c r="E75" s="3"/>
+    </row>
+    <row r="76" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A76" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="B76" s="1">
+        <v>11</v>
+      </c>
+      <c r="C76" s="17" t="s">
+        <v>240</v>
+      </c>
+      <c r="D76" s="14" t="s">
+        <v>282</v>
+      </c>
+      <c r="E76" s="3"/>
+    </row>
+    <row r="77" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A77" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="B77" s="1">
+        <v>11</v>
+      </c>
+      <c r="C77" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="D77" s="14"/>
+      <c r="E77" s="3"/>
+    </row>
+    <row r="78" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A78" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="B78" s="1">
+        <v>11</v>
+      </c>
+      <c r="C78" s="17" t="s">
+        <v>242</v>
+      </c>
+      <c r="D78" s="14" t="s">
+        <v>283</v>
+      </c>
+      <c r="E78" s="3"/>
+    </row>
+    <row r="79" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A79" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="B79" s="1">
+        <v>11</v>
+      </c>
+      <c r="C79" s="17" t="s">
+        <v>243</v>
+      </c>
+      <c r="D79" s="14" t="s">
+        <v>284</v>
+      </c>
+      <c r="E79" s="3"/>
+    </row>
+    <row r="80" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A80" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="B80" s="1">
+        <v>11</v>
+      </c>
+      <c r="C80" s="18" t="s">
+        <v>244</v>
+      </c>
+      <c r="D80" s="14" t="s">
+        <v>285</v>
+      </c>
+      <c r="E80" s="3"/>
+    </row>
+    <row r="81" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A81" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="B81" s="1">
+        <v>11</v>
+      </c>
+      <c r="C81" s="17" t="s">
+        <v>245</v>
+      </c>
+      <c r="D81" s="14" t="s">
+        <v>286</v>
+      </c>
+      <c r="E81" s="3"/>
+    </row>
+    <row r="82" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A82" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="B82" s="1">
+        <v>11</v>
+      </c>
+      <c r="C82" s="18" t="s">
+        <v>246</v>
+      </c>
+      <c r="D82" s="14" t="s">
+        <v>286</v>
+      </c>
+      <c r="E82" s="3"/>
+    </row>
+    <row r="83" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A83" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="B83" s="1">
+        <v>11</v>
+      </c>
+      <c r="C83" s="18" t="s">
+        <v>247</v>
+      </c>
+      <c r="D83" s="14" t="s">
+        <v>286</v>
+      </c>
+      <c r="E83" s="3"/>
+    </row>
+    <row r="84" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A84" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="B84" s="1">
+        <v>11</v>
+      </c>
+      <c r="C84" s="18" t="s">
+        <v>248</v>
+      </c>
+      <c r="D84" s="14" t="s">
+        <v>287</v>
+      </c>
+      <c r="E84" s="3"/>
+    </row>
+    <row r="85" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A85" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="B85" s="1">
+        <v>11</v>
+      </c>
+      <c r="C85" s="18" t="s">
+        <v>249</v>
+      </c>
+      <c r="D85" s="14" t="s">
+        <v>275</v>
+      </c>
+      <c r="E85" s="3"/>
+    </row>
+    <row r="86" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A86" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="B86" s="1">
+        <v>11</v>
+      </c>
+      <c r="C86" s="18" t="s">
+        <v>250</v>
+      </c>
+      <c r="D86" s="14" t="s">
+        <v>288</v>
+      </c>
+      <c r="E86" s="3"/>
+    </row>
+    <row r="87" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A87" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="B87" s="1">
+        <v>11</v>
+      </c>
+      <c r="C87" s="17" t="s">
+        <v>251</v>
+      </c>
+      <c r="D87" s="14" t="s">
+        <v>289</v>
+      </c>
+      <c r="E87" s="3"/>
+    </row>
+    <row r="88" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A88" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="B88" s="1">
+        <v>11</v>
+      </c>
+      <c r="C88" s="17" t="s">
+        <v>252</v>
+      </c>
+      <c r="D88" s="14" t="s">
+        <v>289</v>
+      </c>
+      <c r="E88" s="3"/>
+    </row>
+    <row r="89" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A89" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="B89" s="1">
+        <v>11</v>
+      </c>
+      <c r="C89" s="17" t="s">
+        <v>253</v>
+      </c>
+      <c r="D89" s="14" t="s">
+        <v>289</v>
+      </c>
+      <c r="E89" s="3"/>
+    </row>
+    <row r="90" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A90" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="B90" s="1">
+        <v>11</v>
+      </c>
+      <c r="C90" s="17" t="s">
+        <v>254</v>
+      </c>
+      <c r="D90" s="14" t="s">
+        <v>289</v>
+      </c>
+      <c r="E90" s="3"/>
+    </row>
+    <row r="91" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A91" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="B91" s="1">
+        <v>11</v>
+      </c>
+      <c r="C91" s="17" t="s">
+        <v>255</v>
+      </c>
+      <c r="D91" s="14" t="s">
+        <v>289</v>
+      </c>
+      <c r="E91" s="3"/>
+    </row>
+    <row r="92" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A92" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="B92" s="1">
+        <v>11</v>
+      </c>
+      <c r="C92" s="17" t="s">
+        <v>256</v>
+      </c>
+      <c r="D92" s="14" t="s">
+        <v>289</v>
+      </c>
+      <c r="E92" s="3"/>
+    </row>
+    <row r="93" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A93" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="B93" s="1">
+        <v>11</v>
+      </c>
+      <c r="C93" s="18" t="s">
+        <v>257</v>
+      </c>
+      <c r="D93" s="14"/>
+      <c r="E93" s="3"/>
+    </row>
+    <row r="94" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A94" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="B94" s="1">
+        <v>11</v>
+      </c>
+      <c r="C94" s="17" t="s">
+        <v>258</v>
+      </c>
+      <c r="D94" s="14"/>
+      <c r="E94" s="3"/>
+    </row>
+    <row r="95" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A95" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="B95" s="1">
+        <v>11</v>
+      </c>
+      <c r="C95" s="18" t="s">
+        <v>259</v>
+      </c>
+      <c r="D95" s="14" t="s">
+        <v>290</v>
+      </c>
+      <c r="E95" s="3"/>
+    </row>
+    <row r="96" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A96" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="B96" s="1">
+        <v>11</v>
+      </c>
+      <c r="C96" s="17" t="s">
+        <v>260</v>
+      </c>
+      <c r="D96" s="14" t="s">
+        <v>285</v>
+      </c>
+      <c r="E96" s="3"/>
+    </row>
+    <row r="97" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A97" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="B97" s="1">
+        <v>11</v>
+      </c>
+      <c r="C97" s="17" t="s">
+        <v>261</v>
+      </c>
+      <c r="D97" s="14" t="s">
+        <v>285</v>
+      </c>
+      <c r="E97" s="3"/>
+    </row>
+    <row r="98" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A98" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="B98" s="1">
+        <v>11</v>
+      </c>
+      <c r="C98" s="17" t="s">
+        <v>262</v>
+      </c>
+      <c r="D98" s="14"/>
+      <c r="E98" s="3"/>
+    </row>
+    <row r="99" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A99" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="B99" s="1">
+        <v>11</v>
+      </c>
+      <c r="C99" s="17" t="s">
+        <v>263</v>
+      </c>
+      <c r="D99" s="14" t="s">
+        <v>285</v>
+      </c>
+      <c r="E99" s="3"/>
+    </row>
+    <row r="100" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A100" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="B100" s="1">
+        <v>11</v>
+      </c>
+      <c r="C100" s="18" t="s">
+        <v>264</v>
+      </c>
+      <c r="D100" s="14" t="s">
+        <v>291</v>
+      </c>
+      <c r="E100" s="3"/>
+    </row>
+    <row r="101" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A101" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="B101" s="1">
+        <v>11</v>
+      </c>
+      <c r="C101" s="17" t="s">
+        <v>265</v>
+      </c>
+      <c r="D101" s="14" t="s">
+        <v>292</v>
+      </c>
+      <c r="E101" s="3"/>
+    </row>
+    <row r="102" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A102" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B102" s="1">
+        <v>11</v>
+      </c>
+      <c r="C102" s="17" t="s">
+        <v>266</v>
+      </c>
+      <c r="D102" s="14" t="s">
+        <v>292</v>
+      </c>
+      <c r="E102" s="3"/>
+    </row>
+    <row r="103" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A103" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="B103" s="1">
+        <v>11</v>
+      </c>
+      <c r="C103" s="18" t="s">
+        <v>267</v>
+      </c>
+      <c r="D103" s="14"/>
+      <c r="E103" s="3"/>
+    </row>
+    <row r="104" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A104" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="B104" s="1">
+        <v>11</v>
+      </c>
+      <c r="C104" s="17" t="s">
+        <v>268</v>
+      </c>
+      <c r="D104" s="14" t="s">
+        <v>293</v>
+      </c>
+      <c r="E104" s="3"/>
+    </row>
+    <row r="105" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A105" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="B105" s="1">
+        <v>11</v>
+      </c>
+      <c r="C105" s="17" t="s">
+        <v>269</v>
+      </c>
+      <c r="D105" s="14" t="s">
+        <v>293</v>
+      </c>
+      <c r="E105" s="3"/>
+    </row>
+    <row r="106" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A106" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="B106" s="1">
+        <v>11</v>
+      </c>
+      <c r="C106" s="17" t="s">
+        <v>270</v>
+      </c>
+      <c r="D106" s="14" t="s">
+        <v>293</v>
+      </c>
+      <c r="E106" s="3"/>
+    </row>
+    <row r="107" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A107" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="B107" s="1">
+        <v>11</v>
+      </c>
+      <c r="C107" s="17" t="s">
+        <v>271</v>
+      </c>
+      <c r="D107" s="14" t="s">
+        <v>292</v>
+      </c>
+      <c r="E107" s="3"/>
+    </row>
+    <row r="108" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A108" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="B108" s="1">
+        <v>11</v>
+      </c>
+      <c r="C108" s="17" t="s">
+        <v>272</v>
+      </c>
+      <c r="D108" s="14" t="s">
+        <v>293</v>
+      </c>
+      <c r="E108" s="3"/>
+    </row>
+    <row r="109" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A109" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="B109" s="1">
+        <v>11</v>
+      </c>
+      <c r="C109" s="17" t="s">
+        <v>273</v>
+      </c>
+      <c r="D109" s="14" t="s">
+        <v>293</v>
+      </c>
+      <c r="E109" s="3"/>
+    </row>
+    <row r="110" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A110" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="B110" s="1">
+        <v>11</v>
+      </c>
+      <c r="C110" s="17" t="s">
+        <v>274</v>
+      </c>
+      <c r="D110" s="14" t="s">
+        <v>293</v>
+      </c>
+      <c r="E110" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>

<commit_message>
Updated Requirements sheet to include group 24's requirements.
</commit_message>
<xml_diff>
--- a/FinalRequirements.xlsx
+++ b/FinalRequirements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10413"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raisatasnim/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lancey/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F108DAD8-348D-9842-BB6C-E59B2D17790B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCCB48FA-442C-4A44-9736-5B1E835893C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="332">
   <si>
     <t>Tested By</t>
   </si>
@@ -673,263 +673,377 @@
     <t>R090</t>
   </si>
   <si>
+    <t>R092</t>
+  </si>
+  <si>
+    <t>R093</t>
+  </si>
+  <si>
+    <t>R094</t>
+  </si>
+  <si>
+    <t>R095</t>
+  </si>
+  <si>
+    <t>R096</t>
+  </si>
+  <si>
+    <t>R097</t>
+  </si>
+  <si>
+    <t>R098</t>
+  </si>
+  <si>
+    <t>R099</t>
+  </si>
+  <si>
+    <t>R100</t>
+  </si>
+  <si>
+    <t>R101</t>
+  </si>
+  <si>
+    <t>R102</t>
+  </si>
+  <si>
+    <t>R103</t>
+  </si>
+  <si>
+    <t>R104</t>
+  </si>
+  <si>
+    <t>R105</t>
+  </si>
+  <si>
+    <t>R106</t>
+  </si>
+  <si>
+    <t>R107</t>
+  </si>
+  <si>
+    <t>R108</t>
+  </si>
+  <si>
+    <t>R109</t>
+  </si>
+  <si>
+    <t>The Game should have 8 x 8 array checkers board.</t>
+  </si>
+  <si>
+    <t>The board should display 24 checkers (12 red and 12 black) at the start of the game.</t>
+  </si>
+  <si>
+    <t>Pieces should be clearly distinguishable by color for two players.</t>
+  </si>
+  <si>
+    <t>The board should support different themes that players can choose from.</t>
+  </si>
+  <si>
+    <t>When a piece reaches the last row, it should become a King and be visually distinct.</t>
+  </si>
+  <si>
+    <t>Players should be able to move pieces by dragging and dropping.</t>
+  </si>
+  <si>
+    <t>The game should validate whether a move is legal, and prevent invalid moves.</t>
+  </si>
+  <si>
+    <t>The game should highlight valid moves when a piece is selected.</t>
+  </si>
+  <si>
+    <t>When it is not the player’s turn, their own pieces should be faded or unclickable, while the opponent's pieces are highlighted, and vice versa.</t>
+  </si>
+  <si>
+    <t>The game should track and display the number of pieces captured.</t>
+  </si>
+  <si>
+    <t>The game should indicate whose turn it is at all times.</t>
+  </si>
+  <si>
+    <t>The game should provide clear win/loss/draw notifications at the end of a match.</t>
+  </si>
+  <si>
+    <t>A move history should be maintained, allowing players to view previous game states.</t>
+  </si>
+  <si>
+    <t>The board should display a timer to track the duration of the game.</t>
+  </si>
+  <si>
+    <t>Players should have the option to restart the game after it ends.</t>
+  </si>
+  <si>
+    <t>The game should support username input and display for both players.</t>
+  </si>
+  <si>
+    <t>A sound effect should play when a piece is moved.</t>
+  </si>
+  <si>
+    <t>A distinct sound effect should play when a piece is kinged.</t>
+  </si>
+  <si>
+    <t>A different sound effect should play when a piece is captured.</t>
+  </si>
+  <si>
+    <t>Players should be able to toggle sound effects on or off.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diagonally placement for the checkers. </t>
+  </si>
+  <si>
+    <t>A sound effect should play at the beginning of a game</t>
+  </si>
+  <si>
+    <t>A sound effect should play when a game is won</t>
+  </si>
+  <si>
+    <t>A sound effect should play when a game is lost</t>
+  </si>
+  <si>
+    <t>A sound effect should play when a game is drawn</t>
+  </si>
+  <si>
+    <t>A sound effect should play when a player recieves a draw proposal</t>
+  </si>
+  <si>
+    <t>Players should be able to adjust the volume of sound effects.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The move history of the active game in play should in store in a linked list on the html alongside the turn order. On the main page there should be two buttons, one to go move backwards in the game history and another to go a move forward in the game history. </t>
+  </si>
+  <si>
+    <t>The move history of the game in play should be displayed in checkers notation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A move that is made by the player (Whether it would be dragged or clicked), will be sent to the page manager system for checking if the valid move is legal or not. </t>
+  </si>
+  <si>
+    <t>The usernames for each player (or bot) shall be recieved by the pagemanager</t>
+  </si>
+  <si>
+    <t>If a bot is in game, a unique tag shall be displayed for them, replacing where the ranking would normally be displayed.</t>
+  </si>
+  <si>
+    <t>For the themes, a hashmap shall be used for storage of themes</t>
+  </si>
+  <si>
+    <t>The ranking of each player shall be displayed by their username, this data will be recived from the page manager system</t>
+  </si>
+  <si>
+    <t>Once a move has been verified that it is legal or not via data from the page manager. The gameboard will update with the new positions, if the move was illegal the, the attempted to be moved piece will return to its previous position</t>
+  </si>
+  <si>
+    <t>There shall be a resignation button for when a player wishes to resign</t>
+  </si>
+  <si>
+    <t>Clicking the resignation button will require a second conformation click.</t>
+  </si>
+  <si>
+    <t>When a piece moves multiple times in a single turn, there shall be a small visual update delay between each move the moving piece captures during that turn.</t>
+  </si>
+  <si>
+    <t>Both proposing and accepting a draw will require a second conformation click when clicked.</t>
+  </si>
+  <si>
+    <t>When a player clicks the draw button, on or off their turn, the opposing player will be notified that they are being proposed a draw.</t>
+  </si>
+  <si>
+    <t>There shall be a draw button for when a player wishes to propose a draw</t>
+  </si>
+  <si>
+    <t>The game should automatically restart when a player resigns.</t>
+  </si>
+  <si>
+    <t>The game should automatically restart when a player ACCEPTS a proposed draw.</t>
+  </si>
+  <si>
+    <t>When a draw is proposed there will be a 10 second timer for the draw to be either confirmed or declined.</t>
+  </si>
+  <si>
+    <t>The recently moved piece should be highlighted briefly.</t>
+  </si>
+  <si>
+    <t>createBoard()</t>
+  </si>
+  <si>
+    <t>.red .blue</t>
+  </si>
+  <si>
+    <t>toggleTheme</t>
+  </si>
+  <si>
+    <t>executeValidMove(), .king</t>
+  </si>
+  <si>
+    <t>createPiece()</t>
+  </si>
+  <si>
+    <t>socket.send()</t>
+  </si>
+  <si>
+    <t>displayPlayerTurn()</t>
+  </si>
+  <si>
+    <t>displayEndState(endOfGameState), alert()</t>
+  </si>
+  <si>
+    <t>drawTimer()</t>
+  </si>
+  <si>
+    <t>location.reload()</t>
+  </si>
+  <si>
+    <t>getPlayerdata()</t>
+  </si>
+  <si>
+    <t>soundManager.playsound()</t>
+  </si>
+  <si>
+    <t>soundToggle()</t>
+  </si>
+  <si>
+    <t>soundManager.init()</t>
+  </si>
+  <si>
+    <t>soundsManager.playSound()</t>
+  </si>
+  <si>
+    <t>cell.addEventListener()</t>
+  </si>
+  <si>
+    <t>executeValidMove()</t>
+  </si>
+  <si>
+    <t>resignbtn</t>
+  </si>
+  <si>
+    <t>drawBtn</t>
+  </si>
+  <si>
+    <t>R110</t>
+  </si>
+  <si>
+    <t>R111</t>
+  </si>
+  <si>
+    <t>R112</t>
+  </si>
+  <si>
+    <t>R113</t>
+  </si>
+  <si>
+    <t>R114</t>
+  </si>
+  <si>
+    <t>R115</t>
+  </si>
+  <si>
+    <t>R116</t>
+  </si>
+  <si>
+    <t>R117</t>
+  </si>
+  <si>
+    <t>R118</t>
+  </si>
+  <si>
+    <t>R119</t>
+  </si>
+  <si>
+    <t>R120</t>
+  </si>
+  <si>
+    <t>R121</t>
+  </si>
+  <si>
+    <t>R122</t>
+  </si>
+  <si>
+    <t>R123</t>
+  </si>
+  <si>
+    <t>R124</t>
+  </si>
+  <si>
+    <t>Pieces shall not overlap each other.</t>
+  </si>
+  <si>
+    <t>Regular pieces shall become king pieces once they reach the opponents edge.</t>
+  </si>
+  <si>
+    <t>Normal Pieces shall only move towards the opponent.</t>
+  </si>
+  <si>
+    <t>King Pieces shall be able to move and capture both forward and backward.</t>
+  </si>
+  <si>
+    <t>Pieces shall only be on "dark" squares and within the bounds of the board.</t>
+  </si>
+  <si>
+    <t>Pieces shall not jump over or capture pieces of the same team.</t>
+  </si>
+  <si>
+    <t>The function shall send the updated table state to Game Termination if the move is valid.</t>
+  </si>
+  <si>
+    <t>The function shall return a boolean back to Game Manager.</t>
+  </si>
+  <si>
+    <t>The function shall receive current board state and the move being made from Game Manager.</t>
+  </si>
+  <si>
+    <t>A piece shall only capture an opponent's piece if it makes a diagonal move over the opponent’s piece to a free empty space.</t>
+  </si>
+  <si>
+    <t>The current board state's data structure the class will be receiving is a 2D integer array from Game Manager.</t>
+  </si>
+  <si>
+    <t>The class will receive the proposed move with an array of integers to hold the coordinates of the piece and where it will end up.</t>
+  </si>
+  <si>
+    <t>The class will include a function that receives a proposed move and return back if the move is diagonal from it's current position called isDiagonal()</t>
+  </si>
+  <si>
+    <t>The pieces shall only move diagonally.</t>
+  </si>
+  <si>
+    <t>The isDiagonal() function will verify whether a move is diagonal by comparing the coordinates of the "from" and "to" positions. It calculates the difference between their x and y values and checks that both differences are exactly ±1, indicating a valid diagonal step.</t>
+  </si>
+  <si>
+    <t>The isInBounds() function will check if the destination coordinates of a move are within the 8×8 board limits. It returns true if both x and y of the "to" position are between 0 and 7, inclusive.</t>
+  </si>
+  <si>
+    <t>GamePlay()</t>
+  </si>
+  <si>
+    <t>promotePiece()</t>
+  </si>
+  <si>
+    <t>isInBounds()</t>
+  </si>
+  <si>
+    <t>isSameTeam()</t>
+  </si>
+  <si>
+    <t>notifyTermination()</t>
+  </si>
+  <si>
+    <t>isValidMove()</t>
+  </si>
+  <si>
+    <t>isJump()</t>
+  </si>
+  <si>
+    <t>isDiagonal()</t>
+  </si>
+  <si>
     <t>R091</t>
-  </si>
-  <si>
-    <t>R092</t>
-  </si>
-  <si>
-    <t>R093</t>
-  </si>
-  <si>
-    <t>R094</t>
-  </si>
-  <si>
-    <t>R095</t>
-  </si>
-  <si>
-    <t>R096</t>
-  </si>
-  <si>
-    <t>R097</t>
-  </si>
-  <si>
-    <t>R098</t>
-  </si>
-  <si>
-    <t>R099</t>
-  </si>
-  <si>
-    <t>R100</t>
-  </si>
-  <si>
-    <t>R101</t>
-  </si>
-  <si>
-    <t>R102</t>
-  </si>
-  <si>
-    <t>R103</t>
-  </si>
-  <si>
-    <t>R104</t>
-  </si>
-  <si>
-    <t>R105</t>
-  </si>
-  <si>
-    <t>R106</t>
-  </si>
-  <si>
-    <t>R107</t>
-  </si>
-  <si>
-    <t>R108</t>
-  </si>
-  <si>
-    <t>R109</t>
-  </si>
-  <si>
-    <t>The Game should have 8 x 8 array checkers board.</t>
-  </si>
-  <si>
-    <t>The board should display 24 checkers (12 red and 12 black) at the start of the game.</t>
-  </si>
-  <si>
-    <t>Pieces should be clearly distinguishable by color for two players.</t>
-  </si>
-  <si>
-    <t>The board should support different themes that players can choose from.</t>
-  </si>
-  <si>
-    <t>When a piece reaches the last row, it should become a King and be visually distinct.</t>
-  </si>
-  <si>
-    <t>Players should be able to move pieces by dragging and dropping.</t>
-  </si>
-  <si>
-    <t>The game should validate whether a move is legal, and prevent invalid moves.</t>
-  </si>
-  <si>
-    <t>The game should highlight valid moves when a piece is selected.</t>
-  </si>
-  <si>
-    <t>When it is not the player’s turn, their own pieces should be faded or unclickable, while the opponent's pieces are highlighted, and vice versa.</t>
-  </si>
-  <si>
-    <t>The game should track and display the number of pieces captured.</t>
-  </si>
-  <si>
-    <t>The game should indicate whose turn it is at all times.</t>
-  </si>
-  <si>
-    <t>The game should provide clear win/loss/draw notifications at the end of a match.</t>
-  </si>
-  <si>
-    <t>A move history should be maintained, allowing players to view previous game states.</t>
-  </si>
-  <si>
-    <t>The board should display a timer to track the duration of the game.</t>
-  </si>
-  <si>
-    <t>Players should have the option to restart the game after it ends.</t>
-  </si>
-  <si>
-    <t>The game should support username input and display for both players.</t>
-  </si>
-  <si>
-    <t>A sound effect should play when a piece is moved.</t>
-  </si>
-  <si>
-    <t>A distinct sound effect should play when a piece is kinged.</t>
-  </si>
-  <si>
-    <t>A different sound effect should play when a piece is captured.</t>
-  </si>
-  <si>
-    <t>Players should be able to toggle sound effects on or off.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diagonally placement for the checkers. </t>
-  </si>
-  <si>
-    <t>A sound effect should play at the beginning of a game</t>
-  </si>
-  <si>
-    <t>A sound effect should play when a game is won</t>
-  </si>
-  <si>
-    <t>A sound effect should play when a game is lost</t>
-  </si>
-  <si>
-    <t>A sound effect should play when a game is drawn</t>
-  </si>
-  <si>
-    <t>A sound effect should play when a player recieves a draw proposal</t>
-  </si>
-  <si>
-    <t>Players should be able to adjust the volume of sound effects.</t>
-  </si>
-  <si>
-    <t>A sound effect should play when a piece is captured</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The move history of the active game in play should in store in a linked list on the html alongside the turn order. On the main page there should be two buttons, one to go move backwards in the game history and another to go a move forward in the game history. </t>
-  </si>
-  <si>
-    <t>The move history of the game in play should be displayed in checkers notation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A move that is made by the player (Whether it would be dragged or clicked), will be sent to the page manager system for checking if the valid move is legal or not. </t>
-  </si>
-  <si>
-    <t>The usernames for each player (or bot) shall be recieved by the pagemanager</t>
-  </si>
-  <si>
-    <t>If a bot is in game, a unique tag shall be displayed for them, replacing where the ranking would normally be displayed.</t>
-  </si>
-  <si>
-    <t>For the themes, a hashmap shall be used for storage of themes</t>
-  </si>
-  <si>
-    <t>The ranking of each player shall be displayed by their username, this data will be recived from the page manager system</t>
-  </si>
-  <si>
-    <t>Once a move has been verified that it is legal or not via data from the page manager. The gameboard will update with the new positions, if the move was illegal the, the attempted to be moved piece will return to its previous position</t>
-  </si>
-  <si>
-    <t>There shall be a resignation button for when a player wishes to resign</t>
-  </si>
-  <si>
-    <t>Clicking the resignation button will require a second conformation click.</t>
-  </si>
-  <si>
-    <t>When a piece moves multiple times in a single turn, there shall be a small visual update delay between each move the moving piece captures during that turn.</t>
-  </si>
-  <si>
-    <t>Both proposing and accepting a draw will require a second conformation click when clicked.</t>
-  </si>
-  <si>
-    <t>When a player clicks the draw button, on or off their turn, the opposing player will be notified that they are being proposed a draw.</t>
-  </si>
-  <si>
-    <t>There shall be a draw button for when a player wishes to propose a draw</t>
-  </si>
-  <si>
-    <t>The game should automatically restart when a player resigns.</t>
-  </si>
-  <si>
-    <t>The game should automatically restart when a player ACCEPTS a proposed draw.</t>
-  </si>
-  <si>
-    <t>When a draw is proposed there will be a 10 second timer for the draw to be either confirmed or declined.</t>
-  </si>
-  <si>
-    <t>The recently moved piece should be highlighted briefly.</t>
-  </si>
-  <si>
-    <t>createBoard()</t>
-  </si>
-  <si>
-    <t>.red .blue</t>
-  </si>
-  <si>
-    <t>toggleTheme</t>
-  </si>
-  <si>
-    <t>executeValidMove(), .king</t>
-  </si>
-  <si>
-    <t>createPiece()</t>
-  </si>
-  <si>
-    <t>socket.send()</t>
-  </si>
-  <si>
-    <t>displayPlayerTurn()</t>
-  </si>
-  <si>
-    <t>displayEndState(endOfGameState), alert()</t>
-  </si>
-  <si>
-    <t>drawTimer()</t>
-  </si>
-  <si>
-    <t>location.reload()</t>
-  </si>
-  <si>
-    <t>getPlayerdata()</t>
-  </si>
-  <si>
-    <t>soundManager.playsound()</t>
-  </si>
-  <si>
-    <t>soundToggle()</t>
-  </si>
-  <si>
-    <t>soundManager.init()</t>
-  </si>
-  <si>
-    <t>soundsManager.playSound()</t>
-  </si>
-  <si>
-    <t>cell.addEventListener()</t>
-  </si>
-  <si>
-    <t>executeValidMove()</t>
-  </si>
-  <si>
-    <t>resignbtn</t>
-  </si>
-  <si>
-    <t>drawBtn</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -973,6 +1087,11 @@
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Roboto"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1023,7 +1142,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1076,6 +1195,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1260,8 +1380,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BE40BDEB-2F06-144D-B216-1B597D73F842}" name="Table1" displayName="Table1" ref="A3:E110" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A3:E110" xr:uid="{BE40BDEB-2F06-144D-B216-1B597D73F842}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BE40BDEB-2F06-144D-B216-1B597D73F842}" name="Table1" displayName="Table1" ref="A3:E128" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A3:E128" xr:uid="{BE40BDEB-2F06-144D-B216-1B597D73F842}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{B21B0785-0173-D145-A443-FA0BA41EF992}" name="ID" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{F4BBF6E4-4A05-FE42-95C4-FED1ADB2E7EC}" name="Group" dataDxfId="3"/>
@@ -1590,16 +1710,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S110"/>
+  <dimension ref="A1:S128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="C72" sqref="C72"/>
+    <sheetView tabSelected="1" topLeftCell="A104" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C126" sqref="C126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="8" customWidth="1"/>
-    <col min="3" max="3" width="144.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="231" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="45.6640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="22.1640625" style="1" customWidth="1"/>
     <col min="6" max="6" width="16.5" bestFit="1" customWidth="1"/>
@@ -2032,7 +2152,7 @@
       </c>
       <c r="E27" s="3"/>
     </row>
-    <row r="28" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>89</v>
       </c>
@@ -2587,10 +2707,10 @@
         <v>11</v>
       </c>
       <c r="C65" s="14" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D65" s="14" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="E65" s="3"/>
     </row>
@@ -2602,10 +2722,10 @@
         <v>11</v>
       </c>
       <c r="C66" s="19" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D66" s="14" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="E66" s="3"/>
     </row>
@@ -2617,10 +2737,10 @@
         <v>11</v>
       </c>
       <c r="C67" s="19" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D67" s="14" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E67" s="3"/>
     </row>
@@ -2632,10 +2752,10 @@
         <v>11</v>
       </c>
       <c r="C68" s="17" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D68" s="14" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E68" s="3"/>
     </row>
@@ -2647,10 +2767,10 @@
         <v>11</v>
       </c>
       <c r="C69" s="17" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D69" s="14" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E69" s="3"/>
     </row>
@@ -2662,10 +2782,10 @@
         <v>11</v>
       </c>
       <c r="C70" s="17" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D70" s="14" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="E70" s="3"/>
     </row>
@@ -2677,10 +2797,10 @@
         <v>11</v>
       </c>
       <c r="C71" s="17" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D71" s="14" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="E71" s="3"/>
     </row>
@@ -2692,7 +2812,7 @@
         <v>11</v>
       </c>
       <c r="C72" s="17" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D72" s="14"/>
       <c r="E72" s="3"/>
@@ -2705,7 +2825,7 @@
         <v>11</v>
       </c>
       <c r="C73" s="18" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D73" s="14"/>
       <c r="E73" s="3"/>
@@ -2718,7 +2838,7 @@
         <v>11</v>
       </c>
       <c r="C74" s="17" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D74" s="14"/>
       <c r="E74" s="3"/>
@@ -2731,10 +2851,10 @@
         <v>11</v>
       </c>
       <c r="C75" s="17" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D75" s="14" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E75" s="3"/>
     </row>
@@ -2746,10 +2866,10 @@
         <v>11</v>
       </c>
       <c r="C76" s="17" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D76" s="14" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E76" s="3"/>
     </row>
@@ -2761,7 +2881,7 @@
         <v>11</v>
       </c>
       <c r="C77" s="17" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D77" s="14"/>
       <c r="E77" s="3"/>
@@ -2774,10 +2894,10 @@
         <v>11</v>
       </c>
       <c r="C78" s="17" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D78" s="14" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E78" s="3"/>
     </row>
@@ -2789,10 +2909,10 @@
         <v>11</v>
       </c>
       <c r="C79" s="17" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D79" s="14" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="E79" s="3"/>
     </row>
@@ -2804,10 +2924,10 @@
         <v>11</v>
       </c>
       <c r="C80" s="18" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D80" s="14" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E80" s="3"/>
     </row>
@@ -2819,10 +2939,10 @@
         <v>11</v>
       </c>
       <c r="C81" s="17" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D81" s="14" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E81" s="3"/>
     </row>
@@ -2834,10 +2954,10 @@
         <v>11</v>
       </c>
       <c r="C82" s="18" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D82" s="14" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E82" s="3"/>
     </row>
@@ -2849,10 +2969,10 @@
         <v>11</v>
       </c>
       <c r="C83" s="18" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D83" s="14" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E83" s="3"/>
     </row>
@@ -2864,10 +2984,10 @@
         <v>11</v>
       </c>
       <c r="C84" s="18" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D84" s="14" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="E84" s="3"/>
     </row>
@@ -2879,10 +2999,10 @@
         <v>11</v>
       </c>
       <c r="C85" s="18" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D85" s="14" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="E85" s="3"/>
     </row>
@@ -2894,10 +3014,10 @@
         <v>11</v>
       </c>
       <c r="C86" s="18" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D86" s="14" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E86" s="3"/>
     </row>
@@ -2909,10 +3029,10 @@
         <v>11</v>
       </c>
       <c r="C87" s="17" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D87" s="14" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E87" s="3"/>
     </row>
@@ -2924,10 +3044,10 @@
         <v>11</v>
       </c>
       <c r="C88" s="17" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D88" s="14" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E88" s="3"/>
     </row>
@@ -2939,10 +3059,10 @@
         <v>11</v>
       </c>
       <c r="C89" s="17" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D89" s="14" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E89" s="3"/>
     </row>
@@ -2954,10 +3074,10 @@
         <v>11</v>
       </c>
       <c r="C90" s="17" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D90" s="14" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E90" s="3"/>
     </row>
@@ -2969,289 +3089,535 @@
         <v>11</v>
       </c>
       <c r="C91" s="17" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D91" s="14" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E91" s="3"/>
     </row>
     <row r="92" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A92" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="B92" s="1">
+        <v>11</v>
+      </c>
+      <c r="C92" s="18" t="s">
+        <v>255</v>
+      </c>
+      <c r="D92" s="14"/>
+      <c r="E92" s="3"/>
+    </row>
+    <row r="93" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A93" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="B92" s="1">
-        <v>11</v>
-      </c>
-      <c r="C92" s="17" t="s">
+      <c r="B93" s="1">
+        <v>11</v>
+      </c>
+      <c r="C93" s="17" t="s">
         <v>256</v>
-      </c>
-      <c r="D92" s="14" t="s">
-        <v>289</v>
-      </c>
-      <c r="E92" s="3"/>
-    </row>
-    <row r="93" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A93" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="B93" s="1">
-        <v>11</v>
-      </c>
-      <c r="C93" s="18" t="s">
-        <v>257</v>
       </c>
       <c r="D93" s="14"/>
       <c r="E93" s="3"/>
     </row>
-    <row r="94" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A94" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B94" s="1">
         <v>11</v>
       </c>
-      <c r="C94" s="17" t="s">
-        <v>258</v>
-      </c>
-      <c r="D94" s="14"/>
+      <c r="C94" s="18" t="s">
+        <v>257</v>
+      </c>
+      <c r="D94" s="14" t="s">
+        <v>288</v>
+      </c>
       <c r="E94" s="3"/>
     </row>
     <row r="95" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A95" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B95" s="1">
         <v>11</v>
       </c>
-      <c r="C95" s="18" t="s">
-        <v>259</v>
+      <c r="C95" s="17" t="s">
+        <v>258</v>
       </c>
       <c r="D95" s="14" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="E95" s="3"/>
     </row>
     <row r="96" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A96" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="B96" s="1">
+        <v>11</v>
+      </c>
+      <c r="C96" s="17" t="s">
+        <v>259</v>
+      </c>
+      <c r="D96" s="14" t="s">
+        <v>283</v>
+      </c>
+      <c r="E96" s="3"/>
+    </row>
+    <row r="97" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A97" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="B96" s="1">
-        <v>11</v>
-      </c>
-      <c r="C96" s="17" t="s">
+      <c r="B97" s="1">
+        <v>11</v>
+      </c>
+      <c r="C97" s="17" t="s">
         <v>260</v>
       </c>
-      <c r="D96" s="14" t="s">
-        <v>285</v>
-      </c>
-      <c r="E96" s="3"/>
-    </row>
-    <row r="97" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A97" s="3" t="s">
+      <c r="D97" s="14"/>
+      <c r="E97" s="3"/>
+    </row>
+    <row r="98" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A98" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="B97" s="1">
-        <v>11</v>
-      </c>
-      <c r="C97" s="17" t="s">
+      <c r="B98" s="1">
+        <v>11</v>
+      </c>
+      <c r="C98" s="17" t="s">
         <v>261</v>
       </c>
-      <c r="D97" s="14" t="s">
-        <v>285</v>
-      </c>
-      <c r="E97" s="3"/>
-    </row>
-    <row r="98" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A98" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="B98" s="1">
-        <v>11</v>
-      </c>
-      <c r="C98" s="17" t="s">
-        <v>262</v>
-      </c>
-      <c r="D98" s="14"/>
+      <c r="D98" s="14" t="s">
+        <v>283</v>
+      </c>
       <c r="E98" s="3"/>
     </row>
     <row r="99" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A99" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="B99" s="1">
+        <v>11</v>
+      </c>
+      <c r="C99" s="18" t="s">
+        <v>262</v>
+      </c>
+      <c r="D99" s="14" t="s">
+        <v>289</v>
+      </c>
+      <c r="E99" s="3"/>
+    </row>
+    <row r="100" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A100" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="B99" s="1">
-        <v>11</v>
-      </c>
-      <c r="C99" s="17" t="s">
+      <c r="B100" s="1">
+        <v>11</v>
+      </c>
+      <c r="C100" s="17" t="s">
         <v>263</v>
       </c>
-      <c r="D99" s="14" t="s">
-        <v>285</v>
-      </c>
-      <c r="E99" s="3"/>
-    </row>
-    <row r="100" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A100" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="B100" s="1">
-        <v>11</v>
-      </c>
-      <c r="C100" s="18" t="s">
-        <v>264</v>
-      </c>
       <c r="D100" s="14" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E100" s="3"/>
     </row>
     <row r="101" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A101" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B101" s="1">
         <v>11</v>
       </c>
       <c r="C101" s="17" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D101" s="14" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="E101" s="3"/>
     </row>
     <row r="102" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A102" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B102" s="1">
         <v>11</v>
       </c>
-      <c r="C102" s="17" t="s">
-        <v>266</v>
-      </c>
-      <c r="D102" s="14" t="s">
-        <v>292</v>
-      </c>
+      <c r="C102" s="18" t="s">
+        <v>265</v>
+      </c>
+      <c r="D102" s="14"/>
       <c r="E102" s="3"/>
     </row>
     <row r="103" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A103" s="3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B103" s="1">
         <v>11</v>
       </c>
-      <c r="C103" s="18" t="s">
-        <v>267</v>
-      </c>
-      <c r="D103" s="14"/>
+      <c r="C103" s="17" t="s">
+        <v>266</v>
+      </c>
+      <c r="D103" s="14" t="s">
+        <v>291</v>
+      </c>
       <c r="E103" s="3"/>
     </row>
     <row r="104" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A104" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B104" s="1">
         <v>11</v>
       </c>
       <c r="C104" s="17" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D104" s="14" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="E104" s="3"/>
     </row>
     <row r="105" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A105" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B105" s="1">
         <v>11</v>
       </c>
       <c r="C105" s="17" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D105" s="14" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="E105" s="3"/>
     </row>
     <row r="106" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A106" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B106" s="1">
         <v>11</v>
       </c>
       <c r="C106" s="17" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D106" s="14" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="E106" s="3"/>
     </row>
     <row r="107" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A107" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B107" s="1">
         <v>11</v>
       </c>
       <c r="C107" s="17" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D107" s="14" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E107" s="3"/>
     </row>
     <row r="108" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A108" s="3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B108" s="1">
         <v>11</v>
       </c>
       <c r="C108" s="17" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D108" s="14" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="E108" s="3"/>
     </row>
     <row r="109" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A109" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="B109" s="1">
+        <v>11</v>
+      </c>
+      <c r="C109" s="17" t="s">
+        <v>272</v>
+      </c>
+      <c r="D109" s="14" t="s">
+        <v>291</v>
+      </c>
+      <c r="E109" s="3"/>
+    </row>
+    <row r="110" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A110" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="B109" s="1">
-        <v>11</v>
-      </c>
-      <c r="C109" s="17" t="s">
-        <v>273</v>
-      </c>
-      <c r="D109" s="14" t="s">
+      <c r="B110" s="1">
+        <v>24</v>
+      </c>
+      <c r="C110" s="13" t="s">
+        <v>307</v>
+      </c>
+      <c r="D110" s="20" t="s">
+        <v>323</v>
+      </c>
+      <c r="E110" s="3"/>
+    </row>
+    <row r="111" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A111" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="B111" s="1">
+        <v>24</v>
+      </c>
+      <c r="C111" s="13" t="s">
+        <v>308</v>
+      </c>
+      <c r="D111" s="20" t="s">
+        <v>324</v>
+      </c>
+      <c r="E111" s="3"/>
+    </row>
+    <row r="112" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A112" s="3" t="s">
         <v>293</v>
       </c>
-      <c r="E109" s="3"/>
-    </row>
-    <row r="110" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A110" s="3" t="s">
-        <v>228</v>
-      </c>
-      <c r="B110" s="1">
-        <v>11</v>
-      </c>
-      <c r="C110" s="17" t="s">
-        <v>274</v>
-      </c>
-      <c r="D110" s="14" t="s">
-        <v>293</v>
-      </c>
-      <c r="E110" s="3"/>
+      <c r="B112" s="1">
+        <v>24</v>
+      </c>
+      <c r="C112" s="13" t="s">
+        <v>309</v>
+      </c>
+      <c r="D112" s="20" t="s">
+        <v>323</v>
+      </c>
+      <c r="E112" s="3"/>
+    </row>
+    <row r="113" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A113" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="B113" s="1">
+        <v>24</v>
+      </c>
+      <c r="C113" s="13" t="s">
+        <v>310</v>
+      </c>
+      <c r="D113" s="20" t="s">
+        <v>323</v>
+      </c>
+      <c r="E113" s="3"/>
+    </row>
+    <row r="114" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A114" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="B114" s="1">
+        <v>24</v>
+      </c>
+      <c r="C114" s="13" t="s">
+        <v>311</v>
+      </c>
+      <c r="D114" s="20" t="s">
+        <v>325</v>
+      </c>
+      <c r="E114" s="3"/>
+    </row>
+    <row r="115" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A115" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="B115" s="1">
+        <v>24</v>
+      </c>
+      <c r="C115" s="13" t="s">
+        <v>312</v>
+      </c>
+      <c r="D115" s="20" t="s">
+        <v>326</v>
+      </c>
+      <c r="E115" s="3"/>
+    </row>
+    <row r="116" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A116" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="B116" s="1">
+        <v>24</v>
+      </c>
+      <c r="C116" s="13" t="s">
+        <v>313</v>
+      </c>
+      <c r="D116" s="20" t="s">
+        <v>327</v>
+      </c>
+      <c r="E116" s="3"/>
+    </row>
+    <row r="117" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A117" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="B117" s="1">
+        <v>24</v>
+      </c>
+      <c r="C117" s="13" t="s">
+        <v>314</v>
+      </c>
+      <c r="D117" s="20" t="s">
+        <v>328</v>
+      </c>
+      <c r="E117" s="3"/>
+    </row>
+    <row r="118" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A118" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="B118" s="1">
+        <v>24</v>
+      </c>
+      <c r="C118" s="13" t="s">
+        <v>315</v>
+      </c>
+      <c r="D118" s="20" t="s">
+        <v>323</v>
+      </c>
+      <c r="E118" s="3"/>
+    </row>
+    <row r="119" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A119" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="B119" s="1">
+        <v>24</v>
+      </c>
+      <c r="C119" s="13" t="s">
+        <v>316</v>
+      </c>
+      <c r="D119" s="20" t="s">
+        <v>329</v>
+      </c>
+      <c r="E119" s="3"/>
+    </row>
+    <row r="120" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A120" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="B120" s="1">
+        <v>24</v>
+      </c>
+      <c r="C120" s="13" t="s">
+        <v>317</v>
+      </c>
+      <c r="D120" s="20" t="s">
+        <v>323</v>
+      </c>
+      <c r="E120" s="3"/>
+    </row>
+    <row r="121" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A121" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="B121" s="1">
+        <v>24</v>
+      </c>
+      <c r="C121" s="13" t="s">
+        <v>318</v>
+      </c>
+      <c r="D121" s="20" t="s">
+        <v>323</v>
+      </c>
+      <c r="E121" s="3"/>
+    </row>
+    <row r="122" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A122" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="B122" s="1">
+        <v>24</v>
+      </c>
+      <c r="C122" s="13" t="s">
+        <v>319</v>
+      </c>
+      <c r="D122" s="20" t="s">
+        <v>330</v>
+      </c>
+      <c r="E122" s="3"/>
+    </row>
+    <row r="123" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A123" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="B123" s="1">
+        <v>24</v>
+      </c>
+      <c r="C123" s="13" t="s">
+        <v>320</v>
+      </c>
+      <c r="D123" s="20" t="s">
+        <v>330</v>
+      </c>
+      <c r="E123" s="3"/>
+    </row>
+    <row r="124" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A124" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="B124" s="1">
+        <v>24</v>
+      </c>
+      <c r="C124" s="13" t="s">
+        <v>321</v>
+      </c>
+      <c r="D124" s="20" t="s">
+        <v>330</v>
+      </c>
+      <c r="E124" s="3"/>
+    </row>
+    <row r="125" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A125" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="B125" s="1">
+        <v>24</v>
+      </c>
+      <c r="C125" s="13" t="s">
+        <v>322</v>
+      </c>
+      <c r="D125" s="20" t="s">
+        <v>325</v>
+      </c>
+      <c r="E125" s="3"/>
+    </row>
+    <row r="126" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A126" s="3"/>
+      <c r="B126" s="1"/>
+      <c r="C126" s="17"/>
+      <c r="D126" s="14"/>
+      <c r="E126" s="3"/>
+    </row>
+    <row r="127" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A127" s="3"/>
+      <c r="B127" s="1"/>
+      <c r="C127" s="17"/>
+      <c r="D127" s="14"/>
+      <c r="E127" s="3"/>
+    </row>
+    <row r="128" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A128" s="3"/>
+      <c r="B128" s="1"/>
+      <c r="C128" s="17"/>
+      <c r="D128" s="14"/>
+      <c r="E128" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>

<commit_message>
Updated Final Requirements Sheet with Game Manager Requirements
</commit_message>
<xml_diff>
--- a/FinalRequirements.xlsx
+++ b/FinalRequirements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kritazyaupreti/Desktop/UNIVERSITY/4th Sem/Fundamentals of Software Engineering/Project/cse3310-sp25-003/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\18173\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FB7FE55-53FF-1247-A199-61E39FDC85D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF1BB1AA-319E-498C-864A-0869A05EEA9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="-3100" windowWidth="37260" windowHeight="21100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="435">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="495">
   <si>
     <t>Tested By</t>
   </si>
@@ -1331,13 +1331,256 @@
   </si>
   <si>
     <t>R047</t>
+  </si>
+  <si>
+    <t>Must receive moves from page maneger or gameplay</t>
+  </si>
+  <si>
+    <t>Must vailidate each move played</t>
+  </si>
+  <si>
+    <t>Must update current state of the game</t>
+  </si>
+  <si>
+    <t>Manege multiple activies at once</t>
+  </si>
+  <si>
+    <t>Must store the sate of the game</t>
+  </si>
+  <si>
+    <t>Must Comparair each move with the rules of the game with Game play</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Must reject invalid moves </t>
+  </si>
+  <si>
+    <t>Log all moves made durning the with game play</t>
+  </si>
+  <si>
+    <t>Diplay log of the moves made in the game</t>
+  </si>
+  <si>
+    <t>Communicate with Page maneger, Bot 1 and bot 1, Pair up and Game play</t>
+  </si>
+  <si>
+    <t>Send moves to Bot1 and Bot 2</t>
+  </si>
+  <si>
+    <t>Page Manager should support retry logic for failed communications</t>
+  </si>
+  <si>
+    <t>Must return Java objects responses to calling modules</t>
+  </si>
+  <si>
+    <t>Setep up oour file in git hub to work properly</t>
+  </si>
+  <si>
+    <t>Share Player information with Pair up</t>
+  </si>
+  <si>
+    <t>Share GameSession,Position and Move with Game Play</t>
+  </si>
+  <si>
+    <t>Share Position,Move with Bot 1 and Bot 2</t>
+  </si>
+  <si>
+    <t>Share Position,Move,Session,Move and Player with Page maneger</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Must communicate with the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Pair Up</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> module to assign users to games</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Must route requests and responses to/from the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Game Play</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> module</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Must communicate with </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Bot 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> for automated player moves when required</t>
+    </r>
+  </si>
+  <si>
+    <t>R160</t>
+  </si>
+  <si>
+    <t>R161</t>
+  </si>
+  <si>
+    <t>R162</t>
+  </si>
+  <si>
+    <t>R163</t>
+  </si>
+  <si>
+    <t>R164</t>
+  </si>
+  <si>
+    <t>R165</t>
+  </si>
+  <si>
+    <t>R166</t>
+  </si>
+  <si>
+    <t>R167</t>
+  </si>
+  <si>
+    <t>R168</t>
+  </si>
+  <si>
+    <t>R169</t>
+  </si>
+  <si>
+    <t>R170</t>
+  </si>
+  <si>
+    <t>R171</t>
+  </si>
+  <si>
+    <t>R172</t>
+  </si>
+  <si>
+    <t>R173</t>
+  </si>
+  <si>
+    <t>R174</t>
+  </si>
+  <si>
+    <t>R175</t>
+  </si>
+  <si>
+    <t>R176</t>
+  </si>
+  <si>
+    <t>R177</t>
+  </si>
+  <si>
+    <t>R178</t>
+  </si>
+  <si>
+    <t>R179</t>
+  </si>
+  <si>
+    <t>R180</t>
+  </si>
+  <si>
+    <t>R181</t>
+  </si>
+  <si>
+    <t>Gamefile/Code.GameManager/Files</t>
+  </si>
+  <si>
+    <t>Gamefile/manager.GameManager / receiveMove()</t>
+  </si>
+  <si>
+    <t>Gamefile/rules.Gameplay / validateMove()</t>
+  </si>
+  <si>
+    <t>Gamefile/manager.GameManager / updateGameState()</t>
+  </si>
+  <si>
+    <t>Gamefile/manager.GameManager / manageSessions()</t>
+  </si>
+  <si>
+    <t>Gamefile/storage.GameStateStore / saveState()</t>
+  </si>
+  <si>
+    <t>Gamefile/rules.Gameplay / compareWithRules()</t>
+  </si>
+  <si>
+    <t>Gamefile/manager.GameManager / handleInvalidMove()</t>
+  </si>
+  <si>
+    <t>Gamefile/logging.GameLogger / logMove()</t>
+  </si>
+  <si>
+    <t>Gamefile/ui.MoveLogUI / displayLogs()</t>
+  </si>
+  <si>
+    <t>Gamefile/pairup.PairUp / sendToModule(String target)</t>
+  </si>
+  <si>
+    <t>Gamefile/bot.BotOne / sendMoveToBot(int botId)</t>
+  </si>
+  <si>
+    <t>Gamefile/page.PageManager / retryCommunication()</t>
+  </si>
+  <si>
+    <t>Gamefile/pairup.PairUp / assignPlayers()</t>
+  </si>
+  <si>
+    <t>Gamefile/play.GamePlay / routeToGamePlay()</t>
+  </si>
+  <si>
+    <t>Gamefile/bot.BotOne / getBotMove()</t>
+  </si>
+  <si>
+    <t>Gamefile/page.PageManager / generateResponse()</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1350,39 +1593,12 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-      <charset val="1"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Roboto"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Aptos"/>
     </font>
     <font>
       <i/>
@@ -1390,24 +1606,13 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-      <charset val="1"/>
     </font>
     <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1418,7 +1623,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -1441,149 +1646,230 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1597,14 +1883,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A3:E162" totalsRowShown="0">
-  <autoFilter ref="A3:E162" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A3:E184" totalsRowShown="0" dataDxfId="5">
+  <autoFilter ref="A3:E184" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Group"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Text"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Implemented In"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="UI XREF"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Group" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Text" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Implemented In" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="UI XREF" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1720,28 +2006,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S163"/>
+  <dimension ref="A1:S184"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
-      <selection activeCell="J146" sqref="J146"/>
+    <sheetView tabSelected="1" topLeftCell="A159" zoomScale="56" zoomScaleNormal="65" workbookViewId="0">
+      <selection activeCell="C167" sqref="C167"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="8" customWidth="1"/>
     <col min="3" max="3" width="231" customWidth="1"/>
-    <col min="4" max="4" width="45.6640625" customWidth="1"/>
-    <col min="5" max="5" width="22.1640625" customWidth="1"/>
-    <col min="6" max="6" width="16.5" customWidth="1"/>
-    <col min="19" max="19" width="36.5" customWidth="1"/>
+    <col min="4" max="4" width="64.54296875" customWidth="1"/>
+    <col min="5" max="5" width="22.1796875" customWidth="1"/>
+    <col min="6" max="6" width="16.453125" customWidth="1"/>
+    <col min="19" max="19" width="36.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
       <c r="K1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
       <c r="F2" t="s">
         <v>1</v>
       </c>
@@ -1779,7 +2065,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -1799,2378 +2085,2702 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="48" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="2">
         <v>10</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="5"/>
+      <c r="E4" s="4"/>
       <c r="S4" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="2">
         <v>10</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="5"/>
-    </row>
-    <row r="6" spans="1:19" ht="17" x14ac:dyDescent="0.2">
+      <c r="E5" s="4"/>
+    </row>
+    <row r="6" spans="1:19" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="2">
         <v>10</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="5"/>
-    </row>
-    <row r="7" spans="1:19" ht="17" x14ac:dyDescent="0.2">
+      <c r="E6" s="4"/>
+    </row>
+    <row r="7" spans="1:19" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="2">
         <v>10</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E7" s="6"/>
-    </row>
-    <row r="8" spans="1:19" ht="17" x14ac:dyDescent="0.2">
+      <c r="E7" s="4"/>
+    </row>
+    <row r="8" spans="1:19" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="2">
         <v>10</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="E8" s="5"/>
-    </row>
-    <row r="9" spans="1:19" ht="17" x14ac:dyDescent="0.2">
+      <c r="E8" s="4"/>
+    </row>
+    <row r="9" spans="1:19" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="2">
         <v>10</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="5"/>
-    </row>
-    <row r="10" spans="1:19" ht="17" x14ac:dyDescent="0.2">
+      <c r="E9" s="4"/>
+    </row>
+    <row r="10" spans="1:19" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="2">
         <v>10</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="E10" s="5"/>
-    </row>
-    <row r="11" spans="1:19" ht="17" x14ac:dyDescent="0.2">
+      <c r="E10" s="4"/>
+    </row>
+    <row r="11" spans="1:19" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="2">
         <v>10</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E11" s="7"/>
-    </row>
-    <row r="12" spans="1:19" ht="17" x14ac:dyDescent="0.2">
+      <c r="E11" s="4"/>
+    </row>
+    <row r="12" spans="1:19" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="2">
         <v>10</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="E12" s="5"/>
-    </row>
-    <row r="13" spans="1:19" ht="17" x14ac:dyDescent="0.2">
+      <c r="E12" s="4"/>
+    </row>
+    <row r="13" spans="1:19" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="2">
         <v>10</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="E13" s="7"/>
-    </row>
-    <row r="14" spans="1:19" ht="17" x14ac:dyDescent="0.2">
+      <c r="E13" s="4"/>
+    </row>
+    <row r="14" spans="1:19" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="2">
         <v>10</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="E14" s="5"/>
-    </row>
-    <row r="15" spans="1:19" ht="17" x14ac:dyDescent="0.2">
+      <c r="E14" s="4"/>
+    </row>
+    <row r="15" spans="1:19" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="2">
         <v>10</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E15" s="7"/>
-    </row>
-    <row r="16" spans="1:19" ht="17" x14ac:dyDescent="0.2">
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" spans="1:19" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B16" s="2">
         <v>10</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="E16" s="7"/>
-    </row>
-    <row r="17" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E16" s="4"/>
+    </row>
+    <row r="17" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B17" s="2">
         <v>10</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="E17" s="7"/>
-    </row>
-    <row r="18" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E17" s="4"/>
+    </row>
+    <row r="18" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B18" s="2">
         <v>10</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="E18" s="5"/>
-    </row>
-    <row r="19" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E18" s="4"/>
+    </row>
+    <row r="19" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B19" s="2">
         <v>10</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D19" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="E19" s="7"/>
-    </row>
-    <row r="20" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E19" s="4"/>
+    </row>
+    <row r="20" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B20" s="2">
         <v>10</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D20" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="E20" s="5"/>
-    </row>
-    <row r="21" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E20" s="4"/>
+    </row>
+    <row r="21" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B21" s="3">
+      <c r="B21" s="2">
         <v>10</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D21" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="E21" s="7"/>
-    </row>
-    <row r="22" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E21" s="4"/>
+    </row>
+    <row r="22" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B22" s="2">
         <v>10</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D22" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="E22" s="5"/>
-    </row>
-    <row r="23" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E22" s="4"/>
+    </row>
+    <row r="23" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B23" s="3">
+      <c r="B23" s="2">
         <v>10</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D23" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="E23" s="5"/>
-    </row>
-    <row r="24" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E23" s="4"/>
+    </row>
+    <row r="24" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B24" s="2">
         <v>10</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="D24" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="E24" s="5"/>
-    </row>
-    <row r="25" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E24" s="4"/>
+    </row>
+    <row r="25" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B25" s="3">
+      <c r="B25" s="2">
         <v>10</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C25" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="D25" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="E25" s="7"/>
-    </row>
-    <row r="26" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E25" s="4"/>
+    </row>
+    <row r="26" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B26" s="3">
+      <c r="B26" s="2">
         <v>10</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C26" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="D26" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="E26" s="5"/>
-    </row>
-    <row r="27" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E26" s="4"/>
+    </row>
+    <row r="27" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B27" s="3">
+      <c r="B27" s="2">
         <v>10</v>
       </c>
-      <c r="C27" s="8" t="s">
+      <c r="C27" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D27" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E27" s="5"/>
-    </row>
-    <row r="28" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A28" s="5" t="s">
+      <c r="E27" s="4"/>
+    </row>
+    <row r="28" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A28" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="B28" s="3">
+      <c r="B28" s="2">
         <v>10</v>
       </c>
-      <c r="C28" s="9" t="s">
+      <c r="C28" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="D28" s="10" t="s">
+      <c r="D28" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="E28" s="11"/>
-    </row>
-    <row r="29" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A29" s="5" t="s">
+      <c r="E28" s="4"/>
+    </row>
+    <row r="29" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A29" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="B29" s="3">
+      <c r="B29" s="2">
         <v>10</v>
       </c>
-      <c r="C29" s="12" t="s">
+      <c r="C29" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="D29" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="E29" s="5"/>
-    </row>
-    <row r="30" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A30" s="5" t="s">
+      <c r="E29" s="4"/>
+    </row>
+    <row r="30" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A30" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="B30" s="3">
+      <c r="B30" s="2">
         <v>10</v>
       </c>
-      <c r="C30" s="12" t="s">
+      <c r="C30" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="D30" s="5" t="s">
+      <c r="D30" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="E30" s="5"/>
-    </row>
-    <row r="31" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A31" s="30" t="s">
+      <c r="E30" s="4"/>
+    </row>
+    <row r="31" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A31" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B31" s="31">
+      <c r="B31" s="2">
         <v>10</v>
       </c>
-      <c r="C31" s="30" t="s">
+      <c r="C31" s="2" t="s">
         <v>431</v>
       </c>
-      <c r="D31" s="30" t="s">
+      <c r="D31" s="2" t="s">
         <v>432</v>
       </c>
-      <c r="E31" s="5"/>
-    </row>
-    <row r="32" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A32" s="30" t="s">
+      <c r="E31" s="4"/>
+    </row>
+    <row r="32" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A32" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="B32" s="3">
+      <c r="B32" s="2">
         <v>17</v>
       </c>
-      <c r="C32" s="13" t="s">
+      <c r="C32" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="D32" s="13" t="s">
+      <c r="D32" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="E32" s="5"/>
-    </row>
-    <row r="33" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A33" s="30" t="s">
+      <c r="E32" s="4"/>
+    </row>
+    <row r="33" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A33" s="2" t="s">
         <v>433</v>
       </c>
-      <c r="B33" s="3">
+      <c r="B33" s="2">
         <v>17</v>
       </c>
-      <c r="C33" s="13" t="s">
+      <c r="C33" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="D33" s="13" t="s">
+      <c r="D33" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="E33" s="5"/>
-    </row>
-    <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="30" t="s">
+      <c r="E33" s="4"/>
+    </row>
+    <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="B34" s="3">
+      <c r="B34" s="2">
         <v>17</v>
       </c>
-      <c r="C34" s="13" t="s">
+      <c r="C34" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="D34" s="13" t="s">
+      <c r="D34" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="E34" s="5"/>
-    </row>
-    <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="30" t="s">
+      <c r="E34" s="4"/>
+    </row>
+    <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B35" s="3">
+      <c r="B35" s="2">
         <v>17</v>
       </c>
-      <c r="C35" s="13" t="s">
+      <c r="C35" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D35" s="13" t="s">
+      <c r="D35" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="E35" s="5"/>
-    </row>
-    <row r="36" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A36" s="30" t="s">
+      <c r="E35" s="4"/>
+    </row>
+    <row r="36" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A36" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B36" s="3">
+      <c r="B36" s="2">
         <v>17</v>
       </c>
-      <c r="C36" s="13" t="s">
+      <c r="C36" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="D36" s="13" t="s">
+      <c r="D36" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="E36" s="5"/>
-    </row>
-    <row r="37" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A37" s="30" t="s">
+      <c r="E36" s="4"/>
+    </row>
+    <row r="37" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A37" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="B37" s="3">
+      <c r="B37" s="2">
         <v>17</v>
       </c>
-      <c r="C37" s="13" t="s">
+      <c r="C37" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D37" s="13" t="s">
+      <c r="D37" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="E37" s="5"/>
-    </row>
-    <row r="38" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A38" s="30" t="s">
+      <c r="E37" s="4"/>
+    </row>
+    <row r="38" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A38" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="B38" s="3">
+      <c r="B38" s="2">
         <v>17</v>
       </c>
-      <c r="C38" s="13" t="s">
+      <c r="C38" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="D38" s="13" t="s">
+      <c r="D38" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="E38" s="5"/>
-    </row>
-    <row r="39" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A39" s="30" t="s">
+      <c r="E38" s="4"/>
+    </row>
+    <row r="39" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A39" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="B39" s="3">
+      <c r="B39" s="2">
         <v>17</v>
       </c>
-      <c r="C39" s="13" t="s">
+      <c r="C39" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="D39" s="13" t="s">
+      <c r="D39" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="E39" s="5"/>
-    </row>
-    <row r="40" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A40" s="30" t="s">
+      <c r="E39" s="4"/>
+    </row>
+    <row r="40" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A40" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="B40">
+      <c r="B40" s="2">
         <v>17</v>
       </c>
-      <c r="C40" s="13" t="s">
+      <c r="C40" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="D40" s="13" t="s">
+      <c r="D40" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="E40" s="5"/>
-    </row>
-    <row r="41" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A41" s="30" t="s">
+      <c r="E40" s="4"/>
+    </row>
+    <row r="41" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A41" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="B41">
+      <c r="B41" s="2">
         <v>17</v>
       </c>
-      <c r="C41" s="13" t="s">
+      <c r="C41" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="D41" s="13" t="s">
+      <c r="D41" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="E41" s="5"/>
-    </row>
-    <row r="42" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A42" s="30" t="s">
+      <c r="E41" s="4"/>
+    </row>
+    <row r="42" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A42" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="B42">
+      <c r="B42" s="2">
         <v>17</v>
       </c>
-      <c r="C42" s="13" t="s">
+      <c r="C42" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="D42" s="13" t="s">
+      <c r="D42" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="E42" s="5"/>
-    </row>
-    <row r="43" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A43" s="30" t="s">
+      <c r="E42" s="4"/>
+    </row>
+    <row r="43" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A43" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B43">
+      <c r="B43" s="2">
         <v>17</v>
       </c>
-      <c r="C43" s="13" t="s">
+      <c r="C43" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="D43" s="13" t="s">
+      <c r="D43" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="E43" s="5"/>
-    </row>
-    <row r="44" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A44" s="30" t="s">
+      <c r="E43" s="4"/>
+    </row>
+    <row r="44" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A44" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="B44">
+      <c r="B44" s="2">
         <v>17</v>
       </c>
-      <c r="C44" s="13" t="s">
+      <c r="C44" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="D44" s="13" t="s">
+      <c r="D44" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="E44" s="5"/>
-    </row>
-    <row r="45" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A45" s="30" t="s">
+      <c r="E44" s="4"/>
+    </row>
+    <row r="45" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A45" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="B45">
+      <c r="B45" s="2">
         <v>17</v>
       </c>
-      <c r="C45" s="13" t="s">
+      <c r="C45" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="D45" s="13" t="s">
+      <c r="D45" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="E45" s="5"/>
-    </row>
-    <row r="46" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A46" s="30" t="s">
+      <c r="E45" s="4"/>
+    </row>
+    <row r="46" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A46" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="B46">
+      <c r="B46" s="2">
         <v>17</v>
       </c>
-      <c r="C46" s="13" t="s">
+      <c r="C46" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="D46" s="13" t="s">
+      <c r="D46" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="E46" s="5"/>
-    </row>
-    <row r="47" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A47" s="30" t="s">
+      <c r="E46" s="4"/>
+    </row>
+    <row r="47" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A47" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="B47">
+      <c r="B47" s="2">
         <v>17</v>
       </c>
-      <c r="C47" s="13" t="s">
+      <c r="C47" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="D47" s="13" t="s">
+      <c r="D47" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="E47" s="5"/>
-    </row>
-    <row r="48" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A48" s="30" t="s">
+      <c r="E47" s="4"/>
+    </row>
+    <row r="48" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A48" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="B48">
+      <c r="B48" s="2">
         <v>17</v>
       </c>
-      <c r="C48" s="13" t="s">
+      <c r="C48" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="D48" s="13" t="s">
+      <c r="D48" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="E48" s="5"/>
-    </row>
-    <row r="49" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A49" s="30" t="s">
+      <c r="E48" s="4"/>
+    </row>
+    <row r="49" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A49" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="B49">
+      <c r="B49" s="2">
         <v>17</v>
       </c>
-      <c r="C49" s="13" t="s">
+      <c r="C49" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="D49" s="13" t="s">
+      <c r="D49" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="E49" s="5"/>
-    </row>
-    <row r="50" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A50" s="30" t="s">
+      <c r="E49" s="4"/>
+    </row>
+    <row r="50" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+      <c r="A50" s="2" t="s">
         <v>434</v>
       </c>
-      <c r="B50">
+      <c r="B50" s="2">
         <v>17</v>
       </c>
-      <c r="C50" s="14" t="s">
+      <c r="C50" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="D50" s="13" t="s">
+      <c r="D50" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="E50" s="5"/>
-    </row>
-    <row r="51" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A51" s="30" t="s">
+      <c r="E50" s="4"/>
+    </row>
+    <row r="51" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A51" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="B51">
+      <c r="B51" s="2">
         <v>14</v>
       </c>
-      <c r="C51" s="12" t="s">
+      <c r="C51" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="D51" s="5" t="s">
+      <c r="D51" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="E51" s="5"/>
-    </row>
-    <row r="52" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A52" s="30" t="s">
+      <c r="E51" s="4"/>
+    </row>
+    <row r="52" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A52" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="B52">
+      <c r="B52" s="2">
         <v>14</v>
       </c>
-      <c r="C52" s="12" t="s">
+      <c r="C52" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="D52" s="5" t="s">
+      <c r="D52" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="E52" s="5"/>
-    </row>
-    <row r="53" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A53" s="30" t="s">
+      <c r="E52" s="4"/>
+    </row>
+    <row r="53" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A53" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="B53">
+      <c r="B53" s="2">
         <v>14</v>
       </c>
-      <c r="C53" s="12" t="s">
+      <c r="C53" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="D53" s="5"/>
-      <c r="E53" s="5"/>
-    </row>
-    <row r="54" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A54" s="30" t="s">
+      <c r="D53" s="4"/>
+      <c r="E53" s="4"/>
+    </row>
+    <row r="54" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A54" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="B54">
+      <c r="B54" s="2">
         <v>14</v>
       </c>
-      <c r="C54" s="12" t="s">
+      <c r="C54" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="D54" s="5"/>
-      <c r="E54" s="5"/>
-    </row>
-    <row r="55" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A55" s="30" t="s">
+      <c r="D54" s="4"/>
+      <c r="E54" s="4"/>
+    </row>
+    <row r="55" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A55" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="B55">
+      <c r="B55" s="2">
         <v>14</v>
       </c>
-      <c r="C55" s="12" t="s">
+      <c r="C55" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="D55" s="5" t="s">
+      <c r="D55" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="E55" s="5"/>
-    </row>
-    <row r="56" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A56" s="30" t="s">
+      <c r="E55" s="4"/>
+    </row>
+    <row r="56" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A56" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="B56">
+      <c r="B56" s="2">
         <v>14</v>
       </c>
-      <c r="C56" s="12" t="s">
+      <c r="C56" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="D56" s="5" t="s">
+      <c r="D56" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="E56" s="5"/>
-    </row>
-    <row r="57" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A57" s="30" t="s">
+      <c r="E56" s="4"/>
+    </row>
+    <row r="57" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A57" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="B57">
+      <c r="B57" s="2">
         <v>14</v>
       </c>
-      <c r="C57" s="12" t="s">
+      <c r="C57" s="7" t="s">
         <v>162</v>
       </c>
-      <c r="D57" s="5" t="s">
+      <c r="D57" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="E57" s="5"/>
-    </row>
-    <row r="58" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A58" s="30" t="s">
+      <c r="E57" s="4"/>
+    </row>
+    <row r="58" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A58" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="B58">
+      <c r="B58" s="2">
         <v>14</v>
       </c>
-      <c r="C58" s="12" t="s">
+      <c r="C58" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="D58" s="5" t="s">
+      <c r="D58" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="E58" s="5"/>
-    </row>
-    <row r="59" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A59" s="30" t="s">
+      <c r="E58" s="4"/>
+    </row>
+    <row r="59" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A59" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="B59">
+      <c r="B59" s="2">
         <v>14</v>
       </c>
-      <c r="C59" s="12" t="s">
+      <c r="C59" s="7" t="s">
         <v>168</v>
       </c>
-      <c r="D59" s="5" t="s">
+      <c r="D59" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="E59" s="5"/>
-    </row>
-    <row r="60" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A60" s="30" t="s">
+      <c r="E59" s="4"/>
+    </row>
+    <row r="60" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A60" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="B60">
+      <c r="B60" s="2">
         <v>14</v>
       </c>
-      <c r="C60" s="12" t="s">
+      <c r="C60" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="D60" s="5" t="s">
+      <c r="D60" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="E60" s="5"/>
-    </row>
-    <row r="61" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A61" s="30" t="s">
+      <c r="E60" s="4"/>
+    </row>
+    <row r="61" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A61" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="B61">
+      <c r="B61" s="2">
         <v>14</v>
       </c>
-      <c r="C61" s="12" t="s">
+      <c r="C61" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="D61" s="5" t="s">
+      <c r="D61" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="E61" s="5"/>
-    </row>
-    <row r="62" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A62" s="30" t="s">
+      <c r="E61" s="4"/>
+    </row>
+    <row r="62" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A62" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="B62">
+      <c r="B62" s="2">
         <v>14</v>
       </c>
-      <c r="C62" s="12" t="s">
+      <c r="C62" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="D62" s="5" t="s">
+      <c r="D62" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="E62" s="5"/>
-    </row>
-    <row r="63" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A63" s="30" t="s">
+      <c r="E62" s="4"/>
+    </row>
+    <row r="63" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A63" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="B63">
+      <c r="B63" s="2">
         <v>14</v>
       </c>
-      <c r="C63" s="12" t="s">
+      <c r="C63" s="7" t="s">
         <v>178</v>
       </c>
-      <c r="D63" s="5"/>
-      <c r="E63" s="5"/>
-    </row>
-    <row r="64" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A64" s="30" t="s">
+      <c r="D63" s="4"/>
+      <c r="E63" s="4"/>
+    </row>
+    <row r="64" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A64" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="B64">
+      <c r="B64" s="2">
         <v>14</v>
       </c>
-      <c r="C64" s="12" t="s">
+      <c r="C64" s="7" t="s">
         <v>180</v>
       </c>
-      <c r="D64" s="5"/>
-      <c r="E64" s="5"/>
-    </row>
-    <row r="65" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A65" s="30" t="s">
+      <c r="D64" s="4"/>
+      <c r="E64" s="4"/>
+    </row>
+    <row r="65" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A65" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="B65">
+      <c r="B65" s="2">
         <v>14</v>
       </c>
-      <c r="C65" s="15" t="s">
+      <c r="C65" s="7" t="s">
         <v>182</v>
       </c>
-      <c r="D65" s="16" t="s">
+      <c r="D65" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="E65" s="16"/>
-    </row>
-    <row r="66" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A66" s="30" t="s">
+      <c r="E65" s="4"/>
+    </row>
+    <row r="66" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A66" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="B66">
+      <c r="B66" s="2">
         <v>11</v>
       </c>
-      <c r="C66" s="14" t="s">
+      <c r="C66" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="D66" s="14" t="s">
+      <c r="D66" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="E66" s="5"/>
-    </row>
-    <row r="67" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A67" s="30" t="s">
+      <c r="E66" s="4"/>
+    </row>
+    <row r="67" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A67" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="B67">
+      <c r="B67" s="2">
         <v>11</v>
       </c>
-      <c r="C67" s="17" t="s">
+      <c r="C67" s="9" t="s">
         <v>187</v>
       </c>
-      <c r="D67" s="14" t="s">
+      <c r="D67" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="E67" s="5"/>
-    </row>
-    <row r="68" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A68" s="30" t="s">
+      <c r="E67" s="4"/>
+    </row>
+    <row r="68" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A68" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="B68">
+      <c r="B68" s="2">
         <v>11</v>
       </c>
-      <c r="C68" s="17" t="s">
+      <c r="C68" s="9" t="s">
         <v>189</v>
       </c>
-      <c r="D68" s="14" t="s">
+      <c r="D68" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="E68" s="5"/>
-    </row>
-    <row r="69" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A69" s="30" t="s">
+      <c r="E68" s="4"/>
+    </row>
+    <row r="69" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A69" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="B69">
+      <c r="B69" s="2">
         <v>11</v>
       </c>
-      <c r="C69" s="13" t="s">
+      <c r="C69" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="D69" s="14" t="s">
+      <c r="D69" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="E69" s="5"/>
-    </row>
-    <row r="70" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A70" s="30" t="s">
+      <c r="E69" s="4"/>
+    </row>
+    <row r="70" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A70" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="B70">
+      <c r="B70" s="2">
         <v>11</v>
       </c>
-      <c r="C70" s="13" t="s">
+      <c r="C70" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="D70" s="14" t="s">
+      <c r="D70" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="E70" s="5"/>
-    </row>
-    <row r="71" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A71" s="30" t="s">
+      <c r="E70" s="4"/>
+    </row>
+    <row r="71" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A71" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="B71">
+      <c r="B71" s="2">
         <v>11</v>
       </c>
-      <c r="C71" s="13" t="s">
+      <c r="C71" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="D71" s="14" t="s">
+      <c r="D71" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="E71" s="5"/>
-    </row>
-    <row r="72" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A72" s="30" t="s">
+      <c r="E71" s="4"/>
+    </row>
+    <row r="72" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A72" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="B72">
+      <c r="B72" s="2">
         <v>11</v>
       </c>
-      <c r="C72" s="13" t="s">
+      <c r="C72" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="D72" s="14" t="s">
+      <c r="D72" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="E72" s="5"/>
-    </row>
-    <row r="73" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A73" s="30" t="s">
+      <c r="E72" s="4"/>
+    </row>
+    <row r="73" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A73" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="B73">
+      <c r="B73" s="2">
         <v>11</v>
       </c>
-      <c r="C73" s="13" t="s">
+      <c r="C73" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="D73" s="14"/>
-      <c r="E73" s="5"/>
-    </row>
-    <row r="74" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A74" s="30" t="s">
+      <c r="D73" s="3"/>
+      <c r="E73" s="4"/>
+    </row>
+    <row r="74" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A74" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="B74">
+      <c r="B74" s="2">
         <v>11</v>
       </c>
-      <c r="C74" s="14" t="s">
+      <c r="C74" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="D74" s="14"/>
-      <c r="E74" s="5"/>
-    </row>
-    <row r="75" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A75" s="30" t="s">
+      <c r="D74" s="3"/>
+      <c r="E74" s="4"/>
+    </row>
+    <row r="75" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A75" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="B75">
+      <c r="B75" s="2">
         <v>11</v>
       </c>
-      <c r="C75" s="13" t="s">
+      <c r="C75" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="D75" s="14"/>
-      <c r="E75" s="5"/>
-    </row>
-    <row r="76" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A76" s="30" t="s">
+      <c r="D75" s="3"/>
+      <c r="E75" s="4"/>
+    </row>
+    <row r="76" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A76" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="B76">
+      <c r="B76" s="2">
         <v>11</v>
       </c>
-      <c r="C76" s="13" t="s">
+      <c r="C76" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="D76" s="14" t="s">
+      <c r="D76" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="E76" s="5"/>
-    </row>
-    <row r="77" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A77" s="30" t="s">
+      <c r="E76" s="4"/>
+    </row>
+    <row r="77" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A77" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="B77">
+      <c r="B77" s="2">
         <v>11</v>
       </c>
-      <c r="C77" s="13" t="s">
+      <c r="C77" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="D77" s="14" t="s">
+      <c r="D77" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="E77" s="5"/>
-    </row>
-    <row r="78" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A78" s="30" t="s">
+      <c r="E77" s="4"/>
+    </row>
+    <row r="78" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A78" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="B78">
+      <c r="B78" s="2">
         <v>11</v>
       </c>
-      <c r="C78" s="13" t="s">
+      <c r="C78" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="D78" s="14"/>
-      <c r="E78" s="5"/>
-    </row>
-    <row r="79" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A79" s="30" t="s">
+      <c r="D78" s="3"/>
+      <c r="E78" s="4"/>
+    </row>
+    <row r="79" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A79" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="B79">
+      <c r="B79" s="2">
         <v>11</v>
       </c>
-      <c r="C79" s="13" t="s">
+      <c r="C79" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="D79" s="14" t="s">
+      <c r="D79" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="E79" s="5"/>
-    </row>
-    <row r="80" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A80" s="30" t="s">
+      <c r="E79" s="4"/>
+    </row>
+    <row r="80" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A80" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="B80">
+      <c r="B80" s="2">
         <v>11</v>
       </c>
-      <c r="C80" s="13" t="s">
+      <c r="C80" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="D80" s="14" t="s">
+      <c r="D80" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="E80" s="5"/>
-    </row>
-    <row r="81" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A81" s="30" t="s">
+      <c r="E80" s="4"/>
+    </row>
+    <row r="81" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A81" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="B81">
+      <c r="B81" s="2">
         <v>11</v>
       </c>
-      <c r="C81" s="14" t="s">
+      <c r="C81" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="D81" s="14" t="s">
+      <c r="D81" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="E81" s="5"/>
-    </row>
-    <row r="82" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A82" s="30" t="s">
+      <c r="E81" s="4"/>
+    </row>
+    <row r="82" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A82" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="B82">
+      <c r="B82" s="2">
         <v>11</v>
       </c>
-      <c r="C82" s="13" t="s">
+      <c r="C82" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="D82" s="14" t="s">
+      <c r="D82" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="E82" s="5"/>
-    </row>
-    <row r="83" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A83" s="30" t="s">
+      <c r="E82" s="4"/>
+    </row>
+    <row r="83" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A83" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="B83">
+      <c r="B83" s="2">
         <v>11</v>
       </c>
-      <c r="C83" s="14" t="s">
+      <c r="C83" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="D83" s="14" t="s">
+      <c r="D83" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="E83" s="5"/>
-    </row>
-    <row r="84" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A84" s="30" t="s">
+      <c r="E83" s="4"/>
+    </row>
+    <row r="84" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A84" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="B84">
+      <c r="B84" s="2">
         <v>11</v>
       </c>
-      <c r="C84" s="14" t="s">
+      <c r="C84" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="D84" s="14" t="s">
+      <c r="D84" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="E84" s="5"/>
-    </row>
-    <row r="85" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A85" s="30" t="s">
+      <c r="E84" s="4"/>
+    </row>
+    <row r="85" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A85" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="B85">
+      <c r="B85" s="2">
         <v>11</v>
       </c>
-      <c r="C85" s="14" t="s">
+      <c r="C85" s="3" t="s">
         <v>234</v>
       </c>
-      <c r="D85" s="14" t="s">
+      <c r="D85" s="3" t="s">
         <v>235</v>
       </c>
-      <c r="E85" s="5"/>
-    </row>
-    <row r="86" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A86" s="30" t="s">
+      <c r="E85" s="4"/>
+    </row>
+    <row r="86" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A86" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="B86">
+      <c r="B86" s="2">
         <v>11</v>
       </c>
-      <c r="C86" s="14" t="s">
+      <c r="C86" s="3" t="s">
         <v>237</v>
       </c>
-      <c r="D86" s="14" t="s">
+      <c r="D86" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="E86" s="5"/>
-    </row>
-    <row r="87" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A87" s="30" t="s">
+      <c r="E86" s="4"/>
+    </row>
+    <row r="87" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A87" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="B87">
+      <c r="B87" s="2">
         <v>11</v>
       </c>
-      <c r="C87" s="14" t="s">
+      <c r="C87" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="D87" s="14" t="s">
+      <c r="D87" s="3" t="s">
         <v>240</v>
       </c>
-      <c r="E87" s="5"/>
-    </row>
-    <row r="88" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A88" s="30" t="s">
+      <c r="E87" s="4"/>
+    </row>
+    <row r="88" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A88" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="B88">
+      <c r="B88" s="2">
         <v>11</v>
       </c>
-      <c r="C88" s="13" t="s">
+      <c r="C88" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="D88" s="14" t="s">
+      <c r="D88" s="3" t="s">
         <v>243</v>
       </c>
-      <c r="E88" s="5"/>
-    </row>
-    <row r="89" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A89" s="30" t="s">
+      <c r="E88" s="4"/>
+    </row>
+    <row r="89" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A89" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="B89">
+      <c r="B89" s="2">
         <v>11</v>
       </c>
-      <c r="C89" s="13" t="s">
+      <c r="C89" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="D89" s="14" t="s">
+      <c r="D89" s="3" t="s">
         <v>243</v>
       </c>
-      <c r="E89" s="5"/>
-    </row>
-    <row r="90" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A90" s="30" t="s">
+      <c r="E89" s="4"/>
+    </row>
+    <row r="90" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A90" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="B90">
+      <c r="B90" s="2">
         <v>11</v>
       </c>
-      <c r="C90" s="13" t="s">
+      <c r="C90" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="D90" s="14" t="s">
+      <c r="D90" s="3" t="s">
         <v>243</v>
       </c>
-      <c r="E90" s="5"/>
-    </row>
-    <row r="91" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A91" s="30" t="s">
+      <c r="E90" s="4"/>
+    </row>
+    <row r="91" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A91" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="B91">
+      <c r="B91" s="2">
         <v>11</v>
       </c>
-      <c r="C91" s="13" t="s">
+      <c r="C91" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="D91" s="14" t="s">
+      <c r="D91" s="3" t="s">
         <v>243</v>
       </c>
-      <c r="E91" s="5"/>
-    </row>
-    <row r="92" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A92" s="30" t="s">
+      <c r="E91" s="4"/>
+    </row>
+    <row r="92" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A92" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="B92">
+      <c r="B92" s="2">
         <v>11</v>
       </c>
-      <c r="C92" s="13" t="s">
+      <c r="C92" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="D92" s="14" t="s">
+      <c r="D92" s="3" t="s">
         <v>243</v>
       </c>
-      <c r="E92" s="5"/>
-    </row>
-    <row r="93" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A93" s="30" t="s">
+      <c r="E92" s="4"/>
+    </row>
+    <row r="93" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+      <c r="A93" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="B93">
+      <c r="B93" s="2">
         <v>11</v>
       </c>
-      <c r="C93" s="14" t="s">
+      <c r="C93" s="3" t="s">
         <v>253</v>
       </c>
-      <c r="D93" s="14"/>
-      <c r="E93" s="5"/>
-    </row>
-    <row r="94" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A94" s="30" t="s">
+      <c r="D93" s="3"/>
+      <c r="E93" s="4"/>
+    </row>
+    <row r="94" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A94" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="B94">
+      <c r="B94" s="2">
         <v>11</v>
       </c>
-      <c r="C94" s="13" t="s">
+      <c r="C94" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="D94" s="14"/>
-      <c r="E94" s="5"/>
-    </row>
-    <row r="95" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A95" s="30" t="s">
+      <c r="D94" s="3"/>
+      <c r="E94" s="4"/>
+    </row>
+    <row r="95" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A95" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="B95">
+      <c r="B95" s="2">
         <v>11</v>
       </c>
-      <c r="C95" s="14" t="s">
+      <c r="C95" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="D95" s="14" t="s">
+      <c r="D95" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="E95" s="5"/>
-    </row>
-    <row r="96" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A96" s="30" t="s">
+      <c r="E95" s="4"/>
+    </row>
+    <row r="96" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A96" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="B96">
+      <c r="B96" s="2">
         <v>11</v>
       </c>
-      <c r="C96" s="13" t="s">
+      <c r="C96" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="D96" s="14" t="s">
+      <c r="D96" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="E96" s="5"/>
-    </row>
-    <row r="97" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A97" s="30" t="s">
+      <c r="E96" s="4"/>
+    </row>
+    <row r="97" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A97" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="B97">
+      <c r="B97" s="2">
         <v>11</v>
       </c>
-      <c r="C97" s="13" t="s">
+      <c r="C97" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="D97" s="14" t="s">
+      <c r="D97" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="E97" s="5"/>
-    </row>
-    <row r="98" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A98" s="30" t="s">
+      <c r="E97" s="4"/>
+    </row>
+    <row r="98" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A98" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="B98">
+      <c r="B98" s="2">
         <v>11</v>
       </c>
-      <c r="C98" s="13" t="s">
+      <c r="C98" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="D98" s="14"/>
-      <c r="E98" s="5"/>
-    </row>
-    <row r="99" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A99" s="30" t="s">
+      <c r="D98" s="3"/>
+      <c r="E98" s="4"/>
+    </row>
+    <row r="99" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A99" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="B99">
+      <c r="B99" s="2">
         <v>11</v>
       </c>
-      <c r="C99" s="13" t="s">
+      <c r="C99" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="D99" s="14" t="s">
+      <c r="D99" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="E99" s="5"/>
-    </row>
-    <row r="100" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A100" s="30" t="s">
+      <c r="E99" s="4"/>
+    </row>
+    <row r="100" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A100" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="B100">
+      <c r="B100" s="2">
         <v>11</v>
       </c>
-      <c r="C100" s="14" t="s">
+      <c r="C100" s="3" t="s">
         <v>268</v>
       </c>
-      <c r="D100" s="14" t="s">
+      <c r="D100" s="3" t="s">
         <v>269</v>
       </c>
-      <c r="E100" s="5"/>
-    </row>
-    <row r="101" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A101" s="30" t="s">
+      <c r="E100" s="4"/>
+    </row>
+    <row r="101" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A101" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="B101">
+      <c r="B101" s="2">
         <v>11</v>
       </c>
-      <c r="C101" s="13" t="s">
+      <c r="C101" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="D101" s="14" t="s">
+      <c r="D101" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="E101" s="5"/>
-    </row>
-    <row r="102" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A102" s="30" t="s">
+      <c r="E101" s="4"/>
+    </row>
+    <row r="102" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A102" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="B102">
+      <c r="B102" s="2">
         <v>11</v>
       </c>
-      <c r="C102" s="13" t="s">
+      <c r="C102" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="D102" s="14" t="s">
+      <c r="D102" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="E102" s="5"/>
-    </row>
-    <row r="103" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A103" s="30" t="s">
+      <c r="E102" s="4"/>
+    </row>
+    <row r="103" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A103" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="B103">
+      <c r="B103" s="2">
         <v>11</v>
       </c>
-      <c r="C103" s="14" t="s">
+      <c r="C103" s="3" t="s">
         <v>276</v>
       </c>
-      <c r="D103" s="14"/>
-      <c r="E103" s="5"/>
-    </row>
-    <row r="104" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A104" s="30" t="s">
+      <c r="D103" s="3"/>
+      <c r="E103" s="4"/>
+    </row>
+    <row r="104" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A104" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="B104">
+      <c r="B104" s="2">
         <v>11</v>
       </c>
-      <c r="C104" s="13" t="s">
+      <c r="C104" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="D104" s="14" t="s">
+      <c r="D104" s="3" t="s">
         <v>279</v>
       </c>
-      <c r="E104" s="5"/>
-    </row>
-    <row r="105" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A105" s="30" t="s">
+      <c r="E104" s="4"/>
+    </row>
+    <row r="105" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A105" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="B105">
+      <c r="B105" s="2">
         <v>11</v>
       </c>
-      <c r="C105" s="13" t="s">
+      <c r="C105" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="D105" s="14" t="s">
+      <c r="D105" s="3" t="s">
         <v>279</v>
       </c>
-      <c r="E105" s="5"/>
-    </row>
-    <row r="106" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A106" s="30" t="s">
+      <c r="E105" s="4"/>
+    </row>
+    <row r="106" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A106" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="B106">
+      <c r="B106" s="2">
         <v>11</v>
       </c>
-      <c r="C106" s="13" t="s">
+      <c r="C106" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="D106" s="14" t="s">
+      <c r="D106" s="3" t="s">
         <v>279</v>
       </c>
-      <c r="E106" s="5"/>
-    </row>
-    <row r="107" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A107" s="30" t="s">
+      <c r="E106" s="4"/>
+    </row>
+    <row r="107" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A107" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="B107">
+      <c r="B107" s="2">
         <v>11</v>
       </c>
-      <c r="C107" s="13" t="s">
+      <c r="C107" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="D107" s="14" t="s">
+      <c r="D107" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="E107" s="5"/>
-    </row>
-    <row r="108" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A108" s="30" t="s">
+      <c r="E107" s="4"/>
+    </row>
+    <row r="108" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A108" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B108">
+      <c r="B108" s="2">
         <v>11</v>
       </c>
-      <c r="C108" s="13" t="s">
+      <c r="C108" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="D108" s="14" t="s">
+      <c r="D108" s="3" t="s">
         <v>279</v>
       </c>
-      <c r="E108" s="5"/>
-    </row>
-    <row r="109" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A109" s="30" t="s">
+      <c r="E108" s="4"/>
+    </row>
+    <row r="109" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A109" s="2" t="s">
         <v>286</v>
       </c>
-      <c r="B109">
+      <c r="B109" s="2">
         <v>11</v>
       </c>
-      <c r="C109" s="13" t="s">
+      <c r="C109" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="D109" s="14" t="s">
+      <c r="D109" s="3" t="s">
         <v>279</v>
       </c>
-      <c r="E109" s="5"/>
-    </row>
-    <row r="110" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A110" s="30" t="s">
+      <c r="E109" s="4"/>
+    </row>
+    <row r="110" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A110" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="B110">
+      <c r="B110" s="2">
         <v>11</v>
       </c>
-      <c r="C110" s="13" t="s">
+      <c r="C110" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="D110" s="14" t="s">
+      <c r="D110" s="3" t="s">
         <v>279</v>
       </c>
-      <c r="E110" s="5"/>
-    </row>
-    <row r="111" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A111" s="30" t="s">
+      <c r="E110" s="4"/>
+    </row>
+    <row r="111" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A111" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="B111">
+      <c r="B111" s="2">
         <v>24</v>
       </c>
-      <c r="C111" s="13" t="s">
+      <c r="C111" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="D111" s="18" t="s">
+      <c r="D111" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="E111" s="5"/>
-    </row>
-    <row r="112" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A112" s="30" t="s">
+      <c r="E111" s="4"/>
+    </row>
+    <row r="112" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A112" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="B112">
+      <c r="B112" s="2">
         <v>24</v>
       </c>
-      <c r="C112" s="13" t="s">
+      <c r="C112" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="D112" s="18" t="s">
+      <c r="D112" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="E112" s="5"/>
-    </row>
-    <row r="113" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A113" s="30" t="s">
+      <c r="E112" s="4"/>
+    </row>
+    <row r="113" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A113" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="B113">
+      <c r="B113" s="2">
         <v>24</v>
       </c>
-      <c r="C113" s="13" t="s">
+      <c r="C113" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="D113" s="18" t="s">
+      <c r="D113" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="E113" s="5"/>
-    </row>
-    <row r="114" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A114" s="30" t="s">
+      <c r="E113" s="4"/>
+    </row>
+    <row r="114" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A114" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="B114">
+      <c r="B114" s="2">
         <v>24</v>
       </c>
-      <c r="C114" s="13" t="s">
+      <c r="C114" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="D114" s="18" t="s">
+      <c r="D114" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="E114" s="5"/>
-    </row>
-    <row r="115" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A115" s="30" t="s">
+      <c r="E114" s="4"/>
+    </row>
+    <row r="115" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A115" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="B115">
+      <c r="B115" s="2">
         <v>24</v>
       </c>
-      <c r="C115" s="13" t="s">
+      <c r="C115" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="D115" s="18" t="s">
+      <c r="D115" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="E115" s="5"/>
-    </row>
-    <row r="116" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A116" s="30" t="s">
+      <c r="E115" s="4"/>
+    </row>
+    <row r="116" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A116" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="B116">
+      <c r="B116" s="2">
         <v>24</v>
       </c>
-      <c r="C116" s="13" t="s">
+      <c r="C116" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="D116" s="18" t="s">
+      <c r="D116" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="E116" s="5"/>
-    </row>
-    <row r="117" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A117" s="30" t="s">
+      <c r="E116" s="4"/>
+    </row>
+    <row r="117" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A117" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="B117">
+      <c r="B117" s="2">
         <v>24</v>
       </c>
-      <c r="C117" s="13" t="s">
+      <c r="C117" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="D117" s="18" t="s">
+      <c r="D117" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="E117" s="5"/>
-    </row>
-    <row r="118" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A118" s="30" t="s">
+      <c r="E117" s="4"/>
+    </row>
+    <row r="118" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A118" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="B118">
+      <c r="B118" s="2">
         <v>24</v>
       </c>
-      <c r="C118" s="13" t="s">
+      <c r="C118" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="D118" s="18" t="s">
+      <c r="D118" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="E118" s="5"/>
-    </row>
-    <row r="119" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A119" s="30" t="s">
+      <c r="E118" s="4"/>
+    </row>
+    <row r="119" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A119" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="B119">
+      <c r="B119" s="2">
         <v>24</v>
       </c>
-      <c r="C119" s="13" t="s">
+      <c r="C119" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="D119" s="18" t="s">
+      <c r="D119" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="E119" s="5"/>
-    </row>
-    <row r="120" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A120" s="30" t="s">
+      <c r="E119" s="4"/>
+    </row>
+    <row r="120" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A120" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="B120">
+      <c r="B120" s="2">
         <v>24</v>
       </c>
-      <c r="C120" s="13" t="s">
+      <c r="C120" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="D120" s="18" t="s">
+      <c r="D120" s="2" t="s">
         <v>318</v>
       </c>
-      <c r="E120" s="5"/>
-    </row>
-    <row r="121" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A121" s="30" t="s">
+      <c r="E120" s="4"/>
+    </row>
+    <row r="121" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A121" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="B121">
+      <c r="B121" s="2">
         <v>24</v>
       </c>
-      <c r="C121" s="13" t="s">
+      <c r="C121" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="D121" s="18" t="s">
+      <c r="D121" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="E121" s="5"/>
-    </row>
-    <row r="122" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A122" s="30" t="s">
+      <c r="E121" s="4"/>
+    </row>
+    <row r="122" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A122" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="B122">
+      <c r="B122" s="2">
         <v>24</v>
       </c>
-      <c r="C122" s="13" t="s">
+      <c r="C122" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="D122" s="18" t="s">
+      <c r="D122" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="E122" s="5"/>
-    </row>
-    <row r="123" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A123" s="30" t="s">
+      <c r="E122" s="4"/>
+    </row>
+    <row r="123" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A123" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="B123">
+      <c r="B123" s="2">
         <v>24</v>
       </c>
-      <c r="C123" s="13" t="s">
+      <c r="C123" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="D123" s="18" t="s">
+      <c r="D123" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="E123" s="5"/>
-    </row>
-    <row r="124" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A124" s="30" t="s">
+      <c r="E123" s="4"/>
+    </row>
+    <row r="124" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A124" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="B124">
+      <c r="B124" s="2">
         <v>24</v>
       </c>
-      <c r="C124" s="13" t="s">
+      <c r="C124" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="D124" s="18" t="s">
+      <c r="D124" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="E124" s="5"/>
-    </row>
-    <row r="125" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A125" s="30" t="s">
+      <c r="E124" s="4"/>
+    </row>
+    <row r="125" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A125" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="B125">
+      <c r="B125" s="2">
         <v>24</v>
       </c>
-      <c r="C125" s="13" t="s">
+      <c r="C125" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="D125" s="18" t="s">
+      <c r="D125" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="E125" s="5"/>
-    </row>
-    <row r="126" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A126" s="30" t="s">
+      <c r="E125" s="4"/>
+    </row>
+    <row r="126" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A126" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="B126">
+      <c r="B126" s="2">
         <v>24</v>
       </c>
-      <c r="C126" s="13" t="s">
+      <c r="C126" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="D126" s="18" t="s">
+      <c r="D126" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="E126" s="5"/>
-    </row>
-    <row r="127" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A127" s="30" t="s">
+      <c r="E126" s="4"/>
+    </row>
+    <row r="127" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A127" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="B127">
+      <c r="B127" s="2">
         <v>9</v>
       </c>
-      <c r="C127" s="19" t="s">
+      <c r="C127" s="6" t="s">
         <v>333</v>
       </c>
-      <c r="D127" s="20" t="s">
+      <c r="D127" s="8" t="s">
         <v>334</v>
       </c>
-      <c r="E127" s="5"/>
-    </row>
-    <row r="128" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A128" s="30" t="s">
+      <c r="E127" s="4"/>
+    </row>
+    <row r="128" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A128" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="B128">
+      <c r="B128" s="2">
         <v>9</v>
       </c>
-      <c r="C128" s="21" t="s">
+      <c r="C128" s="6" t="s">
         <v>336</v>
       </c>
-      <c r="D128" s="20" t="s">
+      <c r="D128" s="8" t="s">
         <v>337</v>
       </c>
-      <c r="E128" s="5"/>
-    </row>
-    <row r="129" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A129" s="30" t="s">
+      <c r="E128" s="4"/>
+    </row>
+    <row r="129" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+      <c r="A129" s="2" t="s">
         <v>335</v>
       </c>
-      <c r="B129">
+      <c r="B129" s="2">
         <v>9</v>
       </c>
-      <c r="C129" s="19" t="s">
+      <c r="C129" s="6" t="s">
         <v>339</v>
       </c>
-      <c r="D129" s="20" t="s">
+      <c r="D129" s="8" t="s">
         <v>340</v>
       </c>
-      <c r="E129" s="5"/>
-    </row>
-    <row r="130" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A130" s="30" t="s">
+      <c r="E129" s="4"/>
+    </row>
+    <row r="130" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+      <c r="A130" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="B130">
+      <c r="B130" s="2">
         <v>9</v>
       </c>
-      <c r="C130" s="12" t="s">
+      <c r="C130" s="7" t="s">
         <v>342</v>
       </c>
-      <c r="D130" s="20" t="s">
+      <c r="D130" s="8" t="s">
         <v>340</v>
       </c>
-      <c r="E130" s="5"/>
-    </row>
-    <row r="131" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A131" s="30" t="s">
+      <c r="E130" s="4"/>
+    </row>
+    <row r="131" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+      <c r="A131" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="B131">
+      <c r="B131" s="2">
         <v>9</v>
       </c>
-      <c r="C131" s="12" t="s">
+      <c r="C131" s="7" t="s">
         <v>344</v>
       </c>
-      <c r="D131" s="20" t="s">
+      <c r="D131" s="8" t="s">
         <v>345</v>
       </c>
-      <c r="E131" s="5"/>
-    </row>
-    <row r="132" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A132" s="30" t="s">
+      <c r="E131" s="4"/>
+    </row>
+    <row r="132" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A132" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="B132">
+      <c r="B132" s="2">
         <v>9</v>
       </c>
-      <c r="C132" s="12" t="s">
+      <c r="C132" s="7" t="s">
         <v>347</v>
       </c>
-      <c r="D132" s="20" t="s">
+      <c r="D132" s="8" t="s">
         <v>348</v>
       </c>
-      <c r="E132" s="5"/>
-    </row>
-    <row r="133" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A133" s="30" t="s">
+      <c r="E132" s="4"/>
+    </row>
+    <row r="133" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+      <c r="A133" s="2" t="s">
         <v>346</v>
       </c>
-      <c r="B133">
+      <c r="B133" s="2">
         <v>9</v>
       </c>
-      <c r="C133" s="12" t="s">
+      <c r="C133" s="7" t="s">
         <v>350</v>
       </c>
-      <c r="D133" s="20" t="s">
+      <c r="D133" s="8" t="s">
         <v>351</v>
       </c>
-      <c r="E133" s="5"/>
-    </row>
-    <row r="134" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A134" s="30" t="s">
+      <c r="E133" s="4"/>
+    </row>
+    <row r="134" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A134" s="2" t="s">
         <v>349</v>
       </c>
-      <c r="B134">
+      <c r="B134" s="2">
         <v>9</v>
       </c>
-      <c r="C134" s="22" t="s">
+      <c r="C134" s="7" t="s">
         <v>353</v>
       </c>
-      <c r="D134" s="23" t="s">
+      <c r="D134" s="8" t="s">
         <v>354</v>
       </c>
-      <c r="E134" s="5"/>
-    </row>
-    <row r="135" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A135" s="30" t="s">
+      <c r="E134" s="4"/>
+    </row>
+    <row r="135" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A135" s="2" t="s">
         <v>352</v>
       </c>
-      <c r="B135">
+      <c r="B135" s="2">
         <v>9</v>
       </c>
-      <c r="C135" s="22" t="s">
+      <c r="C135" s="7" t="s">
         <v>356</v>
       </c>
-      <c r="D135" s="24" t="s">
+      <c r="D135" s="10" t="s">
         <v>357</v>
       </c>
-      <c r="E135" s="5"/>
-    </row>
-    <row r="136" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A136" s="30" t="s">
+      <c r="E135" s="4"/>
+    </row>
+    <row r="136" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A136" s="2" t="s">
         <v>355</v>
       </c>
-      <c r="B136">
+      <c r="B136" s="2">
         <v>9</v>
       </c>
-      <c r="C136" s="12" t="s">
+      <c r="C136" s="7" t="s">
         <v>359</v>
       </c>
-      <c r="D136" s="25" t="s">
+      <c r="D136" s="8" t="s">
         <v>360</v>
       </c>
-      <c r="E136" s="5"/>
-    </row>
-    <row r="137" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A137" s="30" t="s">
+      <c r="E136" s="4"/>
+    </row>
+    <row r="137" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A137" s="2" t="s">
         <v>358</v>
       </c>
-      <c r="B137">
+      <c r="B137" s="2">
         <v>9</v>
       </c>
-      <c r="C137" s="12" t="s">
+      <c r="C137" s="7" t="s">
         <v>362</v>
       </c>
-      <c r="D137" s="25" t="s">
+      <c r="D137" s="8" t="s">
         <v>360</v>
       </c>
-      <c r="E137" s="5"/>
-    </row>
-    <row r="138" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A138" s="30" t="s">
+      <c r="E137" s="4"/>
+    </row>
+    <row r="138" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A138" s="2" t="s">
         <v>361</v>
       </c>
-      <c r="B138">
+      <c r="B138" s="2">
         <v>9</v>
       </c>
-      <c r="C138" s="15" t="s">
+      <c r="C138" s="7" t="s">
         <v>364</v>
       </c>
-      <c r="D138" s="26" t="s">
+      <c r="D138" s="8" t="s">
         <v>365</v>
       </c>
-      <c r="E138" s="16"/>
-    </row>
-    <row r="139" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A139" s="30" t="s">
+      <c r="E138" s="4"/>
+    </row>
+    <row r="139" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A139" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="B139">
+      <c r="B139" s="2">
         <v>9</v>
       </c>
-      <c r="C139" s="12" t="s">
+      <c r="C139" s="7" t="s">
         <v>367</v>
       </c>
-      <c r="D139" s="27" t="s">
+      <c r="D139" s="8" t="s">
         <v>360</v>
       </c>
-      <c r="E139" s="5"/>
-    </row>
-    <row r="140" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A140" s="30" t="s">
+      <c r="E139" s="4"/>
+    </row>
+    <row r="140" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A140" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="B140">
+      <c r="B140" s="2">
         <v>9</v>
       </c>
-      <c r="C140" s="12" t="s">
+      <c r="C140" s="7" t="s">
         <v>369</v>
       </c>
-      <c r="D140" s="27" t="s">
+      <c r="D140" s="8" t="s">
         <v>370</v>
       </c>
-      <c r="E140" s="5"/>
-    </row>
-    <row r="141" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A141" s="30" t="s">
+      <c r="E140" s="4"/>
+    </row>
+    <row r="141" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A141" s="2" t="s">
         <v>368</v>
       </c>
-      <c r="B141">
+      <c r="B141" s="2">
         <v>9</v>
       </c>
-      <c r="C141" s="12" t="s">
+      <c r="C141" s="7" t="s">
         <v>372</v>
       </c>
-      <c r="D141" s="27" t="s">
+      <c r="D141" s="8" t="s">
         <v>360</v>
       </c>
-      <c r="E141" s="5"/>
-    </row>
-    <row r="142" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A142" s="30" t="s">
+      <c r="E141" s="4"/>
+    </row>
+    <row r="142" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A142" s="2" t="s">
         <v>371</v>
       </c>
-      <c r="B142">
+      <c r="B142" s="2">
         <v>9</v>
       </c>
-      <c r="C142" s="12" t="s">
+      <c r="C142" s="7" t="s">
         <v>374</v>
       </c>
-      <c r="D142" s="27" t="s">
+      <c r="D142" s="8" t="s">
         <v>360</v>
       </c>
-      <c r="E142" s="5"/>
-    </row>
-    <row r="143" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A143" s="30" t="s">
+      <c r="E142" s="4"/>
+    </row>
+    <row r="143" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A143" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="B143">
+      <c r="B143" s="2">
         <v>9</v>
       </c>
-      <c r="C143" s="15" t="s">
+      <c r="C143" s="7" t="s">
         <v>376</v>
       </c>
-      <c r="D143" s="27" t="s">
+      <c r="D143" s="8" t="s">
         <v>365</v>
       </c>
-      <c r="E143" s="16"/>
-    </row>
-    <row r="144" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A144" s="30" t="s">
+      <c r="E143" s="4"/>
+    </row>
+    <row r="144" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+      <c r="A144" s="2" t="s">
         <v>375</v>
       </c>
-      <c r="B144">
+      <c r="B144" s="2">
         <v>9</v>
       </c>
-      <c r="C144" s="12" t="s">
+      <c r="C144" s="7" t="s">
         <v>378</v>
       </c>
-      <c r="D144" s="27" t="s">
+      <c r="D144" s="8" t="s">
         <v>379</v>
       </c>
-      <c r="E144" s="5"/>
-    </row>
-    <row r="145" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A145" s="30" t="s">
+      <c r="E144" s="4"/>
+    </row>
+    <row r="145" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A145" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="B145">
+      <c r="B145" s="2">
         <v>9</v>
       </c>
-      <c r="C145" s="12" t="s">
+      <c r="C145" s="7" t="s">
         <v>381</v>
       </c>
-      <c r="D145" s="27" t="s">
+      <c r="D145" s="8" t="s">
         <v>382</v>
       </c>
-      <c r="E145" s="5"/>
-    </row>
-    <row r="146" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A146" s="30" t="s">
+      <c r="E145" s="4"/>
+    </row>
+    <row r="146" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+      <c r="A146" s="2" t="s">
         <v>380</v>
       </c>
-      <c r="B146">
+      <c r="B146" s="2">
         <v>9</v>
       </c>
-      <c r="C146" s="12" t="s">
+      <c r="C146" s="7" t="s">
         <v>384</v>
       </c>
-      <c r="D146" s="27" t="s">
+      <c r="D146" s="8" t="s">
         <v>385</v>
       </c>
-      <c r="E146" s="5"/>
-    </row>
-    <row r="147" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A147" s="30" t="s">
+      <c r="E146" s="4"/>
+    </row>
+    <row r="147" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A147" s="2" t="s">
         <v>383</v>
       </c>
-      <c r="B147">
+      <c r="B147" s="2">
         <v>9</v>
       </c>
-      <c r="C147" s="12" t="s">
+      <c r="C147" s="7" t="s">
         <v>387</v>
       </c>
-      <c r="D147" s="27" t="s">
+      <c r="D147" s="8" t="s">
         <v>388</v>
       </c>
-      <c r="E147" s="5"/>
-    </row>
-    <row r="148" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A148" s="30" t="s">
+      <c r="E147" s="4"/>
+    </row>
+    <row r="148" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A148" s="2" t="s">
         <v>386</v>
       </c>
-      <c r="B148">
+      <c r="B148" s="2">
         <v>9</v>
       </c>
-      <c r="C148" s="12" t="s">
+      <c r="C148" s="7" t="s">
         <v>390</v>
       </c>
-      <c r="D148" s="27" t="s">
+      <c r="D148" s="8" t="s">
         <v>391</v>
       </c>
-      <c r="E148" s="5"/>
-    </row>
-    <row r="149" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A149" s="30" t="s">
+      <c r="E148" s="4"/>
+    </row>
+    <row r="149" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+      <c r="A149" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="B149">
+      <c r="B149" s="2">
         <v>9</v>
       </c>
-      <c r="C149" s="12" t="s">
+      <c r="C149" s="7" t="s">
         <v>393</v>
       </c>
-      <c r="D149" s="27" t="s">
+      <c r="D149" s="8" t="s">
         <v>394</v>
       </c>
-      <c r="E149" s="5"/>
-    </row>
-    <row r="150" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A150" s="30" t="s">
+      <c r="E149" s="4"/>
+    </row>
+    <row r="150" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+      <c r="A150" s="2" t="s">
         <v>392</v>
       </c>
-      <c r="B150">
+      <c r="B150" s="2">
         <v>9</v>
       </c>
-      <c r="C150" s="12" t="s">
+      <c r="C150" s="7" t="s">
         <v>396</v>
       </c>
-      <c r="D150" s="27" t="s">
+      <c r="D150" s="8" t="s">
         <v>397</v>
       </c>
-      <c r="E150" s="5"/>
-    </row>
-    <row r="151" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A151" s="30" t="s">
+      <c r="E150" s="4"/>
+    </row>
+    <row r="151" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+      <c r="A151" s="2" t="s">
         <v>395</v>
       </c>
-      <c r="B151">
+      <c r="B151" s="2">
         <v>22</v>
       </c>
-      <c r="C151" s="12" t="s">
+      <c r="C151" s="7" t="s">
         <v>399</v>
       </c>
-      <c r="D151" s="27" t="s">
+      <c r="D151" s="8" t="s">
         <v>400</v>
       </c>
-      <c r="E151" s="5"/>
-    </row>
-    <row r="152" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A152" s="30" t="s">
+      <c r="E151" s="4"/>
+    </row>
+    <row r="152" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A152" s="2" t="s">
         <v>398</v>
       </c>
-      <c r="B152">
+      <c r="B152" s="2">
         <v>22</v>
       </c>
-      <c r="C152" s="12" t="s">
+      <c r="C152" s="7" t="s">
         <v>402</v>
       </c>
-      <c r="D152" s="27" t="s">
+      <c r="D152" s="8" t="s">
         <v>403</v>
       </c>
-      <c r="E152" s="5"/>
-    </row>
-    <row r="153" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A153" s="30" t="s">
+      <c r="E152" s="4"/>
+    </row>
+    <row r="153" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A153" s="2" t="s">
         <v>401</v>
       </c>
-      <c r="B153">
+      <c r="B153" s="2">
         <v>22</v>
       </c>
-      <c r="C153" s="12" t="s">
+      <c r="C153" s="7" t="s">
         <v>405</v>
       </c>
-      <c r="D153" s="27" t="s">
+      <c r="D153" s="8" t="s">
         <v>406</v>
       </c>
-      <c r="E153" s="5"/>
-    </row>
-    <row r="154" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A154" s="30" t="s">
+      <c r="E153" s="4"/>
+    </row>
+    <row r="154" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+      <c r="A154" s="2" t="s">
         <v>404</v>
       </c>
-      <c r="B154">
+      <c r="B154" s="2">
         <v>22</v>
       </c>
-      <c r="C154" s="12" t="s">
+      <c r="C154" s="7" t="s">
         <v>408</v>
       </c>
-      <c r="D154" s="27" t="s">
+      <c r="D154" s="8" t="s">
         <v>409</v>
       </c>
-      <c r="E154" s="5"/>
-    </row>
-    <row r="155" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A155" s="30" t="s">
+      <c r="E154" s="4"/>
+    </row>
+    <row r="155" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A155" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="B155">
+      <c r="B155" s="2">
         <v>22</v>
       </c>
-      <c r="C155" s="12" t="s">
+      <c r="C155" s="7" t="s">
         <v>411</v>
       </c>
-      <c r="D155" s="27" t="s">
+      <c r="D155" s="8" t="s">
         <v>412</v>
       </c>
-      <c r="E155" s="5"/>
-    </row>
-    <row r="156" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A156" s="30" t="s">
+      <c r="E155" s="4"/>
+    </row>
+    <row r="156" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A156" s="2" t="s">
         <v>410</v>
       </c>
-      <c r="B156">
+      <c r="B156" s="2">
         <v>22</v>
       </c>
-      <c r="C156" s="12" t="s">
+      <c r="C156" s="7" t="s">
         <v>414</v>
       </c>
-      <c r="D156" s="27" t="s">
+      <c r="D156" s="8" t="s">
         <v>403</v>
       </c>
-      <c r="E156" s="5"/>
-    </row>
-    <row r="157" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A157" s="30" t="s">
+      <c r="E156" s="4"/>
+    </row>
+    <row r="157" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A157" s="2" t="s">
         <v>413</v>
       </c>
-      <c r="B157">
+      <c r="B157" s="2">
         <v>22</v>
       </c>
-      <c r="C157" s="12" t="s">
+      <c r="C157" s="7" t="s">
         <v>416</v>
       </c>
-      <c r="D157" s="27" t="s">
+      <c r="D157" s="8" t="s">
         <v>403</v>
       </c>
-      <c r="E157" s="5"/>
-    </row>
-    <row r="158" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A158" s="30" t="s">
+      <c r="E157" s="4"/>
+    </row>
+    <row r="158" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A158" s="2" t="s">
         <v>415</v>
       </c>
-      <c r="B158">
+      <c r="B158" s="2">
         <v>22</v>
       </c>
-      <c r="C158" s="12" t="s">
+      <c r="C158" s="7" t="s">
         <v>418</v>
       </c>
-      <c r="D158" s="27" t="s">
+      <c r="D158" s="8" t="s">
         <v>419</v>
       </c>
-      <c r="E158" s="5"/>
-    </row>
-    <row r="159" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A159" s="30" t="s">
+      <c r="E158" s="4"/>
+    </row>
+    <row r="159" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+      <c r="A159" s="2" t="s">
         <v>417</v>
       </c>
-      <c r="B159">
+      <c r="B159" s="2">
         <v>22</v>
       </c>
-      <c r="C159" s="12" t="s">
+      <c r="C159" s="7" t="s">
         <v>421</v>
       </c>
-      <c r="D159" s="27" t="s">
+      <c r="D159" s="8" t="s">
         <v>422</v>
       </c>
-      <c r="E159" s="5"/>
-    </row>
-    <row r="160" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A160" s="30" t="s">
+      <c r="E159" s="4"/>
+    </row>
+    <row r="160" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+      <c r="A160" s="2" t="s">
         <v>420</v>
       </c>
-      <c r="B160">
+      <c r="B160" s="2">
         <v>22</v>
       </c>
-      <c r="C160" s="12" t="s">
+      <c r="C160" s="7" t="s">
         <v>424</v>
       </c>
-      <c r="D160" s="27" t="s">
+      <c r="D160" s="8" t="s">
         <v>425</v>
       </c>
-      <c r="E160" s="5"/>
-    </row>
-    <row r="161" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A161" s="30" t="s">
+      <c r="E160" s="4"/>
+    </row>
+    <row r="161" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+      <c r="A161" s="2" t="s">
         <v>423</v>
       </c>
-      <c r="B161">
+      <c r="B161" s="2">
         <v>22</v>
       </c>
-      <c r="C161" s="12" t="s">
+      <c r="C161" s="7" t="s">
         <v>427</v>
       </c>
-      <c r="D161" s="27" t="s">
+      <c r="D161" s="8" t="s">
         <v>428</v>
       </c>
-      <c r="E161" s="5"/>
-    </row>
-    <row r="162" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A162" s="30" t="s">
+      <c r="E161" s="4"/>
+    </row>
+    <row r="162" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+      <c r="A162" s="2" t="s">
         <v>426</v>
       </c>
-      <c r="B162">
+      <c r="B162" s="2">
         <v>22</v>
       </c>
-      <c r="C162" s="12" t="s">
+      <c r="C162" s="7" t="s">
         <v>429</v>
       </c>
-      <c r="D162" s="20" t="s">
+      <c r="D162" s="8" t="s">
         <v>430</v>
       </c>
-      <c r="E162" s="5"/>
-    </row>
-    <row r="163" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A163" s="30"/>
-      <c r="C163" s="28"/>
-      <c r="D163" s="32"/>
-      <c r="E163" s="29"/>
+      <c r="E162" s="4"/>
+    </row>
+    <row r="163" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A163" s="2" t="s">
+        <v>456</v>
+      </c>
+      <c r="B163" s="2">
+        <v>16</v>
+      </c>
+      <c r="C163" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="D163" s="2" t="s">
+        <v>479</v>
+      </c>
+      <c r="E163" s="4"/>
+    </row>
+    <row r="164" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A164" s="2" t="s">
+        <v>457</v>
+      </c>
+      <c r="B164" s="2">
+        <v>16</v>
+      </c>
+      <c r="C164" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="D164" s="2" t="s">
+        <v>480</v>
+      </c>
+      <c r="E164" s="2"/>
+    </row>
+    <row r="165" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A165" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="B165" s="2">
+        <v>16</v>
+      </c>
+      <c r="C165" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="D165" s="2" t="s">
+        <v>481</v>
+      </c>
+      <c r="E165" s="2"/>
+    </row>
+    <row r="166" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A166" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="B166" s="2">
+        <v>16</v>
+      </c>
+      <c r="C166" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="D166" s="2" t="s">
+        <v>482</v>
+      </c>
+      <c r="E166" s="2"/>
+    </row>
+    <row r="167" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A167" s="2" t="s">
+        <v>460</v>
+      </c>
+      <c r="B167" s="2">
+        <v>16</v>
+      </c>
+      <c r="C167" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="D167" s="2" t="s">
+        <v>483</v>
+      </c>
+      <c r="E167" s="2"/>
+    </row>
+    <row r="168" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A168" s="2" t="s">
+        <v>461</v>
+      </c>
+      <c r="B168" s="2">
+        <v>16</v>
+      </c>
+      <c r="C168" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="D168" s="2" t="s">
+        <v>484</v>
+      </c>
+      <c r="E168" s="2"/>
+    </row>
+    <row r="169" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A169" s="2" t="s">
+        <v>462</v>
+      </c>
+      <c r="B169" s="2">
+        <v>16</v>
+      </c>
+      <c r="C169" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="D169" s="2" t="s">
+        <v>485</v>
+      </c>
+      <c r="E169" s="2"/>
+    </row>
+    <row r="170" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A170" s="2" t="s">
+        <v>463</v>
+      </c>
+      <c r="B170" s="2">
+        <v>16</v>
+      </c>
+      <c r="C170" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="D170" s="2" t="s">
+        <v>486</v>
+      </c>
+      <c r="E170" s="2"/>
+    </row>
+    <row r="171" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A171" s="2" t="s">
+        <v>464</v>
+      </c>
+      <c r="B171" s="2">
+        <v>16</v>
+      </c>
+      <c r="C171" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="D171" s="2" t="s">
+        <v>487</v>
+      </c>
+      <c r="E171" s="2"/>
+    </row>
+    <row r="172" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A172" s="2" t="s">
+        <v>465</v>
+      </c>
+      <c r="B172" s="2">
+        <v>16</v>
+      </c>
+      <c r="C172" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="D172" s="2" t="s">
+        <v>488</v>
+      </c>
+      <c r="E172" s="2"/>
+    </row>
+    <row r="173" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A173" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="B173" s="2">
+        <v>16</v>
+      </c>
+      <c r="C173" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="D173" s="2" t="s">
+        <v>489</v>
+      </c>
+      <c r="E173" s="2"/>
+    </row>
+    <row r="174" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A174" s="2" t="s">
+        <v>467</v>
+      </c>
+      <c r="B174" s="2">
+        <v>16</v>
+      </c>
+      <c r="C174" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="D174" s="2" t="s">
+        <v>490</v>
+      </c>
+      <c r="E174" s="2"/>
+    </row>
+    <row r="175" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A175" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="B175" s="2">
+        <v>16</v>
+      </c>
+      <c r="C175" s="2" t="s">
+        <v>453</v>
+      </c>
+      <c r="D175" s="2" t="s">
+        <v>491</v>
+      </c>
+      <c r="E175" s="2"/>
+    </row>
+    <row r="176" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A176" s="2" t="s">
+        <v>469</v>
+      </c>
+      <c r="B176" s="2">
+        <v>16</v>
+      </c>
+      <c r="C176" s="2" t="s">
+        <v>454</v>
+      </c>
+      <c r="D176" s="2" t="s">
+        <v>492</v>
+      </c>
+      <c r="E176" s="2"/>
+    </row>
+    <row r="177" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A177" s="2" t="s">
+        <v>470</v>
+      </c>
+      <c r="B177" s="2">
+        <v>16</v>
+      </c>
+      <c r="C177" s="2" t="s">
+        <v>455</v>
+      </c>
+      <c r="D177" s="2" t="s">
+        <v>493</v>
+      </c>
+      <c r="E177" s="2"/>
+    </row>
+    <row r="178" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A178" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="B178" s="2">
+        <v>16</v>
+      </c>
+      <c r="C178" s="2" t="s">
+        <v>447</v>
+      </c>
+      <c r="D178" s="2" t="s">
+        <v>494</v>
+      </c>
+      <c r="E178" s="2"/>
+    </row>
+    <row r="179" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A179" s="2" t="s">
+        <v>472</v>
+      </c>
+      <c r="B179" s="2">
+        <v>16</v>
+      </c>
+      <c r="C179" s="5" t="s">
+        <v>446</v>
+      </c>
+      <c r="D179" s="2" t="s">
+        <v>478</v>
+      </c>
+      <c r="E179" s="2"/>
+    </row>
+    <row r="180" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A180" s="2" t="s">
+        <v>473</v>
+      </c>
+      <c r="B180" s="2">
+        <v>16</v>
+      </c>
+      <c r="C180" s="2" t="s">
+        <v>448</v>
+      </c>
+      <c r="D180" s="2" t="s">
+        <v>490</v>
+      </c>
+      <c r="E180" s="2"/>
+    </row>
+    <row r="181" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A181" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="B181" s="2">
+        <v>16</v>
+      </c>
+      <c r="C181" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="D181" s="2" t="s">
+        <v>491</v>
+      </c>
+      <c r="E181" s="2"/>
+    </row>
+    <row r="182" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A182" s="2" t="s">
+        <v>475</v>
+      </c>
+      <c r="B182" s="2">
+        <v>16</v>
+      </c>
+      <c r="C182" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="D182" s="2" t="s">
+        <v>492</v>
+      </c>
+      <c r="E182" s="2"/>
+    </row>
+    <row r="183" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A183" s="2" t="s">
+        <v>476</v>
+      </c>
+      <c r="B183" s="2">
+        <v>16</v>
+      </c>
+      <c r="C183" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="D183" s="2" t="s">
+        <v>489</v>
+      </c>
+      <c r="E183" s="2"/>
+    </row>
+    <row r="184" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A184" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="B184" s="2">
+        <v>16</v>
+      </c>
+      <c r="C184" s="2" t="s">
+        <v>452</v>
+      </c>
+      <c r="D184" s="2" t="s">
+        <v>490</v>
+      </c>
+      <c r="E184" s="2"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="10" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Updated the UI picture formatting for Group 10
</commit_message>
<xml_diff>
--- a/FinalRequirements.xlsx
+++ b/FinalRequirements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meomeomeo/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EFEBB529-3717-D445-BEAA-72A654A20E85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{03E800A6-D1CC-3943-8EA4-FEB3A3D8E0A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3480" yWindow="6740" windowWidth="16380" windowHeight="8200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
   <metadataTypes count="1">
     <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
-  <futureMetadata name="XLRICHVALUE" count="5">
+  <futureMetadata name="XLRICHVALUE" count="8">
     <bk>
       <extLst>
         <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
@@ -65,8 +65,29 @@
         </ext>
       </extLst>
     </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="5"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="6"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="7"/>
+        </ext>
+      </extLst>
+    </bk>
   </futureMetadata>
-  <valueMetadata count="5">
+  <valueMetadata count="8">
     <bk>
       <rc t="1" v="0"/>
     </bk>
@@ -81,6 +102,15 @@
     </bk>
     <bk>
       <rc t="1" v="4"/>
+    </bk>
+    <bk>
+      <rc t="1" v="5"/>
+    </bk>
+    <bk>
+      <rc t="1" v="6"/>
+    </bk>
+    <bk>
+      <rc t="1" v="7"/>
     </bk>
   </valueMetadata>
 </metadata>
@@ -1938,18 +1968,12 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -2029,19 +2053,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2100,7 +2124,7 @@
 </file>
 
 <file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
-<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="5">
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="8">
   <rv s="0">
     <v>0</v>
     <v>5</v>
@@ -2119,6 +2143,18 @@
   </rv>
   <rv s="0">
     <v>4</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>5</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>6</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>7</v>
     <v>5</v>
   </rv>
 </rvData>
@@ -2140,6 +2176,9 @@
   <rel r:id="rId3"/>
   <rel r:id="rId4"/>
   <rel r:id="rId5"/>
+  <rel r:id="rId6"/>
+  <rel r:id="rId7"/>
+  <rel r:id="rId8"/>
 </richValueRels>
 </file>
 
@@ -2269,8 +2308,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S213"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C21" zoomScale="132" zoomScaleNormal="132" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" topLeftCell="C19" zoomScale="50" zoomScaleNormal="132" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2278,7 +2317,7 @@
     <col min="2" max="2" width="8" customWidth="1"/>
     <col min="3" max="3" width="231" customWidth="1"/>
     <col min="4" max="4" width="64.5" customWidth="1"/>
-    <col min="5" max="5" width="22.1640625" customWidth="1"/>
+    <col min="5" max="5" width="48.5" customWidth="1"/>
     <col min="6" max="6" width="16.5" customWidth="1"/>
     <col min="19" max="19" width="36.5" customWidth="1"/>
   </cols>
@@ -2619,14 +2658,14 @@
       </c>
       <c r="E21" s="4"/>
     </row>
-    <row r="22" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" ht="135" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B22" s="14">
+      <c r="B22" s="18">
         <v>10</v>
       </c>
-      <c r="C22" s="15" t="s">
+      <c r="C22" s="14" t="s">
         <v>74</v>
       </c>
       <c r="D22" s="4" t="s">
@@ -2636,156 +2675,156 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" ht="78" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B23" s="14">
+      <c r="B23" s="18">
         <v>10</v>
       </c>
-      <c r="C23" s="15" t="s">
+      <c r="C23" s="14" t="s">
         <v>77</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="E23" s="4" t="e" vm="1">
+      <c r="E23" s="4" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" ht="125" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B24" s="14">
+      <c r="B24" s="18">
         <v>10</v>
       </c>
-      <c r="C24" s="15" t="s">
+      <c r="C24" s="14" t="s">
         <v>80</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="E24" s="4" t="e" vm="2">
+      <c r="E24" s="4" t="e" vm="3">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" ht="125" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B25" s="14">
+      <c r="B25" s="18">
         <v>10</v>
       </c>
-      <c r="C25" s="15" t="s">
+      <c r="C25" s="14" t="s">
         <v>83</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="E25" s="4" t="e" vm="2">
+      <c r="E25" s="4" t="e" vm="4">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" ht="99" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B26" s="14">
+      <c r="B26" s="18">
         <v>10</v>
       </c>
-      <c r="C26" s="15" t="s">
+      <c r="C26" s="14" t="s">
         <v>86</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="E26" s="4" t="e" vm="3">
+      <c r="E26" s="4" t="e" vm="5">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" ht="126" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B27" s="14">
+      <c r="B27" s="18">
         <v>10</v>
       </c>
-      <c r="C27" s="16" t="s">
+      <c r="C27" s="15" t="s">
         <v>89</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E27" s="4" t="e" vm="2">
+      <c r="E27" s="4" t="e" vm="6">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" ht="112" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="B28" s="14">
+      <c r="B28" s="18">
         <v>10</v>
       </c>
-      <c r="C28" s="17" t="s">
+      <c r="C28" s="16" t="s">
         <v>92</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="E28" s="4" t="e" vm="4">
+      <c r="E28" s="4" t="e" vm="7">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" ht="95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="B29" s="14">
+      <c r="B29" s="18">
         <v>10</v>
       </c>
-      <c r="C29" s="18" t="s">
+      <c r="C29" s="17" t="s">
         <v>95</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="E29" s="4" t="e" vm="5">
+      <c r="E29" s="4" t="e" vm="8">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" ht="98" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="B30" s="14">
+      <c r="B30" s="18">
         <v>10</v>
       </c>
-      <c r="C30" s="18" t="s">
+      <c r="C30" s="17" t="s">
         <v>98</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="E30" s="4" t="e" vm="3">
+      <c r="E30" s="4" t="e" vm="5">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" ht="194" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B31" s="14">
+      <c r="B31" s="18">
         <v>10</v>
       </c>
-      <c r="C31" s="14" t="s">
+      <c r="C31" s="18" t="s">
         <v>101</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="E31" s="4" t="e" vm="2">
+      <c r="E31" s="4" t="e" vm="4">
         <v>#VALUE!</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated UI picture formatting for group 10
</commit_message>
<xml_diff>
--- a/FinalRequirements.xlsx
+++ b/FinalRequirements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meomeomeo/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lucyguerrero/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{03E800A6-D1CC-3943-8EA4-FEB3A3D8E0A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95D25B5E-AF76-CE40-8261-16654EDF207D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16360" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
   <metadataTypes count="1">
     <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
-  <futureMetadata name="XLRICHVALUE" count="8">
+  <futureMetadata name="XLRICHVALUE" count="14">
     <bk>
       <extLst>
         <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
@@ -86,8 +86,50 @@
         </ext>
       </extLst>
     </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="8"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="9"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="10"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="11"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="12"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="13"/>
+        </ext>
+      </extLst>
+    </bk>
   </futureMetadata>
-  <valueMetadata count="8">
+  <valueMetadata count="14">
     <bk>
       <rc t="1" v="0"/>
     </bk>
@@ -111,6 +153,24 @@
     </bk>
     <bk>
       <rc t="1" v="7"/>
+    </bk>
+    <bk>
+      <rc t="1" v="8"/>
+    </bk>
+    <bk>
+      <rc t="1" v="9"/>
+    </bk>
+    <bk>
+      <rc t="1" v="10"/>
+    </bk>
+    <bk>
+      <rc t="1" v="11"/>
+    </bk>
+    <bk>
+      <rc t="1" v="12"/>
+    </bk>
+    <bk>
+      <rc t="1" v="13"/>
     </bk>
   </valueMetadata>
 </metadata>
@@ -2016,7 +2076,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2053,19 +2113,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2124,7 +2171,7 @@
 </file>
 
 <file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
-<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="8">
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="14">
   <rv s="0">
     <v>0</v>
     <v>5</v>
@@ -2157,6 +2204,30 @@
     <v>7</v>
     <v>5</v>
   </rv>
+  <rv s="0">
+    <v>8</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>9</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>10</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>11</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>12</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>13</v>
+    <v>5</v>
+  </rv>
 </rvData>
 </file>
 
@@ -2179,6 +2250,12 @@
   <rel r:id="rId6"/>
   <rel r:id="rId7"/>
   <rel r:id="rId8"/>
+  <rel r:id="rId9"/>
+  <rel r:id="rId10"/>
+  <rel r:id="rId11"/>
+  <rel r:id="rId12"/>
+  <rel r:id="rId13"/>
+  <rel r:id="rId14"/>
 </richValueRels>
 </file>
 
@@ -2308,8 +2385,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S213"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C19" zoomScale="50" zoomScaleNormal="132" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2317,7 +2394,7 @@
     <col min="2" max="2" width="8" customWidth="1"/>
     <col min="3" max="3" width="231" customWidth="1"/>
     <col min="4" max="4" width="64.5" customWidth="1"/>
-    <col min="5" max="5" width="48.5" customWidth="1"/>
+    <col min="5" max="5" width="80.83203125" customWidth="1"/>
     <col min="6" max="6" width="16.5" customWidth="1"/>
     <col min="19" max="19" width="36.5" customWidth="1"/>
   </cols>
@@ -2538,7 +2615,7 @@
       </c>
       <c r="E13" s="4"/>
     </row>
-    <row r="14" spans="1:19" ht="17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:19" ht="200" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>49</v>
       </c>
@@ -2551,9 +2628,11 @@
       <c r="D14" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="E14" s="4"/>
-    </row>
-    <row r="15" spans="1:19" ht="17" x14ac:dyDescent="0.2">
+      <c r="E14" s="4" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" ht="300" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>52</v>
       </c>
@@ -2566,7 +2645,9 @@
       <c r="D15" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E15" s="4"/>
+      <c r="E15" s="4" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
     </row>
     <row r="16" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
@@ -2583,7 +2664,7 @@
       </c>
       <c r="E16" s="4"/>
     </row>
-    <row r="17" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" ht="200" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>58</v>
       </c>
@@ -2596,9 +2677,11 @@
       <c r="D17" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="E17" s="4"/>
-    </row>
-    <row r="18" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E17" s="4" t="e" vm="3">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="150" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>61</v>
       </c>
@@ -2611,7 +2694,9 @@
       <c r="D18" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="E18" s="4"/>
+      <c r="E18" s="4" t="e" vm="4">
+        <v>#VALUE!</v>
+      </c>
     </row>
     <row r="19" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
@@ -2628,7 +2713,7 @@
       </c>
       <c r="E19" s="4"/>
     </row>
-    <row r="20" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" ht="200" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>67</v>
       </c>
@@ -2641,9 +2726,11 @@
       <c r="D20" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="E20" s="4"/>
-    </row>
-    <row r="21" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E20" s="4" t="e" vm="5">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="200" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>70</v>
       </c>
@@ -2656,22 +2743,24 @@
       <c r="D21" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="E21" s="4"/>
+      <c r="E21" s="4" t="e" vm="6">
+        <v>#VALUE!</v>
+      </c>
     </row>
     <row r="22" spans="1:5" ht="135" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B22" s="18">
+      <c r="B22" s="2">
         <v>10</v>
       </c>
-      <c r="C22" s="14" t="s">
+      <c r="C22" s="3" t="s">
         <v>74</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="E22" s="4" t="e" vm="1">
+      <c r="E22" s="4" t="e" vm="7">
         <v>#VALUE!</v>
       </c>
     </row>
@@ -2679,16 +2768,16 @@
       <c r="A23" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B23" s="18">
+      <c r="B23" s="2">
         <v>10</v>
       </c>
-      <c r="C23" s="14" t="s">
+      <c r="C23" s="3" t="s">
         <v>77</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="E23" s="4" t="e" vm="2">
+      <c r="E23" s="4" t="e" vm="8">
         <v>#VALUE!</v>
       </c>
     </row>
@@ -2696,16 +2785,16 @@
       <c r="A24" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B24" s="18">
+      <c r="B24" s="2">
         <v>10</v>
       </c>
-      <c r="C24" s="14" t="s">
+      <c r="C24" s="3" t="s">
         <v>80</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="E24" s="4" t="e" vm="3">
+      <c r="E24" s="4" t="e" vm="9">
         <v>#VALUE!</v>
       </c>
     </row>
@@ -2713,16 +2802,16 @@
       <c r="A25" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B25" s="18">
+      <c r="B25" s="2">
         <v>10</v>
       </c>
-      <c r="C25" s="14" t="s">
+      <c r="C25" s="3" t="s">
         <v>83</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="E25" s="4" t="e" vm="4">
+      <c r="E25" s="4" t="e" vm="10">
         <v>#VALUE!</v>
       </c>
     </row>
@@ -2730,16 +2819,16 @@
       <c r="A26" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B26" s="18">
+      <c r="B26" s="2">
         <v>10</v>
       </c>
-      <c r="C26" s="14" t="s">
+      <c r="C26" s="3" t="s">
         <v>86</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="E26" s="4" t="e" vm="5">
+      <c r="E26" s="4" t="e" vm="11">
         <v>#VALUE!</v>
       </c>
     </row>
@@ -2747,16 +2836,16 @@
       <c r="A27" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B27" s="18">
+      <c r="B27" s="2">
         <v>10</v>
       </c>
-      <c r="C27" s="15" t="s">
+      <c r="C27" s="5" t="s">
         <v>89</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E27" s="4" t="e" vm="6">
+      <c r="E27" s="4" t="e" vm="12">
         <v>#VALUE!</v>
       </c>
     </row>
@@ -2764,16 +2853,16 @@
       <c r="A28" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="B28" s="18">
+      <c r="B28" s="2">
         <v>10</v>
       </c>
-      <c r="C28" s="16" t="s">
+      <c r="C28" s="6" t="s">
         <v>92</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="E28" s="4" t="e" vm="7">
+      <c r="E28" s="4" t="e" vm="13">
         <v>#VALUE!</v>
       </c>
     </row>
@@ -2781,16 +2870,16 @@
       <c r="A29" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="B29" s="18">
+      <c r="B29" s="2">
         <v>10</v>
       </c>
-      <c r="C29" s="17" t="s">
+      <c r="C29" s="7" t="s">
         <v>95</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="E29" s="4" t="e" vm="8">
+      <c r="E29" s="4" t="e" vm="14">
         <v>#VALUE!</v>
       </c>
     </row>
@@ -2798,16 +2887,16 @@
       <c r="A30" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="B30" s="18">
+      <c r="B30" s="2">
         <v>10</v>
       </c>
-      <c r="C30" s="17" t="s">
+      <c r="C30" s="7" t="s">
         <v>98</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="E30" s="4" t="e" vm="5">
+      <c r="E30" s="4" t="e" vm="11">
         <v>#VALUE!</v>
       </c>
     </row>
@@ -2815,16 +2904,16 @@
       <c r="A31" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B31" s="18">
+      <c r="B31" s="2">
         <v>10</v>
       </c>
-      <c r="C31" s="18" t="s">
+      <c r="C31" s="2" t="s">
         <v>101</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="E31" s="4" t="e" vm="4">
+      <c r="E31" s="4" t="e" vm="10">
         <v>#VALUE!</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added final requirememts for Group23; GameTermination
</commit_message>
<xml_diff>
--- a/FinalRequirements.xlsx
+++ b/FinalRequirements.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="579">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="762" uniqueCount="619">
   <si>
     <t xml:space="preserve">Tested By</t>
   </si>
@@ -1457,7 +1457,7 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
         <charset val="1"/>
@@ -1468,7 +1468,7 @@
       <rPr>
         <b val="true"/>
         <sz val="12"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
         <charset val="1"/>
@@ -1478,7 +1478,7 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
         <charset val="1"/>
@@ -1496,7 +1496,7 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
         <charset val="1"/>
@@ -1507,7 +1507,7 @@
       <rPr>
         <b val="true"/>
         <sz val="12"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
         <charset val="1"/>
@@ -1517,7 +1517,7 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
         <charset val="1"/>
@@ -1535,7 +1535,7 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
         <charset val="1"/>
@@ -1546,7 +1546,7 @@
       <rPr>
         <b val="true"/>
         <sz val="12"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
         <charset val="1"/>
@@ -1556,7 +1556,7 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
         <charset val="1"/>
@@ -1848,6 +1848,126 @@
   </si>
   <si>
     <t xml:space="preserve">The leaderboard shall display player statistics such as number of wins and losses.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R211</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The Game must follow the rules the official rules of English draughts </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GameTermination.checkForGameEnd(), hasAnyValiMoves()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R212</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The System shall support 10 consecutive games </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GameTermination.checkForGameEnd()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R213</t>
+  </si>
+  <si>
+    <t xml:space="preserve">After a game concludes players go to the end of the line </t>
+  </si>
+  <si>
+    <t xml:space="preserve">R214</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A leaderboard will be displayed after each game </t>
+  </si>
+  <si>
+    <t xml:space="preserve">R215</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Results of every game played must be stored in a database</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R216</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No game login in HTML/JS; all in java</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R217</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Java Subsystems communicate via methid calls </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GameManager → checkForGameEnd()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R218</t>
+  </si>
+  <si>
+    <t xml:space="preserve">After each move the state is processed and sent ti the client </t>
+  </si>
+  <si>
+    <t xml:space="preserve">checkForGameEnd(), hasAnyValidMoves(), countPieces()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R219</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Java is event driven</t>
+  </si>
+  <si>
+    <t xml:space="preserve">checkForGameEnd()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R220</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Return GameStatus enum in based on board state and move history</t>
+  </si>
+  <si>
+    <t xml:space="preserve">checkForGameEnd(BoardState, List &lt;Move&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R221</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The system shall detect if a player no legal moves left</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GameTermination.hasAnyValidMoves()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R222</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The system shall detec draw by 40-move rule </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GameTermination.is40moveRuleDraw()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R223</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The system shall detect draw by 25 king-only non-capturing moves</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GameTermination.check25MoveRuleKingOnly()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R224</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The system shall detect draw due to threefold board state repetition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GameTermination.checkForThreefoldRepetition()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R225</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The system shall detect mutual stalemate when both players cannot move</t>
   </si>
 </sst>
 </file>
@@ -1904,7 +2024,7 @@
     </font>
     <font>
       <sz val="12"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
@@ -1912,7 +2032,7 @@
     <font>
       <b val="true"/>
       <sz val="12"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
@@ -2202,14 +2322,14 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>324000</xdr:colOff>
-      <xdr:row>203</xdr:row>
-      <xdr:rowOff>104760</xdr:rowOff>
+      <xdr:row>183</xdr:row>
+      <xdr:rowOff>545040</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>5256720</xdr:colOff>
-      <xdr:row>203</xdr:row>
-      <xdr:rowOff>4370760</xdr:rowOff>
+      <xdr:colOff>5255640</xdr:colOff>
+      <xdr:row>191</xdr:row>
+      <xdr:rowOff>85320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2223,8 +2343,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="29116080" y="190997280"/>
-          <a:ext cx="4932720" cy="4266000"/>
+          <a:off x="29116080" y="187175880"/>
+          <a:ext cx="4931640" cy="4264920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2241,14 +2361,14 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>37800</xdr:colOff>
-      <xdr:row>212</xdr:row>
-      <xdr:rowOff>714240</xdr:rowOff>
+      <xdr:row>210</xdr:row>
+      <xdr:rowOff>352080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>990360</xdr:colOff>
-      <xdr:row>215</xdr:row>
-      <xdr:rowOff>18720</xdr:rowOff>
+      <xdr:row>210</xdr:row>
+      <xdr:rowOff>2104560</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp>
       <xdr:nvCxnSpPr>
@@ -2263,7 +2383,7 @@
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
         </a:prstGeom>
-        <a:ln w="6350">
+        <a:ln w="6480">
           <a:noFill/>
         </a:ln>
       </xdr:spPr>
@@ -2274,14 +2394,14 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>212</xdr:row>
-      <xdr:rowOff>904680</xdr:rowOff>
+      <xdr:row>210</xdr:row>
+      <xdr:rowOff>542520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1180800</xdr:colOff>
-      <xdr:row>216</xdr:row>
-      <xdr:rowOff>18720</xdr:rowOff>
+      <xdr:row>210</xdr:row>
+      <xdr:rowOff>2695320</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp>
       <xdr:nvCxnSpPr>
@@ -2296,7 +2416,7 @@
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
         </a:prstGeom>
-        <a:ln w="6350">
+        <a:ln w="6480">
           <a:noFill/>
         </a:ln>
       </xdr:spPr>
@@ -2307,14 +2427,14 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>419040</xdr:colOff>
-      <xdr:row>212</xdr:row>
-      <xdr:rowOff>1095120</xdr:rowOff>
+      <xdr:row>210</xdr:row>
+      <xdr:rowOff>732960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1371600</xdr:colOff>
-      <xdr:row>217</xdr:row>
-      <xdr:rowOff>18720</xdr:rowOff>
+      <xdr:row>210</xdr:row>
+      <xdr:rowOff>3285720</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp>
       <xdr:nvCxnSpPr>
@@ -2329,7 +2449,7 @@
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
         </a:prstGeom>
-        <a:ln w="6350">
+        <a:ln w="6480">
           <a:noFill/>
         </a:ln>
       </xdr:spPr>
@@ -2340,14 +2460,14 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>133200</xdr:colOff>
-      <xdr:row>212</xdr:row>
-      <xdr:rowOff>714240</xdr:rowOff>
+      <xdr:row>210</xdr:row>
+      <xdr:rowOff>352080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1085760</xdr:colOff>
-      <xdr:row>215</xdr:row>
-      <xdr:rowOff>18720</xdr:rowOff>
+      <xdr:row>210</xdr:row>
+      <xdr:rowOff>2104560</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp>
       <xdr:nvCxnSpPr>
@@ -2362,7 +2482,7 @@
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
         </a:prstGeom>
-        <a:ln w="6350">
+        <a:ln w="6480">
           <a:noFill/>
         </a:ln>
       </xdr:spPr>
@@ -2373,14 +2493,14 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>323640</xdr:colOff>
-      <xdr:row>212</xdr:row>
-      <xdr:rowOff>904680</xdr:rowOff>
+      <xdr:row>210</xdr:row>
+      <xdr:rowOff>542520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1276200</xdr:colOff>
-      <xdr:row>216</xdr:row>
-      <xdr:rowOff>18720</xdr:rowOff>
+      <xdr:row>210</xdr:row>
+      <xdr:rowOff>2695320</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp>
       <xdr:nvCxnSpPr>
@@ -2395,7 +2515,7 @@
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
         </a:prstGeom>
-        <a:ln w="6350">
+        <a:ln w="6480">
           <a:noFill/>
         </a:ln>
       </xdr:spPr>
@@ -2406,14 +2526,14 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>212</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>209</xdr:row>
+      <xdr:rowOff>486720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>4628160</xdr:colOff>
-      <xdr:row>213</xdr:row>
-      <xdr:rowOff>37080</xdr:rowOff>
+      <xdr:colOff>4627080</xdr:colOff>
+      <xdr:row>209</xdr:row>
+      <xdr:rowOff>1789560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2426,8 +2546,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="28792080" y="227087280"/>
-          <a:ext cx="4628160" cy="1303920"/>
+          <a:off x="28792080" y="222859440"/>
+          <a:ext cx="4627080" cy="1302840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2444,14 +2564,14 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>38160</xdr:colOff>
-      <xdr:row>204</xdr:row>
-      <xdr:rowOff>66600</xdr:rowOff>
+      <xdr:row>190</xdr:row>
+      <xdr:rowOff>536400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>3285000</xdr:colOff>
-      <xdr:row>204</xdr:row>
-      <xdr:rowOff>2227680</xdr:rowOff>
+      <xdr:colOff>3283920</xdr:colOff>
+      <xdr:row>194</xdr:row>
+      <xdr:rowOff>334080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2464,8 +2584,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="28830240" y="195407280"/>
-          <a:ext cx="3246840" cy="2161080"/>
+          <a:off x="28830240" y="191301120"/>
+          <a:ext cx="3245760" cy="2160000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2482,14 +2602,14 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>3029040</xdr:colOff>
-      <xdr:row>206</xdr:row>
-      <xdr:rowOff>47520</xdr:rowOff>
+      <xdr:row>202</xdr:row>
+      <xdr:rowOff>496440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>5590080</xdr:colOff>
-      <xdr:row>206</xdr:row>
-      <xdr:rowOff>3599280</xdr:rowOff>
+      <xdr:colOff>5589000</xdr:colOff>
+      <xdr:row>203</xdr:row>
+      <xdr:rowOff>3456360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2502,8 +2622,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="31821120" y="203007960"/>
-          <a:ext cx="2561040" cy="3551760"/>
+          <a:off x="31821120" y="198780120"/>
+          <a:ext cx="2559960" cy="3550680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2520,14 +2640,14 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>206</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>202</xdr:row>
+      <xdr:rowOff>448920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>2923200</xdr:colOff>
-      <xdr:row>206</xdr:row>
-      <xdr:rowOff>1703880</xdr:rowOff>
+      <xdr:colOff>2922120</xdr:colOff>
+      <xdr:row>203</xdr:row>
+      <xdr:rowOff>1560960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2540,8 +2660,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="28792080" y="202960440"/>
-          <a:ext cx="2923200" cy="1703880"/>
+          <a:off x="28792080" y="198732600"/>
+          <a:ext cx="2922120" cy="1702800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2558,14 +2678,14 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>204</xdr:row>
-      <xdr:rowOff>3695760</xdr:rowOff>
+      <xdr:row>196</xdr:row>
+      <xdr:rowOff>500400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>5618520</xdr:colOff>
-      <xdr:row>205</xdr:row>
-      <xdr:rowOff>3504240</xdr:rowOff>
+      <xdr:colOff>5617440</xdr:colOff>
+      <xdr:row>202</xdr:row>
+      <xdr:rowOff>142200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2578,8 +2698,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="28792080" y="199036440"/>
-          <a:ext cx="5618520" cy="3618360"/>
+          <a:off x="28792080" y="194808600"/>
+          <a:ext cx="5617440" cy="3617280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2596,14 +2716,14 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>207</xdr:row>
-      <xdr:rowOff>152280</xdr:rowOff>
+      <xdr:row>203</xdr:row>
+      <xdr:rowOff>3820680</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>5637600</xdr:colOff>
-      <xdr:row>207</xdr:row>
-      <xdr:rowOff>3285000</xdr:rowOff>
+      <xdr:colOff>5636520</xdr:colOff>
+      <xdr:row>204</xdr:row>
+      <xdr:rowOff>2504160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2616,8 +2736,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="28792080" y="206922960"/>
-          <a:ext cx="5637600" cy="3132720"/>
+          <a:off x="28792080" y="202695120"/>
+          <a:ext cx="5636520" cy="3131640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2634,14 +2754,14 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>981000</xdr:colOff>
-      <xdr:row>208</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>204</xdr:row>
+      <xdr:rowOff>3030120</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>4047120</xdr:colOff>
-      <xdr:row>208</xdr:row>
-      <xdr:rowOff>3456360</xdr:rowOff>
+      <xdr:colOff>4046040</xdr:colOff>
+      <xdr:row>205</xdr:row>
+      <xdr:rowOff>2675520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2655,8 +2775,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="29773080" y="210580560"/>
-          <a:ext cx="3066120" cy="3456360"/>
+          <a:off x="29773080" y="206352720"/>
+          <a:ext cx="3065040" cy="3455280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2673,14 +2793,14 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>208</xdr:row>
-      <xdr:rowOff>3800520</xdr:rowOff>
+      <xdr:row>205</xdr:row>
+      <xdr:rowOff>3020760</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>3932640</xdr:colOff>
-      <xdr:row>209</xdr:row>
-      <xdr:rowOff>494640</xdr:rowOff>
+      <xdr:colOff>3931560</xdr:colOff>
+      <xdr:row>205</xdr:row>
+      <xdr:rowOff>3523680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2693,8 +2813,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="28792080" y="214381080"/>
-          <a:ext cx="3932640" cy="504000"/>
+          <a:off x="28792080" y="210153240"/>
+          <a:ext cx="3931560" cy="502920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2711,14 +2831,14 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>990720</xdr:colOff>
-      <xdr:row>209</xdr:row>
-      <xdr:rowOff>95400</xdr:rowOff>
+      <xdr:row>205</xdr:row>
+      <xdr:rowOff>3125520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>5561640</xdr:colOff>
-      <xdr:row>209</xdr:row>
-      <xdr:rowOff>1722960</xdr:rowOff>
+      <xdr:colOff>5560560</xdr:colOff>
+      <xdr:row>206</xdr:row>
+      <xdr:rowOff>941760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2731,8 +2851,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="29782800" y="214485840"/>
-          <a:ext cx="4570920" cy="1627560"/>
+          <a:off x="29782800" y="210258000"/>
+          <a:ext cx="4569840" cy="1626480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2749,14 +2869,14 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>295200</xdr:colOff>
-      <xdr:row>209</xdr:row>
-      <xdr:rowOff>1762200</xdr:rowOff>
+      <xdr:row>206</xdr:row>
+      <xdr:rowOff>982080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>5542560</xdr:colOff>
-      <xdr:row>209</xdr:row>
-      <xdr:rowOff>4923360</xdr:rowOff>
+      <xdr:colOff>5541480</xdr:colOff>
+      <xdr:row>207</xdr:row>
+      <xdr:rowOff>332280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2769,8 +2889,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="29087280" y="216152640"/>
-          <a:ext cx="5247360" cy="3161160"/>
+          <a:off x="29087280" y="211924800"/>
+          <a:ext cx="5246280" cy="3160080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2787,14 +2907,14 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>771480</xdr:colOff>
-      <xdr:row>210</xdr:row>
-      <xdr:rowOff>162000</xdr:rowOff>
+      <xdr:row>207</xdr:row>
+      <xdr:rowOff>649080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>4151880</xdr:colOff>
-      <xdr:row>210</xdr:row>
-      <xdr:rowOff>3542400</xdr:rowOff>
+      <xdr:colOff>4150800</xdr:colOff>
+      <xdr:row>208</xdr:row>
+      <xdr:rowOff>218520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2807,8 +2927,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="29563560" y="219629520"/>
-          <a:ext cx="3380400" cy="3380400"/>
+          <a:off x="29563560" y="215401680"/>
+          <a:ext cx="3379320" cy="3379320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2825,14 +2945,14 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>504720</xdr:colOff>
-      <xdr:row>211</xdr:row>
-      <xdr:rowOff>114480</xdr:rowOff>
+      <xdr:row>208</xdr:row>
+      <xdr:rowOff>601560</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>4142160</xdr:colOff>
-      <xdr:row>211</xdr:row>
-      <xdr:rowOff>3742560</xdr:rowOff>
+      <xdr:colOff>4141080</xdr:colOff>
+      <xdr:row>209</xdr:row>
+      <xdr:rowOff>418320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2845,8 +2965,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="29296800" y="223391880"/>
-          <a:ext cx="3637440" cy="3628080"/>
+          <a:off x="29296800" y="219164040"/>
+          <a:ext cx="3636360" cy="3627000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2863,14 +2983,14 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>429840</xdr:colOff>
-      <xdr:row>126</xdr:row>
-      <xdr:rowOff>308520</xdr:rowOff>
+      <xdr:row>119</xdr:row>
+      <xdr:rowOff>867960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>4134240</xdr:colOff>
-      <xdr:row>126</xdr:row>
-      <xdr:rowOff>2250720</xdr:rowOff>
+      <xdr:colOff>4133160</xdr:colOff>
+      <xdr:row>121</xdr:row>
+      <xdr:rowOff>762840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2883,8 +3003,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="29221920" y="118696680"/>
-          <a:ext cx="3704400" cy="1942200"/>
+          <a:off x="29221920" y="116134920"/>
+          <a:ext cx="3703320" cy="1941120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2901,14 +3021,14 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>4822920</xdr:colOff>
-      <xdr:row>125</xdr:row>
-      <xdr:rowOff>567360</xdr:rowOff>
+      <xdr:row>119</xdr:row>
+      <xdr:rowOff>179640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>8170560</xdr:colOff>
-      <xdr:row>126</xdr:row>
-      <xdr:rowOff>1998000</xdr:rowOff>
+      <xdr:colOff>8169480</xdr:colOff>
+      <xdr:row>121</xdr:row>
+      <xdr:rowOff>510480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2921,8 +3041,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="33615000" y="118008000"/>
-          <a:ext cx="3347640" cy="2378160"/>
+          <a:off x="33615000" y="115446600"/>
+          <a:ext cx="3346560" cy="2377080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2939,14 +3059,14 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>522360</xdr:colOff>
-      <xdr:row>128</xdr:row>
-      <xdr:rowOff>225720</xdr:rowOff>
+      <xdr:row>122</xdr:row>
+      <xdr:rowOff>992160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>6807240</xdr:colOff>
-      <xdr:row>128</xdr:row>
-      <xdr:rowOff>1271520</xdr:rowOff>
+      <xdr:colOff>6806160</xdr:colOff>
+      <xdr:row>124</xdr:row>
+      <xdr:rowOff>423360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2959,8 +3079,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="29314440" y="121930560"/>
-          <a:ext cx="6284880" cy="1045800"/>
+          <a:off x="29314440" y="119328120"/>
+          <a:ext cx="6283800" cy="1044720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2977,14 +3097,14 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>675720</xdr:colOff>
-      <xdr:row>131</xdr:row>
-      <xdr:rowOff>232920</xdr:rowOff>
+      <xdr:row>126</xdr:row>
+      <xdr:rowOff>1100880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>7973640</xdr:colOff>
-      <xdr:row>131</xdr:row>
-      <xdr:rowOff>1165320</xdr:rowOff>
+      <xdr:colOff>7972560</xdr:colOff>
+      <xdr:row>126</xdr:row>
+      <xdr:rowOff>2032200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2997,8 +3117,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="29467800" y="126200880"/>
-          <a:ext cx="7297920" cy="932400"/>
+          <a:off x="29467800" y="123598800"/>
+          <a:ext cx="7296840" cy="931320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3015,14 +3135,14 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>214920</xdr:colOff>
-      <xdr:row>133</xdr:row>
-      <xdr:rowOff>198360</xdr:rowOff>
+      <xdr:row>128</xdr:row>
+      <xdr:rowOff>1154880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>6112440</xdr:colOff>
-      <xdr:row>133</xdr:row>
-      <xdr:rowOff>911520</xdr:rowOff>
+      <xdr:colOff>6111360</xdr:colOff>
+      <xdr:row>129</xdr:row>
+      <xdr:rowOff>342000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3035,8 +3155,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="29007000" y="129808800"/>
-          <a:ext cx="5897520" cy="713160"/>
+          <a:off x="29007000" y="127206360"/>
+          <a:ext cx="5896440" cy="712080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3053,14 +3173,14 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>214920</xdr:colOff>
-      <xdr:row>135</xdr:row>
-      <xdr:rowOff>227880</xdr:rowOff>
+      <xdr:row>130</xdr:row>
+      <xdr:rowOff>977040</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>6730560</xdr:colOff>
-      <xdr:row>135</xdr:row>
-      <xdr:rowOff>799200</xdr:rowOff>
+      <xdr:colOff>6729480</xdr:colOff>
+      <xdr:row>131</xdr:row>
+      <xdr:rowOff>21960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3073,8 +3193,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="29007000" y="132681240"/>
-          <a:ext cx="6515640" cy="571320"/>
+          <a:off x="29007000" y="130078800"/>
+          <a:ext cx="6514560" cy="570240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3091,14 +3211,14 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>338040</xdr:colOff>
-      <xdr:row>136</xdr:row>
-      <xdr:rowOff>188280</xdr:rowOff>
+      <xdr:row>131</xdr:row>
+      <xdr:rowOff>359640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>6876360</xdr:colOff>
-      <xdr:row>136</xdr:row>
-      <xdr:rowOff>789840</xdr:rowOff>
+      <xdr:colOff>6875280</xdr:colOff>
+      <xdr:row>131</xdr:row>
+      <xdr:rowOff>960120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3111,8 +3231,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="29130120" y="133589160"/>
-          <a:ext cx="6538320" cy="601560"/>
+          <a:off x="29130120" y="130986720"/>
+          <a:ext cx="6537240" cy="600480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3129,14 +3249,14 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>676080</xdr:colOff>
-      <xdr:row>136</xdr:row>
-      <xdr:rowOff>936000</xdr:rowOff>
+      <xdr:row>131</xdr:row>
+      <xdr:rowOff>1107360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>4085280</xdr:colOff>
-      <xdr:row>138</xdr:row>
-      <xdr:rowOff>9720</xdr:rowOff>
+      <xdr:colOff>4084200</xdr:colOff>
+      <xdr:row>132</xdr:row>
+      <xdr:rowOff>549360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3149,8 +3269,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="29468160" y="134336880"/>
-          <a:ext cx="3409200" cy="968400"/>
+          <a:off x="29468160" y="131734440"/>
+          <a:ext cx="3408120" cy="967320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3167,14 +3287,14 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>276480</xdr:colOff>
-      <xdr:row>138</xdr:row>
-      <xdr:rowOff>334440</xdr:rowOff>
+      <xdr:row>132</xdr:row>
+      <xdr:rowOff>875520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>6530040</xdr:colOff>
-      <xdr:row>139</xdr:row>
-      <xdr:rowOff>48600</xdr:rowOff>
+      <xdr:colOff>6528960</xdr:colOff>
+      <xdr:row>132</xdr:row>
+      <xdr:rowOff>1536120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3187,8 +3307,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="29068560" y="135630000"/>
-          <a:ext cx="6253560" cy="661680"/>
+          <a:off x="29068560" y="133027920"/>
+          <a:ext cx="6252480" cy="660600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3205,14 +3325,14 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>614520</xdr:colOff>
-      <xdr:row>139</xdr:row>
-      <xdr:rowOff>170640</xdr:rowOff>
+      <xdr:row>132</xdr:row>
+      <xdr:rowOff>1659240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>7310160</xdr:colOff>
-      <xdr:row>140</xdr:row>
-      <xdr:rowOff>35280</xdr:rowOff>
+      <xdr:colOff>7309080</xdr:colOff>
+      <xdr:row>133</xdr:row>
+      <xdr:rowOff>249120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3225,8 +3345,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="29406600" y="136413720"/>
-          <a:ext cx="6695640" cy="812160"/>
+          <a:off x="29406600" y="133811640"/>
+          <a:ext cx="6694560" cy="811080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3243,14 +3363,14 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>362520</xdr:colOff>
-      <xdr:row>140</xdr:row>
-      <xdr:rowOff>355320</xdr:rowOff>
+      <xdr:row>133</xdr:row>
+      <xdr:rowOff>570240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>6900840</xdr:colOff>
-      <xdr:row>141</xdr:row>
-      <xdr:rowOff>9720</xdr:rowOff>
+      <xdr:colOff>6899760</xdr:colOff>
+      <xdr:row>134</xdr:row>
+      <xdr:rowOff>147600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3263,8 +3383,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="29154600" y="137545920"/>
-          <a:ext cx="6538320" cy="601560"/>
+          <a:off x="29154600" y="134943840"/>
+          <a:ext cx="6537240" cy="600480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3281,14 +3401,14 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>767880</xdr:colOff>
-      <xdr:row>141</xdr:row>
-      <xdr:rowOff>158760</xdr:rowOff>
+      <xdr:row>134</xdr:row>
+      <xdr:rowOff>297720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>8220240</xdr:colOff>
-      <xdr:row>141</xdr:row>
-      <xdr:rowOff>730080</xdr:rowOff>
+      <xdr:colOff>8219160</xdr:colOff>
+      <xdr:row>134</xdr:row>
+      <xdr:rowOff>867960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3301,8 +3421,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="29559960" y="138296520"/>
-          <a:ext cx="7452360" cy="571320"/>
+          <a:off x="29559960" y="135694440"/>
+          <a:ext cx="7451280" cy="570240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3319,14 +3439,14 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1229040</xdr:colOff>
-      <xdr:row>142</xdr:row>
-      <xdr:rowOff>271080</xdr:rowOff>
+      <xdr:row>134</xdr:row>
+      <xdr:rowOff>1357200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>6082200</xdr:colOff>
-      <xdr:row>143</xdr:row>
-      <xdr:rowOff>286200</xdr:rowOff>
+      <xdr:colOff>6081120</xdr:colOff>
+      <xdr:row>135</xdr:row>
+      <xdr:rowOff>290520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3339,8 +3459,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="30021120" y="139356360"/>
-          <a:ext cx="4853160" cy="962640"/>
+          <a:off x="30021120" y="136753920"/>
+          <a:ext cx="4852080" cy="961560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3357,14 +3477,14 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>583560</xdr:colOff>
-      <xdr:row>147</xdr:row>
-      <xdr:rowOff>790920</xdr:rowOff>
+      <xdr:row>142</xdr:row>
+      <xdr:rowOff>268560</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>8041680</xdr:colOff>
-      <xdr:row>147</xdr:row>
-      <xdr:rowOff>1693080</xdr:rowOff>
+      <xdr:colOff>8040600</xdr:colOff>
+      <xdr:row>143</xdr:row>
+      <xdr:rowOff>146520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3377,8 +3497,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="29375640" y="147456360"/>
-          <a:ext cx="7458120" cy="902160"/>
+          <a:off x="29375640" y="144854280"/>
+          <a:ext cx="7457040" cy="901080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3395,14 +3515,14 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>61200</xdr:colOff>
-      <xdr:row>132</xdr:row>
-      <xdr:rowOff>155880</xdr:rowOff>
+      <xdr:row>126</xdr:row>
+      <xdr:rowOff>2445120</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>5933520</xdr:colOff>
-      <xdr:row>132</xdr:row>
-      <xdr:rowOff>847080</xdr:rowOff>
+      <xdr:colOff>5932440</xdr:colOff>
+      <xdr:row>127</xdr:row>
+      <xdr:rowOff>604800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3415,8 +3535,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="28853280" y="127545120"/>
-          <a:ext cx="5872320" cy="691200"/>
+          <a:off x="28853280" y="124943040"/>
+          <a:ext cx="5871240" cy="690120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3433,14 +3553,14 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>30960</xdr:colOff>
-      <xdr:row>132</xdr:row>
-      <xdr:rowOff>1211400</xdr:rowOff>
+      <xdr:row>127</xdr:row>
+      <xdr:rowOff>970200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>5643000</xdr:colOff>
-      <xdr:row>132</xdr:row>
-      <xdr:rowOff>1876680</xdr:rowOff>
+      <xdr:colOff>5641920</xdr:colOff>
+      <xdr:row>128</xdr:row>
+      <xdr:rowOff>611280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3453,8 +3573,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="28823040" y="128600640"/>
-          <a:ext cx="5612040" cy="665280"/>
+          <a:off x="28823040" y="125998560"/>
+          <a:ext cx="5610960" cy="664200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3471,14 +3591,14 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>6175800</xdr:colOff>
-      <xdr:row>132</xdr:row>
-      <xdr:rowOff>291240</xdr:rowOff>
+      <xdr:row>127</xdr:row>
+      <xdr:rowOff>50040</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>11786400</xdr:colOff>
-      <xdr:row>132</xdr:row>
-      <xdr:rowOff>938160</xdr:rowOff>
+      <xdr:colOff>11785320</xdr:colOff>
+      <xdr:row>127</xdr:row>
+      <xdr:rowOff>695880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3491,8 +3611,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="34967880" y="127680480"/>
-          <a:ext cx="5610600" cy="646920"/>
+          <a:off x="34967880" y="125078400"/>
+          <a:ext cx="5609520" cy="645840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3509,14 +3629,14 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>5838480</xdr:colOff>
-      <xdr:row>132</xdr:row>
-      <xdr:rowOff>1362600</xdr:rowOff>
+      <xdr:row>128</xdr:row>
+      <xdr:rowOff>98280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>10252440</xdr:colOff>
-      <xdr:row>132</xdr:row>
-      <xdr:rowOff>1967400</xdr:rowOff>
+      <xdr:colOff>10251360</xdr:colOff>
+      <xdr:row>128</xdr:row>
+      <xdr:rowOff>702000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3529,8 +3649,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="34630560" y="128751840"/>
-          <a:ext cx="4413960" cy="604800"/>
+          <a:off x="34630560" y="126149760"/>
+          <a:ext cx="4412880" cy="603720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3547,14 +3667,14 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>552960</xdr:colOff>
-      <xdr:row>129</xdr:row>
-      <xdr:rowOff>374760</xdr:rowOff>
+      <xdr:row>124</xdr:row>
+      <xdr:rowOff>948960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>8340480</xdr:colOff>
-      <xdr:row>129</xdr:row>
-      <xdr:rowOff>1307520</xdr:rowOff>
+      <xdr:colOff>8339400</xdr:colOff>
+      <xdr:row>125</xdr:row>
+      <xdr:rowOff>355320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3567,8 +3687,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="29345040" y="123500520"/>
-          <a:ext cx="7787520" cy="932760"/>
+          <a:off x="29345040" y="120898440"/>
+          <a:ext cx="7786440" cy="931680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3585,14 +3705,14 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>616680</xdr:colOff>
-      <xdr:row>146</xdr:row>
-      <xdr:rowOff>930600</xdr:rowOff>
+      <xdr:row>140</xdr:row>
+      <xdr:rowOff>84960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>8404200</xdr:colOff>
-      <xdr:row>146</xdr:row>
-      <xdr:rowOff>1863360</xdr:rowOff>
+      <xdr:colOff>8403120</xdr:colOff>
+      <xdr:row>140</xdr:row>
+      <xdr:rowOff>1016640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3605,8 +3725,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="29408760" y="145226880"/>
-          <a:ext cx="7787520" cy="932760"/>
+          <a:off x="29408760" y="142624800"/>
+          <a:ext cx="7786440" cy="931680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3623,14 +3743,14 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>430200</xdr:colOff>
-      <xdr:row>145</xdr:row>
-      <xdr:rowOff>357840</xdr:rowOff>
+      <xdr:row>138</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>8218800</xdr:colOff>
-      <xdr:row>146</xdr:row>
-      <xdr:rowOff>49680</xdr:rowOff>
+      <xdr:colOff>8217720</xdr:colOff>
+      <xdr:row>139</xdr:row>
+      <xdr:rowOff>226080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3643,8 +3763,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="29222280" y="143232840"/>
-          <a:ext cx="7788600" cy="1113120"/>
+          <a:off x="29222280" y="140630760"/>
+          <a:ext cx="7787520" cy="1112040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3661,14 +3781,14 @@
     <xdr:from>
       <xdr:col>19</xdr:col>
       <xdr:colOff>218520</xdr:colOff>
-      <xdr:row>135</xdr:row>
-      <xdr:rowOff>168120</xdr:rowOff>
+      <xdr:row>130</xdr:row>
+      <xdr:rowOff>917280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>489960</xdr:colOff>
-      <xdr:row>140</xdr:row>
-      <xdr:rowOff>843840</xdr:rowOff>
+      <xdr:colOff>488880</xdr:colOff>
+      <xdr:row>134</xdr:row>
+      <xdr:rowOff>34200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3681,8 +3801,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="77369760" y="132621480"/>
-          <a:ext cx="14655600" cy="5412960"/>
+          <a:off x="77370480" y="130019040"/>
+          <a:ext cx="14654160" cy="5411880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3820,10 +3940,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:T213"/>
+  <dimension ref="A1:T228"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="32" zoomScaleNormal="32" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R3" activeCellId="0" sqref="R3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A211" colorId="64" zoomScale="32" zoomScaleNormal="32" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C230" activeCellId="0" sqref="C230"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="46.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3893,7 +4013,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="46.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
@@ -4465,7 +4585,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="74.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="3" t="s">
         <v>107</v>
       </c>
@@ -4535,7 +4655,7 @@
       <c r="E36" s="5"/>
       <c r="F36" s="5"/>
     </row>
-    <row r="37" customFormat="false" ht="74.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="3" t="s">
         <v>117</v>
       </c>
@@ -4551,7 +4671,7 @@
       <c r="E37" s="5"/>
       <c r="F37" s="5"/>
     </row>
-    <row r="38" customFormat="false" ht="74.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="3" t="s">
         <v>119</v>
       </c>
@@ -4567,7 +4687,7 @@
       <c r="E38" s="5"/>
       <c r="F38" s="5"/>
     </row>
-    <row r="39" customFormat="false" ht="74.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="3" t="s">
         <v>122</v>
       </c>
@@ -4619,7 +4739,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="74.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="3" t="s">
         <v>131</v>
       </c>
@@ -4637,7 +4757,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="74.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="3" t="s">
         <v>134</v>
       </c>
@@ -4669,7 +4789,7 @@
       <c r="E44" s="5"/>
       <c r="F44" s="5"/>
     </row>
-    <row r="45" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="3" t="s">
         <v>139</v>
       </c>
@@ -4701,7 +4821,7 @@
       <c r="E46" s="5"/>
       <c r="F46" s="5"/>
     </row>
-    <row r="47" customFormat="false" ht="74.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="3" t="s">
         <v>144</v>
       </c>
@@ -4751,7 +4871,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="120.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="3" t="s">
         <v>150</v>
       </c>
@@ -4769,7 +4889,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="74.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="3" t="s">
         <v>152</v>
       </c>
@@ -5131,7 +5251,7 @@
       <c r="E73" s="5"/>
       <c r="F73" s="5"/>
     </row>
-    <row r="74" customFormat="false" ht="74.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="3" t="s">
         <v>210</v>
       </c>
@@ -5175,7 +5295,7 @@
       <c r="E76" s="5"/>
       <c r="F76" s="5"/>
     </row>
-    <row r="77" customFormat="false" ht="74.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="3" t="s">
         <v>217</v>
       </c>
@@ -5253,7 +5373,7 @@
       <c r="E81" s="5"/>
       <c r="F81" s="5"/>
     </row>
-    <row r="82" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="3" t="s">
         <v>231</v>
       </c>
@@ -5269,7 +5389,7 @@
       <c r="E82" s="5"/>
       <c r="F82" s="5"/>
     </row>
-    <row r="83" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="3" t="s">
         <v>234</v>
       </c>
@@ -5285,7 +5405,7 @@
       <c r="E83" s="5"/>
       <c r="F83" s="5"/>
     </row>
-    <row r="84" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="3" t="s">
         <v>236</v>
       </c>
@@ -5349,7 +5469,7 @@
       <c r="E87" s="5"/>
       <c r="F87" s="5"/>
     </row>
-    <row r="88" customFormat="false" ht="74.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="3" t="s">
         <v>246</v>
       </c>
@@ -5365,7 +5485,7 @@
       <c r="E88" s="5"/>
       <c r="F88" s="5"/>
     </row>
-    <row r="89" customFormat="false" ht="74.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="3" t="s">
         <v>249</v>
       </c>
@@ -5381,7 +5501,7 @@
       <c r="E89" s="5"/>
       <c r="F89" s="5"/>
     </row>
-    <row r="90" customFormat="false" ht="74.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="3" t="s">
         <v>251</v>
       </c>
@@ -5397,7 +5517,7 @@
       <c r="E90" s="5"/>
       <c r="F90" s="5"/>
     </row>
-    <row r="91" customFormat="false" ht="74.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="3" t="s">
         <v>253</v>
       </c>
@@ -5413,7 +5533,7 @@
       <c r="E91" s="5"/>
       <c r="F91" s="5"/>
     </row>
-    <row r="92" customFormat="false" ht="74.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="3" t="s">
         <v>255</v>
       </c>
@@ -5429,7 +5549,7 @@
       <c r="E92" s="5"/>
       <c r="F92" s="5"/>
     </row>
-    <row r="93" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" customFormat="false" ht="120.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="3" t="s">
         <v>257</v>
       </c>
@@ -5457,7 +5577,7 @@
       <c r="E94" s="5"/>
       <c r="F94" s="5"/>
     </row>
-    <row r="95" customFormat="false" ht="74.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="3" t="s">
         <v>261</v>
       </c>
@@ -5493,7 +5613,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="74.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="3" t="s">
         <v>266</v>
       </c>
@@ -5525,7 +5645,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="74.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="3" t="s">
         <v>270</v>
       </c>
@@ -5541,7 +5661,7 @@
       <c r="E99" s="5"/>
       <c r="F99" s="5"/>
     </row>
-    <row r="100" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="120.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="3" t="s">
         <v>272</v>
       </c>
@@ -5589,7 +5709,7 @@
       <c r="E102" s="5"/>
       <c r="F102" s="5"/>
     </row>
-    <row r="103" customFormat="false" ht="74.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="103" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="3" t="s">
         <v>280</v>
       </c>
@@ -5619,7 +5739,7 @@
       <c r="E104" s="5"/>
       <c r="F104" s="5"/>
     </row>
-    <row r="105" customFormat="false" ht="74.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="105" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="3" t="s">
         <v>285</v>
       </c>
@@ -5683,7 +5803,7 @@
       <c r="E108" s="5"/>
       <c r="F108" s="5"/>
     </row>
-    <row r="109" customFormat="false" ht="74.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="109" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="3" t="s">
         <v>293</v>
       </c>
@@ -5863,7 +5983,7 @@
       <c r="E119" s="5"/>
       <c r="F119" s="5"/>
     </row>
-    <row r="120" customFormat="false" ht="74.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="120" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="3" t="s">
         <v>321</v>
       </c>
@@ -5879,7 +5999,7 @@
       <c r="E120" s="5"/>
       <c r="F120" s="5"/>
     </row>
-    <row r="121" customFormat="false" ht="74.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="121" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="3" t="s">
         <v>324</v>
       </c>
@@ -5897,7 +6017,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="122" customFormat="false" ht="74.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="122" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="3" t="s">
         <v>326</v>
       </c>
@@ -5915,7 +6035,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="123" customFormat="false" ht="74.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="123" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="3" t="s">
         <v>328</v>
       </c>
@@ -5949,7 +6069,7 @@
       <c r="E124" s="5"/>
       <c r="F124" s="5"/>
     </row>
-    <row r="125" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="125" customFormat="false" ht="120.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="3" t="s">
         <v>333</v>
       </c>
@@ -5967,7 +6087,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="126" customFormat="false" ht="74.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="126" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="3" t="s">
         <v>335</v>
       </c>
@@ -5985,7 +6105,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="127" customFormat="false" ht="186.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="127" customFormat="false" ht="199.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="3" t="s">
         <v>337</v>
       </c>
@@ -6001,7 +6121,7 @@
       <c r="E127" s="5"/>
       <c r="F127" s="5"/>
     </row>
-    <row r="128" s="15" customFormat="true" ht="74.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="128" s="15" customFormat="true" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="11" t="s">
         <v>340</v>
       </c>
@@ -6019,7 +6139,7 @@
       </c>
       <c r="F128" s="14"/>
     </row>
-    <row r="129" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="129" customFormat="false" ht="120.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="3" t="s">
         <v>344</v>
       </c>
@@ -6035,7 +6155,7 @@
       <c r="E129" s="5"/>
       <c r="F129" s="5"/>
     </row>
-    <row r="130" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="130" customFormat="false" ht="120.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="3" t="s">
         <v>347</v>
       </c>
@@ -6051,7 +6171,7 @@
       <c r="E130" s="5"/>
       <c r="F130" s="5"/>
     </row>
-    <row r="131" s="15" customFormat="true" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="131" s="15" customFormat="true" ht="120.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="11" t="s">
         <v>349</v>
       </c>
@@ -6069,7 +6189,7 @@
       </c>
       <c r="F131" s="14"/>
     </row>
-    <row r="132" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="132" customFormat="false" ht="120.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="3" t="s">
         <v>352</v>
       </c>
@@ -6101,7 +6221,7 @@
       <c r="E133" s="5"/>
       <c r="F133" s="5"/>
     </row>
-    <row r="134" customFormat="false" ht="74.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="134" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="3" t="s">
         <v>358</v>
       </c>
@@ -6117,7 +6237,7 @@
       <c r="E134" s="5"/>
       <c r="F134" s="5"/>
     </row>
-    <row r="135" customFormat="false" ht="149.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="135" customFormat="false" ht="159.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="11" t="s">
         <v>361</v>
       </c>
@@ -6135,7 +6255,7 @@
       </c>
       <c r="F135" s="14"/>
     </row>
-    <row r="136" customFormat="false" ht="74.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="136" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="3" t="s">
         <v>365</v>
       </c>
@@ -6151,7 +6271,7 @@
       <c r="E136" s="5"/>
       <c r="F136" s="5"/>
     </row>
-    <row r="137" customFormat="false" ht="74.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="137" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="3" t="s">
         <v>368</v>
       </c>
@@ -6167,7 +6287,7 @@
       <c r="E137" s="5"/>
       <c r="F137" s="5"/>
     </row>
-    <row r="138" customFormat="false" ht="74.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="138" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="3" t="s">
         <v>370</v>
       </c>
@@ -6183,7 +6303,7 @@
       <c r="E138" s="5"/>
       <c r="F138" s="5"/>
     </row>
-    <row r="139" customFormat="false" ht="74.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="139" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="3" t="s">
         <v>373</v>
       </c>
@@ -6199,7 +6319,7 @@
       <c r="E139" s="5"/>
       <c r="F139" s="5"/>
     </row>
-    <row r="140" customFormat="false" ht="74.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="140" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="3" t="s">
         <v>375</v>
       </c>
@@ -6215,7 +6335,7 @@
       <c r="E140" s="5"/>
       <c r="F140" s="5"/>
     </row>
-    <row r="141" customFormat="false" ht="74.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="141" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="3" t="s">
         <v>378</v>
       </c>
@@ -6231,7 +6351,7 @@
       <c r="E141" s="5"/>
       <c r="F141" s="5"/>
     </row>
-    <row r="142" customFormat="false" ht="74.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="142" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="3" t="s">
         <v>380</v>
       </c>
@@ -6247,7 +6367,7 @@
       <c r="E142" s="5"/>
       <c r="F142" s="5"/>
     </row>
-    <row r="143" customFormat="false" ht="74.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="143" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="3" t="s">
         <v>382</v>
       </c>
@@ -6263,7 +6383,7 @@
       <c r="E143" s="5"/>
       <c r="F143" s="5"/>
     </row>
-    <row r="144" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="144" customFormat="false" ht="120.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="18" t="s">
         <v>384</v>
       </c>
@@ -6281,7 +6401,7 @@
       </c>
       <c r="F144" s="21"/>
     </row>
-    <row r="145" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="145" customFormat="false" ht="120.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="3" t="s">
         <v>388</v>
       </c>
@@ -6297,7 +6417,7 @@
       <c r="E145" s="5"/>
       <c r="F145" s="5"/>
     </row>
-    <row r="146" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="146" customFormat="false" ht="120.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="3" t="s">
         <v>391</v>
       </c>
@@ -6313,7 +6433,7 @@
       <c r="E146" s="5"/>
       <c r="F146" s="5"/>
     </row>
-    <row r="147" customFormat="false" ht="186.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="147" customFormat="false" ht="199.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="3" t="s">
         <v>394</v>
       </c>
@@ -6329,7 +6449,7 @@
       <c r="E147" s="5"/>
       <c r="F147" s="5"/>
     </row>
-    <row r="148" customFormat="false" ht="186.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="148" customFormat="false" ht="199.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="3" t="s">
         <v>397</v>
       </c>
@@ -6345,7 +6465,7 @@
       <c r="E148" s="5"/>
       <c r="F148" s="5"/>
     </row>
-    <row r="149" s="15" customFormat="true" ht="149.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="149" s="15" customFormat="true" ht="159.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="11" t="s">
         <v>400</v>
       </c>
@@ -6363,7 +6483,7 @@
       </c>
       <c r="F149" s="14"/>
     </row>
-    <row r="150" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="150" customFormat="false" ht="120.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="3" t="s">
         <v>403</v>
       </c>
@@ -6379,7 +6499,7 @@
       <c r="E150" s="5"/>
       <c r="F150" s="5"/>
     </row>
-    <row r="151" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="151" customFormat="false" ht="120.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="3" t="s">
         <v>406</v>
       </c>
@@ -6411,7 +6531,7 @@
       <c r="E152" s="5"/>
       <c r="F152" s="5"/>
     </row>
-    <row r="153" customFormat="false" ht="74.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="153" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="3" t="s">
         <v>412</v>
       </c>
@@ -6429,7 +6549,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="154" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="154" customFormat="false" ht="120.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="3" t="s">
         <v>415</v>
       </c>
@@ -6447,7 +6567,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="155" customFormat="false" ht="74.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="155" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="3" t="s">
         <v>418</v>
       </c>
@@ -6465,7 +6585,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="156" customFormat="false" ht="74.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="156" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="3" t="s">
         <v>421</v>
       </c>
@@ -6501,7 +6621,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="158" customFormat="false" ht="74.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="158" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="3" t="s">
         <v>425</v>
       </c>
@@ -6519,7 +6639,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="159" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="159" customFormat="false" ht="120.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="3" t="s">
         <v>428</v>
       </c>
@@ -6537,7 +6657,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="160" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="160" customFormat="false" ht="120.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="3" t="s">
         <v>431</v>
       </c>
@@ -6555,7 +6675,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="161" customFormat="false" ht="149.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="161" customFormat="false" ht="159.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="3" t="s">
         <v>434</v>
       </c>
@@ -6573,7 +6693,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="162" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="162" customFormat="false" ht="159.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="3" t="s">
         <v>437</v>
       </c>
@@ -7237,7 +7357,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="199" customFormat="false" ht="74.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="199" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="3" t="s">
         <v>542</v>
       </c>
@@ -7474,6 +7594,210 @@
       </c>
       <c r="D213" s="1" t="s">
         <v>559</v>
+      </c>
+    </row>
+    <row r="214" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A214" s="1" t="s">
+        <v>579</v>
+      </c>
+      <c r="B214" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="C214" s="2" t="s">
+        <v>580</v>
+      </c>
+      <c r="D214" s="1" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="215" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A215" s="1" t="s">
+        <v>582</v>
+      </c>
+      <c r="B215" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="C215" s="2" t="s">
+        <v>583</v>
+      </c>
+      <c r="D215" s="1" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="216" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A216" s="1" t="s">
+        <v>585</v>
+      </c>
+      <c r="B216" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="C216" s="2" t="s">
+        <v>586</v>
+      </c>
+      <c r="D216" s="1" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="217" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A217" s="1" t="s">
+        <v>587</v>
+      </c>
+      <c r="B217" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="C217" s="2" t="s">
+        <v>588</v>
+      </c>
+      <c r="D217" s="1" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="218" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A218" s="1" t="s">
+        <v>589</v>
+      </c>
+      <c r="B218" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="C218" s="2" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="219" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A219" s="1" t="s">
+        <v>591</v>
+      </c>
+      <c r="B219" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="C219" s="2" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="220" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A220" s="1" t="s">
+        <v>593</v>
+      </c>
+      <c r="B220" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="C220" s="2" t="s">
+        <v>594</v>
+      </c>
+      <c r="D220" s="1" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="221" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A221" s="1" t="s">
+        <v>596</v>
+      </c>
+      <c r="B221" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="C221" s="2" t="s">
+        <v>597</v>
+      </c>
+      <c r="D221" s="1" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="222" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A222" s="1" t="s">
+        <v>599</v>
+      </c>
+      <c r="B222" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="C222" s="2" t="s">
+        <v>600</v>
+      </c>
+      <c r="D222" s="1" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="223" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A223" s="1" t="s">
+        <v>602</v>
+      </c>
+      <c r="B223" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="C223" s="2" t="s">
+        <v>603</v>
+      </c>
+      <c r="D223" s="1" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="224" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A224" s="1" t="s">
+        <v>605</v>
+      </c>
+      <c r="B224" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="C224" s="2" t="s">
+        <v>606</v>
+      </c>
+      <c r="D224" s="1" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="225" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A225" s="1" t="s">
+        <v>608</v>
+      </c>
+      <c r="B225" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="C225" s="2" t="s">
+        <v>609</v>
+      </c>
+      <c r="D225" s="1" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="226" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A226" s="1" t="s">
+        <v>611</v>
+      </c>
+      <c r="B226" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="C226" s="2" t="s">
+        <v>612</v>
+      </c>
+      <c r="D226" s="1" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="227" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A227" s="1" t="s">
+        <v>614</v>
+      </c>
+      <c r="B227" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="C227" s="2" t="s">
+        <v>615</v>
+      </c>
+      <c r="D227" s="1" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="228" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A228" s="1" t="s">
+        <v>617</v>
+      </c>
+      <c r="B228" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="C228" s="2" t="s">
+        <v>618</v>
+      </c>
+      <c r="D228" s="1" t="s">
+        <v>607</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Test Database.db file in Final Requirements from Group 23
</commit_message>
<xml_diff>
--- a/FinalRequirements.xlsx
+++ b/FinalRequirements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mavsuta-my.sharepoint.com/personal/axr0602_mavs_uta_edu/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Khang Lam\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B5BA81BC-3A1C-694D-9C2C-F3A4D232CB4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EB38EA5-6F38-466D-80ED-212B2710E0EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="740" windowWidth="20960" windowHeight="9720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51480" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="983" uniqueCount="647">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="997" uniqueCount="649">
   <si>
     <t>Testing</t>
   </si>
@@ -1579,7 +1579,6 @@
         <sz val="12"/>
         <color indexed="64"/>
         <rFont val="Times New Roman"/>
-        <family val="1"/>
       </rPr>
       <t xml:space="preserve">Must communicate with the </t>
     </r>
@@ -1589,7 +1588,6 @@
         <sz val="12"/>
         <color indexed="64"/>
         <rFont val="Times New Roman"/>
-        <family val="1"/>
       </rPr>
       <t>Pair Up</t>
     </r>
@@ -1598,7 +1596,6 @@
         <sz val="12"/>
         <color indexed="64"/>
         <rFont val="Times New Roman"/>
-        <family val="1"/>
       </rPr>
       <t xml:space="preserve"> module to assign users to games</t>
     </r>
@@ -1615,7 +1612,6 @@
         <sz val="12"/>
         <color indexed="64"/>
         <rFont val="Times New Roman"/>
-        <family val="1"/>
       </rPr>
       <t xml:space="preserve">Must route requests and responses to/from the </t>
     </r>
@@ -1625,7 +1621,6 @@
         <sz val="12"/>
         <color indexed="64"/>
         <rFont val="Times New Roman"/>
-        <family val="1"/>
       </rPr>
       <t>Game Play</t>
     </r>
@@ -1634,7 +1629,6 @@
         <sz val="12"/>
         <color indexed="64"/>
         <rFont val="Times New Roman"/>
-        <family val="1"/>
       </rPr>
       <t xml:space="preserve"> module</t>
     </r>
@@ -1651,7 +1645,6 @@
         <sz val="12"/>
         <color indexed="64"/>
         <rFont val="Times New Roman"/>
-        <family val="1"/>
       </rPr>
       <t xml:space="preserve">Must communicate with </t>
     </r>
@@ -1661,7 +1654,6 @@
         <sz val="12"/>
         <color indexed="64"/>
         <rFont val="Times New Roman"/>
-        <family val="1"/>
       </rPr>
       <t>Bot 1</t>
     </r>
@@ -1670,7 +1662,6 @@
         <sz val="12"/>
         <color indexed="64"/>
         <rFont val="Times New Roman"/>
-        <family val="1"/>
       </rPr>
       <t xml:space="preserve"> for automated player moves when required</t>
     </r>
@@ -2091,13 +2082,19 @@
   </si>
   <si>
     <t>The system shall detect mutual stalemate when both players cannot move</t>
+  </si>
+  <si>
+    <t>User DB has 5 rows and 6 columns and Match DB have only 1 rows and 6 clumns (no data records)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BoardState is in 4th column correctly </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2112,40 +2109,33 @@
       <sz val="36"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
-      <family val="1"/>
     </font>
     <font>
       <sz val="36"/>
       <color theme="1"/>
       <name val="ＭＳ 明朝"/>
-      <family val="1"/>
-      <charset val="128"/>
     </font>
     <font>
       <sz val="36"/>
       <color indexed="64"/>
       <name val="Times New Roman"/>
-      <family val="1"/>
     </font>
     <font>
       <i/>
       <sz val="36"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
-      <family val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color indexed="64"/>
       <name val="Times New Roman"/>
-      <family val="1"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color indexed="64"/>
       <name val="Times New Roman"/>
-      <family val="1"/>
     </font>
   </fonts>
   <fills count="10">
@@ -2839,7 +2829,7 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>6804799</xdr:colOff>
       <xdr:row>124</xdr:row>
-      <xdr:rowOff>423361</xdr:rowOff>
+      <xdr:rowOff>423362</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2883,7 +2873,7 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>7973921</xdr:colOff>
       <xdr:row>127</xdr:row>
-      <xdr:rowOff>591883</xdr:rowOff>
+      <xdr:rowOff>591884</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2927,7 +2917,7 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>6114081</xdr:colOff>
       <xdr:row>129</xdr:row>
-      <xdr:rowOff>342001</xdr:rowOff>
+      <xdr:rowOff>342002</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2971,7 +2961,7 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>6728118</xdr:colOff>
       <xdr:row>131</xdr:row>
-      <xdr:rowOff>40974</xdr:rowOff>
+      <xdr:rowOff>40975</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3015,7 +3005,7 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>6878001</xdr:colOff>
       <xdr:row>132</xdr:row>
-      <xdr:rowOff>10568</xdr:rowOff>
+      <xdr:rowOff>10567</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3059,7 +3049,7 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>4085560</xdr:colOff>
       <xdr:row>132</xdr:row>
-      <xdr:rowOff>552079</xdr:rowOff>
+      <xdr:rowOff>552078</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3147,7 +3137,7 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>7307719</xdr:colOff>
       <xdr:row>133</xdr:row>
-      <xdr:rowOff>251840</xdr:rowOff>
+      <xdr:rowOff>251841</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3191,7 +3181,7 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>6899759</xdr:colOff>
       <xdr:row>134</xdr:row>
-      <xdr:rowOff>146239</xdr:rowOff>
+      <xdr:rowOff>146238</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3279,7 +3269,7 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>6083841</xdr:colOff>
       <xdr:row>135</xdr:row>
-      <xdr:rowOff>289160</xdr:rowOff>
+      <xdr:rowOff>289161</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3455,7 +3445,7 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>10245161</xdr:colOff>
       <xdr:row>128</xdr:row>
-      <xdr:rowOff>8028</xdr:rowOff>
+      <xdr:rowOff>8027</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3499,7 +3489,7 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>10248861</xdr:colOff>
       <xdr:row>129</xdr:row>
-      <xdr:rowOff>6449</xdr:rowOff>
+      <xdr:rowOff>6450</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3543,7 +3533,7 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>8339400</xdr:colOff>
       <xdr:row>125</xdr:row>
-      <xdr:rowOff>356680</xdr:rowOff>
+      <xdr:rowOff>356679</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3631,7 +3621,7 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>8216359</xdr:colOff>
       <xdr:row>139</xdr:row>
-      <xdr:rowOff>226078</xdr:rowOff>
+      <xdr:rowOff>226077</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3917,7 +3907,7 @@
       <xdr:col>11</xdr:col>
       <xdr:colOff>3534268</xdr:colOff>
       <xdr:row>132</xdr:row>
-      <xdr:rowOff>210902</xdr:rowOff>
+      <xdr:rowOff>210901</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4127,7 +4117,7 @@
       <xdr:col>11</xdr:col>
       <xdr:colOff>3553321</xdr:colOff>
       <xdr:row>134</xdr:row>
-      <xdr:rowOff>296639</xdr:rowOff>
+      <xdr:rowOff>296638</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4295,7 +4285,7 @@
       <xdr:col>11</xdr:col>
       <xdr:colOff>3515216</xdr:colOff>
       <xdr:row>139</xdr:row>
-      <xdr:rowOff>31225</xdr:rowOff>
+      <xdr:rowOff>31224</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4620,6 +4610,94 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>309561</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>23813</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>9492943</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>2548290</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="52" name="Picture 51">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{997A4CD6-72FC-88E0-57E8-ABACB5D1BE5E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId38"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="87368061" y="124515563"/>
+          <a:ext cx="9183382" cy="2524477"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>166688</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>5349011</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>2824533</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Picture 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4182A9BC-C76E-3AA9-A7E1-8355FCB0B4F0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId39"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="87225188" y="130968750"/>
+          <a:ext cx="5182323" cy="2657846"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4765,41 +4843,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:T228"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G152" zoomScale="23" workbookViewId="0">
-      <selection activeCell="P153" sqref="P153"/>
+    <sheetView tabSelected="1" topLeftCell="F50" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="Q55" sqref="Q55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="47"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="46.5" x14ac:dyDescent="0.7"/>
   <cols>
     <col min="1" max="1" width="21" style="1" customWidth="1"/>
-    <col min="2" max="2" width="19.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="161.5" style="2" customWidth="1"/>
-    <col min="4" max="4" width="250.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="210.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="164.33203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="161.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="250.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="210.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="164.28515625" style="3" customWidth="1"/>
     <col min="7" max="7" width="34" style="1" customWidth="1"/>
-    <col min="8" max="8" width="34.83203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="30.1640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="38.6640625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="34.1640625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="131" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="34.85546875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="30.140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="38.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="34.140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="167.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="33" style="1" customWidth="1"/>
-    <col min="14" max="14" width="46.5" style="1" customWidth="1"/>
+    <col min="14" max="14" width="46.42578125" style="1" customWidth="1"/>
     <col min="15" max="15" width="33" style="1" customWidth="1"/>
-    <col min="16" max="16" width="27.5" style="1" customWidth="1"/>
-    <col min="17" max="17" width="30.1640625" style="1" customWidth="1"/>
-    <col min="18" max="18" width="40.1640625" style="1" customWidth="1"/>
-    <col min="19" max="19" width="8.83203125" style="1"/>
-    <col min="20" max="20" width="153.1640625" style="1" customWidth="1"/>
-    <col min="21" max="16384" width="8.83203125" style="1"/>
+    <col min="16" max="16" width="27.42578125" style="1" customWidth="1"/>
+    <col min="17" max="17" width="255.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="40.140625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="8.85546875" style="1"/>
+    <col min="20" max="20" width="153.140625" style="1" customWidth="1"/>
+    <col min="21" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.7">
       <c r="L2" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="48">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.7">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -4855,7 +4933,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="96">
+    <row r="4" spans="1:20" ht="139.5" x14ac:dyDescent="0.7">
       <c r="A4" s="9" t="s">
         <v>19</v>
       </c>
@@ -4891,7 +4969,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="291" customHeight="1">
+    <row r="5" spans="1:20" ht="92.25" x14ac:dyDescent="0.7">
       <c r="A5" s="9" t="s">
         <v>24</v>
       </c>
@@ -4923,7 +5001,7 @@
       <c r="Q5" s="4"/>
       <c r="R5" s="4"/>
     </row>
-    <row r="6" spans="1:20" ht="285.75" customHeight="1">
+    <row r="6" spans="1:20" ht="285.75" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A6" s="9" t="s">
         <v>27</v>
       </c>
@@ -4955,7 +5033,7 @@
       <c r="Q6" s="4"/>
       <c r="R6" s="4"/>
     </row>
-    <row r="7" spans="1:20" ht="287.25" customHeight="1">
+    <row r="7" spans="1:20" ht="287.25" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A7" s="9" t="s">
         <v>30</v>
       </c>
@@ -4987,7 +5065,7 @@
       <c r="Q7" s="4"/>
       <c r="R7" s="4"/>
     </row>
-    <row r="8" spans="1:20" ht="329.25" customHeight="1">
+    <row r="8" spans="1:20" ht="329.25" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A8" s="9" t="s">
         <v>33</v>
       </c>
@@ -5019,7 +5097,7 @@
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
     </row>
-    <row r="9" spans="1:20" ht="140">
+    <row r="9" spans="1:20" ht="138" x14ac:dyDescent="0.7">
       <c r="A9" s="9" t="s">
         <v>36</v>
       </c>
@@ -5048,10 +5126,12 @@
       <c r="N9" s="4"/>
       <c r="O9" s="4"/>
       <c r="P9" s="4"/>
-      <c r="Q9" s="4"/>
+      <c r="Q9" s="4" t="s">
+        <v>38</v>
+      </c>
       <c r="R9" s="4"/>
     </row>
-    <row r="10" spans="1:20" ht="318" customHeight="1">
+    <row r="10" spans="1:20" ht="318" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A10" s="9" t="s">
         <v>39</v>
       </c>
@@ -5083,7 +5163,7 @@
       <c r="Q10" s="4"/>
       <c r="R10" s="4"/>
     </row>
-    <row r="11" spans="1:20" ht="318" customHeight="1">
+    <row r="11" spans="1:20" ht="318" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A11" s="9" t="s">
         <v>43</v>
       </c>
@@ -5115,7 +5195,7 @@
       <c r="Q11" s="4"/>
       <c r="R11" s="4"/>
     </row>
-    <row r="12" spans="1:20" ht="334.5" customHeight="1">
+    <row r="12" spans="1:20" ht="334.5" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A12" s="9" t="s">
         <v>47</v>
       </c>
@@ -5147,7 +5227,7 @@
       <c r="Q12" s="4"/>
       <c r="R12" s="4"/>
     </row>
-    <row r="13" spans="1:20" ht="313.5" customHeight="1">
+    <row r="13" spans="1:20" ht="313.5" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A13" s="9" t="s">
         <v>50</v>
       </c>
@@ -5179,7 +5259,7 @@
       <c r="Q13" s="4"/>
       <c r="R13" s="4"/>
     </row>
-    <row r="14" spans="1:20" ht="250" customHeight="1">
+    <row r="14" spans="1:20" ht="249.95" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A14" s="9" t="s">
         <v>54</v>
       </c>
@@ -5211,7 +5291,7 @@
       <c r="Q14" s="4"/>
       <c r="R14" s="4"/>
     </row>
-    <row r="15" spans="1:20" ht="400" customHeight="1">
+    <row r="15" spans="1:20" ht="399.95" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A15" s="9" t="s">
         <v>58</v>
       </c>
@@ -5243,7 +5323,7 @@
       <c r="Q15" s="4"/>
       <c r="R15" s="4"/>
     </row>
-    <row r="16" spans="1:20" ht="94">
+    <row r="16" spans="1:20" ht="92.25" x14ac:dyDescent="0.7">
       <c r="A16" s="9" t="s">
         <v>62</v>
       </c>
@@ -5273,7 +5353,7 @@
       <c r="Q16" s="4"/>
       <c r="R16" s="4"/>
     </row>
-    <row r="17" spans="1:18" ht="250" customHeight="1">
+    <row r="17" spans="1:18" ht="249.95" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A17" s="9" t="s">
         <v>66</v>
       </c>
@@ -5305,7 +5385,7 @@
       <c r="Q17" s="4"/>
       <c r="R17" s="4"/>
     </row>
-    <row r="18" spans="1:18" ht="250" customHeight="1">
+    <row r="18" spans="1:18" ht="249.95" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A18" s="9" t="s">
         <v>70</v>
       </c>
@@ -5337,7 +5417,7 @@
       <c r="Q18" s="4"/>
       <c r="R18" s="4"/>
     </row>
-    <row r="19" spans="1:18" ht="94">
+    <row r="19" spans="1:18" ht="92.25" x14ac:dyDescent="0.7">
       <c r="A19" s="9" t="s">
         <v>73</v>
       </c>
@@ -5367,7 +5447,7 @@
       <c r="Q19" s="4"/>
       <c r="R19" s="4"/>
     </row>
-    <row r="20" spans="1:18" ht="250" customHeight="1">
+    <row r="20" spans="1:18" ht="249.95" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A20" s="9" t="s">
         <v>76</v>
       </c>
@@ -5399,7 +5479,7 @@
       <c r="Q20" s="4"/>
       <c r="R20" s="4"/>
     </row>
-    <row r="21" spans="1:18" ht="199.5" customHeight="1">
+    <row r="21" spans="1:18" ht="199.5" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A21" s="9" t="s">
         <v>80</v>
       </c>
@@ -5431,7 +5511,7 @@
       <c r="Q21" s="4"/>
       <c r="R21" s="4"/>
     </row>
-    <row r="22" spans="1:18" ht="350" customHeight="1">
+    <row r="22" spans="1:18" ht="350.1" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A22" s="9" t="s">
         <v>84</v>
       </c>
@@ -5463,7 +5543,7 @@
       <c r="Q22" s="4"/>
       <c r="R22" s="4"/>
     </row>
-    <row r="23" spans="1:18" ht="300" customHeight="1">
+    <row r="23" spans="1:18" ht="300" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A23" s="9" t="s">
         <v>87</v>
       </c>
@@ -5495,7 +5575,7 @@
       <c r="Q23" s="4"/>
       <c r="R23" s="4"/>
     </row>
-    <row r="24" spans="1:18" ht="350" customHeight="1">
+    <row r="24" spans="1:18" ht="350.1" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A24" s="9" t="s">
         <v>90</v>
       </c>
@@ -5527,7 +5607,7 @@
       <c r="Q24" s="4"/>
       <c r="R24" s="4"/>
     </row>
-    <row r="25" spans="1:18" ht="350" customHeight="1">
+    <row r="25" spans="1:18" ht="350.1" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A25" s="9" t="s">
         <v>93</v>
       </c>
@@ -5559,7 +5639,7 @@
       <c r="Q25" s="4"/>
       <c r="R25" s="4"/>
     </row>
-    <row r="26" spans="1:18" ht="350" customHeight="1">
+    <row r="26" spans="1:18" ht="350.1" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A26" s="9" t="s">
         <v>96</v>
       </c>
@@ -5591,7 +5671,7 @@
       <c r="Q26" s="4"/>
       <c r="R26" s="4"/>
     </row>
-    <row r="27" spans="1:18" ht="400" customHeight="1">
+    <row r="27" spans="1:18" ht="399.95" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A27" s="9" t="s">
         <v>99</v>
       </c>
@@ -5623,7 +5703,7 @@
       <c r="Q27" s="4"/>
       <c r="R27" s="4"/>
     </row>
-    <row r="28" spans="1:18" ht="300" customHeight="1">
+    <row r="28" spans="1:18" ht="300" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A28" s="11" t="s">
         <v>102</v>
       </c>
@@ -5655,7 +5735,7 @@
       <c r="Q28" s="4"/>
       <c r="R28" s="4"/>
     </row>
-    <row r="29" spans="1:18" ht="94.5" customHeight="1">
+    <row r="29" spans="1:18" ht="94.5" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A29" s="11" t="s">
         <v>105</v>
       </c>
@@ -5687,10 +5767,12 @@
       <c r="N29" s="4"/>
       <c r="O29" s="4"/>
       <c r="P29" s="4"/>
-      <c r="Q29" s="4"/>
+      <c r="Q29" s="4" t="s">
+        <v>38</v>
+      </c>
       <c r="R29" s="4"/>
     </row>
-    <row r="30" spans="1:18" ht="350" customHeight="1">
+    <row r="30" spans="1:18" ht="350.1" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A30" s="11" t="s">
         <v>108</v>
       </c>
@@ -5722,7 +5804,7 @@
       <c r="Q30" s="4"/>
       <c r="R30" s="4"/>
     </row>
-    <row r="31" spans="1:18" ht="350" customHeight="1">
+    <row r="31" spans="1:18" ht="350.1" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A31" s="9" t="s">
         <v>111</v>
       </c>
@@ -5754,7 +5836,7 @@
       <c r="Q31" s="4"/>
       <c r="R31" s="4"/>
     </row>
-    <row r="32" spans="1:18" ht="94">
+    <row r="32" spans="1:18" ht="92.25" x14ac:dyDescent="0.7">
       <c r="A32" s="9" t="s">
         <v>114</v>
       </c>
@@ -5783,10 +5865,12 @@
       <c r="N32" s="4"/>
       <c r="O32" s="4"/>
       <c r="P32" s="4"/>
-      <c r="Q32" s="4"/>
+      <c r="Q32" s="4" t="s">
+        <v>119</v>
+      </c>
       <c r="R32" s="4"/>
     </row>
-    <row r="33" spans="1:18" ht="94">
+    <row r="33" spans="1:18" ht="138" x14ac:dyDescent="0.7">
       <c r="A33" s="9" t="s">
         <v>117</v>
       </c>
@@ -5815,10 +5899,12 @@
       <c r="N33" s="4"/>
       <c r="O33" s="4"/>
       <c r="P33" s="4"/>
-      <c r="Q33" s="4"/>
+      <c r="Q33" s="4" t="s">
+        <v>119</v>
+      </c>
       <c r="R33" s="4"/>
     </row>
-    <row r="34" spans="1:18" ht="92.5" customHeight="1">
+    <row r="34" spans="1:18" ht="92.45" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A34" s="9" t="s">
         <v>120</v>
       </c>
@@ -5847,10 +5933,12 @@
       <c r="N34" s="4"/>
       <c r="O34" s="4"/>
       <c r="P34" s="4"/>
-      <c r="Q34" s="4"/>
+      <c r="Q34" s="4" t="s">
+        <v>119</v>
+      </c>
       <c r="R34" s="4"/>
     </row>
-    <row r="35" spans="1:18" ht="99.5" customHeight="1">
+    <row r="35" spans="1:18" ht="99.6" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A35" s="9" t="s">
         <v>123</v>
       </c>
@@ -5879,10 +5967,12 @@
       <c r="N35" s="4"/>
       <c r="O35" s="4"/>
       <c r="P35" s="4"/>
-      <c r="Q35" s="4"/>
+      <c r="Q35" s="4" t="s">
+        <v>119</v>
+      </c>
       <c r="R35" s="4"/>
     </row>
-    <row r="36" spans="1:18" ht="96">
+    <row r="36" spans="1:18" ht="93" x14ac:dyDescent="0.7">
       <c r="A36" s="9" t="s">
         <v>125</v>
       </c>
@@ -5912,7 +6002,7 @@
       <c r="Q36" s="4"/>
       <c r="R36" s="4"/>
     </row>
-    <row r="37" spans="1:18" ht="96">
+    <row r="37" spans="1:18" ht="138" x14ac:dyDescent="0.7">
       <c r="A37" s="9" t="s">
         <v>128</v>
       </c>
@@ -5942,7 +6032,7 @@
       <c r="Q37" s="4"/>
       <c r="R37" s="4"/>
     </row>
-    <row r="38" spans="1:18" ht="96">
+    <row r="38" spans="1:18" ht="138" x14ac:dyDescent="0.7">
       <c r="A38" s="9" t="s">
         <v>130</v>
       </c>
@@ -5972,7 +6062,7 @@
       <c r="Q38" s="4"/>
       <c r="R38" s="4"/>
     </row>
-    <row r="39" spans="1:18" ht="96">
+    <row r="39" spans="1:18" ht="138" x14ac:dyDescent="0.7">
       <c r="A39" s="9" t="s">
         <v>133</v>
       </c>
@@ -6002,7 +6092,7 @@
       <c r="Q39" s="4"/>
       <c r="R39" s="4"/>
     </row>
-    <row r="40" spans="1:18" ht="96">
+    <row r="40" spans="1:18" ht="93" x14ac:dyDescent="0.7">
       <c r="A40" s="9" t="s">
         <v>136</v>
       </c>
@@ -6031,10 +6121,12 @@
       <c r="N40" s="4"/>
       <c r="O40" s="4"/>
       <c r="P40" s="4"/>
-      <c r="Q40" s="4"/>
+      <c r="Q40" s="4" t="s">
+        <v>119</v>
+      </c>
       <c r="R40" s="4"/>
     </row>
-    <row r="41" spans="1:18" ht="96">
+    <row r="41" spans="1:18" ht="93" x14ac:dyDescent="0.7">
       <c r="A41" s="9" t="s">
         <v>139</v>
       </c>
@@ -6063,10 +6155,12 @@
       <c r="N41" s="4"/>
       <c r="O41" s="4"/>
       <c r="P41" s="4"/>
-      <c r="Q41" s="4"/>
+      <c r="Q41" s="4" t="s">
+        <v>119</v>
+      </c>
       <c r="R41" s="4"/>
     </row>
-    <row r="42" spans="1:18" ht="140">
+    <row r="42" spans="1:18" ht="138" x14ac:dyDescent="0.7">
       <c r="A42" s="9" t="s">
         <v>142</v>
       </c>
@@ -6095,10 +6189,12 @@
       <c r="N42" s="4"/>
       <c r="O42" s="4"/>
       <c r="P42" s="4"/>
-      <c r="Q42" s="4"/>
+      <c r="Q42" s="4" t="s">
+        <v>119</v>
+      </c>
       <c r="R42" s="4"/>
     </row>
-    <row r="43" spans="1:18" ht="96">
+    <row r="43" spans="1:18" ht="93" x14ac:dyDescent="0.7">
       <c r="A43" s="9" t="s">
         <v>145</v>
       </c>
@@ -6128,7 +6224,7 @@
       <c r="Q43" s="4"/>
       <c r="R43" s="4"/>
     </row>
-    <row r="44" spans="1:18" ht="96">
+    <row r="44" spans="1:18" ht="93" x14ac:dyDescent="0.7">
       <c r="A44" s="9" t="s">
         <v>148</v>
       </c>
@@ -6158,7 +6254,7 @@
       <c r="Q44" s="4"/>
       <c r="R44" s="4"/>
     </row>
-    <row r="45" spans="1:18" ht="96">
+    <row r="45" spans="1:18" ht="93" x14ac:dyDescent="0.7">
       <c r="A45" s="9" t="s">
         <v>150</v>
       </c>
@@ -6188,7 +6284,7 @@
       <c r="Q45" s="4"/>
       <c r="R45" s="4"/>
     </row>
-    <row r="46" spans="1:18" ht="96">
+    <row r="46" spans="1:18" ht="93" x14ac:dyDescent="0.7">
       <c r="A46" s="9" t="s">
         <v>153</v>
       </c>
@@ -6218,7 +6314,7 @@
       <c r="Q46" s="4"/>
       <c r="R46" s="4"/>
     </row>
-    <row r="47" spans="1:18" ht="140">
+    <row r="47" spans="1:18" ht="138" x14ac:dyDescent="0.7">
       <c r="A47" s="9" t="s">
         <v>155</v>
       </c>
@@ -6248,7 +6344,7 @@
       <c r="Q47" s="4"/>
       <c r="R47" s="4"/>
     </row>
-    <row r="48" spans="1:18" ht="96">
+    <row r="48" spans="1:18" ht="93" x14ac:dyDescent="0.7">
       <c r="A48" s="9" t="s">
         <v>157</v>
       </c>
@@ -6278,7 +6374,7 @@
       <c r="Q48" s="4"/>
       <c r="R48" s="4"/>
     </row>
-    <row r="49" spans="1:18" ht="94">
+    <row r="49" spans="1:18" ht="92.25" x14ac:dyDescent="0.7">
       <c r="A49" s="9" t="s">
         <v>159</v>
       </c>
@@ -6307,10 +6403,12 @@
       <c r="N49" s="4"/>
       <c r="O49" s="4"/>
       <c r="P49" s="4"/>
-      <c r="Q49" s="4"/>
+      <c r="Q49" s="4" t="s">
+        <v>38</v>
+      </c>
       <c r="R49" s="4"/>
     </row>
-    <row r="50" spans="1:18" ht="186">
+    <row r="50" spans="1:18" ht="183.75" x14ac:dyDescent="0.7">
       <c r="A50" s="9" t="s">
         <v>161</v>
       </c>
@@ -6339,10 +6437,12 @@
       <c r="N50" s="4"/>
       <c r="O50" s="4"/>
       <c r="P50" s="4"/>
-      <c r="Q50" s="4"/>
+      <c r="Q50" s="4" t="s">
+        <v>38</v>
+      </c>
       <c r="R50" s="4"/>
     </row>
-    <row r="51" spans="1:18" ht="235.25" customHeight="1">
+    <row r="51" spans="1:18" ht="267" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A51" s="9" t="s">
         <v>163</v>
       </c>
@@ -6370,10 +6470,12 @@
       <c r="N51" s="4"/>
       <c r="O51" s="4"/>
       <c r="P51" s="4"/>
-      <c r="Q51" s="4"/>
+      <c r="Q51" s="4" t="s">
+        <v>647</v>
+      </c>
       <c r="R51" s="4"/>
     </row>
-    <row r="52" spans="1:18" ht="94">
+    <row r="52" spans="1:18" ht="92.25" x14ac:dyDescent="0.7">
       <c r="A52" s="9" t="s">
         <v>167</v>
       </c>
@@ -6402,10 +6504,12 @@
       <c r="N52" s="4"/>
       <c r="O52" s="4"/>
       <c r="P52" s="4"/>
-      <c r="Q52" s="4"/>
+      <c r="Q52" s="4" t="s">
+        <v>38</v>
+      </c>
       <c r="R52" s="4"/>
     </row>
-    <row r="53" spans="1:18" ht="48">
+    <row r="53" spans="1:18" ht="92.25" x14ac:dyDescent="0.7">
       <c r="A53" s="23" t="s">
         <v>169</v>
       </c>
@@ -6435,7 +6539,7 @@
       <c r="Q53" s="4"/>
       <c r="R53" s="4"/>
     </row>
-    <row r="54" spans="1:18" ht="48">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.7">
       <c r="A54" s="23" t="s">
         <v>172</v>
       </c>
@@ -6465,7 +6569,7 @@
       <c r="Q54" s="4"/>
       <c r="R54" s="4"/>
     </row>
-    <row r="55" spans="1:18" ht="232">
+    <row r="55" spans="1:18" ht="275.25" x14ac:dyDescent="0.7">
       <c r="A55" s="9" t="s">
         <v>175</v>
       </c>
@@ -6494,10 +6598,12 @@
       <c r="N55" s="4"/>
       <c r="O55" s="4"/>
       <c r="P55" s="4"/>
-      <c r="Q55" s="4"/>
+      <c r="Q55" s="4" t="s">
+        <v>648</v>
+      </c>
       <c r="R55" s="4"/>
     </row>
-    <row r="56" spans="1:18" ht="48">
+    <row r="56" spans="1:18" x14ac:dyDescent="0.7">
       <c r="A56" s="23" t="s">
         <v>179</v>
       </c>
@@ -6529,7 +6635,7 @@
       <c r="Q56" s="4"/>
       <c r="R56" s="4"/>
     </row>
-    <row r="57" spans="1:18" ht="278">
+    <row r="57" spans="1:18" ht="275.25" x14ac:dyDescent="0.7">
       <c r="A57" s="9" t="s">
         <v>182</v>
       </c>
@@ -6561,7 +6667,7 @@
       <c r="Q57" s="4"/>
       <c r="R57" s="4"/>
     </row>
-    <row r="58" spans="1:18" ht="48">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.7">
       <c r="A58" s="9" t="s">
         <v>186</v>
       </c>
@@ -6593,7 +6699,7 @@
       <c r="Q58" s="4"/>
       <c r="R58" s="4"/>
     </row>
-    <row r="59" spans="1:18" ht="278">
+    <row r="59" spans="1:18" ht="275.25" x14ac:dyDescent="0.7">
       <c r="A59" s="9" t="s">
         <v>189</v>
       </c>
@@ -6625,7 +6731,7 @@
       <c r="Q59" s="4"/>
       <c r="R59" s="4"/>
     </row>
-    <row r="60" spans="1:18" ht="186">
+    <row r="60" spans="1:18" ht="183.75" x14ac:dyDescent="0.7">
       <c r="A60" s="9" t="s">
         <v>192</v>
       </c>
@@ -6657,7 +6763,7 @@
       <c r="Q60" s="4"/>
       <c r="R60" s="4"/>
     </row>
-    <row r="61" spans="1:18" ht="94">
+    <row r="61" spans="1:18" ht="92.25" x14ac:dyDescent="0.7">
       <c r="A61" s="23" t="s">
         <v>197</v>
       </c>
@@ -6689,7 +6795,7 @@
       <c r="Q61" s="4"/>
       <c r="R61" s="4"/>
     </row>
-    <row r="62" spans="1:18" ht="232">
+    <row r="62" spans="1:18" ht="275.25" x14ac:dyDescent="0.7">
       <c r="A62" s="9" t="s">
         <v>199</v>
       </c>
@@ -6721,7 +6827,7 @@
       <c r="Q62" s="4"/>
       <c r="R62" s="4"/>
     </row>
-    <row r="63" spans="1:18" ht="48">
+    <row r="63" spans="1:18" x14ac:dyDescent="0.7">
       <c r="A63" s="23" t="s">
         <v>203</v>
       </c>
@@ -6751,7 +6857,7 @@
       <c r="Q63" s="4"/>
       <c r="R63" s="4"/>
     </row>
-    <row r="64" spans="1:18" ht="48">
+    <row r="64" spans="1:18" ht="92.25" x14ac:dyDescent="0.7">
       <c r="A64" s="23" t="s">
         <v>205</v>
       </c>
@@ -6781,7 +6887,7 @@
       <c r="Q64" s="4"/>
       <c r="R64" s="4"/>
     </row>
-    <row r="65" spans="1:18" ht="94">
+    <row r="65" spans="1:18" ht="92.25" x14ac:dyDescent="0.7">
       <c r="A65" s="9" t="s">
         <v>208</v>
       </c>
@@ -6813,7 +6919,7 @@
       <c r="Q65" s="4"/>
       <c r="R65" s="4"/>
     </row>
-    <row r="66" spans="1:18" ht="48">
+    <row r="66" spans="1:18" x14ac:dyDescent="0.7">
       <c r="A66" s="9" t="s">
         <v>211</v>
       </c>
@@ -6845,7 +6951,7 @@
       <c r="Q66" s="4"/>
       <c r="R66" s="4"/>
     </row>
-    <row r="67" spans="1:18" ht="92">
+    <row r="67" spans="1:18" ht="91.5" x14ac:dyDescent="0.7">
       <c r="A67" s="9" t="s">
         <v>214</v>
       </c>
@@ -6875,7 +6981,7 @@
       <c r="Q67" s="4"/>
       <c r="R67" s="4"/>
     </row>
-    <row r="68" spans="1:18" ht="92">
+    <row r="68" spans="1:18" ht="91.5" x14ac:dyDescent="0.7">
       <c r="A68" s="9" t="s">
         <v>216</v>
       </c>
@@ -6905,7 +7011,7 @@
       <c r="Q68" s="4"/>
       <c r="R68" s="4"/>
     </row>
-    <row r="69" spans="1:18" ht="94">
+    <row r="69" spans="1:18" ht="92.25" x14ac:dyDescent="0.7">
       <c r="A69" s="9" t="s">
         <v>219</v>
       </c>
@@ -6935,7 +7041,7 @@
       <c r="Q69" s="4"/>
       <c r="R69" s="4"/>
     </row>
-    <row r="70" spans="1:18" ht="94">
+    <row r="70" spans="1:18" ht="92.25" x14ac:dyDescent="0.7">
       <c r="A70" s="9" t="s">
         <v>222</v>
       </c>
@@ -6965,7 +7071,7 @@
       <c r="Q70" s="4"/>
       <c r="R70" s="4"/>
     </row>
-    <row r="71" spans="1:18" ht="94">
+    <row r="71" spans="1:18" ht="92.25" x14ac:dyDescent="0.7">
       <c r="A71" s="9" t="s">
         <v>225</v>
       </c>
@@ -6995,7 +7101,7 @@
       <c r="Q71" s="4"/>
       <c r="R71" s="4"/>
     </row>
-    <row r="72" spans="1:18" ht="94">
+    <row r="72" spans="1:18" ht="92.25" x14ac:dyDescent="0.7">
       <c r="A72" s="9" t="s">
         <v>228</v>
       </c>
@@ -7025,7 +7131,7 @@
       <c r="Q72" s="4"/>
       <c r="R72" s="4"/>
     </row>
-    <row r="73" spans="1:18" ht="94">
+    <row r="73" spans="1:18" ht="92.25" x14ac:dyDescent="0.7">
       <c r="A73" s="9" t="s">
         <v>231</v>
       </c>
@@ -7053,7 +7159,7 @@
       <c r="Q73" s="4"/>
       <c r="R73" s="4"/>
     </row>
-    <row r="74" spans="1:18" ht="140">
+    <row r="74" spans="1:18" ht="138" x14ac:dyDescent="0.7">
       <c r="A74" s="9" t="s">
         <v>233</v>
       </c>
@@ -7081,7 +7187,7 @@
       <c r="Q74" s="4"/>
       <c r="R74" s="4"/>
     </row>
-    <row r="75" spans="1:18" ht="94">
+    <row r="75" spans="1:18" ht="92.25" x14ac:dyDescent="0.7">
       <c r="A75" s="9" t="s">
         <v>235</v>
       </c>
@@ -7109,7 +7215,7 @@
       <c r="Q75" s="4"/>
       <c r="R75" s="4"/>
     </row>
-    <row r="76" spans="1:18" ht="48">
+    <row r="76" spans="1:18" x14ac:dyDescent="0.7">
       <c r="A76" s="9" t="s">
         <v>237</v>
       </c>
@@ -7139,7 +7245,7 @@
       <c r="Q76" s="4"/>
       <c r="R76" s="4"/>
     </row>
-    <row r="77" spans="1:18" ht="94">
+    <row r="77" spans="1:18" ht="92.25" x14ac:dyDescent="0.7">
       <c r="A77" s="9" t="s">
         <v>240</v>
       </c>
@@ -7169,7 +7275,7 @@
       <c r="Q77" s="4"/>
       <c r="R77" s="4"/>
     </row>
-    <row r="78" spans="1:18" ht="94">
+    <row r="78" spans="1:18" ht="92.25" x14ac:dyDescent="0.7">
       <c r="A78" s="9" t="s">
         <v>243</v>
       </c>
@@ -7197,7 +7303,7 @@
       <c r="Q78" s="4"/>
       <c r="R78" s="4"/>
     </row>
-    <row r="79" spans="1:18" ht="94">
+    <row r="79" spans="1:18" ht="92.25" x14ac:dyDescent="0.7">
       <c r="A79" s="9" t="s">
         <v>245</v>
       </c>
@@ -7227,7 +7333,7 @@
       <c r="Q79" s="4"/>
       <c r="R79" s="4"/>
     </row>
-    <row r="80" spans="1:18" ht="94">
+    <row r="80" spans="1:18" ht="92.25" x14ac:dyDescent="0.7">
       <c r="A80" s="9" t="s">
         <v>248</v>
       </c>
@@ -7257,7 +7363,7 @@
       <c r="Q80" s="4"/>
       <c r="R80" s="4"/>
     </row>
-    <row r="81" spans="1:18" ht="94">
+    <row r="81" spans="1:18" ht="92.25" x14ac:dyDescent="0.7">
       <c r="A81" s="9" t="s">
         <v>251</v>
       </c>
@@ -7287,7 +7393,7 @@
       <c r="Q81" s="4"/>
       <c r="R81" s="4"/>
     </row>
-    <row r="82" spans="1:18" ht="48">
+    <row r="82" spans="1:18" x14ac:dyDescent="0.7">
       <c r="A82" s="9" t="s">
         <v>254</v>
       </c>
@@ -7317,7 +7423,7 @@
       <c r="Q82" s="4"/>
       <c r="R82" s="4"/>
     </row>
-    <row r="83" spans="1:18" ht="48">
+    <row r="83" spans="1:18" ht="92.25" x14ac:dyDescent="0.7">
       <c r="A83" s="9" t="s">
         <v>257</v>
       </c>
@@ -7347,7 +7453,7 @@
       <c r="Q83" s="4"/>
       <c r="R83" s="4"/>
     </row>
-    <row r="84" spans="1:18" ht="94">
+    <row r="84" spans="1:18" ht="92.25" x14ac:dyDescent="0.7">
       <c r="A84" s="9" t="s">
         <v>259</v>
       </c>
@@ -7377,7 +7483,7 @@
       <c r="Q84" s="4"/>
       <c r="R84" s="4"/>
     </row>
-    <row r="85" spans="1:18" ht="48">
+    <row r="85" spans="1:18" ht="92.25" x14ac:dyDescent="0.7">
       <c r="A85" s="9" t="s">
         <v>261</v>
       </c>
@@ -7407,7 +7513,7 @@
       <c r="Q85" s="4"/>
       <c r="R85" s="4"/>
     </row>
-    <row r="86" spans="1:18" ht="48">
+    <row r="86" spans="1:18" x14ac:dyDescent="0.7">
       <c r="A86" s="9" t="s">
         <v>264</v>
       </c>
@@ -7437,7 +7543,7 @@
       <c r="Q86" s="4"/>
       <c r="R86" s="4"/>
     </row>
-    <row r="87" spans="1:18" ht="48">
+    <row r="87" spans="1:18" x14ac:dyDescent="0.7">
       <c r="A87" s="9" t="s">
         <v>266</v>
       </c>
@@ -7467,7 +7573,7 @@
       <c r="Q87" s="4"/>
       <c r="R87" s="4"/>
     </row>
-    <row r="88" spans="1:18" ht="48">
+    <row r="88" spans="1:18" x14ac:dyDescent="0.7">
       <c r="A88" s="9" t="s">
         <v>269</v>
       </c>
@@ -7497,7 +7603,7 @@
       <c r="Q88" s="4"/>
       <c r="R88" s="4"/>
     </row>
-    <row r="89" spans="1:18" ht="48">
+    <row r="89" spans="1:18" x14ac:dyDescent="0.7">
       <c r="A89" s="9" t="s">
         <v>272</v>
       </c>
@@ -7527,7 +7633,7 @@
       <c r="Q89" s="4"/>
       <c r="R89" s="4"/>
     </row>
-    <row r="90" spans="1:18" ht="48">
+    <row r="90" spans="1:18" x14ac:dyDescent="0.7">
       <c r="A90" s="9" t="s">
         <v>274</v>
       </c>
@@ -7557,7 +7663,7 @@
       <c r="Q90" s="4"/>
       <c r="R90" s="4"/>
     </row>
-    <row r="91" spans="1:18" ht="94">
+    <row r="91" spans="1:18" ht="92.25" x14ac:dyDescent="0.7">
       <c r="A91" s="9" t="s">
         <v>276</v>
       </c>
@@ -7587,7 +7693,7 @@
       <c r="Q91" s="4"/>
       <c r="R91" s="4"/>
     </row>
-    <row r="92" spans="1:18" ht="94">
+    <row r="92" spans="1:18" ht="92.25" x14ac:dyDescent="0.7">
       <c r="A92" s="9" t="s">
         <v>278</v>
       </c>
@@ -7617,7 +7723,7 @@
       <c r="Q92" s="4"/>
       <c r="R92" s="4"/>
     </row>
-    <row r="93" spans="1:18" ht="232">
+    <row r="93" spans="1:18" ht="229.5" x14ac:dyDescent="0.7">
       <c r="A93" s="9" t="s">
         <v>280</v>
       </c>
@@ -7645,7 +7751,7 @@
       <c r="Q93" s="4"/>
       <c r="R93" s="4"/>
     </row>
-    <row r="94" spans="1:18" ht="94">
+    <row r="94" spans="1:18" ht="92.25" x14ac:dyDescent="0.7">
       <c r="A94" s="9" t="s">
         <v>282</v>
       </c>
@@ -7673,7 +7779,7 @@
       <c r="Q94" s="4"/>
       <c r="R94" s="4"/>
     </row>
-    <row r="95" spans="1:18" ht="140">
+    <row r="95" spans="1:18" ht="183.75" x14ac:dyDescent="0.7">
       <c r="A95" s="9" t="s">
         <v>284</v>
       </c>
@@ -7705,7 +7811,7 @@
       <c r="Q95" s="4"/>
       <c r="R95" s="4"/>
     </row>
-    <row r="96" spans="1:18" ht="94">
+    <row r="96" spans="1:18" ht="92.25" x14ac:dyDescent="0.7">
       <c r="A96" s="9" t="s">
         <v>287</v>
       </c>
@@ -7737,7 +7843,7 @@
       <c r="Q96" s="4"/>
       <c r="R96" s="4"/>
     </row>
-    <row r="97" spans="1:18" ht="94">
+    <row r="97" spans="1:18" ht="138" x14ac:dyDescent="0.7">
       <c r="A97" s="9" t="s">
         <v>289</v>
       </c>
@@ -7765,7 +7871,7 @@
       <c r="Q97" s="4"/>
       <c r="R97" s="4"/>
     </row>
-    <row r="98" spans="1:18" ht="94">
+    <row r="98" spans="1:18" ht="92.25" x14ac:dyDescent="0.7">
       <c r="A98" s="9" t="s">
         <v>291</v>
       </c>
@@ -7795,7 +7901,7 @@
       <c r="Q98" s="4"/>
       <c r="R98" s="4"/>
     </row>
-    <row r="99" spans="1:18" ht="140">
+    <row r="99" spans="1:18" ht="138" x14ac:dyDescent="0.7">
       <c r="A99" s="9" t="s">
         <v>293</v>
       </c>
@@ -7825,7 +7931,7 @@
       <c r="Q99" s="4"/>
       <c r="R99" s="4"/>
     </row>
-    <row r="100" spans="1:18" ht="186">
+    <row r="100" spans="1:18" ht="229.5" x14ac:dyDescent="0.7">
       <c r="A100" s="9" t="s">
         <v>295</v>
       </c>
@@ -7855,7 +7961,7 @@
       <c r="Q100" s="4"/>
       <c r="R100" s="4"/>
     </row>
-    <row r="101" spans="1:18" ht="94">
+    <row r="101" spans="1:18" ht="92.25" x14ac:dyDescent="0.7">
       <c r="A101" s="9" t="s">
         <v>298</v>
       </c>
@@ -7885,7 +7991,7 @@
       <c r="Q101" s="4"/>
       <c r="R101" s="4"/>
     </row>
-    <row r="102" spans="1:18" ht="94">
+    <row r="102" spans="1:18" ht="92.25" x14ac:dyDescent="0.7">
       <c r="A102" s="9" t="s">
         <v>301</v>
       </c>
@@ -7915,7 +8021,7 @@
       <c r="Q102" s="4"/>
       <c r="R102" s="4"/>
     </row>
-    <row r="103" spans="1:18" ht="140">
+    <row r="103" spans="1:18" ht="138" x14ac:dyDescent="0.7">
       <c r="A103" s="9" t="s">
         <v>303</v>
       </c>
@@ -7943,7 +8049,7 @@
       <c r="Q103" s="4"/>
       <c r="R103" s="4"/>
     </row>
-    <row r="104" spans="1:18" ht="94">
+    <row r="104" spans="1:18" ht="92.25" x14ac:dyDescent="0.7">
       <c r="A104" s="9" t="s">
         <v>305</v>
       </c>
@@ -7973,7 +8079,7 @@
       <c r="Q104" s="4"/>
       <c r="R104" s="4"/>
     </row>
-    <row r="105" spans="1:18" ht="140">
+    <row r="105" spans="1:18" ht="138" x14ac:dyDescent="0.7">
       <c r="A105" s="9" t="s">
         <v>308</v>
       </c>
@@ -8003,7 +8109,7 @@
       <c r="Q105" s="4"/>
       <c r="R105" s="4"/>
     </row>
-    <row r="106" spans="1:18" ht="94">
+    <row r="106" spans="1:18" ht="92.25" x14ac:dyDescent="0.7">
       <c r="A106" s="9" t="s">
         <v>310</v>
       </c>
@@ -8033,7 +8139,7 @@
       <c r="Q106" s="4"/>
       <c r="R106" s="4"/>
     </row>
-    <row r="107" spans="1:18" ht="94">
+    <row r="107" spans="1:18" ht="92.25" x14ac:dyDescent="0.7">
       <c r="A107" s="9" t="s">
         <v>312</v>
       </c>
@@ -8063,7 +8169,7 @@
       <c r="Q107" s="4"/>
       <c r="R107" s="4"/>
     </row>
-    <row r="108" spans="1:18" ht="94">
+    <row r="108" spans="1:18" ht="92.25" x14ac:dyDescent="0.7">
       <c r="A108" s="9" t="s">
         <v>314</v>
       </c>
@@ -8093,7 +8199,7 @@
       <c r="Q108" s="4"/>
       <c r="R108" s="4"/>
     </row>
-    <row r="109" spans="1:18" ht="94">
+    <row r="109" spans="1:18" ht="92.25" x14ac:dyDescent="0.7">
       <c r="A109" s="9" t="s">
         <v>316</v>
       </c>
@@ -8123,7 +8229,7 @@
       <c r="Q109" s="4"/>
       <c r="R109" s="4"/>
     </row>
-    <row r="110" spans="1:18" ht="48">
+    <row r="110" spans="1:18" ht="92.25" x14ac:dyDescent="0.7">
       <c r="A110" s="9" t="s">
         <v>318</v>
       </c>
@@ -8153,7 +8259,7 @@
       <c r="Q110" s="4"/>
       <c r="R110" s="4"/>
     </row>
-    <row r="111" spans="1:18" ht="48">
+    <row r="111" spans="1:18" x14ac:dyDescent="0.7">
       <c r="A111" s="9" t="s">
         <v>320</v>
       </c>
@@ -8183,7 +8289,7 @@
       <c r="Q111" s="4"/>
       <c r="R111" s="4"/>
     </row>
-    <row r="112" spans="1:18" ht="94">
+    <row r="112" spans="1:18" ht="92.25" x14ac:dyDescent="0.7">
       <c r="A112" s="9" t="s">
         <v>323</v>
       </c>
@@ -8213,7 +8319,7 @@
       <c r="Q112" s="4"/>
       <c r="R112" s="4"/>
     </row>
-    <row r="113" spans="1:20" ht="48">
+    <row r="113" spans="1:20" x14ac:dyDescent="0.7">
       <c r="A113" s="9" t="s">
         <v>326</v>
       </c>
@@ -8243,7 +8349,7 @@
       <c r="Q113" s="4"/>
       <c r="R113" s="4"/>
     </row>
-    <row r="114" spans="1:20" ht="94">
+    <row r="114" spans="1:20" ht="92.25" x14ac:dyDescent="0.7">
       <c r="A114" s="9" t="s">
         <v>328</v>
       </c>
@@ -8273,7 +8379,7 @@
       <c r="Q114" s="4"/>
       <c r="R114" s="4"/>
     </row>
-    <row r="115" spans="1:20" ht="94">
+    <row r="115" spans="1:20" ht="92.25" x14ac:dyDescent="0.7">
       <c r="A115" s="9" t="s">
         <v>330</v>
       </c>
@@ -8303,7 +8409,7 @@
       <c r="Q115" s="4"/>
       <c r="R115" s="4"/>
     </row>
-    <row r="116" spans="1:20" ht="94">
+    <row r="116" spans="1:20" ht="92.25" x14ac:dyDescent="0.7">
       <c r="A116" s="9" t="s">
         <v>333</v>
       </c>
@@ -8333,7 +8439,7 @@
       <c r="Q116" s="4"/>
       <c r="R116" s="4"/>
     </row>
-    <row r="117" spans="1:20" ht="94">
+    <row r="117" spans="1:20" ht="92.25" x14ac:dyDescent="0.7">
       <c r="A117" s="9" t="s">
         <v>336</v>
       </c>
@@ -8365,7 +8471,7 @@
       <c r="Q117" s="4"/>
       <c r="R117" s="4"/>
     </row>
-    <row r="118" spans="1:20" ht="48">
+    <row r="118" spans="1:20" ht="92.25" x14ac:dyDescent="0.7">
       <c r="A118" s="9" t="s">
         <v>339</v>
       </c>
@@ -8397,7 +8503,7 @@
       <c r="Q118" s="4"/>
       <c r="R118" s="4"/>
     </row>
-    <row r="119" spans="1:20" ht="94">
+    <row r="119" spans="1:20" ht="92.25" x14ac:dyDescent="0.7">
       <c r="A119" s="9" t="s">
         <v>342</v>
       </c>
@@ -8427,7 +8533,7 @@
       <c r="Q119" s="4"/>
       <c r="R119" s="4"/>
     </row>
-    <row r="120" spans="1:20" ht="140">
+    <row r="120" spans="1:20" ht="138" x14ac:dyDescent="0.7">
       <c r="A120" s="9" t="s">
         <v>344</v>
       </c>
@@ -8457,7 +8563,7 @@
       <c r="Q120" s="4"/>
       <c r="R120" s="4"/>
     </row>
-    <row r="121" spans="1:20" ht="94">
+    <row r="121" spans="1:20" ht="138" x14ac:dyDescent="0.7">
       <c r="A121" s="9" t="s">
         <v>347</v>
       </c>
@@ -8489,7 +8595,7 @@
       <c r="Q121" s="4"/>
       <c r="R121" s="4"/>
     </row>
-    <row r="122" spans="1:20" ht="140">
+    <row r="122" spans="1:20" ht="138" x14ac:dyDescent="0.7">
       <c r="A122" s="9" t="s">
         <v>349</v>
       </c>
@@ -8521,7 +8627,7 @@
       <c r="Q122" s="4"/>
       <c r="R122" s="4"/>
     </row>
-    <row r="123" spans="1:20" ht="140">
+    <row r="123" spans="1:20" ht="138" x14ac:dyDescent="0.7">
       <c r="A123" s="9" t="s">
         <v>351</v>
       </c>
@@ -8553,7 +8659,7 @@
       <c r="Q123" s="4"/>
       <c r="R123" s="4"/>
     </row>
-    <row r="124" spans="1:20" ht="48">
+    <row r="124" spans="1:20" x14ac:dyDescent="0.7">
       <c r="A124" s="9" t="s">
         <v>354</v>
       </c>
@@ -8581,7 +8687,7 @@
       <c r="Q124" s="4"/>
       <c r="R124" s="4"/>
     </row>
-    <row r="125" spans="1:20" ht="232">
+    <row r="125" spans="1:20" ht="229.5" x14ac:dyDescent="0.7">
       <c r="A125" s="9" t="s">
         <v>356</v>
       </c>
@@ -8613,7 +8719,7 @@
       <c r="Q125" s="4"/>
       <c r="R125" s="4"/>
     </row>
-    <row r="126" spans="1:20" ht="186">
+    <row r="126" spans="1:20" ht="183.75" x14ac:dyDescent="0.7">
       <c r="A126" s="9" t="s">
         <v>358</v>
       </c>
@@ -8645,7 +8751,7 @@
       <c r="Q126" s="4"/>
       <c r="R126" s="4"/>
     </row>
-    <row r="127" spans="1:20" ht="92">
+    <row r="127" spans="1:20" ht="137.25" x14ac:dyDescent="0.7">
       <c r="A127" s="9" t="s">
         <v>360</v>
       </c>
@@ -8677,7 +8783,7 @@
       <c r="Q127" s="4"/>
       <c r="R127" s="4"/>
     </row>
-    <row r="128" spans="1:20" s="33" customFormat="1">
+    <row r="128" spans="1:20" s="33" customFormat="1" ht="91.5" x14ac:dyDescent="0.7">
       <c r="A128" s="34" t="s">
         <v>363</v>
       </c>
@@ -8711,7 +8817,7 @@
       <c r="S128" s="41"/>
       <c r="T128" s="41"/>
     </row>
-    <row r="129" spans="1:20" ht="92">
+    <row r="129" spans="1:20" ht="91.5" x14ac:dyDescent="0.7">
       <c r="A129" s="9" t="s">
         <v>367</v>
       </c>
@@ -8743,7 +8849,7 @@
       <c r="S129" s="44"/>
       <c r="T129" s="44"/>
     </row>
-    <row r="130" spans="1:20" ht="94">
+    <row r="130" spans="1:20" ht="92.25" x14ac:dyDescent="0.7">
       <c r="A130" s="9" t="s">
         <v>370</v>
       </c>
@@ -8775,7 +8881,7 @@
       <c r="S130" s="44"/>
       <c r="T130" s="44"/>
     </row>
-    <row r="131" spans="1:20" s="33" customFormat="1" ht="94">
+    <row r="131" spans="1:20" s="33" customFormat="1" ht="92.25" x14ac:dyDescent="0.7">
       <c r="A131" s="34" t="s">
         <v>372</v>
       </c>
@@ -8809,7 +8915,7 @@
       <c r="S131" s="41"/>
       <c r="T131" s="41"/>
     </row>
-    <row r="132" spans="1:20" ht="48">
+    <row r="132" spans="1:20" x14ac:dyDescent="0.7">
       <c r="A132" s="9" t="s">
         <v>375</v>
       </c>
@@ -8841,7 +8947,7 @@
       <c r="S132" s="44"/>
       <c r="T132" s="44"/>
     </row>
-    <row r="133" spans="1:20" ht="175" customHeight="1">
+    <row r="133" spans="1:20" ht="174.95" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A133" s="9" t="s">
         <v>378</v>
       </c>
@@ -8873,7 +8979,7 @@
       <c r="S133" s="44"/>
       <c r="T133" s="44"/>
     </row>
-    <row r="134" spans="1:20" ht="48">
+    <row r="134" spans="1:20" x14ac:dyDescent="0.7">
       <c r="A134" s="9" t="s">
         <v>381</v>
       </c>
@@ -8905,7 +9011,7 @@
       <c r="S134" s="44"/>
       <c r="T134" s="44"/>
     </row>
-    <row r="135" spans="1:20" ht="94">
+    <row r="135" spans="1:20" ht="92.25" x14ac:dyDescent="0.7">
       <c r="A135" s="34" t="s">
         <v>384</v>
       </c>
@@ -8939,7 +9045,7 @@
       <c r="S135" s="44"/>
       <c r="T135" s="44"/>
     </row>
-    <row r="136" spans="1:20" ht="94">
+    <row r="136" spans="1:20" ht="92.25" x14ac:dyDescent="0.7">
       <c r="A136" s="9" t="s">
         <v>388</v>
       </c>
@@ -8969,7 +9075,7 @@
       <c r="Q136" s="4"/>
       <c r="R136" s="4"/>
     </row>
-    <row r="137" spans="1:20" ht="94">
+    <row r="137" spans="1:20" ht="92.25" x14ac:dyDescent="0.7">
       <c r="A137" s="9" t="s">
         <v>391</v>
       </c>
@@ -8999,7 +9105,7 @@
       <c r="Q137" s="4"/>
       <c r="R137" s="4"/>
     </row>
-    <row r="138" spans="1:20" ht="140">
+    <row r="138" spans="1:20" ht="138" x14ac:dyDescent="0.7">
       <c r="A138" s="9" t="s">
         <v>393</v>
       </c>
@@ -9029,7 +9135,7 @@
       <c r="Q138" s="4"/>
       <c r="R138" s="4"/>
     </row>
-    <row r="139" spans="1:20" ht="94">
+    <row r="139" spans="1:20" ht="92.25" x14ac:dyDescent="0.7">
       <c r="A139" s="9" t="s">
         <v>396</v>
       </c>
@@ -9059,7 +9165,7 @@
       <c r="Q139" s="4"/>
       <c r="R139" s="4"/>
     </row>
-    <row r="140" spans="1:20" ht="94">
+    <row r="140" spans="1:20" ht="138" x14ac:dyDescent="0.7">
       <c r="A140" s="9" t="s">
         <v>398</v>
       </c>
@@ -9089,7 +9195,7 @@
       <c r="Q140" s="4"/>
       <c r="R140" s="4"/>
     </row>
-    <row r="141" spans="1:20" ht="94">
+    <row r="141" spans="1:20" ht="92.25" x14ac:dyDescent="0.7">
       <c r="A141" s="9" t="s">
         <v>401</v>
       </c>
@@ -9119,7 +9225,7 @@
       <c r="Q141" s="4"/>
       <c r="R141" s="4"/>
     </row>
-    <row r="142" spans="1:20" ht="94">
+    <row r="142" spans="1:20" ht="92.25" x14ac:dyDescent="0.7">
       <c r="A142" s="9" t="s">
         <v>403</v>
       </c>
@@ -9149,7 +9255,7 @@
       <c r="Q142" s="4"/>
       <c r="R142" s="4"/>
     </row>
-    <row r="143" spans="1:20" ht="140">
+    <row r="143" spans="1:20" ht="138" x14ac:dyDescent="0.7">
       <c r="A143" s="9" t="s">
         <v>405</v>
       </c>
@@ -9179,7 +9285,7 @@
       <c r="Q143" s="4"/>
       <c r="R143" s="4"/>
     </row>
-    <row r="144" spans="1:20" ht="94">
+    <row r="144" spans="1:20" ht="138" x14ac:dyDescent="0.7">
       <c r="A144" s="47" t="s">
         <v>407</v>
       </c>
@@ -9211,7 +9317,7 @@
       <c r="S144" s="44"/>
       <c r="T144" s="44"/>
     </row>
-    <row r="145" spans="1:20" ht="94">
+    <row r="145" spans="1:20" ht="138" x14ac:dyDescent="0.7">
       <c r="A145" s="9" t="s">
         <v>411</v>
       </c>
@@ -9245,7 +9351,7 @@
       <c r="S145" s="44"/>
       <c r="T145" s="44"/>
     </row>
-    <row r="146" spans="1:20" ht="140">
+    <row r="146" spans="1:20" ht="138" x14ac:dyDescent="0.7">
       <c r="A146" s="9" t="s">
         <v>414</v>
       </c>
@@ -9279,7 +9385,7 @@
       <c r="S146" s="44"/>
       <c r="T146" s="44"/>
     </row>
-    <row r="147" spans="1:20" ht="140">
+    <row r="147" spans="1:20" ht="138" x14ac:dyDescent="0.7">
       <c r="A147" s="9" t="s">
         <v>417</v>
       </c>
@@ -9311,7 +9417,7 @@
       <c r="S147" s="44"/>
       <c r="T147" s="44"/>
     </row>
-    <row r="148" spans="1:20" ht="140">
+    <row r="148" spans="1:20" ht="138" x14ac:dyDescent="0.7">
       <c r="A148" s="9" t="s">
         <v>420</v>
       </c>
@@ -9343,7 +9449,7 @@
       <c r="S148" s="44"/>
       <c r="T148" s="44"/>
     </row>
-    <row r="149" spans="1:20" s="33" customFormat="1" ht="94">
+    <row r="149" spans="1:20" s="33" customFormat="1" ht="138" x14ac:dyDescent="0.7">
       <c r="A149" s="34" t="s">
         <v>423</v>
       </c>
@@ -9375,7 +9481,7 @@
       <c r="S149" s="41"/>
       <c r="T149" s="41"/>
     </row>
-    <row r="150" spans="1:20" ht="140">
+    <row r="150" spans="1:20" ht="138" x14ac:dyDescent="0.7">
       <c r="A150" s="9" t="s">
         <v>426</v>
       </c>
@@ -9407,7 +9513,7 @@
       <c r="S150" s="44"/>
       <c r="T150" s="44"/>
     </row>
-    <row r="151" spans="1:20" ht="140">
+    <row r="151" spans="1:20" ht="138" x14ac:dyDescent="0.7">
       <c r="A151" s="9" t="s">
         <v>429</v>
       </c>
@@ -9441,7 +9547,7 @@
       <c r="S151" s="44"/>
       <c r="T151" s="44"/>
     </row>
-    <row r="152" spans="1:20" ht="94">
+    <row r="152" spans="1:20" ht="92.25" x14ac:dyDescent="0.7">
       <c r="A152" s="9" t="s">
         <v>433</v>
       </c>
@@ -9475,7 +9581,7 @@
       <c r="S152" s="44"/>
       <c r="T152" s="44"/>
     </row>
-    <row r="153" spans="1:20" ht="140">
+    <row r="153" spans="1:20" ht="138" x14ac:dyDescent="0.7">
       <c r="A153" s="9" t="s">
         <v>436</v>
       </c>
@@ -9511,7 +9617,7 @@
       <c r="S153" s="44"/>
       <c r="T153" s="44"/>
     </row>
-    <row r="154" spans="1:20" ht="140">
+    <row r="154" spans="1:20" ht="138" x14ac:dyDescent="0.7">
       <c r="A154" s="9" t="s">
         <v>439</v>
       </c>
@@ -9547,7 +9653,7 @@
       <c r="S154" s="44"/>
       <c r="T154" s="44"/>
     </row>
-    <row r="155" spans="1:20" ht="94">
+    <row r="155" spans="1:20" ht="92.25" x14ac:dyDescent="0.7">
       <c r="A155" s="9" t="s">
         <v>442</v>
       </c>
@@ -9583,7 +9689,7 @@
       <c r="S155" s="44"/>
       <c r="T155" s="44"/>
     </row>
-    <row r="156" spans="1:20" ht="94">
+    <row r="156" spans="1:20" ht="138" x14ac:dyDescent="0.7">
       <c r="A156" s="9" t="s">
         <v>445</v>
       </c>
@@ -9619,7 +9725,7 @@
       <c r="S156" s="44"/>
       <c r="T156" s="44"/>
     </row>
-    <row r="157" spans="1:20" ht="94">
+    <row r="157" spans="1:20" ht="92.25" x14ac:dyDescent="0.7">
       <c r="A157" s="9" t="s">
         <v>447</v>
       </c>
@@ -9655,7 +9761,7 @@
       <c r="S157" s="44"/>
       <c r="T157" s="44"/>
     </row>
-    <row r="158" spans="1:20" ht="94">
+    <row r="158" spans="1:20" ht="92.25" x14ac:dyDescent="0.7">
       <c r="A158" s="9" t="s">
         <v>449</v>
       </c>
@@ -9691,7 +9797,7 @@
       <c r="S158" s="44"/>
       <c r="T158" s="44"/>
     </row>
-    <row r="159" spans="1:20" ht="94">
+    <row r="159" spans="1:20" ht="92.25" x14ac:dyDescent="0.7">
       <c r="A159" s="9" t="s">
         <v>452</v>
       </c>
@@ -9727,7 +9833,7 @@
       <c r="S159" s="44"/>
       <c r="T159" s="44"/>
     </row>
-    <row r="160" spans="1:20" ht="94">
+    <row r="160" spans="1:20" ht="92.25" x14ac:dyDescent="0.7">
       <c r="A160" s="9" t="s">
         <v>455</v>
       </c>
@@ -9763,7 +9869,7 @@
       <c r="S160" s="44"/>
       <c r="T160" s="44"/>
     </row>
-    <row r="161" spans="1:20" ht="94">
+    <row r="161" spans="1:20" ht="92.25" x14ac:dyDescent="0.7">
       <c r="A161" s="9" t="s">
         <v>458</v>
       </c>
@@ -9799,7 +9905,7 @@
       <c r="S161" s="44"/>
       <c r="T161" s="44"/>
     </row>
-    <row r="162" spans="1:20" ht="48">
+    <row r="162" spans="1:20" x14ac:dyDescent="0.7">
       <c r="A162" s="9" t="s">
         <v>461</v>
       </c>
@@ -9835,7 +9941,7 @@
       <c r="S162" s="44"/>
       <c r="T162" s="44"/>
     </row>
-    <row r="163" spans="1:20" ht="48">
+    <row r="163" spans="1:20" x14ac:dyDescent="0.7">
       <c r="A163" s="9" t="s">
         <v>464</v>
       </c>
@@ -9869,7 +9975,7 @@
       <c r="S163" s="44"/>
       <c r="T163" s="44"/>
     </row>
-    <row r="164" spans="1:20" ht="48">
+    <row r="164" spans="1:20" x14ac:dyDescent="0.7">
       <c r="A164" s="9" t="s">
         <v>467</v>
       </c>
@@ -9903,7 +10009,7 @@
       <c r="S164" s="44"/>
       <c r="T164" s="44"/>
     </row>
-    <row r="165" spans="1:20" ht="48">
+    <row r="165" spans="1:20" x14ac:dyDescent="0.7">
       <c r="A165" s="9" t="s">
         <v>470</v>
       </c>
@@ -9937,7 +10043,7 @@
       <c r="S165" s="44"/>
       <c r="T165" s="44"/>
     </row>
-    <row r="166" spans="1:20" ht="48">
+    <row r="166" spans="1:20" x14ac:dyDescent="0.7">
       <c r="A166" s="9" t="s">
         <v>473</v>
       </c>
@@ -9971,7 +10077,7 @@
       <c r="S166" s="44"/>
       <c r="T166" s="44"/>
     </row>
-    <row r="167" spans="1:20" ht="48">
+    <row r="167" spans="1:20" x14ac:dyDescent="0.7">
       <c r="A167" s="9" t="s">
         <v>476</v>
       </c>
@@ -10005,7 +10111,7 @@
       <c r="S167" s="44"/>
       <c r="T167" s="44"/>
     </row>
-    <row r="168" spans="1:20" ht="94">
+    <row r="168" spans="1:20" ht="92.25" x14ac:dyDescent="0.7">
       <c r="A168" s="9" t="s">
         <v>479</v>
       </c>
@@ -10039,7 +10145,7 @@
       <c r="S168" s="44"/>
       <c r="T168" s="44"/>
     </row>
-    <row r="169" spans="1:20" ht="48">
+    <row r="169" spans="1:20" x14ac:dyDescent="0.7">
       <c r="A169" s="9" t="s">
         <v>482</v>
       </c>
@@ -10073,7 +10179,7 @@
       <c r="S169" s="44"/>
       <c r="T169" s="44"/>
     </row>
-    <row r="170" spans="1:20" ht="48">
+    <row r="170" spans="1:20" x14ac:dyDescent="0.7">
       <c r="A170" s="9" t="s">
         <v>485</v>
       </c>
@@ -10107,7 +10213,7 @@
       <c r="S170" s="44"/>
       <c r="T170" s="44"/>
     </row>
-    <row r="171" spans="1:20" ht="48">
+    <row r="171" spans="1:20" x14ac:dyDescent="0.7">
       <c r="A171" s="9" t="s">
         <v>488</v>
       </c>
@@ -10137,7 +10243,7 @@
       <c r="S171" s="44"/>
       <c r="T171" s="44"/>
     </row>
-    <row r="172" spans="1:20" ht="94">
+    <row r="172" spans="1:20" ht="92.25" x14ac:dyDescent="0.7">
       <c r="A172" s="9" t="s">
         <v>491</v>
       </c>
@@ -10171,7 +10277,7 @@
       <c r="S172" s="44"/>
       <c r="T172" s="44"/>
     </row>
-    <row r="173" spans="1:20" ht="48">
+    <row r="173" spans="1:20" x14ac:dyDescent="0.7">
       <c r="A173" s="9" t="s">
         <v>494</v>
       </c>
@@ -10205,7 +10311,7 @@
       <c r="S173" s="44"/>
       <c r="T173" s="44"/>
     </row>
-    <row r="174" spans="1:20" ht="94">
+    <row r="174" spans="1:20" ht="92.25" x14ac:dyDescent="0.7">
       <c r="A174" s="9" t="s">
         <v>497</v>
       </c>
@@ -10239,7 +10345,7 @@
       <c r="S174" s="44"/>
       <c r="T174" s="44"/>
     </row>
-    <row r="175" spans="1:20">
+    <row r="175" spans="1:20" x14ac:dyDescent="0.7">
       <c r="A175" s="9" t="s">
         <v>500</v>
       </c>
@@ -10273,7 +10379,7 @@
       <c r="S175" s="44"/>
       <c r="T175" s="44"/>
     </row>
-    <row r="176" spans="1:20">
+    <row r="176" spans="1:20" x14ac:dyDescent="0.7">
       <c r="A176" s="9" t="s">
         <v>503</v>
       </c>
@@ -10307,7 +10413,7 @@
       <c r="S176" s="44"/>
       <c r="T176" s="44"/>
     </row>
-    <row r="177" spans="1:20">
+    <row r="177" spans="1:20" x14ac:dyDescent="0.7">
       <c r="A177" s="9" t="s">
         <v>506</v>
       </c>
@@ -10341,7 +10447,7 @@
       <c r="S177" s="44"/>
       <c r="T177" s="44"/>
     </row>
-    <row r="178" spans="1:20" ht="48">
+    <row r="178" spans="1:20" x14ac:dyDescent="0.7">
       <c r="A178" s="9" t="s">
         <v>509</v>
       </c>
@@ -10375,7 +10481,7 @@
       <c r="S178" s="44"/>
       <c r="T178" s="44"/>
     </row>
-    <row r="179" spans="1:20" ht="92">
+    <row r="179" spans="1:20" ht="91.5" x14ac:dyDescent="0.7">
       <c r="A179" s="9" t="s">
         <v>512</v>
       </c>
@@ -10409,7 +10515,7 @@
       <c r="S179" s="44"/>
       <c r="T179" s="44"/>
     </row>
-    <row r="180" spans="1:20" ht="48">
+    <row r="180" spans="1:20" x14ac:dyDescent="0.7">
       <c r="A180" s="9" t="s">
         <v>514</v>
       </c>
@@ -10443,7 +10549,7 @@
       <c r="S180" s="44"/>
       <c r="T180" s="44"/>
     </row>
-    <row r="181" spans="1:20" ht="48">
+    <row r="181" spans="1:20" x14ac:dyDescent="0.7">
       <c r="A181" s="9" t="s">
         <v>516</v>
       </c>
@@ -10477,7 +10583,7 @@
       <c r="S181" s="44"/>
       <c r="T181" s="44"/>
     </row>
-    <row r="182" spans="1:20" ht="48">
+    <row r="182" spans="1:20" ht="92.25" x14ac:dyDescent="0.7">
       <c r="A182" s="9" t="s">
         <v>518</v>
       </c>
@@ -10511,7 +10617,7 @@
       <c r="S182" s="44"/>
       <c r="T182" s="44"/>
     </row>
-    <row r="183" spans="1:20" ht="48">
+    <row r="183" spans="1:20" x14ac:dyDescent="0.7">
       <c r="A183" s="9" t="s">
         <v>520</v>
       </c>
@@ -10545,7 +10651,7 @@
       <c r="S183" s="44"/>
       <c r="T183" s="44"/>
     </row>
-    <row r="184" spans="1:20" ht="94">
+    <row r="184" spans="1:20" ht="92.25" x14ac:dyDescent="0.7">
       <c r="A184" s="9" t="s">
         <v>522</v>
       </c>
@@ -10579,7 +10685,7 @@
       <c r="S184" s="44"/>
       <c r="T184" s="44"/>
     </row>
-    <row r="185" spans="1:20" ht="94">
+    <row r="185" spans="1:20" ht="92.25" x14ac:dyDescent="0.7">
       <c r="A185" s="9" t="s">
         <v>524</v>
       </c>
@@ -10613,7 +10719,7 @@
       <c r="S185" s="44"/>
       <c r="T185" s="44"/>
     </row>
-    <row r="186" spans="1:20" ht="94">
+    <row r="186" spans="1:20" ht="92.25" x14ac:dyDescent="0.7">
       <c r="A186" s="9" t="s">
         <v>527</v>
       </c>
@@ -10647,7 +10753,7 @@
       <c r="S186" s="44"/>
       <c r="T186" s="44"/>
     </row>
-    <row r="187" spans="1:20" ht="48">
+    <row r="187" spans="1:20" ht="92.25" x14ac:dyDescent="0.7">
       <c r="A187" s="9" t="s">
         <v>530</v>
       </c>
@@ -10681,7 +10787,7 @@
       <c r="S187" s="44"/>
       <c r="T187" s="44"/>
     </row>
-    <row r="188" spans="1:20" ht="94">
+    <row r="188" spans="1:20" ht="92.25" x14ac:dyDescent="0.7">
       <c r="A188" s="9" t="s">
         <v>533</v>
       </c>
@@ -10715,7 +10821,7 @@
       <c r="S188" s="44"/>
       <c r="T188" s="44"/>
     </row>
-    <row r="189" spans="1:20" ht="94">
+    <row r="189" spans="1:20" ht="92.25" x14ac:dyDescent="0.7">
       <c r="A189" s="9" t="s">
         <v>536</v>
       </c>
@@ -10749,7 +10855,7 @@
       <c r="S189" s="44"/>
       <c r="T189" s="44"/>
     </row>
-    <row r="190" spans="1:20" ht="94">
+    <row r="190" spans="1:20" ht="92.25" x14ac:dyDescent="0.7">
       <c r="A190" s="9" t="s">
         <v>539</v>
       </c>
@@ -10783,7 +10889,7 @@
       <c r="S190" s="44"/>
       <c r="T190" s="44"/>
     </row>
-    <row r="191" spans="1:20" ht="94">
+    <row r="191" spans="1:20" ht="92.25" x14ac:dyDescent="0.7">
       <c r="A191" s="9" t="s">
         <v>542</v>
       </c>
@@ -10817,7 +10923,7 @@
       <c r="S191" s="44"/>
       <c r="T191" s="44"/>
     </row>
-    <row r="192" spans="1:20" ht="94">
+    <row r="192" spans="1:20" ht="92.25" x14ac:dyDescent="0.7">
       <c r="A192" s="9" t="s">
         <v>545</v>
       </c>
@@ -10851,7 +10957,7 @@
       <c r="S192" s="44"/>
       <c r="T192" s="44"/>
     </row>
-    <row r="193" spans="1:20" ht="94">
+    <row r="193" spans="1:20" ht="92.25" x14ac:dyDescent="0.7">
       <c r="A193" s="9" t="s">
         <v>548</v>
       </c>
@@ -10885,7 +10991,7 @@
       <c r="S193" s="44"/>
       <c r="T193" s="44"/>
     </row>
-    <row r="194" spans="1:20" ht="94">
+    <row r="194" spans="1:20" ht="92.25" x14ac:dyDescent="0.7">
       <c r="A194" s="9" t="s">
         <v>551</v>
       </c>
@@ -10919,7 +11025,7 @@
       <c r="S194" s="44"/>
       <c r="T194" s="44"/>
     </row>
-    <row r="195" spans="1:20" ht="48">
+    <row r="195" spans="1:20" ht="92.25" x14ac:dyDescent="0.7">
       <c r="A195" s="9" t="s">
         <v>554</v>
       </c>
@@ -10953,7 +11059,7 @@
       <c r="S195" s="44"/>
       <c r="T195" s="44"/>
     </row>
-    <row r="196" spans="1:20" ht="48">
+    <row r="196" spans="1:20" x14ac:dyDescent="0.7">
       <c r="A196" s="9" t="s">
         <v>557</v>
       </c>
@@ -10987,7 +11093,7 @@
       <c r="S196" s="44"/>
       <c r="T196" s="44"/>
     </row>
-    <row r="197" spans="1:20" ht="94">
+    <row r="197" spans="1:20" ht="92.25" x14ac:dyDescent="0.7">
       <c r="A197" s="9" t="s">
         <v>560</v>
       </c>
@@ -11021,7 +11127,7 @@
       <c r="S197" s="44"/>
       <c r="T197" s="44"/>
     </row>
-    <row r="198" spans="1:20" ht="94">
+    <row r="198" spans="1:20" ht="92.25" x14ac:dyDescent="0.7">
       <c r="A198" s="9" t="s">
         <v>563</v>
       </c>
@@ -11055,7 +11161,7 @@
       <c r="S198" s="44"/>
       <c r="T198" s="44"/>
     </row>
-    <row r="199" spans="1:20" ht="94">
+    <row r="199" spans="1:20" ht="138" x14ac:dyDescent="0.7">
       <c r="A199" s="9" t="s">
         <v>566</v>
       </c>
@@ -11089,7 +11195,7 @@
       <c r="S199" s="44"/>
       <c r="T199" s="44"/>
     </row>
-    <row r="200" spans="1:20" ht="94">
+    <row r="200" spans="1:20" ht="92.25" x14ac:dyDescent="0.7">
       <c r="A200" s="9" t="s">
         <v>569</v>
       </c>
@@ -11123,7 +11229,7 @@
       <c r="S200" s="44"/>
       <c r="T200" s="44"/>
     </row>
-    <row r="201" spans="1:20" ht="48">
+    <row r="201" spans="1:20" ht="92.25" x14ac:dyDescent="0.7">
       <c r="A201" s="9" t="s">
         <v>572</v>
       </c>
@@ -11157,7 +11263,7 @@
       <c r="S201" s="44"/>
       <c r="T201" s="44"/>
     </row>
-    <row r="202" spans="1:20" ht="94">
+    <row r="202" spans="1:20" ht="92.25" x14ac:dyDescent="0.7">
       <c r="A202" s="9" t="s">
         <v>575</v>
       </c>
@@ -11191,7 +11297,7 @@
       <c r="S202" s="44"/>
       <c r="T202" s="44"/>
     </row>
-    <row r="203" spans="1:20" ht="94">
+    <row r="203" spans="1:20" ht="92.25" x14ac:dyDescent="0.7">
       <c r="A203" s="9" t="s">
         <v>578</v>
       </c>
@@ -11225,7 +11331,7 @@
       <c r="S203" s="44"/>
       <c r="T203" s="44"/>
     </row>
-    <row r="204" spans="1:20" ht="350.25" customHeight="1">
+    <row r="204" spans="1:20" ht="350.25" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A204" s="9" t="s">
         <v>581</v>
       </c>
@@ -11259,7 +11365,7 @@
       <c r="S204" s="44"/>
       <c r="T204" s="44"/>
     </row>
-    <row r="205" spans="1:20" ht="300" customHeight="1">
+    <row r="205" spans="1:20" ht="300" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A205" s="9" t="s">
         <v>584</v>
       </c>
@@ -11297,7 +11403,7 @@
       <c r="S205" s="44"/>
       <c r="T205" s="44"/>
     </row>
-    <row r="206" spans="1:20" ht="300" customHeight="1">
+    <row r="206" spans="1:20" ht="300" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A206" s="9" t="s">
         <v>587</v>
       </c>
@@ -11335,7 +11441,7 @@
       <c r="S206" s="44"/>
       <c r="T206" s="44"/>
     </row>
-    <row r="207" spans="1:20" ht="300" customHeight="1">
+    <row r="207" spans="1:20" ht="300" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A207" s="9" t="s">
         <v>589</v>
       </c>
@@ -11369,7 +11475,7 @@
       <c r="S207" s="44"/>
       <c r="T207" s="44"/>
     </row>
-    <row r="208" spans="1:20" ht="300" customHeight="1">
+    <row r="208" spans="1:20" ht="300" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A208" s="9" t="s">
         <v>591</v>
       </c>
@@ -11407,7 +11513,7 @@
       <c r="S208" s="44"/>
       <c r="T208" s="44"/>
     </row>
-    <row r="209" spans="1:20" ht="300" customHeight="1">
+    <row r="209" spans="1:20" ht="300" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A209" s="9" t="s">
         <v>593</v>
       </c>
@@ -11441,7 +11547,7 @@
       <c r="S209" s="44"/>
       <c r="T209" s="44"/>
     </row>
-    <row r="210" spans="1:20" ht="399.75" customHeight="1">
+    <row r="210" spans="1:20" ht="399.75" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A210" s="9" t="s">
         <v>595</v>
       </c>
@@ -11473,7 +11579,7 @@
       <c r="Q210" s="4"/>
       <c r="R210" s="4"/>
     </row>
-    <row r="211" spans="1:20" ht="300" customHeight="1">
+    <row r="211" spans="1:20" ht="300" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A211" s="9" t="s">
         <v>597</v>
       </c>
@@ -11505,7 +11611,7 @@
       <c r="Q211" s="4"/>
       <c r="R211" s="4"/>
     </row>
-    <row r="212" spans="1:20" ht="300" customHeight="1">
+    <row r="212" spans="1:20" ht="300" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A212" s="9" t="s">
         <v>599</v>
       </c>
@@ -11537,7 +11643,7 @@
       <c r="Q212" s="4"/>
       <c r="R212" s="4"/>
     </row>
-    <row r="213" spans="1:20" ht="150" customHeight="1">
+    <row r="213" spans="1:20" ht="150" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A213" s="9" t="s">
         <v>601</v>
       </c>
@@ -11569,7 +11675,7 @@
       <c r="Q213" s="4"/>
       <c r="R213" s="4"/>
     </row>
-    <row r="214" spans="1:20" ht="96">
+    <row r="214" spans="1:20" ht="93" x14ac:dyDescent="0.7">
       <c r="A214" s="4" t="s">
         <v>603</v>
       </c>
@@ -11599,7 +11705,7 @@
       <c r="Q214" s="4"/>
       <c r="R214" s="4"/>
     </row>
-    <row r="215" spans="1:20" ht="48">
+    <row r="215" spans="1:20" x14ac:dyDescent="0.7">
       <c r="A215" s="4" t="s">
         <v>606</v>
       </c>
@@ -11629,7 +11735,7 @@
       <c r="Q215" s="4"/>
       <c r="R215" s="4"/>
     </row>
-    <row r="216" spans="1:20" ht="48">
+    <row r="216" spans="1:20" ht="93" x14ac:dyDescent="0.7">
       <c r="A216" s="4" t="s">
         <v>609</v>
       </c>
@@ -11659,7 +11765,7 @@
       <c r="Q216" s="4"/>
       <c r="R216" s="4"/>
     </row>
-    <row r="217" spans="1:20" ht="48">
+    <row r="217" spans="1:20" x14ac:dyDescent="0.7">
       <c r="A217" s="4" t="s">
         <v>611</v>
       </c>
@@ -11689,7 +11795,7 @@
       <c r="Q217" s="4"/>
       <c r="R217" s="4"/>
     </row>
-    <row r="218" spans="1:20" ht="48">
+    <row r="218" spans="1:20" ht="93" x14ac:dyDescent="0.7">
       <c r="A218" s="4" t="s">
         <v>613</v>
       </c>
@@ -11717,7 +11823,7 @@
       <c r="Q218" s="4"/>
       <c r="R218" s="4"/>
     </row>
-    <row r="219" spans="1:20" ht="48">
+    <row r="219" spans="1:20" x14ac:dyDescent="0.7">
       <c r="A219" s="4" t="s">
         <v>615</v>
       </c>
@@ -11745,7 +11851,7 @@
       <c r="Q219" s="4"/>
       <c r="R219" s="4"/>
     </row>
-    <row r="220" spans="1:20" ht="48">
+    <row r="220" spans="1:20" x14ac:dyDescent="0.7">
       <c r="A220" s="4" t="s">
         <v>618</v>
       </c>
@@ -11775,7 +11881,7 @@
       <c r="Q220" s="4"/>
       <c r="R220" s="4"/>
     </row>
-    <row r="221" spans="1:20" ht="48">
+    <row r="221" spans="1:20" ht="93" x14ac:dyDescent="0.7">
       <c r="A221" s="4" t="s">
         <v>622</v>
       </c>
@@ -11805,7 +11911,7 @@
       <c r="Q221" s="4"/>
       <c r="R221" s="4"/>
     </row>
-    <row r="222" spans="1:20" ht="48">
+    <row r="222" spans="1:20" x14ac:dyDescent="0.7">
       <c r="A222" s="4" t="s">
         <v>626</v>
       </c>
@@ -11835,7 +11941,7 @@
       <c r="Q222" s="4"/>
       <c r="R222" s="4"/>
     </row>
-    <row r="223" spans="1:20" ht="96">
+    <row r="223" spans="1:20" ht="93" x14ac:dyDescent="0.7">
       <c r="A223" s="4" t="s">
         <v>629</v>
       </c>
@@ -11867,7 +11973,7 @@
       <c r="Q223" s="4"/>
       <c r="R223" s="4"/>
     </row>
-    <row r="224" spans="1:20" ht="48">
+    <row r="224" spans="1:20" x14ac:dyDescent="0.7">
       <c r="A224" s="4" t="s">
         <v>633</v>
       </c>
@@ -11897,7 +12003,7 @@
       <c r="Q224" s="4"/>
       <c r="R224" s="4"/>
     </row>
-    <row r="225" spans="1:18" ht="48">
+    <row r="225" spans="1:18" x14ac:dyDescent="0.7">
       <c r="A225" s="4" t="s">
         <v>636</v>
       </c>
@@ -11927,7 +12033,7 @@
       <c r="Q225" s="4"/>
       <c r="R225" s="4"/>
     </row>
-    <row r="226" spans="1:18" ht="96">
+    <row r="226" spans="1:18" ht="93" x14ac:dyDescent="0.7">
       <c r="A226" s="4" t="s">
         <v>639</v>
       </c>
@@ -11957,7 +12063,7 @@
       <c r="Q226" s="4"/>
       <c r="R226" s="4"/>
     </row>
-    <row r="227" spans="1:18" ht="96">
+    <row r="227" spans="1:18" ht="93" x14ac:dyDescent="0.7">
       <c r="A227" s="4" t="s">
         <v>642</v>
       </c>
@@ -11987,7 +12093,7 @@
       <c r="Q227" s="4"/>
       <c r="R227" s="4"/>
     </row>
-    <row r="228" spans="1:18" ht="96">
+    <row r="228" spans="1:18" ht="93" x14ac:dyDescent="0.7">
       <c r="A228" s="4" t="s">
         <v>645</v>
       </c>
@@ -12036,15 +12142,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F5DF915EA4BB084DB5AFDEC09381A8FB" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a8bfd8294cc6ef9580ab498b0ea1a4b0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="4d8d79fe-4947-4674-81e0-6583e9bfe4f8" xmlns:ns4="c2641e0b-4c18-4c38-a43e-68190c3edb42" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6a9b76ea4862c7452c415f65ac2c735a" ns3:_="" ns4:_="">
     <xsd:import namespace="4d8d79fe-4947-4674-81e0-6583e9bfe4f8"/>
@@ -12277,6 +12374,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0EA954FC-C7AE-4DD6-BF3A-FC1E0C3B7857}">
   <ds:schemaRefs>
@@ -12288,14 +12394,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C8131CB9-B24D-4314-824E-AB1327ACF550}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C93AC341-3165-48FE-919E-1B8955D5F238}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -12312,4 +12410,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C8131CB9-B24D-4314-824E-AB1327ACF550}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added group 10 testing requirements spreadsheet
</commit_message>
<xml_diff>
--- a/FinalRequirements.xlsx
+++ b/FinalRequirements.xlsx
@@ -5,17 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yukes\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\18173\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8BFADDBF-BECC-49C7-967B-0CE0BF4A4BDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DB00B3E-0FD8-4F25-B30E-ABB22CB0DA9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -40,7 +40,7 @@
   <metadataTypes count="1">
     <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
-  <futureMetadata name="XLRICHVALUE" count="15">
+  <futureMetadata name="XLRICHVALUE" count="20">
     <bk>
       <extLst>
         <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
@@ -146,8 +146,43 @@
         </ext>
       </extLst>
     </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="15"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="16"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="17"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="18"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="19"/>
+        </ext>
+      </extLst>
+    </bk>
   </futureMetadata>
-  <valueMetadata count="15">
+  <valueMetadata count="20">
     <bk>
       <rc t="1" v="0"/>
     </bk>
@@ -193,12 +228,27 @@
     <bk>
       <rc t="1" v="14"/>
     </bk>
+    <bk>
+      <rc t="1" v="15"/>
+    </bk>
+    <bk>
+      <rc t="1" v="16"/>
+    </bk>
+    <bk>
+      <rc t="1" v="17"/>
+    </bk>
+    <bk>
+      <rc t="1" v="18"/>
+    </bk>
+    <bk>
+      <rc t="1" v="19"/>
+    </bk>
   </valueMetadata>
 </metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1214" uniqueCount="699">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1238" uniqueCount="716">
   <si>
     <t>Testing</t>
   </si>
@@ -2448,14 +2498,76 @@
     <t>cannot join game, therefore cannot test it</t>
   </si>
   <si>
-    <t>it shows error message.</t>
+    <t>The page is not showing 
+the username of the player
+who joined, it is just showing 
+Player 1 or player 2</t>
+  </si>
+  <si>
+    <t>Yes the page shows the 
+2 bots are in the lobby</t>
+  </si>
+  <si>
+    <t>Yes the page shows the 
+10 lobbies that users can join</t>
+  </si>
+  <si>
+    <t>Yes the page shows the 
+back button but it is not functioning , i.e nothing happens.</t>
+  </si>
+  <si>
+    <t>Yes the page shows the 
+list of available lobbies</t>
+  </si>
+  <si>
+    <t>Single user is not able to join the lobby, if 2 players/Bot is there then directly enter the game but can't wait in lobby</t>
+  </si>
+  <si>
+    <t>No the page does not show the current status of the lobby.</t>
+  </si>
+  <si>
+    <t>Page does not shows the number of players in the lobby</t>
+  </si>
+  <si>
+    <t>Since there is no any interface for lobby, user cannot leave the lobby</t>
+  </si>
+  <si>
+    <t>Does not have "Start Game" button</t>
+  </si>
+  <si>
+    <t>No any error message</t>
+  </si>
+  <si>
+    <t>Color of the button
+changes but button has no function</t>
+  </si>
+  <si>
+    <t>User can add the 
+Bot I/BotII</t>
+  </si>
+  <si>
+    <t>No any waiting message
+was displayed</t>
+  </si>
+  <si>
+    <t>Since there is no any interface for lobby, user cannot see which lobby they are in</t>
+  </si>
+  <si>
+    <t>User are able to leave the game but it goes to create account/login page</t>
+  </si>
+  <si>
+    <t>Since there is no any interface for lobby, user cannot see any progress</t>
+  </si>
+  <si>
+    <t>Page is not showing any 
+users</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2511,6 +2623,12 @@
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="36"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -2671,7 +2789,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -2791,6 +2909,12 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3125,9 +3249,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>487080</xdr:colOff>
-      <xdr:row>132</xdr:row>
-      <xdr:rowOff>3049740</xdr:rowOff>
+      <xdr:colOff>487079</xdr:colOff>
+      <xdr:row>134</xdr:row>
+      <xdr:rowOff>192240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3342,7 +3466,7 @@
       <xdr:col>11</xdr:col>
       <xdr:colOff>3925440</xdr:colOff>
       <xdr:row>130</xdr:row>
-      <xdr:rowOff>463690</xdr:rowOff>
+      <xdr:rowOff>463680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3385,7 +3509,7 @@
       <xdr:col>11</xdr:col>
       <xdr:colOff>3533760</xdr:colOff>
       <xdr:row>132</xdr:row>
-      <xdr:rowOff>210610</xdr:rowOff>
+      <xdr:rowOff>210601</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3600,7 +3724,7 @@
       <xdr:col>11</xdr:col>
       <xdr:colOff>3552840</xdr:colOff>
       <xdr:row>134</xdr:row>
-      <xdr:rowOff>296280</xdr:rowOff>
+      <xdr:rowOff>296279</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4030,7 +4154,7 @@
       <xdr:col>11</xdr:col>
       <xdr:colOff>3916080</xdr:colOff>
       <xdr:row>148</xdr:row>
-      <xdr:rowOff>235080</xdr:rowOff>
+      <xdr:rowOff>235079</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4363,6 +4487,206 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>1333500</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>187502</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>4788377</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>2146475</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="37" name="Picture 36">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{072C8681-ED7B-4EA1-98E1-F0107EFE65F1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId29">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="82556350" y="7502702"/>
+          <a:ext cx="3457885" cy="1958973"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>253999</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>5643144</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>1585450</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="38" name="Picture 37">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{393F08E4-EF31-42BA-96AC-2A5876B05ABD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId30">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="81794350" y="28867099"/>
+          <a:ext cx="5073650" cy="1331451"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>1333500</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>187502</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>4791385</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>2146475</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="39" name="Picture 38">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A241152-7450-4945-9AFB-94B2EF873200}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId29">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="82556350" y="7502702"/>
+          <a:ext cx="3457885" cy="1958973"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>253999</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>1585450</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="40" name="Picture 39">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5669CA3A-8928-44DB-A304-9CF3103B58AB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId30">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="81794350" y="28867099"/>
+          <a:ext cx="5073650" cy="1331451"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4407,7 +4731,7 @@
 </file>
 
 <file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
-<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="15">
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="20">
   <rv s="0">
     <v>0</v>
     <v>5</v>
@@ -4468,6 +4792,26 @@
     <v>14</v>
     <v>5</v>
   </rv>
+  <rv s="0">
+    <v>15</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>16</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>17</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>18</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>19</v>
+    <v>5</v>
+  </rv>
 </rvData>
 </file>
 
@@ -4497,6 +4841,11 @@
   <rel r:id="rId13"/>
   <rel r:id="rId14"/>
   <rel r:id="rId15"/>
+  <rel r:id="rId16"/>
+  <rel r:id="rId17"/>
+  <rel r:id="rId18"/>
+  <rel r:id="rId19"/>
+  <rel r:id="rId20"/>
 </richValueRels>
 </file>
 
@@ -4624,41 +4973,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:T232"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A116" zoomScale="10" zoomScaleNormal="10" workbookViewId="0">
-      <selection activeCell="P150" sqref="P150"/>
+    <sheetView tabSelected="1" topLeftCell="F140" zoomScale="19" zoomScaleNormal="28" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="46.9" x14ac:dyDescent="1.4"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="47.5" x14ac:dyDescent="1.1000000000000001"/>
   <cols>
     <col min="1" max="1" width="21" style="1" customWidth="1"/>
-    <col min="2" max="2" width="19.46484375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="161.46484375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="250.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="210.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="164.33203125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="104.19921875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="34.796875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="30.1328125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="165.33203125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="34.1328125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.453125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="161.453125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="250.36328125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="210.6328125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="164.36328125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="104.1796875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="34.81640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="30.08984375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="165.36328125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="34.08984375" style="1" customWidth="1"/>
     <col min="12" max="12" width="131" style="1" customWidth="1"/>
     <col min="13" max="13" width="33" style="1" customWidth="1"/>
-    <col min="14" max="14" width="46.46484375" style="1" customWidth="1"/>
+    <col min="14" max="14" width="107.1796875" style="55" customWidth="1"/>
     <col min="15" max="15" width="33" style="1" customWidth="1"/>
     <col min="16" max="16" width="133" style="1" customWidth="1"/>
     <col min="17" max="17" width="158" style="1" customWidth="1"/>
-    <col min="18" max="18" width="40.1328125" style="1" customWidth="1"/>
-    <col min="19" max="19" width="8.796875" style="1"/>
-    <col min="20" max="20" width="153.1328125" style="1" customWidth="1"/>
-    <col min="21" max="16384" width="8.796875" style="1"/>
+    <col min="18" max="18" width="40.08984375" style="1" customWidth="1"/>
+    <col min="19" max="19" width="8.81640625" style="1"/>
+    <col min="20" max="20" width="153.08984375" style="1" customWidth="1"/>
+    <col min="21" max="16384" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:20" x14ac:dyDescent="1.4">
+    <row r="2" spans="1:20" x14ac:dyDescent="1.1000000000000001">
       <c r="L2" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="1.4">
+    <row r="3" spans="1:20" x14ac:dyDescent="1.1000000000000001">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -4698,7 +5047,7 @@
       <c r="M3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="N3" s="56" t="s">
         <v>14</v>
       </c>
       <c r="O3" s="3" t="s">
@@ -4714,7 +5063,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="140.65" x14ac:dyDescent="1.4">
+    <row r="4" spans="1:20" ht="142.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A4" s="8" t="s">
         <v>19</v>
       </c>
@@ -4745,7 +5094,9 @@
       <c r="M4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="N4" s="3"/>
+      <c r="N4" s="53" t="s">
+        <v>23</v>
+      </c>
       <c r="O4" s="3"/>
       <c r="P4" s="3" t="s">
         <v>22</v>
@@ -4756,7 +5107,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="291" customHeight="1" x14ac:dyDescent="1.4">
+    <row r="5" spans="1:20" ht="291" customHeight="1" x14ac:dyDescent="1.1000000000000001">
       <c r="A5" s="8" t="s">
         <v>25</v>
       </c>
@@ -4784,13 +5135,15 @@
         <v>#VALUE!</v>
       </c>
       <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
+      <c r="N5" s="54" t="s">
+        <v>698</v>
+      </c>
       <c r="O5" s="3"/>
       <c r="P5" s="3"/>
       <c r="Q5" s="3"/>
       <c r="R5" s="3"/>
     </row>
-    <row r="6" spans="1:20" ht="285.75" customHeight="1" x14ac:dyDescent="1.4">
+    <row r="6" spans="1:20" ht="285.75" customHeight="1" x14ac:dyDescent="1.1000000000000001">
       <c r="A6" s="8" t="s">
         <v>28</v>
       </c>
@@ -4818,13 +5171,15 @@
         <v>#VALUE!</v>
       </c>
       <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
+      <c r="N6" s="54" t="s">
+        <v>699</v>
+      </c>
       <c r="O6" s="3"/>
       <c r="P6" s="3"/>
       <c r="Q6" s="3"/>
       <c r="R6" s="3"/>
     </row>
-    <row r="7" spans="1:20" ht="287.25" customHeight="1" x14ac:dyDescent="1.4">
+    <row r="7" spans="1:20" ht="287.25" customHeight="1" x14ac:dyDescent="1.1000000000000001">
       <c r="A7" s="8" t="s">
         <v>31</v>
       </c>
@@ -4852,13 +5207,15 @@
         <v>#VALUE!</v>
       </c>
       <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
+      <c r="N7" s="54" t="s">
+        <v>700</v>
+      </c>
       <c r="O7" s="3"/>
       <c r="P7" s="3"/>
       <c r="Q7" s="3"/>
       <c r="R7" s="3"/>
     </row>
-    <row r="8" spans="1:20" ht="329.25" customHeight="1" x14ac:dyDescent="1.4">
+    <row r="8" spans="1:20" ht="329.25" customHeight="1" x14ac:dyDescent="1.1000000000000001">
       <c r="A8" s="8" t="s">
         <v>34</v>
       </c>
@@ -4886,13 +5243,15 @@
         <v>#VALUE!</v>
       </c>
       <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
+      <c r="N8" s="54" t="s">
+        <v>701</v>
+      </c>
       <c r="O8" s="3"/>
       <c r="P8" s="3"/>
       <c r="Q8" s="3"/>
       <c r="R8" s="3"/>
     </row>
-    <row r="9" spans="1:20" ht="138.4" x14ac:dyDescent="1.4">
+    <row r="9" spans="1:20" ht="139.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A9" s="8" t="s">
         <v>37</v>
       </c>
@@ -4920,7 +5279,9 @@
         <v>39</v>
       </c>
       <c r="M9" s="3"/>
-      <c r="N9" s="3"/>
+      <c r="N9" s="53" t="s">
+        <v>39</v>
+      </c>
       <c r="O9" s="3"/>
       <c r="P9" s="3" t="s">
         <v>39</v>
@@ -4928,7 +5289,7 @@
       <c r="Q9" s="3"/>
       <c r="R9" s="3"/>
     </row>
-    <row r="10" spans="1:20" ht="318" customHeight="1" x14ac:dyDescent="1.4">
+    <row r="10" spans="1:20" ht="318" customHeight="1" x14ac:dyDescent="1.1000000000000001">
       <c r="A10" s="8" t="s">
         <v>40</v>
       </c>
@@ -4959,13 +5320,15 @@
       <c r="M10" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="N10" s="3"/>
+      <c r="N10" s="53" t="s">
+        <v>23</v>
+      </c>
       <c r="O10" s="3"/>
       <c r="P10" s="3"/>
       <c r="Q10" s="3"/>
       <c r="R10" s="3"/>
     </row>
-    <row r="11" spans="1:20" ht="318" customHeight="1" x14ac:dyDescent="1.4">
+    <row r="11" spans="1:20" ht="318" customHeight="1" x14ac:dyDescent="1.1000000000000001">
       <c r="A11" s="8" t="s">
         <v>44</v>
       </c>
@@ -4996,7 +5359,9 @@
       <c r="M11" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="N11" s="3"/>
+      <c r="N11" s="54" t="s">
+        <v>702</v>
+      </c>
       <c r="O11" s="3"/>
       <c r="P11" s="3" t="s">
         <v>49</v>
@@ -5004,7 +5369,7 @@
       <c r="Q11" s="3"/>
       <c r="R11" s="3"/>
     </row>
-    <row r="12" spans="1:20" ht="334.5" customHeight="1" x14ac:dyDescent="1.4">
+    <row r="12" spans="1:20" ht="334.5" customHeight="1" x14ac:dyDescent="1.1000000000000001">
       <c r="A12" s="8" t="s">
         <v>50</v>
       </c>
@@ -5034,7 +5399,9 @@
         <v>#VALUE!</v>
       </c>
       <c r="M12" s="3"/>
-      <c r="N12" s="3"/>
+      <c r="N12" s="54" t="s">
+        <v>703</v>
+      </c>
       <c r="O12" s="3"/>
       <c r="P12" s="3" t="s">
         <v>54</v>
@@ -5042,7 +5409,7 @@
       <c r="Q12" s="3"/>
       <c r="R12" s="3"/>
     </row>
-    <row r="13" spans="1:20" ht="313.5" customHeight="1" x14ac:dyDescent="1.4">
+    <row r="13" spans="1:20" ht="313.5" customHeight="1" x14ac:dyDescent="1.1000000000000001">
       <c r="A13" s="8" t="s">
         <v>55</v>
       </c>
@@ -5073,13 +5440,15 @@
       <c r="M13" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="N13" s="3"/>
+      <c r="N13" s="54" t="s">
+        <v>704</v>
+      </c>
       <c r="O13" s="3"/>
       <c r="P13" s="3"/>
       <c r="Q13" s="3"/>
       <c r="R13" s="3"/>
     </row>
-    <row r="14" spans="1:20" ht="249.75" customHeight="1" x14ac:dyDescent="1.4">
+    <row r="14" spans="1:20" ht="249.75" customHeight="1" x14ac:dyDescent="1.1000000000000001">
       <c r="A14" s="8" t="s">
         <v>60</v>
       </c>
@@ -5110,13 +5479,15 @@
       <c r="M14" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="N14" s="3"/>
+      <c r="N14" s="54" t="s">
+        <v>705</v>
+      </c>
       <c r="O14" s="3"/>
       <c r="P14" s="3"/>
       <c r="Q14" s="3"/>
       <c r="R14" s="3"/>
     </row>
-    <row r="15" spans="1:20" ht="399.75" customHeight="1" x14ac:dyDescent="1.4">
+    <row r="15" spans="1:20" ht="399.75" customHeight="1" x14ac:dyDescent="1.1000000000000001">
       <c r="A15" s="8" t="s">
         <v>65</v>
       </c>
@@ -5147,7 +5518,9 @@
       <c r="M15" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="N15" s="3"/>
+      <c r="N15" s="54" t="s">
+        <v>706</v>
+      </c>
       <c r="O15" s="3"/>
       <c r="P15" s="3" t="s">
         <v>70</v>
@@ -5155,7 +5528,7 @@
       <c r="Q15" s="3"/>
       <c r="R15" s="3"/>
     </row>
-    <row r="16" spans="1:20" ht="138.4" x14ac:dyDescent="1.4">
+    <row r="16" spans="1:20" ht="185.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A16" s="8" t="s">
         <v>71</v>
       </c>
@@ -5183,13 +5556,15 @@
       <c r="M16" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="N16" s="3"/>
+      <c r="N16" s="54" t="s">
+        <v>707</v>
+      </c>
       <c r="O16" s="3"/>
       <c r="P16" s="3"/>
       <c r="Q16" s="3"/>
       <c r="R16" s="3"/>
     </row>
-    <row r="17" spans="1:18" ht="249.75" customHeight="1" x14ac:dyDescent="1.4">
+    <row r="17" spans="1:18" ht="249.75" customHeight="1" x14ac:dyDescent="1.1000000000000001">
       <c r="A17" s="8" t="s">
         <v>76</v>
       </c>
@@ -5218,13 +5593,15 @@
       <c r="M17" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="N17" s="3"/>
+      <c r="N17" s="53" t="s">
+        <v>708</v>
+      </c>
       <c r="O17" s="3"/>
       <c r="P17" s="3"/>
       <c r="Q17" s="3"/>
       <c r="R17" s="3"/>
     </row>
-    <row r="18" spans="1:18" ht="249.75" customHeight="1" x14ac:dyDescent="1.4">
+    <row r="18" spans="1:18" ht="249.75" customHeight="1" x14ac:dyDescent="1.1000000000000001">
       <c r="A18" s="8" t="s">
         <v>81</v>
       </c>
@@ -5251,13 +5628,15 @@
         <v>23</v>
       </c>
       <c r="M18" s="10"/>
-      <c r="N18" s="3"/>
+      <c r="N18" s="53" t="s">
+        <v>23</v>
+      </c>
       <c r="O18" s="3"/>
       <c r="P18" s="3"/>
       <c r="Q18" s="3"/>
       <c r="R18" s="3"/>
     </row>
-    <row r="19" spans="1:18" ht="92.65" x14ac:dyDescent="1.4">
+    <row r="19" spans="1:18" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A19" s="8" t="s">
         <v>84</v>
       </c>
@@ -5283,13 +5662,15 @@
       <c r="M19" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="N19" s="3"/>
+      <c r="N19" s="53" t="s">
+        <v>23</v>
+      </c>
       <c r="O19" s="3"/>
       <c r="P19" s="3"/>
       <c r="Q19" s="3"/>
       <c r="R19" s="3"/>
     </row>
-    <row r="20" spans="1:18" ht="249.75" customHeight="1" x14ac:dyDescent="1.4">
+    <row r="20" spans="1:18" ht="249.75" customHeight="1" x14ac:dyDescent="1.1000000000000001">
       <c r="A20" s="8" t="s">
         <v>87</v>
       </c>
@@ -5318,13 +5699,15 @@
       <c r="M20" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="N20" s="3"/>
+      <c r="N20" s="54" t="s">
+        <v>709</v>
+      </c>
       <c r="O20" s="3"/>
       <c r="P20" s="3"/>
       <c r="Q20" s="3"/>
       <c r="R20" s="3"/>
     </row>
-    <row r="21" spans="1:18" ht="199.5" customHeight="1" x14ac:dyDescent="1.4">
+    <row r="21" spans="1:18" ht="199.5" customHeight="1" x14ac:dyDescent="1.1000000000000001">
       <c r="A21" s="8" t="s">
         <v>91</v>
       </c>
@@ -5353,13 +5736,15 @@
       <c r="M21" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="N21" s="3"/>
+      <c r="N21" s="54" t="s">
+        <v>710</v>
+      </c>
       <c r="O21" s="3"/>
       <c r="P21" s="3"/>
       <c r="Q21" s="3"/>
       <c r="R21" s="3"/>
     </row>
-    <row r="22" spans="1:18" ht="349.5" customHeight="1" x14ac:dyDescent="1.4">
+    <row r="22" spans="1:18" ht="349.5" customHeight="1" x14ac:dyDescent="1.1000000000000001">
       <c r="A22" s="8" t="s">
         <v>95</v>
       </c>
@@ -5386,13 +5771,15 @@
         <v>23</v>
       </c>
       <c r="M22" s="10"/>
-      <c r="N22" s="3"/>
+      <c r="N22" s="53" t="s">
+        <v>23</v>
+      </c>
       <c r="O22" s="3"/>
       <c r="P22" s="3"/>
       <c r="Q22" s="3"/>
       <c r="R22" s="3"/>
     </row>
-    <row r="23" spans="1:18" ht="300" customHeight="1" x14ac:dyDescent="1.4">
+    <row r="23" spans="1:18" ht="300" customHeight="1" x14ac:dyDescent="1.1000000000000001">
       <c r="A23" s="8" t="s">
         <v>98</v>
       </c>
@@ -5419,13 +5806,15 @@
         <v>23</v>
       </c>
       <c r="M23" s="10"/>
-      <c r="N23" s="3"/>
+      <c r="N23" s="54" t="s">
+        <v>711</v>
+      </c>
       <c r="O23" s="3"/>
       <c r="P23" s="3"/>
       <c r="Q23" s="3"/>
       <c r="R23" s="3"/>
     </row>
-    <row r="24" spans="1:18" ht="349.5" customHeight="1" x14ac:dyDescent="1.4">
+    <row r="24" spans="1:18" ht="349.5" customHeight="1" x14ac:dyDescent="1.1000000000000001">
       <c r="A24" s="8" t="s">
         <v>101</v>
       </c>
@@ -5452,13 +5841,15 @@
         <v>23</v>
       </c>
       <c r="M24" s="10"/>
-      <c r="N24" s="3"/>
+      <c r="N24" s="54" t="s">
+        <v>712</v>
+      </c>
       <c r="O24" s="3"/>
       <c r="P24" s="3"/>
       <c r="Q24" s="3"/>
       <c r="R24" s="3"/>
     </row>
-    <row r="25" spans="1:18" ht="349.5" customHeight="1" x14ac:dyDescent="1.4">
+    <row r="25" spans="1:18" ht="349.5" customHeight="1" x14ac:dyDescent="1.1000000000000001">
       <c r="A25" s="8" t="s">
         <v>104</v>
       </c>
@@ -5485,13 +5876,15 @@
         <v>23</v>
       </c>
       <c r="M25" s="10"/>
-      <c r="N25" s="3"/>
+      <c r="N25" s="54" t="s">
+        <v>713</v>
+      </c>
       <c r="O25" s="3"/>
       <c r="P25" s="3"/>
       <c r="Q25" s="3"/>
       <c r="R25" s="3"/>
     </row>
-    <row r="26" spans="1:18" ht="349.5" customHeight="1" x14ac:dyDescent="1.4">
+    <row r="26" spans="1:18" ht="349.5" customHeight="1" x14ac:dyDescent="1.1000000000000001">
       <c r="A26" s="8" t="s">
         <v>107</v>
       </c>
@@ -5518,13 +5911,15 @@
         <v>23</v>
       </c>
       <c r="M26" s="10"/>
-      <c r="N26" s="3"/>
+      <c r="N26" s="53" t="s">
+        <v>23</v>
+      </c>
       <c r="O26" s="3"/>
       <c r="P26" s="3"/>
       <c r="Q26" s="3"/>
       <c r="R26" s="3"/>
     </row>
-    <row r="27" spans="1:18" ht="399.75" customHeight="1" x14ac:dyDescent="1.4">
+    <row r="27" spans="1:18" ht="399.75" customHeight="1" x14ac:dyDescent="1.1000000000000001">
       <c r="A27" s="8" t="s">
         <v>110</v>
       </c>
@@ -5551,13 +5946,15 @@
         <v>23</v>
       </c>
       <c r="M27" s="10"/>
-      <c r="N27" s="3"/>
+      <c r="N27" s="54" t="s">
+        <v>714</v>
+      </c>
       <c r="O27" s="3"/>
       <c r="P27" s="3"/>
       <c r="Q27" s="3"/>
       <c r="R27" s="3"/>
     </row>
-    <row r="28" spans="1:18" ht="300" customHeight="1" x14ac:dyDescent="1.4">
+    <row r="28" spans="1:18" ht="300" customHeight="1" x14ac:dyDescent="1.1000000000000001">
       <c r="A28" s="10" t="s">
         <v>113</v>
       </c>
@@ -5584,13 +5981,15 @@
         <v>23</v>
       </c>
       <c r="M28" s="10"/>
-      <c r="N28" s="3"/>
+      <c r="N28" s="53" t="s">
+        <v>23</v>
+      </c>
       <c r="O28" s="3"/>
       <c r="P28" s="3"/>
       <c r="Q28" s="3"/>
       <c r="R28" s="3"/>
     </row>
-    <row r="29" spans="1:18" ht="94.5" customHeight="1" x14ac:dyDescent="1.4">
+    <row r="29" spans="1:18" ht="94.5" customHeight="1" x14ac:dyDescent="1.1000000000000001">
       <c r="A29" s="10" t="s">
         <v>116</v>
       </c>
@@ -5619,7 +6018,9 @@
         <v>39</v>
       </c>
       <c r="M29" s="10"/>
-      <c r="N29" s="3"/>
+      <c r="N29" s="53" t="s">
+        <v>39</v>
+      </c>
       <c r="O29" s="3"/>
       <c r="P29" s="3" t="s">
         <v>39</v>
@@ -5629,7 +6030,7 @@
       </c>
       <c r="R29" s="3"/>
     </row>
-    <row r="30" spans="1:18" ht="349.5" customHeight="1" x14ac:dyDescent="1.4">
+    <row r="30" spans="1:18" ht="349.5" customHeight="1" x14ac:dyDescent="1.1000000000000001">
       <c r="A30" s="10" t="s">
         <v>119</v>
       </c>
@@ -5656,7 +6057,9 @@
         <v>23</v>
       </c>
       <c r="M30" s="10"/>
-      <c r="N30" s="3"/>
+      <c r="N30" s="54" t="s">
+        <v>715</v>
+      </c>
       <c r="O30" s="3"/>
       <c r="P30" s="3" t="s">
         <v>39</v>
@@ -5666,7 +6069,7 @@
       </c>
       <c r="R30" s="3"/>
     </row>
-    <row r="31" spans="1:18" ht="349.5" customHeight="1" x14ac:dyDescent="1.4">
+    <row r="31" spans="1:18" ht="349.5" customHeight="1" x14ac:dyDescent="1.1000000000000001">
       <c r="A31" s="8" t="s">
         <v>122</v>
       </c>
@@ -5693,7 +6096,9 @@
         <v>23</v>
       </c>
       <c r="M31" s="10"/>
-      <c r="N31" s="3"/>
+      <c r="N31" s="53" t="s">
+        <v>23</v>
+      </c>
       <c r="O31" s="3"/>
       <c r="P31" s="3" t="s">
         <v>39</v>
@@ -5703,7 +6108,7 @@
       </c>
       <c r="R31" s="3"/>
     </row>
-    <row r="32" spans="1:18" ht="92.65" x14ac:dyDescent="1.4">
+    <row r="32" spans="1:18" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A32" s="8" t="s">
         <v>125</v>
       </c>
@@ -5731,7 +6136,7 @@
         <v>39</v>
       </c>
       <c r="M32" s="20"/>
-      <c r="N32" s="3"/>
+      <c r="N32" s="53"/>
       <c r="O32" s="3"/>
       <c r="P32" s="3" t="s">
         <v>39</v>
@@ -5741,7 +6146,7 @@
       </c>
       <c r="R32" s="3"/>
     </row>
-    <row r="33" spans="1:18" ht="92.65" x14ac:dyDescent="1.4">
+    <row r="33" spans="1:18" ht="139.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A33" s="8" t="s">
         <v>128</v>
       </c>
@@ -5769,7 +6174,7 @@
         <v>130</v>
       </c>
       <c r="M33" s="10"/>
-      <c r="N33" s="3"/>
+      <c r="N33" s="53"/>
       <c r="O33" s="3"/>
       <c r="P33" s="3" t="s">
         <v>39</v>
@@ -5779,7 +6184,7 @@
       </c>
       <c r="R33" s="3"/>
     </row>
-    <row r="34" spans="1:18" ht="92.25" customHeight="1" x14ac:dyDescent="1.4">
+    <row r="34" spans="1:18" ht="92.25" customHeight="1" x14ac:dyDescent="1.1000000000000001">
       <c r="A34" s="8" t="s">
         <v>131</v>
       </c>
@@ -5807,7 +6212,7 @@
         <v>39</v>
       </c>
       <c r="M34" s="10"/>
-      <c r="N34" s="3"/>
+      <c r="N34" s="53"/>
       <c r="O34" s="3"/>
       <c r="P34" s="3" t="s">
         <v>39</v>
@@ -5817,7 +6222,7 @@
       </c>
       <c r="R34" s="3"/>
     </row>
-    <row r="35" spans="1:18" ht="99" customHeight="1" x14ac:dyDescent="1.4">
+    <row r="35" spans="1:18" ht="99" customHeight="1" x14ac:dyDescent="1.1000000000000001">
       <c r="A35" s="8" t="s">
         <v>134</v>
       </c>
@@ -5845,7 +6250,7 @@
         <v>39</v>
       </c>
       <c r="M35" s="10"/>
-      <c r="N35" s="3"/>
+      <c r="N35" s="53"/>
       <c r="O35" s="3"/>
       <c r="P35" s="3" t="s">
         <v>39</v>
@@ -5855,7 +6260,7 @@
       </c>
       <c r="R35" s="3"/>
     </row>
-    <row r="36" spans="1:18" ht="93.75" x14ac:dyDescent="1.4">
+    <row r="36" spans="1:18" ht="95" x14ac:dyDescent="1.1000000000000001">
       <c r="A36" s="8" t="s">
         <v>136</v>
       </c>
@@ -5879,7 +6284,7 @@
         <v>138</v>
       </c>
       <c r="M36" s="4"/>
-      <c r="N36" s="3"/>
+      <c r="N36" s="53"/>
       <c r="O36" s="3"/>
       <c r="P36" s="3" t="s">
         <v>39</v>
@@ -5889,7 +6294,7 @@
       </c>
       <c r="R36" s="3"/>
     </row>
-    <row r="37" spans="1:18" ht="93.75" x14ac:dyDescent="1.4">
+    <row r="37" spans="1:18" ht="139.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A37" s="8" t="s">
         <v>139</v>
       </c>
@@ -5913,7 +6318,7 @@
         <v>138</v>
       </c>
       <c r="M37" s="4"/>
-      <c r="N37" s="3"/>
+      <c r="N37" s="53"/>
       <c r="O37" s="3"/>
       <c r="P37" s="3" t="s">
         <v>39</v>
@@ -5923,7 +6328,7 @@
       </c>
       <c r="R37" s="3"/>
     </row>
-    <row r="38" spans="1:18" ht="93.75" x14ac:dyDescent="1.4">
+    <row r="38" spans="1:18" ht="139.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A38" s="8" t="s">
         <v>141</v>
       </c>
@@ -5947,7 +6352,7 @@
         <v>138</v>
       </c>
       <c r="M38" s="4"/>
-      <c r="N38" s="3"/>
+      <c r="N38" s="53"/>
       <c r="O38" s="3"/>
       <c r="P38" s="3" t="s">
         <v>39</v>
@@ -5957,7 +6362,7 @@
       </c>
       <c r="R38" s="3"/>
     </row>
-    <row r="39" spans="1:18" ht="93.75" x14ac:dyDescent="1.4">
+    <row r="39" spans="1:18" ht="139.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A39" s="8" t="s">
         <v>144</v>
       </c>
@@ -5981,7 +6386,7 @@
         <v>138</v>
       </c>
       <c r="M39" s="4"/>
-      <c r="N39" s="3"/>
+      <c r="N39" s="53"/>
       <c r="O39" s="3"/>
       <c r="P39" s="3" t="s">
         <v>39</v>
@@ -5991,7 +6396,7 @@
       </c>
       <c r="R39" s="3"/>
     </row>
-    <row r="40" spans="1:18" ht="93.75" x14ac:dyDescent="1.4">
+    <row r="40" spans="1:18" ht="95" x14ac:dyDescent="1.1000000000000001">
       <c r="A40" s="8" t="s">
         <v>147</v>
       </c>
@@ -6019,7 +6424,7 @@
         <v>138</v>
       </c>
       <c r="M40" s="4"/>
-      <c r="N40" s="3"/>
+      <c r="N40" s="53"/>
       <c r="O40" s="3"/>
       <c r="P40" s="3" t="s">
         <v>39</v>
@@ -6029,7 +6434,7 @@
       </c>
       <c r="R40" s="3"/>
     </row>
-    <row r="41" spans="1:18" ht="93.75" x14ac:dyDescent="1.4">
+    <row r="41" spans="1:18" ht="95" x14ac:dyDescent="1.1000000000000001">
       <c r="A41" s="8" t="s">
         <v>150</v>
       </c>
@@ -6057,7 +6462,7 @@
         <v>138</v>
       </c>
       <c r="M41" s="4"/>
-      <c r="N41" s="3"/>
+      <c r="N41" s="53"/>
       <c r="O41" s="3"/>
       <c r="P41" s="3" t="s">
         <v>39</v>
@@ -6067,7 +6472,7 @@
       </c>
       <c r="R41" s="3"/>
     </row>
-    <row r="42" spans="1:18" ht="138.4" x14ac:dyDescent="1.4">
+    <row r="42" spans="1:18" ht="139.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A42" s="8" t="s">
         <v>153</v>
       </c>
@@ -6095,7 +6500,7 @@
         <v>138</v>
       </c>
       <c r="M42" s="4"/>
-      <c r="N42" s="3"/>
+      <c r="N42" s="53"/>
       <c r="O42" s="3"/>
       <c r="P42" s="3" t="s">
         <v>39</v>
@@ -6105,7 +6510,7 @@
       </c>
       <c r="R42" s="3"/>
     </row>
-    <row r="43" spans="1:18" ht="93.75" x14ac:dyDescent="1.4">
+    <row r="43" spans="1:18" ht="95" x14ac:dyDescent="1.1000000000000001">
       <c r="A43" s="8" t="s">
         <v>156</v>
       </c>
@@ -6129,7 +6534,7 @@
         <v>138</v>
       </c>
       <c r="M43" s="4"/>
-      <c r="N43" s="3"/>
+      <c r="N43" s="53"/>
       <c r="O43" s="3"/>
       <c r="P43" s="3" t="s">
         <v>39</v>
@@ -6139,7 +6544,7 @@
       </c>
       <c r="R43" s="3"/>
     </row>
-    <row r="44" spans="1:18" ht="93.75" x14ac:dyDescent="1.4">
+    <row r="44" spans="1:18" ht="95" x14ac:dyDescent="1.1000000000000001">
       <c r="A44" s="8" t="s">
         <v>159</v>
       </c>
@@ -6163,7 +6568,7 @@
         <v>138</v>
       </c>
       <c r="M44" s="4"/>
-      <c r="N44" s="3"/>
+      <c r="N44" s="53"/>
       <c r="O44" s="3"/>
       <c r="P44" s="3" t="s">
         <v>39</v>
@@ -6173,7 +6578,7 @@
       </c>
       <c r="R44" s="3"/>
     </row>
-    <row r="45" spans="1:18" ht="93.75" x14ac:dyDescent="1.4">
+    <row r="45" spans="1:18" ht="95" x14ac:dyDescent="1.1000000000000001">
       <c r="A45" s="8" t="s">
         <v>161</v>
       </c>
@@ -6197,7 +6602,7 @@
         <v>138</v>
       </c>
       <c r="M45" s="4"/>
-      <c r="N45" s="3"/>
+      <c r="N45" s="53"/>
       <c r="O45" s="3"/>
       <c r="P45" s="3" t="s">
         <v>39</v>
@@ -6207,7 +6612,7 @@
       </c>
       <c r="R45" s="3"/>
     </row>
-    <row r="46" spans="1:18" ht="93.75" x14ac:dyDescent="1.4">
+    <row r="46" spans="1:18" ht="95" x14ac:dyDescent="1.1000000000000001">
       <c r="A46" s="8" t="s">
         <v>164</v>
       </c>
@@ -6231,7 +6636,7 @@
         <v>138</v>
       </c>
       <c r="M46" s="4"/>
-      <c r="N46" s="3"/>
+      <c r="N46" s="53"/>
       <c r="O46" s="3"/>
       <c r="P46" s="3" t="s">
         <v>39</v>
@@ -6241,7 +6646,7 @@
       </c>
       <c r="R46" s="3"/>
     </row>
-    <row r="47" spans="1:18" ht="138.4" x14ac:dyDescent="1.4">
+    <row r="47" spans="1:18" ht="139.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A47" s="8" t="s">
         <v>166</v>
       </c>
@@ -6265,7 +6670,7 @@
         <v>138</v>
       </c>
       <c r="M47" s="4"/>
-      <c r="N47" s="3"/>
+      <c r="N47" s="53"/>
       <c r="O47" s="3"/>
       <c r="P47" s="3" t="s">
         <v>39</v>
@@ -6275,7 +6680,7 @@
       </c>
       <c r="R47" s="3"/>
     </row>
-    <row r="48" spans="1:18" ht="93.75" x14ac:dyDescent="1.4">
+    <row r="48" spans="1:18" ht="95" x14ac:dyDescent="1.1000000000000001">
       <c r="A48" s="8" t="s">
         <v>168</v>
       </c>
@@ -6299,7 +6704,7 @@
         <v>138</v>
       </c>
       <c r="M48" s="4"/>
-      <c r="N48" s="3"/>
+      <c r="N48" s="53"/>
       <c r="O48" s="3"/>
       <c r="P48" s="3" t="s">
         <v>39</v>
@@ -6309,7 +6714,7 @@
       </c>
       <c r="R48" s="3"/>
     </row>
-    <row r="49" spans="1:18" ht="92.65" x14ac:dyDescent="1.4">
+    <row r="49" spans="1:18" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A49" s="8" t="s">
         <v>170</v>
       </c>
@@ -6337,7 +6742,7 @@
         <v>39</v>
       </c>
       <c r="M49" s="10"/>
-      <c r="N49" s="3"/>
+      <c r="N49" s="53"/>
       <c r="O49" s="3"/>
       <c r="P49" s="3" t="s">
         <v>39</v>
@@ -6347,7 +6752,7 @@
       </c>
       <c r="R49" s="3"/>
     </row>
-    <row r="50" spans="1:18" ht="184.15" x14ac:dyDescent="1.4">
+    <row r="50" spans="1:18" ht="185.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A50" s="8" t="s">
         <v>172</v>
       </c>
@@ -6375,7 +6780,7 @@
         <v>39</v>
       </c>
       <c r="M50" s="10"/>
-      <c r="N50" s="3"/>
+      <c r="N50" s="53"/>
       <c r="O50" s="3"/>
       <c r="P50" s="3" t="s">
         <v>39</v>
@@ -6385,7 +6790,7 @@
       </c>
       <c r="R50" s="3"/>
     </row>
-    <row r="51" spans="1:18" ht="234.75" customHeight="1" x14ac:dyDescent="1.4">
+    <row r="51" spans="1:18" ht="234.75" customHeight="1" x14ac:dyDescent="1.1000000000000001">
       <c r="A51" s="8" t="s">
         <v>174</v>
       </c>
@@ -6411,13 +6816,13 @@
         <v>#VALUE!</v>
       </c>
       <c r="M51" s="3"/>
-      <c r="N51" s="3"/>
+      <c r="N51" s="53"/>
       <c r="O51" s="3"/>
       <c r="P51" s="3"/>
       <c r="Q51" s="3"/>
       <c r="R51" s="3"/>
     </row>
-    <row r="52" spans="1:18" ht="92.65" x14ac:dyDescent="1.4">
+    <row r="52" spans="1:18" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A52" s="8" t="s">
         <v>178</v>
       </c>
@@ -6443,7 +6848,7 @@
         <v>39</v>
       </c>
       <c r="M52" s="3"/>
-      <c r="N52" s="3"/>
+      <c r="N52" s="53"/>
       <c r="O52" s="3"/>
       <c r="P52" s="3"/>
       <c r="Q52" s="3" t="s">
@@ -6451,7 +6856,7 @@
       </c>
       <c r="R52" s="3"/>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="1.4">
+    <row r="53" spans="1:18" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A53" s="23" t="s">
         <v>180</v>
       </c>
@@ -6475,13 +6880,13 @@
         <v>23</v>
       </c>
       <c r="M53" s="3"/>
-      <c r="N53" s="3"/>
+      <c r="N53" s="53"/>
       <c r="O53" s="3"/>
       <c r="P53" s="3"/>
       <c r="Q53" s="3"/>
       <c r="R53" s="3"/>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="1.4">
+    <row r="54" spans="1:18" x14ac:dyDescent="1.1000000000000001">
       <c r="A54" s="23" t="s">
         <v>183</v>
       </c>
@@ -6505,13 +6910,13 @@
         <v>185</v>
       </c>
       <c r="M54" s="3"/>
-      <c r="N54" s="3"/>
+      <c r="N54" s="53"/>
       <c r="O54" s="3"/>
       <c r="P54" s="3"/>
       <c r="Q54" s="3"/>
       <c r="R54" s="3"/>
     </row>
-    <row r="55" spans="1:18" ht="275.64999999999998" x14ac:dyDescent="1.4">
+    <row r="55" spans="1:18" ht="277.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A55" s="8" t="s">
         <v>186</v>
       </c>
@@ -6538,13 +6943,13 @@
         <v>#VALUE!</v>
       </c>
       <c r="M55" s="3"/>
-      <c r="N55" s="3"/>
+      <c r="N55" s="53"/>
       <c r="O55" s="3"/>
       <c r="P55" s="3"/>
       <c r="Q55" s="3"/>
       <c r="R55" s="3"/>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="1.4">
+    <row r="56" spans="1:18" x14ac:dyDescent="1.1000000000000001">
       <c r="A56" s="23" t="s">
         <v>190</v>
       </c>
@@ -6570,7 +6975,7 @@
         <v>192</v>
       </c>
       <c r="M56" s="3"/>
-      <c r="N56" s="3"/>
+      <c r="N56" s="53"/>
       <c r="O56" s="3"/>
       <c r="P56" s="3"/>
       <c r="Q56" s="3" t="s">
@@ -6578,7 +6983,7 @@
       </c>
       <c r="R56" s="3"/>
     </row>
-    <row r="57" spans="1:18" ht="275.64999999999998" x14ac:dyDescent="1.4">
+    <row r="57" spans="1:18" ht="277.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A57" s="8" t="s">
         <v>193</v>
       </c>
@@ -6605,13 +7010,13 @@
         <v>#VALUE!</v>
       </c>
       <c r="M57" s="3"/>
-      <c r="N57" s="3"/>
+      <c r="N57" s="53"/>
       <c r="O57" s="3"/>
       <c r="P57" s="3"/>
       <c r="Q57" s="3"/>
       <c r="R57" s="3"/>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="1.4">
+    <row r="58" spans="1:18" x14ac:dyDescent="1.1000000000000001">
       <c r="A58" s="8" t="s">
         <v>197</v>
       </c>
@@ -6637,7 +7042,7 @@
         <v>130</v>
       </c>
       <c r="M58" s="3"/>
-      <c r="N58" s="3"/>
+      <c r="N58" s="53"/>
       <c r="O58" s="3"/>
       <c r="P58" s="3"/>
       <c r="Q58" s="3" t="s">
@@ -6645,7 +7050,7 @@
       </c>
       <c r="R58" s="3"/>
     </row>
-    <row r="59" spans="1:18" ht="275.64999999999998" x14ac:dyDescent="1.4">
+    <row r="59" spans="1:18" ht="277.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A59" s="8" t="s">
         <v>200</v>
       </c>
@@ -6672,13 +7077,13 @@
         <v>#VALUE!</v>
       </c>
       <c r="M59" s="3"/>
-      <c r="N59" s="3"/>
+      <c r="N59" s="53"/>
       <c r="O59" s="3"/>
       <c r="P59" s="3"/>
       <c r="Q59" s="3"/>
       <c r="R59" s="3"/>
     </row>
-    <row r="60" spans="1:18" ht="408.75" customHeight="1" x14ac:dyDescent="1.4">
+    <row r="60" spans="1:18" ht="408.75" customHeight="1" x14ac:dyDescent="1.1000000000000001">
       <c r="A60" s="8" t="s">
         <v>203</v>
       </c>
@@ -6704,13 +7109,13 @@
         <v>207</v>
       </c>
       <c r="M60" s="3"/>
-      <c r="N60" s="3"/>
+      <c r="N60" s="53"/>
       <c r="O60" s="3"/>
       <c r="P60" s="3"/>
       <c r="Q60" s="3"/>
       <c r="R60" s="3"/>
     </row>
-    <row r="61" spans="1:18" ht="92.65" x14ac:dyDescent="1.4">
+    <row r="61" spans="1:18" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A61" s="23" t="s">
         <v>208</v>
       </c>
@@ -6736,7 +7141,7 @@
         <v>192</v>
       </c>
       <c r="M61" s="3"/>
-      <c r="N61" s="3"/>
+      <c r="N61" s="53"/>
       <c r="O61" s="3"/>
       <c r="P61" s="3"/>
       <c r="Q61" s="3" t="s">
@@ -6744,7 +7149,7 @@
       </c>
       <c r="R61" s="3"/>
     </row>
-    <row r="62" spans="1:18" ht="408.75" customHeight="1" x14ac:dyDescent="1.4">
+    <row r="62" spans="1:18" ht="408.75" customHeight="1" x14ac:dyDescent="1.1000000000000001">
       <c r="A62" s="8" t="s">
         <v>210</v>
       </c>
@@ -6770,13 +7175,13 @@
         <v>207</v>
       </c>
       <c r="M62" s="3"/>
-      <c r="N62" s="3"/>
+      <c r="N62" s="53"/>
       <c r="O62" s="3"/>
       <c r="P62" s="3"/>
       <c r="Q62" s="3"/>
       <c r="R62" s="3"/>
     </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="1.4">
+    <row r="63" spans="1:18" x14ac:dyDescent="1.1000000000000001">
       <c r="A63" s="23" t="s">
         <v>214</v>
       </c>
@@ -6800,13 +7205,13 @@
         <v>207</v>
       </c>
       <c r="M63" s="3"/>
-      <c r="N63" s="3"/>
+      <c r="N63" s="53"/>
       <c r="O63" s="3"/>
       <c r="P63" s="3"/>
       <c r="Q63" s="3"/>
       <c r="R63" s="3"/>
     </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="1.4">
+    <row r="64" spans="1:18" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A64" s="23" t="s">
         <v>216</v>
       </c>
@@ -6830,13 +7235,13 @@
         <v>207</v>
       </c>
       <c r="M64" s="3"/>
-      <c r="N64" s="3"/>
+      <c r="N64" s="53"/>
       <c r="O64" s="3"/>
       <c r="P64" s="3"/>
       <c r="Q64" s="3"/>
       <c r="R64" s="3"/>
     </row>
-    <row r="65" spans="1:18" ht="92.65" x14ac:dyDescent="1.4">
+    <row r="65" spans="1:18" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A65" s="8" t="s">
         <v>219</v>
       </c>
@@ -6862,7 +7267,7 @@
         <v>130</v>
       </c>
       <c r="M65" s="3"/>
-      <c r="N65" s="3"/>
+      <c r="N65" s="53"/>
       <c r="O65" s="3"/>
       <c r="P65" s="3"/>
       <c r="Q65" s="3" t="s">
@@ -6870,7 +7275,7 @@
       </c>
       <c r="R65" s="3"/>
     </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="1.4">
+    <row r="66" spans="1:18" x14ac:dyDescent="1.1000000000000001">
       <c r="A66" s="8" t="s">
         <v>222</v>
       </c>
@@ -6896,7 +7301,7 @@
         <v>39</v>
       </c>
       <c r="M66" s="3"/>
-      <c r="N66" s="3"/>
+      <c r="N66" s="53"/>
       <c r="O66" s="3"/>
       <c r="P66" s="3"/>
       <c r="Q66" s="3" t="s">
@@ -6904,7 +7309,7 @@
       </c>
       <c r="R66" s="3"/>
     </row>
-    <row r="67" spans="1:18" ht="91.5" x14ac:dyDescent="1.4">
+    <row r="67" spans="1:18" ht="92" x14ac:dyDescent="1.1000000000000001">
       <c r="A67" s="8" t="s">
         <v>225</v>
       </c>
@@ -6931,13 +7336,13 @@
         <f>#VALUE!</f>
         <v>#VALUE!</v>
       </c>
-      <c r="N67" s="3"/>
+      <c r="N67" s="53"/>
       <c r="O67" s="3"/>
       <c r="P67" s="3"/>
       <c r="Q67" s="3"/>
       <c r="R67" s="3"/>
     </row>
-    <row r="68" spans="1:18" ht="91.5" x14ac:dyDescent="1.4">
+    <row r="68" spans="1:18" ht="92" x14ac:dyDescent="1.1000000000000001">
       <c r="A68" s="8" t="s">
         <v>227</v>
       </c>
@@ -6964,13 +7369,13 @@
         <f>#VALUE!</f>
         <v>#VALUE!</v>
       </c>
-      <c r="N68" s="3"/>
+      <c r="N68" s="53"/>
       <c r="O68" s="3"/>
       <c r="P68" s="3"/>
       <c r="Q68" s="3"/>
       <c r="R68" s="3"/>
     </row>
-    <row r="69" spans="1:18" ht="92.65" x14ac:dyDescent="1.4">
+    <row r="69" spans="1:18" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A69" s="8" t="s">
         <v>230</v>
       </c>
@@ -6997,13 +7402,13 @@
         <f>#VALUE!</f>
         <v>#VALUE!</v>
       </c>
-      <c r="N69" s="3"/>
+      <c r="N69" s="53"/>
       <c r="O69" s="3"/>
       <c r="P69" s="3"/>
       <c r="Q69" s="3"/>
       <c r="R69" s="3"/>
     </row>
-    <row r="70" spans="1:18" ht="92.65" x14ac:dyDescent="1.4">
+    <row r="70" spans="1:18" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A70" s="8" t="s">
         <v>233</v>
       </c>
@@ -7029,13 +7434,13 @@
       <c r="M70" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="N70" s="3"/>
+      <c r="N70" s="53"/>
       <c r="O70" s="3"/>
       <c r="P70" s="3"/>
       <c r="Q70" s="3"/>
       <c r="R70" s="3"/>
     </row>
-    <row r="71" spans="1:18" ht="92.65" x14ac:dyDescent="1.4">
+    <row r="71" spans="1:18" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A71" s="8" t="s">
         <v>237</v>
       </c>
@@ -7061,13 +7466,13 @@
       <c r="M71" s="3" t="s">
         <v>240</v>
       </c>
-      <c r="N71" s="3"/>
+      <c r="N71" s="53"/>
       <c r="O71" s="3"/>
       <c r="P71" s="3"/>
       <c r="Q71" s="3"/>
       <c r="R71" s="3"/>
     </row>
-    <row r="72" spans="1:18" ht="92.65" x14ac:dyDescent="1.4">
+    <row r="72" spans="1:18" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A72" s="8" t="s">
         <v>241</v>
       </c>
@@ -7093,13 +7498,13 @@
       <c r="M72" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="N72" s="3"/>
+      <c r="N72" s="53"/>
       <c r="O72" s="3"/>
       <c r="P72" s="3"/>
       <c r="Q72" s="3"/>
       <c r="R72" s="3"/>
     </row>
-    <row r="73" spans="1:18" ht="92.65" x14ac:dyDescent="1.4">
+    <row r="73" spans="1:18" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A73" s="8" t="s">
         <v>244</v>
       </c>
@@ -7124,13 +7529,13 @@
         <f>#VALUE!</f>
         <v>#VALUE!</v>
       </c>
-      <c r="N73" s="3"/>
+      <c r="N73" s="53"/>
       <c r="O73" s="3"/>
       <c r="P73" s="3"/>
       <c r="Q73" s="3"/>
       <c r="R73" s="3"/>
     </row>
-    <row r="74" spans="1:18" ht="138.4" x14ac:dyDescent="1.4">
+    <row r="74" spans="1:18" ht="139.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A74" s="8" t="s">
         <v>246</v>
       </c>
@@ -7152,13 +7557,13 @@
         <v>207</v>
       </c>
       <c r="M74" s="3"/>
-      <c r="N74" s="3"/>
+      <c r="N74" s="53"/>
       <c r="O74" s="3"/>
       <c r="P74" s="3"/>
       <c r="Q74" s="3"/>
       <c r="R74" s="3"/>
     </row>
-    <row r="75" spans="1:18" ht="92.65" x14ac:dyDescent="1.4">
+    <row r="75" spans="1:18" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A75" s="8" t="s">
         <v>248</v>
       </c>
@@ -7182,13 +7587,13 @@
       <c r="M75" s="3" t="s">
         <v>250</v>
       </c>
-      <c r="N75" s="3"/>
+      <c r="N75" s="53"/>
       <c r="O75" s="3"/>
       <c r="P75" s="3"/>
       <c r="Q75" s="3"/>
       <c r="R75" s="3"/>
     </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="1.4">
+    <row r="76" spans="1:18" x14ac:dyDescent="1.1000000000000001">
       <c r="A76" s="8" t="s">
         <v>251</v>
       </c>
@@ -7214,13 +7619,13 @@
       <c r="M76" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="N76" s="3"/>
+      <c r="N76" s="53"/>
       <c r="O76" s="3"/>
       <c r="P76" s="3"/>
       <c r="Q76" s="3"/>
       <c r="R76" s="3"/>
     </row>
-    <row r="77" spans="1:18" ht="92.65" x14ac:dyDescent="1.4">
+    <row r="77" spans="1:18" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A77" s="8" t="s">
         <v>255</v>
       </c>
@@ -7246,13 +7651,13 @@
       <c r="M77" s="3" t="s">
         <v>250</v>
       </c>
-      <c r="N77" s="3"/>
+      <c r="N77" s="53"/>
       <c r="O77" s="3"/>
       <c r="P77" s="3"/>
       <c r="Q77" s="3"/>
       <c r="R77" s="3"/>
     </row>
-    <row r="78" spans="1:18" ht="92.65" x14ac:dyDescent="1.4">
+    <row r="78" spans="1:18" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A78" s="8" t="s">
         <v>258</v>
       </c>
@@ -7276,13 +7681,13 @@
       <c r="M78" s="3" t="s">
         <v>250</v>
       </c>
-      <c r="N78" s="3"/>
+      <c r="N78" s="53"/>
       <c r="O78" s="3"/>
       <c r="P78" s="3"/>
       <c r="Q78" s="3"/>
       <c r="R78" s="3"/>
     </row>
-    <row r="79" spans="1:18" ht="92.65" x14ac:dyDescent="1.4">
+    <row r="79" spans="1:18" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A79" s="8" t="s">
         <v>260</v>
       </c>
@@ -7308,13 +7713,13 @@
       <c r="M79" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="N79" s="3"/>
+      <c r="N79" s="53"/>
       <c r="O79" s="3"/>
       <c r="P79" s="3"/>
       <c r="Q79" s="3"/>
       <c r="R79" s="3"/>
     </row>
-    <row r="80" spans="1:18" ht="92.65" x14ac:dyDescent="1.4">
+    <row r="80" spans="1:18" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A80" s="8" t="s">
         <v>263</v>
       </c>
@@ -7340,13 +7745,13 @@
       <c r="M80" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="N80" s="3"/>
+      <c r="N80" s="53"/>
       <c r="O80" s="3"/>
       <c r="P80" s="3"/>
       <c r="Q80" s="3"/>
       <c r="R80" s="3"/>
     </row>
-    <row r="81" spans="1:18" ht="92.65" x14ac:dyDescent="1.4">
+    <row r="81" spans="1:18" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A81" s="8" t="s">
         <v>266</v>
       </c>
@@ -7372,13 +7777,13 @@
       <c r="M81" s="3" t="s">
         <v>269</v>
       </c>
-      <c r="N81" s="3"/>
+      <c r="N81" s="53"/>
       <c r="O81" s="3"/>
       <c r="P81" s="3"/>
       <c r="Q81" s="3"/>
       <c r="R81" s="3"/>
     </row>
-    <row r="82" spans="1:18" x14ac:dyDescent="1.4">
+    <row r="82" spans="1:18" x14ac:dyDescent="1.1000000000000001">
       <c r="A82" s="8" t="s">
         <v>270</v>
       </c>
@@ -7404,13 +7809,13 @@
       <c r="M82" s="3" t="s">
         <v>250</v>
       </c>
-      <c r="N82" s="3"/>
+      <c r="N82" s="53"/>
       <c r="O82" s="3"/>
       <c r="P82" s="3"/>
       <c r="Q82" s="3"/>
       <c r="R82" s="3"/>
     </row>
-    <row r="83" spans="1:18" ht="92.65" x14ac:dyDescent="1.4">
+    <row r="83" spans="1:18" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A83" s="8" t="s">
         <v>273</v>
       </c>
@@ -7436,13 +7841,13 @@
       <c r="M83" s="3" t="s">
         <v>250</v>
       </c>
-      <c r="N83" s="3"/>
+      <c r="N83" s="53"/>
       <c r="O83" s="3"/>
       <c r="P83" s="3"/>
       <c r="Q83" s="3"/>
       <c r="R83" s="3"/>
     </row>
-    <row r="84" spans="1:18" ht="92.65" x14ac:dyDescent="1.4">
+    <row r="84" spans="1:18" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A84" s="8" t="s">
         <v>275</v>
       </c>
@@ -7468,13 +7873,13 @@
       <c r="M84" s="3" t="s">
         <v>250</v>
       </c>
-      <c r="N84" s="3"/>
+      <c r="N84" s="53"/>
       <c r="O84" s="3"/>
       <c r="P84" s="3"/>
       <c r="Q84" s="3"/>
       <c r="R84" s="3"/>
     </row>
-    <row r="85" spans="1:18" x14ac:dyDescent="1.4">
+    <row r="85" spans="1:18" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A85" s="8" t="s">
         <v>277</v>
       </c>
@@ -7500,13 +7905,13 @@
       <c r="M85" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="N85" s="3"/>
+      <c r="N85" s="53"/>
       <c r="O85" s="3"/>
       <c r="P85" s="3"/>
       <c r="Q85" s="3"/>
       <c r="R85" s="3"/>
     </row>
-    <row r="86" spans="1:18" x14ac:dyDescent="1.4">
+    <row r="86" spans="1:18" x14ac:dyDescent="1.1000000000000001">
       <c r="A86" s="8" t="s">
         <v>281</v>
       </c>
@@ -7530,13 +7935,13 @@
         <v>207</v>
       </c>
       <c r="M86" s="3"/>
-      <c r="N86" s="3"/>
+      <c r="N86" s="53"/>
       <c r="O86" s="3"/>
       <c r="P86" s="3"/>
       <c r="Q86" s="3"/>
       <c r="R86" s="3"/>
     </row>
-    <row r="87" spans="1:18" x14ac:dyDescent="1.4">
+    <row r="87" spans="1:18" x14ac:dyDescent="1.1000000000000001">
       <c r="A87" s="8" t="s">
         <v>283</v>
       </c>
@@ -7560,13 +7965,13 @@
         <v>207</v>
       </c>
       <c r="M87" s="3"/>
-      <c r="N87" s="3"/>
+      <c r="N87" s="53"/>
       <c r="O87" s="3"/>
       <c r="P87" s="3"/>
       <c r="Q87" s="3"/>
       <c r="R87" s="3"/>
     </row>
-    <row r="88" spans="1:18" x14ac:dyDescent="1.4">
+    <row r="88" spans="1:18" x14ac:dyDescent="1.1000000000000001">
       <c r="A88" s="8" t="s">
         <v>286</v>
       </c>
@@ -7590,13 +7995,13 @@
         <v>207</v>
       </c>
       <c r="M88" s="3"/>
-      <c r="N88" s="3"/>
+      <c r="N88" s="53"/>
       <c r="O88" s="3"/>
       <c r="P88" s="3"/>
       <c r="Q88" s="3"/>
       <c r="R88" s="3"/>
     </row>
-    <row r="89" spans="1:18" x14ac:dyDescent="1.4">
+    <row r="89" spans="1:18" x14ac:dyDescent="1.1000000000000001">
       <c r="A89" s="8" t="s">
         <v>289</v>
       </c>
@@ -7622,13 +8027,13 @@
       <c r="M89" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="N89" s="3"/>
+      <c r="N89" s="53"/>
       <c r="O89" s="3"/>
       <c r="P89" s="3"/>
       <c r="Q89" s="3"/>
       <c r="R89" s="3"/>
     </row>
-    <row r="90" spans="1:18" x14ac:dyDescent="1.4">
+    <row r="90" spans="1:18" x14ac:dyDescent="1.1000000000000001">
       <c r="A90" s="8" t="s">
         <v>291</v>
       </c>
@@ -7654,13 +8059,13 @@
       <c r="M90" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="N90" s="3"/>
+      <c r="N90" s="53"/>
       <c r="O90" s="3"/>
       <c r="P90" s="3"/>
       <c r="Q90" s="3"/>
       <c r="R90" s="3"/>
     </row>
-    <row r="91" spans="1:18" ht="92.65" x14ac:dyDescent="1.4">
+    <row r="91" spans="1:18" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A91" s="8" t="s">
         <v>293</v>
       </c>
@@ -7686,13 +8091,13 @@
       <c r="M91" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="N91" s="3"/>
+      <c r="N91" s="53"/>
       <c r="O91" s="3"/>
       <c r="P91" s="3"/>
       <c r="Q91" s="3"/>
       <c r="R91" s="3"/>
     </row>
-    <row r="92" spans="1:18" ht="92.65" x14ac:dyDescent="1.4">
+    <row r="92" spans="1:18" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A92" s="8" t="s">
         <v>295</v>
       </c>
@@ -7718,13 +8123,13 @@
       <c r="M92" s="3" t="s">
         <v>297</v>
       </c>
-      <c r="N92" s="3"/>
+      <c r="N92" s="53"/>
       <c r="O92" s="3"/>
       <c r="P92" s="3"/>
       <c r="Q92" s="3"/>
       <c r="R92" s="3"/>
     </row>
-    <row r="93" spans="1:18" ht="229.9" x14ac:dyDescent="1.4">
+    <row r="93" spans="1:18" ht="231.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A93" s="8" t="s">
         <v>298</v>
       </c>
@@ -7746,13 +8151,13 @@
         <v>207</v>
       </c>
       <c r="M93" s="3"/>
-      <c r="N93" s="3"/>
+      <c r="N93" s="53"/>
       <c r="O93" s="3"/>
       <c r="P93" s="3"/>
       <c r="Q93" s="3"/>
       <c r="R93" s="3"/>
     </row>
-    <row r="94" spans="1:18" ht="92.65" x14ac:dyDescent="1.4">
+    <row r="94" spans="1:18" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A94" s="8" t="s">
         <v>300</v>
       </c>
@@ -7774,13 +8179,13 @@
         <v>207</v>
       </c>
       <c r="M94" s="3"/>
-      <c r="N94" s="3"/>
+      <c r="N94" s="53"/>
       <c r="O94" s="3"/>
       <c r="P94" s="3"/>
       <c r="Q94" s="3"/>
       <c r="R94" s="3"/>
     </row>
-    <row r="95" spans="1:18" ht="138.4" x14ac:dyDescent="1.4">
+    <row r="95" spans="1:18" ht="185.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A95" s="8" t="s">
         <v>302</v>
       </c>
@@ -7808,7 +8213,7 @@
         <v>39</v>
       </c>
       <c r="M95" s="3"/>
-      <c r="N95" s="3"/>
+      <c r="N95" s="53"/>
       <c r="O95" s="3"/>
       <c r="P95" s="3" t="s">
         <v>39</v>
@@ -7816,7 +8221,7 @@
       <c r="Q95" s="3"/>
       <c r="R95" s="3"/>
     </row>
-    <row r="96" spans="1:18" ht="92.65" x14ac:dyDescent="1.4">
+    <row r="96" spans="1:18" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A96" s="8" t="s">
         <v>305</v>
       </c>
@@ -7844,7 +8249,7 @@
         <v>39</v>
       </c>
       <c r="M96" s="3"/>
-      <c r="N96" s="3"/>
+      <c r="N96" s="53"/>
       <c r="O96" s="3"/>
       <c r="P96" s="3" t="s">
         <v>39</v>
@@ -7852,7 +8257,7 @@
       <c r="Q96" s="3"/>
       <c r="R96" s="3"/>
     </row>
-    <row r="97" spans="1:18" ht="138.4" x14ac:dyDescent="1.4">
+    <row r="97" spans="1:18" ht="139.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A97" s="8" t="s">
         <v>307</v>
       </c>
@@ -7874,13 +8279,13 @@
       <c r="K97" s="3"/>
       <c r="L97" s="10"/>
       <c r="M97" s="3"/>
-      <c r="N97" s="3"/>
+      <c r="N97" s="53"/>
       <c r="O97" s="3"/>
       <c r="P97" s="3"/>
       <c r="Q97" s="3"/>
       <c r="R97" s="3"/>
     </row>
-    <row r="98" spans="1:18" ht="92.65" x14ac:dyDescent="1.4">
+    <row r="98" spans="1:18" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A98" s="8" t="s">
         <v>309</v>
       </c>
@@ -7906,13 +8311,13 @@
         <v>39</v>
       </c>
       <c r="M98" s="3"/>
-      <c r="N98" s="3"/>
+      <c r="N98" s="53"/>
       <c r="O98" s="3"/>
       <c r="P98" s="3"/>
       <c r="Q98" s="3"/>
       <c r="R98" s="3"/>
     </row>
-    <row r="99" spans="1:18" ht="138.4" x14ac:dyDescent="1.4">
+    <row r="99" spans="1:18" ht="139.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A99" s="8" t="s">
         <v>311</v>
       </c>
@@ -7938,13 +8343,13 @@
         <v>207</v>
       </c>
       <c r="M99" s="3"/>
-      <c r="N99" s="3"/>
+      <c r="N99" s="53"/>
       <c r="O99" s="3"/>
       <c r="P99" s="3"/>
       <c r="Q99" s="3"/>
       <c r="R99" s="3"/>
     </row>
-    <row r="100" spans="1:18" ht="229.9" x14ac:dyDescent="1.4">
+    <row r="100" spans="1:18" ht="231.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A100" s="8" t="s">
         <v>314</v>
       </c>
@@ -7968,13 +8373,13 @@
         <v>207</v>
       </c>
       <c r="M100" s="3"/>
-      <c r="N100" s="3"/>
+      <c r="N100" s="53"/>
       <c r="O100" s="3"/>
       <c r="P100" s="3"/>
       <c r="Q100" s="3"/>
       <c r="R100" s="3"/>
     </row>
-    <row r="101" spans="1:18" ht="92.65" x14ac:dyDescent="1.4">
+    <row r="101" spans="1:18" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A101" s="8" t="s">
         <v>317</v>
       </c>
@@ -8001,13 +8406,13 @@
         <f>#VALUE!</f>
         <v>#VALUE!</v>
       </c>
-      <c r="N101" s="3"/>
+      <c r="N101" s="53"/>
       <c r="O101" s="3"/>
       <c r="P101" s="3"/>
       <c r="Q101" s="3"/>
       <c r="R101" s="3"/>
     </row>
-    <row r="102" spans="1:18" ht="92.65" x14ac:dyDescent="1.4">
+    <row r="102" spans="1:18" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A102" s="8" t="s">
         <v>320</v>
       </c>
@@ -8034,13 +8439,13 @@
         <f>#VALUE!</f>
         <v>#VALUE!</v>
       </c>
-      <c r="N102" s="3"/>
+      <c r="N102" s="53"/>
       <c r="O102" s="3"/>
       <c r="P102" s="3"/>
       <c r="Q102" s="3"/>
       <c r="R102" s="3"/>
     </row>
-    <row r="103" spans="1:18" ht="138.4" x14ac:dyDescent="1.4">
+    <row r="103" spans="1:18" ht="139.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A103" s="8" t="s">
         <v>322</v>
       </c>
@@ -8064,13 +8469,13 @@
       <c r="M103" s="3" t="s">
         <v>324</v>
       </c>
-      <c r="N103" s="3"/>
+      <c r="N103" s="53"/>
       <c r="O103" s="3"/>
       <c r="P103" s="3"/>
       <c r="Q103" s="3"/>
       <c r="R103" s="3"/>
     </row>
-    <row r="104" spans="1:18" ht="92.65" x14ac:dyDescent="1.4">
+    <row r="104" spans="1:18" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A104" s="8" t="s">
         <v>325</v>
       </c>
@@ -8097,13 +8502,13 @@
         <f>#VALUE!</f>
         <v>#VALUE!</v>
       </c>
-      <c r="N104" s="3"/>
+      <c r="N104" s="53"/>
       <c r="O104" s="3"/>
       <c r="P104" s="3"/>
       <c r="Q104" s="3"/>
       <c r="R104" s="3"/>
     </row>
-    <row r="105" spans="1:18" ht="138.4" x14ac:dyDescent="1.4">
+    <row r="105" spans="1:18" ht="139.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A105" s="8" t="s">
         <v>328</v>
       </c>
@@ -8127,13 +8532,13 @@
         <v>207</v>
       </c>
       <c r="M105" s="3"/>
-      <c r="N105" s="3"/>
+      <c r="N105" s="53"/>
       <c r="O105" s="3"/>
       <c r="P105" s="3"/>
       <c r="Q105" s="3"/>
       <c r="R105" s="3"/>
     </row>
-    <row r="106" spans="1:18" ht="92.65" x14ac:dyDescent="1.4">
+    <row r="106" spans="1:18" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A106" s="8" t="s">
         <v>330</v>
       </c>
@@ -8160,13 +8565,13 @@
         <f>#VALUE!</f>
         <v>#VALUE!</v>
       </c>
-      <c r="N106" s="3"/>
+      <c r="N106" s="53"/>
       <c r="O106" s="3"/>
       <c r="P106" s="3"/>
       <c r="Q106" s="3"/>
       <c r="R106" s="3"/>
     </row>
-    <row r="107" spans="1:18" ht="92.65" x14ac:dyDescent="1.4">
+    <row r="107" spans="1:18" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A107" s="8" t="s">
         <v>332</v>
       </c>
@@ -8190,13 +8595,13 @@
         <v>207</v>
       </c>
       <c r="M107" s="3"/>
-      <c r="N107" s="3"/>
+      <c r="N107" s="53"/>
       <c r="O107" s="3"/>
       <c r="P107" s="3"/>
       <c r="Q107" s="3"/>
       <c r="R107" s="3"/>
     </row>
-    <row r="108" spans="1:18" ht="92.65" x14ac:dyDescent="1.4">
+    <row r="108" spans="1:18" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A108" s="8" t="s">
         <v>334</v>
       </c>
@@ -8220,13 +8625,13 @@
         <v>207</v>
       </c>
       <c r="M108" s="3"/>
-      <c r="N108" s="3"/>
+      <c r="N108" s="53"/>
       <c r="O108" s="3"/>
       <c r="P108" s="3"/>
       <c r="Q108" s="3"/>
       <c r="R108" s="3"/>
     </row>
-    <row r="109" spans="1:18" ht="92.65" x14ac:dyDescent="1.4">
+    <row r="109" spans="1:18" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A109" s="8" t="s">
         <v>336</v>
       </c>
@@ -8253,13 +8658,13 @@
         <f>#VALUE!</f>
         <v>#VALUE!</v>
       </c>
-      <c r="N109" s="3"/>
+      <c r="N109" s="53"/>
       <c r="O109" s="3"/>
       <c r="P109" s="3"/>
       <c r="Q109" s="3"/>
       <c r="R109" s="3"/>
     </row>
-    <row r="110" spans="1:18" x14ac:dyDescent="1.4">
+    <row r="110" spans="1:18" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A110" s="8" t="s">
         <v>338</v>
       </c>
@@ -8283,13 +8688,13 @@
         <v>207</v>
       </c>
       <c r="M110" s="3"/>
-      <c r="N110" s="3"/>
+      <c r="N110" s="53"/>
       <c r="O110" s="3"/>
       <c r="P110" s="3"/>
       <c r="Q110" s="3"/>
       <c r="R110" s="3"/>
     </row>
-    <row r="111" spans="1:18" x14ac:dyDescent="1.4">
+    <row r="111" spans="1:18" x14ac:dyDescent="1.1000000000000001">
       <c r="A111" s="8" t="s">
         <v>340</v>
       </c>
@@ -8315,7 +8720,7 @@
         <v>207</v>
       </c>
       <c r="M111" s="3"/>
-      <c r="N111" s="3"/>
+      <c r="N111" s="53"/>
       <c r="O111" s="3"/>
       <c r="P111" s="3"/>
       <c r="Q111" s="3"/>
@@ -8324,7 +8729,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="112" spans="1:18" ht="92.65" x14ac:dyDescent="1.4">
+    <row r="112" spans="1:18" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A112" s="8" t="s">
         <v>344</v>
       </c>
@@ -8350,13 +8755,13 @@
         <v>207</v>
       </c>
       <c r="M112" s="3"/>
-      <c r="N112" s="3"/>
+      <c r="N112" s="53"/>
       <c r="O112" s="3"/>
       <c r="P112" s="3"/>
       <c r="Q112" s="3"/>
       <c r="R112" s="3"/>
     </row>
-    <row r="113" spans="1:20" x14ac:dyDescent="1.4">
+    <row r="113" spans="1:20" x14ac:dyDescent="1.1000000000000001">
       <c r="A113" s="8" t="s">
         <v>348</v>
       </c>
@@ -8382,13 +8787,13 @@
         <v>207</v>
       </c>
       <c r="M113" s="3"/>
-      <c r="N113" s="3"/>
+      <c r="N113" s="53"/>
       <c r="O113" s="3"/>
       <c r="P113" s="3"/>
       <c r="Q113" s="3"/>
       <c r="R113" s="3"/>
     </row>
-    <row r="114" spans="1:20" ht="92.65" x14ac:dyDescent="1.4">
+    <row r="114" spans="1:20" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A114" s="8" t="s">
         <v>350</v>
       </c>
@@ -8414,13 +8819,13 @@
         <v>207</v>
       </c>
       <c r="M114" s="3"/>
-      <c r="N114" s="3"/>
+      <c r="N114" s="53"/>
       <c r="O114" s="3"/>
       <c r="P114" s="3"/>
       <c r="Q114" s="3"/>
       <c r="R114" s="3"/>
     </row>
-    <row r="115" spans="1:20" ht="92.65" x14ac:dyDescent="1.4">
+    <row r="115" spans="1:20" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A115" s="8" t="s">
         <v>352</v>
       </c>
@@ -8446,13 +8851,13 @@
         <v>207</v>
       </c>
       <c r="M115" s="3"/>
-      <c r="N115" s="3"/>
+      <c r="N115" s="53"/>
       <c r="O115" s="3"/>
       <c r="P115" s="3"/>
       <c r="Q115" s="3"/>
       <c r="R115" s="3"/>
     </row>
-    <row r="116" spans="1:20" ht="92.65" x14ac:dyDescent="1.4">
+    <row r="116" spans="1:20" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A116" s="8" t="s">
         <v>356</v>
       </c>
@@ -8478,7 +8883,7 @@
         <v>207</v>
       </c>
       <c r="M116" s="3"/>
-      <c r="N116" s="3"/>
+      <c r="N116" s="53"/>
       <c r="O116" s="3"/>
       <c r="P116" s="3"/>
       <c r="Q116" s="3"/>
@@ -8487,7 +8892,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="117" spans="1:20" ht="92.65" x14ac:dyDescent="1.4">
+    <row r="117" spans="1:20" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A117" s="8" t="s">
         <v>359</v>
       </c>
@@ -8513,13 +8918,13 @@
         <v>39</v>
       </c>
       <c r="M117" s="3"/>
-      <c r="N117" s="3"/>
+      <c r="N117" s="53"/>
       <c r="O117" s="3"/>
       <c r="P117" s="3"/>
       <c r="Q117" s="3"/>
       <c r="R117" s="3"/>
     </row>
-    <row r="118" spans="1:20" ht="92.65" x14ac:dyDescent="1.4">
+    <row r="118" spans="1:20" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A118" s="8" t="s">
         <v>362</v>
       </c>
@@ -8545,7 +8950,7 @@
         <v>39</v>
       </c>
       <c r="M118" s="3"/>
-      <c r="N118" s="3"/>
+      <c r="N118" s="53"/>
       <c r="O118" s="3"/>
       <c r="P118" s="3"/>
       <c r="Q118" s="3"/>
@@ -8554,7 +8959,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="119" spans="1:20" ht="92.65" x14ac:dyDescent="1.4">
+    <row r="119" spans="1:20" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A119" s="8" t="s">
         <v>366</v>
       </c>
@@ -8580,13 +8985,13 @@
         <v>207</v>
       </c>
       <c r="M119" s="3"/>
-      <c r="N119" s="3"/>
+      <c r="N119" s="53"/>
       <c r="O119" s="3"/>
       <c r="P119" s="3"/>
       <c r="Q119" s="3"/>
       <c r="R119" s="3"/>
     </row>
-    <row r="120" spans="1:20" ht="138.4" x14ac:dyDescent="1.4">
+    <row r="120" spans="1:20" ht="139.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A120" s="8" t="s">
         <v>368</v>
       </c>
@@ -8612,7 +9017,7 @@
         <v>207</v>
       </c>
       <c r="M120" s="3"/>
-      <c r="N120" s="3"/>
+      <c r="N120" s="53"/>
       <c r="O120" s="3"/>
       <c r="P120" s="3"/>
       <c r="Q120" s="3"/>
@@ -8621,7 +9026,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="121" spans="1:20" ht="92.65" x14ac:dyDescent="1.4">
+    <row r="121" spans="1:20" ht="139.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A121" s="8" t="s">
         <v>372</v>
       </c>
@@ -8647,13 +9052,13 @@
         <v>39</v>
       </c>
       <c r="M121" s="3"/>
-      <c r="N121" s="3"/>
+      <c r="N121" s="53"/>
       <c r="O121" s="3"/>
       <c r="P121" s="3"/>
       <c r="Q121" s="3"/>
       <c r="R121" s="3"/>
     </row>
-    <row r="122" spans="1:20" ht="138.4" x14ac:dyDescent="1.4">
+    <row r="122" spans="1:20" ht="139.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A122" s="8" t="s">
         <v>374</v>
       </c>
@@ -8679,13 +9084,13 @@
         <v>39</v>
       </c>
       <c r="M122" s="3"/>
-      <c r="N122" s="3"/>
+      <c r="N122" s="53"/>
       <c r="O122" s="3"/>
       <c r="P122" s="3"/>
       <c r="Q122" s="3"/>
       <c r="R122" s="3"/>
     </row>
-    <row r="123" spans="1:20" ht="138.4" x14ac:dyDescent="1.4">
+    <row r="123" spans="1:20" ht="139.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A123" s="8" t="s">
         <v>376</v>
       </c>
@@ -8711,7 +9116,7 @@
         <v>39</v>
       </c>
       <c r="M123" s="3"/>
-      <c r="N123" s="3"/>
+      <c r="N123" s="53"/>
       <c r="O123" s="3"/>
       <c r="P123" s="3"/>
       <c r="Q123" s="3"/>
@@ -8720,7 +9125,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="124" spans="1:20" x14ac:dyDescent="1.4">
+    <row r="124" spans="1:20" x14ac:dyDescent="1.1000000000000001">
       <c r="A124" s="8" t="s">
         <v>379</v>
       </c>
@@ -8744,7 +9149,7 @@
       <c r="K124" s="3"/>
       <c r="L124" s="10"/>
       <c r="M124" s="3"/>
-      <c r="N124" s="3"/>
+      <c r="N124" s="53"/>
       <c r="O124" s="3"/>
       <c r="P124" s="3"/>
       <c r="Q124" s="3"/>
@@ -8753,7 +9158,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="125" spans="1:20" ht="229.9" x14ac:dyDescent="1.4">
+    <row r="125" spans="1:20" ht="277.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A125" s="8" t="s">
         <v>381</v>
       </c>
@@ -8779,7 +9184,7 @@
         <v>39</v>
       </c>
       <c r="M125" s="3"/>
-      <c r="N125" s="3"/>
+      <c r="N125" s="53"/>
       <c r="O125" s="3"/>
       <c r="P125" s="3"/>
       <c r="Q125" s="3"/>
@@ -8788,7 +9193,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="126" spans="1:20" ht="184.15" x14ac:dyDescent="1.4">
+    <row r="126" spans="1:20" ht="185.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A126" s="8" t="s">
         <v>383</v>
       </c>
@@ -8814,13 +9219,13 @@
         <v>39</v>
       </c>
       <c r="M126" s="3"/>
-      <c r="N126" s="3"/>
+      <c r="N126" s="53"/>
       <c r="O126" s="3"/>
       <c r="P126" s="3"/>
       <c r="Q126" s="3"/>
       <c r="R126" s="3"/>
     </row>
-    <row r="127" spans="1:20" ht="219" customHeight="1" x14ac:dyDescent="1.4">
+    <row r="127" spans="1:20" ht="138" x14ac:dyDescent="1.1000000000000001">
       <c r="A127" s="8" t="s">
         <v>385</v>
       </c>
@@ -8846,8 +9251,7 @@
         <v>207</v>
       </c>
       <c r="M127" s="3"/>
-      <c r="N127" s="3" t="e">
-        <f>#VALUE!</f>
+      <c r="N127" s="53" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
       <c r="O127" s="3"/>
@@ -8855,7 +9259,7 @@
       <c r="Q127" s="3"/>
       <c r="R127" s="3"/>
     </row>
-    <row r="128" spans="1:20" s="40" customFormat="1" ht="208.15" customHeight="1" x14ac:dyDescent="1.4">
+    <row r="128" spans="1:20" s="40" customFormat="1" ht="92" x14ac:dyDescent="1.1000000000000001">
       <c r="A128" s="33" t="s">
         <v>389</v>
       </c>
@@ -8879,20 +9283,17 @@
       <c r="K128" s="38"/>
       <c r="L128" s="10"/>
       <c r="M128" s="38"/>
-      <c r="N128" s="3" t="e">
-        <f>#VALUE!</f>
+      <c r="N128" s="53" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
       <c r="O128" s="38"/>
-      <c r="P128" s="38" t="e" vm="1">
-        <v>#VALUE!</v>
-      </c>
+      <c r="P128" s="38"/>
       <c r="Q128" s="38"/>
       <c r="R128" s="38"/>
       <c r="S128" s="39"/>
       <c r="T128" s="39"/>
     </row>
-    <row r="129" spans="1:20" ht="91.5" x14ac:dyDescent="1.4">
+    <row r="129" spans="1:20" ht="92" x14ac:dyDescent="1.1000000000000001">
       <c r="A129" s="8" t="s">
         <v>393</v>
       </c>
@@ -8916,20 +9317,17 @@
       <c r="K129" s="38"/>
       <c r="L129" s="10"/>
       <c r="M129" s="38"/>
-      <c r="N129" s="3" t="e">
-        <f>#VALUE!</f>
+      <c r="N129" s="53" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
       <c r="O129" s="38"/>
-      <c r="P129" s="38" t="e" vm="2">
-        <v>#VALUE!</v>
-      </c>
+      <c r="P129" s="38"/>
       <c r="Q129" s="38"/>
       <c r="R129" s="38"/>
       <c r="S129" s="39"/>
       <c r="T129" s="39"/>
     </row>
-    <row r="130" spans="1:20" ht="92.65" x14ac:dyDescent="1.4">
+    <row r="130" spans="1:20" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A130" s="8" t="s">
         <v>397</v>
       </c>
@@ -8953,20 +9351,17 @@
       <c r="K130" s="38"/>
       <c r="L130" s="10"/>
       <c r="M130" s="38"/>
-      <c r="N130" s="3" t="e">
-        <f>#VALUE!</f>
+      <c r="N130" s="53" t="e" vm="3">
         <v>#VALUE!</v>
       </c>
       <c r="O130" s="38"/>
-      <c r="P130" s="38" t="e" vm="3">
-        <v>#VALUE!</v>
-      </c>
+      <c r="P130" s="38"/>
       <c r="Q130" s="38"/>
       <c r="R130" s="38"/>
       <c r="S130" s="39"/>
       <c r="T130" s="39"/>
     </row>
-    <row r="131" spans="1:20" s="40" customFormat="1" ht="92.65" x14ac:dyDescent="1.4">
+    <row r="131" spans="1:20" s="40" customFormat="1" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A131" s="33" t="s">
         <v>400</v>
       </c>
@@ -8990,20 +9385,17 @@
       <c r="K131" s="38"/>
       <c r="L131" s="10"/>
       <c r="M131" s="38"/>
-      <c r="N131" s="3" t="e">
-        <f>#VALUE!</f>
+      <c r="N131" s="53" t="e" vm="3">
         <v>#VALUE!</v>
       </c>
       <c r="O131" s="38"/>
-      <c r="P131" s="38" t="e" vm="4">
-        <v>#VALUE!</v>
-      </c>
+      <c r="P131" s="38"/>
       <c r="Q131" s="38"/>
       <c r="R131" s="38"/>
       <c r="S131" s="39"/>
       <c r="T131" s="39"/>
     </row>
-    <row r="132" spans="1:20" x14ac:dyDescent="1.4">
+    <row r="132" spans="1:20" x14ac:dyDescent="1.1000000000000001">
       <c r="A132" s="8" t="s">
         <v>403</v>
       </c>
@@ -9027,20 +9419,17 @@
       <c r="K132" s="38"/>
       <c r="L132" s="10"/>
       <c r="M132" s="38"/>
-      <c r="N132" s="3" t="e">
-        <f>#VALUE!</f>
+      <c r="N132" s="53" t="e" vm="4">
         <v>#VALUE!</v>
       </c>
       <c r="O132" s="38"/>
-      <c r="P132" s="38" t="e" vm="5">
-        <v>#VALUE!</v>
-      </c>
+      <c r="P132" s="38"/>
       <c r="Q132" s="38"/>
       <c r="R132" s="38"/>
       <c r="S132" s="39"/>
       <c r="T132" s="39"/>
     </row>
-    <row r="133" spans="1:20" ht="358.5" customHeight="1" x14ac:dyDescent="1.4">
+    <row r="133" spans="1:20" ht="174.75" customHeight="1" x14ac:dyDescent="1.1000000000000001">
       <c r="A133" s="8" t="s">
         <v>407</v>
       </c>
@@ -9064,20 +9453,17 @@
       <c r="K133" s="38"/>
       <c r="L133" s="10"/>
       <c r="M133" s="38"/>
-      <c r="N133" s="3" t="e">
-        <f>#VALUE!</f>
+      <c r="N133" s="53" t="e" vm="5">
         <v>#VALUE!</v>
       </c>
       <c r="O133" s="38"/>
-      <c r="P133" s="38" t="e" vm="6">
-        <v>#VALUE!</v>
-      </c>
+      <c r="P133" s="38"/>
       <c r="Q133" s="38"/>
       <c r="R133" s="38"/>
       <c r="S133" s="39"/>
       <c r="T133" s="39"/>
     </row>
-    <row r="134" spans="1:20" x14ac:dyDescent="1.4">
+    <row r="134" spans="1:20" x14ac:dyDescent="1.1000000000000001">
       <c r="A134" s="8" t="s">
         <v>411</v>
       </c>
@@ -9101,20 +9487,17 @@
       <c r="K134" s="38"/>
       <c r="L134" s="10"/>
       <c r="M134" s="38"/>
-      <c r="N134" s="3" t="e">
-        <f>#VALUE!</f>
+      <c r="N134" s="53" t="e" vm="6">
         <v>#VALUE!</v>
       </c>
       <c r="O134" s="38"/>
-      <c r="P134" s="38" t="e" vm="7">
-        <v>#VALUE!</v>
-      </c>
+      <c r="P134" s="38"/>
       <c r="Q134" s="38"/>
       <c r="R134" s="38"/>
       <c r="S134" s="39"/>
       <c r="T134" s="39"/>
     </row>
-    <row r="135" spans="1:20" x14ac:dyDescent="1.4">
+    <row r="135" spans="1:20" x14ac:dyDescent="1.1000000000000001">
       <c r="A135" s="8" t="s">
         <v>415</v>
       </c>
@@ -9138,20 +9521,17 @@
       <c r="K135" s="38"/>
       <c r="L135" s="10"/>
       <c r="M135" s="38"/>
-      <c r="N135" s="3" t="e">
-        <f>#VALUE!</f>
+      <c r="N135" s="53" t="e" vm="7">
         <v>#VALUE!</v>
       </c>
       <c r="O135" s="38"/>
-      <c r="P135" s="38" t="e" vm="8">
-        <v>#VALUE!</v>
-      </c>
+      <c r="P135" s="38"/>
       <c r="Q135" s="38"/>
       <c r="R135" s="38"/>
       <c r="S135" s="39"/>
       <c r="T135" s="39"/>
     </row>
-    <row r="136" spans="1:20" ht="92.65" x14ac:dyDescent="1.4">
+    <row r="136" spans="1:20" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A136" s="8" t="s">
         <v>419</v>
       </c>
@@ -9175,8 +9555,7 @@
       <c r="K136" s="3"/>
       <c r="L136" s="10"/>
       <c r="M136" s="3"/>
-      <c r="N136" s="3" t="e">
-        <f>#VALUE!</f>
+      <c r="N136" s="53" t="e" vm="8">
         <v>#VALUE!</v>
       </c>
       <c r="O136" s="3"/>
@@ -9184,7 +9563,7 @@
       <c r="Q136" s="3"/>
       <c r="R136" s="3"/>
     </row>
-    <row r="137" spans="1:20" ht="92.65" x14ac:dyDescent="1.4">
+    <row r="137" spans="1:20" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A137" s="8" t="s">
         <v>423</v>
       </c>
@@ -9208,8 +9587,7 @@
       <c r="K137" s="3"/>
       <c r="L137" s="10"/>
       <c r="M137" s="3"/>
-      <c r="N137" s="3" t="e">
-        <f>#VALUE!</f>
+      <c r="N137" s="53" t="e" vm="9">
         <v>#VALUE!</v>
       </c>
       <c r="O137" s="3"/>
@@ -9217,7 +9595,7 @@
       <c r="Q137" s="3"/>
       <c r="R137" s="3"/>
     </row>
-    <row r="138" spans="1:20" ht="138.4" x14ac:dyDescent="1.4">
+    <row r="138" spans="1:20" ht="139.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A138" s="8" t="s">
         <v>426</v>
       </c>
@@ -9241,18 +9619,15 @@
       <c r="K138" s="3"/>
       <c r="L138" s="10"/>
       <c r="M138" s="3"/>
-      <c r="N138" s="3" t="e">
-        <f>#VALUE!</f>
+      <c r="N138" s="53" t="e" vm="10">
         <v>#VALUE!</v>
       </c>
       <c r="O138" s="3"/>
-      <c r="P138" s="3" t="e" vm="9">
-        <v>#VALUE!</v>
-      </c>
+      <c r="P138" s="3"/>
       <c r="Q138" s="3"/>
       <c r="R138" s="3"/>
     </row>
-    <row r="139" spans="1:20" ht="92.65" x14ac:dyDescent="1.4">
+    <row r="139" spans="1:20" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A139" s="8" t="s">
         <v>430</v>
       </c>
@@ -9276,18 +9651,15 @@
       <c r="K139" s="3"/>
       <c r="L139" s="10"/>
       <c r="M139" s="3"/>
-      <c r="N139" s="3" t="e">
-        <f>#VALUE!</f>
+      <c r="N139" s="53" t="e" vm="11">
         <v>#VALUE!</v>
       </c>
       <c r="O139" s="3"/>
-      <c r="P139" s="3" t="e" vm="10">
-        <v>#VALUE!</v>
-      </c>
+      <c r="P139" s="3"/>
       <c r="Q139" s="3"/>
       <c r="R139" s="3"/>
     </row>
-    <row r="140" spans="1:20" ht="138.4" x14ac:dyDescent="1.4">
+    <row r="140" spans="1:20" ht="139.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A140" s="8" t="s">
         <v>433</v>
       </c>
@@ -9311,18 +9683,15 @@
       <c r="K140" s="3"/>
       <c r="L140" s="10"/>
       <c r="M140" s="3"/>
-      <c r="N140" s="3" t="e">
-        <f>#VALUE!</f>
+      <c r="N140" s="53" t="e" vm="12">
         <v>#VALUE!</v>
       </c>
       <c r="O140" s="3"/>
-      <c r="P140" s="3" t="e" vm="11">
-        <v>#VALUE!</v>
-      </c>
+      <c r="P140" s="3"/>
       <c r="Q140" s="3"/>
       <c r="R140" s="3"/>
     </row>
-    <row r="141" spans="1:20" ht="92.65" x14ac:dyDescent="1.4">
+    <row r="141" spans="1:20" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A141" s="8" t="s">
         <v>437</v>
       </c>
@@ -9346,18 +9715,15 @@
       <c r="K141" s="3"/>
       <c r="L141" s="10"/>
       <c r="M141" s="3"/>
-      <c r="N141" s="3" t="e">
-        <f>#VALUE!</f>
+      <c r="N141" s="53" t="e" vm="13">
         <v>#VALUE!</v>
       </c>
       <c r="O141" s="3"/>
-      <c r="P141" s="3" t="e" vm="12">
-        <v>#VALUE!</v>
-      </c>
+      <c r="P141" s="3"/>
       <c r="Q141" s="3"/>
       <c r="R141" s="3"/>
     </row>
-    <row r="142" spans="1:20" ht="92.65" x14ac:dyDescent="1.4">
+    <row r="142" spans="1:20" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A142" s="8" t="s">
         <v>440</v>
       </c>
@@ -9381,18 +9747,15 @@
       <c r="K142" s="3"/>
       <c r="L142" s="10"/>
       <c r="M142" s="3"/>
-      <c r="N142" s="3" t="e">
-        <f>#VALUE!</f>
+      <c r="N142" s="53" t="e" vm="14">
         <v>#VALUE!</v>
       </c>
       <c r="O142" s="3"/>
-      <c r="P142" s="3" t="e" vm="13">
-        <v>#VALUE!</v>
-      </c>
+      <c r="P142" s="3"/>
       <c r="Q142" s="3"/>
       <c r="R142" s="3"/>
     </row>
-    <row r="143" spans="1:20" ht="138.4" x14ac:dyDescent="1.4">
+    <row r="143" spans="1:20" ht="139.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A143" s="8" t="s">
         <v>443</v>
       </c>
@@ -9416,18 +9779,15 @@
       <c r="K143" s="3"/>
       <c r="L143" s="10"/>
       <c r="M143" s="3"/>
-      <c r="N143" s="3" t="e">
-        <f>#VALUE!</f>
+      <c r="N143" s="53" t="e" vm="15">
         <v>#VALUE!</v>
       </c>
       <c r="O143" s="3"/>
-      <c r="P143" s="3" t="e" vm="14">
-        <v>#VALUE!</v>
-      </c>
+      <c r="P143" s="3"/>
       <c r="Q143" s="3"/>
       <c r="R143" s="3"/>
     </row>
-    <row r="144" spans="1:20" ht="138.4" x14ac:dyDescent="1.4">
+    <row r="144" spans="1:20" ht="139.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A144" s="42" t="s">
         <v>446</v>
       </c>
@@ -9451,17 +9811,15 @@
       <c r="K144" s="38"/>
       <c r="L144" s="10"/>
       <c r="M144" s="38"/>
-      <c r="N144" s="3"/>
+      <c r="N144" s="53"/>
       <c r="O144" s="38"/>
-      <c r="P144" s="10" t="s">
-        <v>39</v>
-      </c>
+      <c r="P144" s="38"/>
       <c r="Q144" s="38"/>
       <c r="R144" s="38"/>
       <c r="S144" s="39"/>
       <c r="T144" s="39"/>
     </row>
-    <row r="145" spans="1:20" ht="92.65" x14ac:dyDescent="1.4">
+    <row r="145" spans="1:20" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A145" s="8" t="s">
         <v>450</v>
       </c>
@@ -9487,20 +9845,17 @@
         <v>207</v>
       </c>
       <c r="M145" s="38"/>
-      <c r="N145" s="3" t="e">
-        <f>#VALUE!</f>
+      <c r="N145" s="53" t="e" vm="16">
         <v>#VALUE!</v>
       </c>
       <c r="O145" s="38"/>
-      <c r="P145" s="10" t="s">
-        <v>39</v>
-      </c>
+      <c r="P145" s="38"/>
       <c r="Q145" s="38"/>
       <c r="R145" s="38"/>
       <c r="S145" s="39"/>
       <c r="T145" s="39"/>
     </row>
-    <row r="146" spans="1:20" ht="138.4" x14ac:dyDescent="1.4">
+    <row r="146" spans="1:20" ht="139.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A146" s="8" t="s">
         <v>454</v>
       </c>
@@ -9526,20 +9881,17 @@
         <v>207</v>
       </c>
       <c r="M146" s="38"/>
-      <c r="N146" s="3" t="e">
-        <f>#VALUE!</f>
+      <c r="N146" s="53" t="e" vm="17">
         <v>#VALUE!</v>
       </c>
       <c r="O146" s="38"/>
-      <c r="P146" s="10" t="s">
-        <v>39</v>
-      </c>
+      <c r="P146" s="38"/>
       <c r="Q146" s="38"/>
       <c r="R146" s="38"/>
       <c r="S146" s="39"/>
       <c r="T146" s="39"/>
     </row>
-    <row r="147" spans="1:20" ht="138.4" x14ac:dyDescent="1.4">
+    <row r="147" spans="1:20" ht="139.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A147" s="8" t="s">
         <v>458</v>
       </c>
@@ -9563,20 +9915,17 @@
       <c r="K147" s="38"/>
       <c r="L147" s="10"/>
       <c r="M147" s="38"/>
-      <c r="N147" s="3" t="e">
-        <f>#VALUE!</f>
+      <c r="N147" s="53" t="e" vm="18">
         <v>#VALUE!</v>
       </c>
       <c r="O147" s="38"/>
-      <c r="P147" s="38" t="e" vm="2">
-        <v>#VALUE!</v>
-      </c>
+      <c r="P147" s="38"/>
       <c r="Q147" s="38"/>
       <c r="R147" s="38"/>
       <c r="S147" s="39"/>
       <c r="T147" s="39"/>
     </row>
-    <row r="148" spans="1:20" ht="138.4" x14ac:dyDescent="1.4">
+    <row r="148" spans="1:20" ht="139.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A148" s="8" t="s">
         <v>462</v>
       </c>
@@ -9600,20 +9949,17 @@
       <c r="K148" s="38"/>
       <c r="L148" s="10"/>
       <c r="M148" s="38"/>
-      <c r="N148" s="3" t="e">
-        <f>#VALUE!</f>
+      <c r="N148" s="53" t="e" vm="19">
         <v>#VALUE!</v>
       </c>
       <c r="O148" s="38"/>
-      <c r="P148" s="38" t="e" vm="7">
-        <v>#VALUE!</v>
-      </c>
+      <c r="P148" s="38"/>
       <c r="Q148" s="38"/>
       <c r="R148" s="38"/>
       <c r="S148" s="39"/>
       <c r="T148" s="39"/>
     </row>
-    <row r="149" spans="1:20" s="40" customFormat="1" ht="138.4" x14ac:dyDescent="1.4">
+    <row r="149" spans="1:20" s="40" customFormat="1" ht="139.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A149" s="33" t="s">
         <v>466</v>
       </c>
@@ -9637,17 +9983,15 @@
       <c r="K149" s="38"/>
       <c r="L149" s="10"/>
       <c r="M149" s="38"/>
-      <c r="N149" s="3"/>
+      <c r="N149" s="53"/>
       <c r="O149" s="38"/>
-      <c r="P149" s="38" t="e" vm="15">
-        <v>#VALUE!</v>
-      </c>
+      <c r="P149" s="38"/>
       <c r="Q149" s="38"/>
       <c r="R149" s="38"/>
       <c r="S149" s="39"/>
       <c r="T149" s="39"/>
     </row>
-    <row r="150" spans="1:20" ht="138.4" x14ac:dyDescent="1.4">
+    <row r="150" spans="1:20" ht="139.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A150" s="8" t="s">
         <v>470</v>
       </c>
@@ -9671,20 +10015,17 @@
       <c r="K150" s="38"/>
       <c r="L150" s="10"/>
       <c r="M150" s="38"/>
-      <c r="N150" s="3" t="e">
-        <f>#VALUE!</f>
+      <c r="N150" s="53" t="e" vm="20">
         <v>#VALUE!</v>
       </c>
       <c r="O150" s="38"/>
-      <c r="P150" s="38" t="s">
-        <v>698</v>
-      </c>
+      <c r="P150" s="38"/>
       <c r="Q150" s="38"/>
       <c r="R150" s="38"/>
       <c r="S150" s="39"/>
       <c r="T150" s="39"/>
     </row>
-    <row r="151" spans="1:20" ht="138.4" x14ac:dyDescent="1.4">
+    <row r="151" spans="1:20" ht="139.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A151" s="8" t="s">
         <v>474</v>
       </c>
@@ -9708,7 +10049,7 @@
         <v>207</v>
       </c>
       <c r="M151" s="38"/>
-      <c r="N151" s="3"/>
+      <c r="N151" s="53"/>
       <c r="O151" s="38"/>
       <c r="P151" s="38"/>
       <c r="Q151" s="38"/>
@@ -9716,7 +10057,7 @@
       <c r="S151" s="39"/>
       <c r="T151" s="39"/>
     </row>
-    <row r="152" spans="1:20" ht="92.65" x14ac:dyDescent="1.4">
+    <row r="152" spans="1:20" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A152" s="8" t="s">
         <v>477</v>
       </c>
@@ -9740,7 +10081,7 @@
         <v>207</v>
       </c>
       <c r="M152" s="38"/>
-      <c r="N152" s="3"/>
+      <c r="N152" s="53"/>
       <c r="O152" s="38"/>
       <c r="P152" s="38"/>
       <c r="Q152" s="38"/>
@@ -9748,7 +10089,7 @@
       <c r="S152" s="39"/>
       <c r="T152" s="39"/>
     </row>
-    <row r="153" spans="1:20" ht="138.4" x14ac:dyDescent="1.4">
+    <row r="153" spans="1:20" ht="139.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A153" s="8" t="s">
         <v>480</v>
       </c>
@@ -9776,7 +10117,7 @@
         <v>39</v>
       </c>
       <c r="M153" s="38"/>
-      <c r="N153" s="3"/>
+      <c r="N153" s="53"/>
       <c r="O153" s="38"/>
       <c r="P153" s="38" t="s">
         <v>39</v>
@@ -9786,7 +10127,7 @@
       <c r="S153" s="39"/>
       <c r="T153" s="39"/>
     </row>
-    <row r="154" spans="1:20" ht="138.4" x14ac:dyDescent="1.4">
+    <row r="154" spans="1:20" ht="139.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A154" s="8" t="s">
         <v>483</v>
       </c>
@@ -9814,7 +10155,7 @@
         <v>39</v>
       </c>
       <c r="M154" s="38"/>
-      <c r="N154" s="3"/>
+      <c r="N154" s="53"/>
       <c r="O154" s="38"/>
       <c r="P154" s="38" t="s">
         <v>39</v>
@@ -9824,7 +10165,7 @@
       <c r="S154" s="39"/>
       <c r="T154" s="39"/>
     </row>
-    <row r="155" spans="1:20" ht="92.65" x14ac:dyDescent="1.4">
+    <row r="155" spans="1:20" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A155" s="8" t="s">
         <v>486</v>
       </c>
@@ -9852,7 +10193,7 @@
         <v>39</v>
       </c>
       <c r="M155" s="38"/>
-      <c r="N155" s="3"/>
+      <c r="N155" s="53"/>
       <c r="O155" s="38"/>
       <c r="P155" s="38" t="s">
         <v>39</v>
@@ -9862,7 +10203,7 @@
       <c r="S155" s="39"/>
       <c r="T155" s="39"/>
     </row>
-    <row r="156" spans="1:20" ht="138.4" x14ac:dyDescent="1.4">
+    <row r="156" spans="1:20" ht="139.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A156" s="8" t="s">
         <v>489</v>
       </c>
@@ -9890,7 +10231,7 @@
         <v>39</v>
       </c>
       <c r="M156" s="38"/>
-      <c r="N156" s="3"/>
+      <c r="N156" s="53"/>
       <c r="O156" s="38"/>
       <c r="P156" s="38" t="s">
         <v>39</v>
@@ -9900,7 +10241,7 @@
       <c r="S156" s="39"/>
       <c r="T156" s="39"/>
     </row>
-    <row r="157" spans="1:20" ht="92.65" x14ac:dyDescent="1.4">
+    <row r="157" spans="1:20" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A157" s="8" t="s">
         <v>491</v>
       </c>
@@ -9928,7 +10269,7 @@
         <v>39</v>
       </c>
       <c r="M157" s="38"/>
-      <c r="N157" s="3"/>
+      <c r="N157" s="53"/>
       <c r="O157" s="38"/>
       <c r="P157" s="38" t="s">
         <v>39</v>
@@ -9938,7 +10279,7 @@
       <c r="S157" s="39"/>
       <c r="T157" s="39"/>
     </row>
-    <row r="158" spans="1:20" ht="92.65" x14ac:dyDescent="1.4">
+    <row r="158" spans="1:20" ht="139.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A158" s="8" t="s">
         <v>493</v>
       </c>
@@ -9966,7 +10307,7 @@
         <v>39</v>
       </c>
       <c r="M158" s="38"/>
-      <c r="N158" s="3"/>
+      <c r="N158" s="53"/>
       <c r="O158" s="38"/>
       <c r="P158" s="38" t="s">
         <v>39</v>
@@ -9976,7 +10317,7 @@
       <c r="S158" s="39"/>
       <c r="T158" s="39"/>
     </row>
-    <row r="159" spans="1:20" ht="92.65" x14ac:dyDescent="1.4">
+    <row r="159" spans="1:20" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A159" s="8" t="s">
         <v>496</v>
       </c>
@@ -10004,7 +10345,7 @@
         <v>39</v>
       </c>
       <c r="M159" s="38"/>
-      <c r="N159" s="3"/>
+      <c r="N159" s="53"/>
       <c r="O159" s="38"/>
       <c r="P159" s="38" t="s">
         <v>39</v>
@@ -10014,7 +10355,7 @@
       <c r="S159" s="39"/>
       <c r="T159" s="39"/>
     </row>
-    <row r="160" spans="1:20" ht="92.65" x14ac:dyDescent="1.4">
+    <row r="160" spans="1:20" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A160" s="8" t="s">
         <v>499</v>
       </c>
@@ -10042,7 +10383,7 @@
         <v>39</v>
       </c>
       <c r="M160" s="38"/>
-      <c r="N160" s="3"/>
+      <c r="N160" s="53"/>
       <c r="O160" s="38"/>
       <c r="P160" s="38" t="s">
         <v>39</v>
@@ -10052,7 +10393,7 @@
       <c r="S160" s="39"/>
       <c r="T160" s="39"/>
     </row>
-    <row r="161" spans="1:20" ht="92.65" x14ac:dyDescent="1.4">
+    <row r="161" spans="1:20" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A161" s="8" t="s">
         <v>502</v>
       </c>
@@ -10080,7 +10421,7 @@
         <v>39</v>
       </c>
       <c r="M161" s="38"/>
-      <c r="N161" s="3"/>
+      <c r="N161" s="53"/>
       <c r="O161" s="38"/>
       <c r="P161" s="38" t="s">
         <v>39</v>
@@ -10090,7 +10431,7 @@
       <c r="S161" s="39"/>
       <c r="T161" s="39"/>
     </row>
-    <row r="162" spans="1:20" x14ac:dyDescent="1.4">
+    <row r="162" spans="1:20" x14ac:dyDescent="1.1000000000000001">
       <c r="A162" s="8" t="s">
         <v>505</v>
       </c>
@@ -10118,7 +10459,7 @@
         <v>39</v>
       </c>
       <c r="M162" s="38"/>
-      <c r="N162" s="3"/>
+      <c r="N162" s="53"/>
       <c r="O162" s="38"/>
       <c r="P162" s="38" t="s">
         <v>39</v>
@@ -10128,7 +10469,7 @@
       <c r="S162" s="39"/>
       <c r="T162" s="39"/>
     </row>
-    <row r="163" spans="1:20" x14ac:dyDescent="1.4">
+    <row r="163" spans="1:20" x14ac:dyDescent="1.1000000000000001">
       <c r="A163" s="8" t="s">
         <v>508</v>
       </c>
@@ -10156,7 +10497,7 @@
         <v>39</v>
       </c>
       <c r="M163" s="38"/>
-      <c r="N163" s="3"/>
+      <c r="N163" s="53"/>
       <c r="O163" s="38"/>
       <c r="P163" s="38" t="s">
         <v>39</v>
@@ -10166,7 +10507,7 @@
       <c r="S163" s="39"/>
       <c r="T163" s="39"/>
     </row>
-    <row r="164" spans="1:20" x14ac:dyDescent="1.4">
+    <row r="164" spans="1:20" x14ac:dyDescent="1.1000000000000001">
       <c r="A164" s="8" t="s">
         <v>511</v>
       </c>
@@ -10194,7 +10535,7 @@
         <v>39</v>
       </c>
       <c r="M164" s="38"/>
-      <c r="N164" s="3"/>
+      <c r="N164" s="53"/>
       <c r="O164" s="38"/>
       <c r="P164" s="38" t="s">
         <v>39</v>
@@ -10204,7 +10545,7 @@
       <c r="S164" s="39"/>
       <c r="T164" s="39"/>
     </row>
-    <row r="165" spans="1:20" x14ac:dyDescent="1.4">
+    <row r="165" spans="1:20" x14ac:dyDescent="1.1000000000000001">
       <c r="A165" s="8" t="s">
         <v>514</v>
       </c>
@@ -10232,7 +10573,7 @@
         <v>39</v>
       </c>
       <c r="M165" s="38"/>
-      <c r="N165" s="3"/>
+      <c r="N165" s="53"/>
       <c r="O165" s="38"/>
       <c r="P165" s="38" t="s">
         <v>39</v>
@@ -10242,7 +10583,7 @@
       <c r="S165" s="39"/>
       <c r="T165" s="39"/>
     </row>
-    <row r="166" spans="1:20" x14ac:dyDescent="1.4">
+    <row r="166" spans="1:20" x14ac:dyDescent="1.1000000000000001">
       <c r="A166" s="8" t="s">
         <v>517</v>
       </c>
@@ -10270,7 +10611,7 @@
         <v>39</v>
       </c>
       <c r="M166" s="38"/>
-      <c r="N166" s="3"/>
+      <c r="N166" s="53"/>
       <c r="O166" s="38"/>
       <c r="P166" s="38" t="s">
         <v>39</v>
@@ -10280,7 +10621,7 @@
       <c r="S166" s="39"/>
       <c r="T166" s="39"/>
     </row>
-    <row r="167" spans="1:20" x14ac:dyDescent="1.4">
+    <row r="167" spans="1:20" x14ac:dyDescent="1.1000000000000001">
       <c r="A167" s="8" t="s">
         <v>520</v>
       </c>
@@ -10308,7 +10649,7 @@
         <v>39</v>
       </c>
       <c r="M167" s="38"/>
-      <c r="N167" s="3"/>
+      <c r="N167" s="53"/>
       <c r="O167" s="38"/>
       <c r="P167" s="38" t="s">
         <v>39</v>
@@ -10318,7 +10659,7 @@
       <c r="S167" s="39"/>
       <c r="T167" s="39"/>
     </row>
-    <row r="168" spans="1:20" ht="92.65" x14ac:dyDescent="1.4">
+    <row r="168" spans="1:20" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A168" s="8" t="s">
         <v>523</v>
       </c>
@@ -10346,7 +10687,7 @@
         <v>39</v>
       </c>
       <c r="M168" s="38"/>
-      <c r="N168" s="3"/>
+      <c r="N168" s="53"/>
       <c r="O168" s="38"/>
       <c r="P168" s="38"/>
       <c r="Q168" s="38"/>
@@ -10354,7 +10695,7 @@
       <c r="S168" s="39"/>
       <c r="T168" s="39"/>
     </row>
-    <row r="169" spans="1:20" x14ac:dyDescent="1.4">
+    <row r="169" spans="1:20" x14ac:dyDescent="1.1000000000000001">
       <c r="A169" s="8" t="s">
         <v>526</v>
       </c>
@@ -10382,7 +10723,7 @@
         <v>39</v>
       </c>
       <c r="M169" s="38"/>
-      <c r="N169" s="3"/>
+      <c r="N169" s="53"/>
       <c r="O169" s="38"/>
       <c r="P169" s="38"/>
       <c r="Q169" s="38"/>
@@ -10390,7 +10731,7 @@
       <c r="S169" s="39"/>
       <c r="T169" s="39"/>
     </row>
-    <row r="170" spans="1:20" x14ac:dyDescent="1.4">
+    <row r="170" spans="1:20" x14ac:dyDescent="1.1000000000000001">
       <c r="A170" s="8" t="s">
         <v>529</v>
       </c>
@@ -10418,7 +10759,7 @@
         <v>39</v>
       </c>
       <c r="M170" s="38"/>
-      <c r="N170" s="3"/>
+      <c r="N170" s="53"/>
       <c r="O170" s="38"/>
       <c r="P170" s="38"/>
       <c r="Q170" s="38"/>
@@ -10426,7 +10767,7 @@
       <c r="S170" s="39"/>
       <c r="T170" s="39"/>
     </row>
-    <row r="171" spans="1:20" x14ac:dyDescent="1.4">
+    <row r="171" spans="1:20" x14ac:dyDescent="1.1000000000000001">
       <c r="A171" s="8" t="s">
         <v>532</v>
       </c>
@@ -10450,7 +10791,7 @@
       <c r="K171" s="38"/>
       <c r="L171" s="8"/>
       <c r="M171" s="38"/>
-      <c r="N171" s="3"/>
+      <c r="N171" s="53"/>
       <c r="O171" s="38"/>
       <c r="P171" s="38"/>
       <c r="Q171" s="38"/>
@@ -10458,7 +10799,7 @@
       <c r="S171" s="39"/>
       <c r="T171" s="39"/>
     </row>
-    <row r="172" spans="1:20" ht="92.65" x14ac:dyDescent="1.4">
+    <row r="172" spans="1:20" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A172" s="8" t="s">
         <v>535</v>
       </c>
@@ -10486,7 +10827,7 @@
         <v>39</v>
       </c>
       <c r="M172" s="38"/>
-      <c r="N172" s="3"/>
+      <c r="N172" s="53"/>
       <c r="O172" s="38"/>
       <c r="P172" s="38"/>
       <c r="Q172" s="38"/>
@@ -10494,7 +10835,7 @@
       <c r="S172" s="39"/>
       <c r="T172" s="39"/>
     </row>
-    <row r="173" spans="1:20" x14ac:dyDescent="1.4">
+    <row r="173" spans="1:20" x14ac:dyDescent="1.1000000000000001">
       <c r="A173" s="8" t="s">
         <v>538</v>
       </c>
@@ -10522,7 +10863,7 @@
         <v>39</v>
       </c>
       <c r="M173" s="38"/>
-      <c r="N173" s="3"/>
+      <c r="N173" s="53"/>
       <c r="O173" s="38"/>
       <c r="P173" s="38"/>
       <c r="Q173" s="38"/>
@@ -10530,7 +10871,7 @@
       <c r="S173" s="39"/>
       <c r="T173" s="39"/>
     </row>
-    <row r="174" spans="1:20" ht="92.65" x14ac:dyDescent="1.4">
+    <row r="174" spans="1:20" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A174" s="8" t="s">
         <v>541</v>
       </c>
@@ -10558,7 +10899,7 @@
         <v>39</v>
       </c>
       <c r="M174" s="38"/>
-      <c r="N174" s="3"/>
+      <c r="N174" s="53"/>
       <c r="O174" s="38"/>
       <c r="P174" s="38" t="s">
         <v>39</v>
@@ -10568,7 +10909,7 @@
       <c r="S174" s="39"/>
       <c r="T174" s="39"/>
     </row>
-    <row r="175" spans="1:20" x14ac:dyDescent="1.4">
+    <row r="175" spans="1:20" x14ac:dyDescent="1.1000000000000001">
       <c r="A175" s="8" t="s">
         <v>544</v>
       </c>
@@ -10596,7 +10937,7 @@
         <v>39</v>
       </c>
       <c r="M175" s="38"/>
-      <c r="N175" s="3"/>
+      <c r="N175" s="53"/>
       <c r="O175" s="38"/>
       <c r="P175" s="38" t="s">
         <v>39</v>
@@ -10606,7 +10947,7 @@
       <c r="S175" s="39"/>
       <c r="T175" s="39"/>
     </row>
-    <row r="176" spans="1:20" x14ac:dyDescent="1.4">
+    <row r="176" spans="1:20" x14ac:dyDescent="1.1000000000000001">
       <c r="A176" s="8" t="s">
         <v>547</v>
       </c>
@@ -10634,7 +10975,7 @@
         <v>39</v>
       </c>
       <c r="M176" s="38"/>
-      <c r="N176" s="3"/>
+      <c r="N176" s="53"/>
       <c r="O176" s="38"/>
       <c r="P176" s="38" t="s">
         <v>39</v>
@@ -10644,7 +10985,7 @@
       <c r="S176" s="39"/>
       <c r="T176" s="39"/>
     </row>
-    <row r="177" spans="1:20" x14ac:dyDescent="1.4">
+    <row r="177" spans="1:20" x14ac:dyDescent="1.1000000000000001">
       <c r="A177" s="8" t="s">
         <v>550</v>
       </c>
@@ -10672,7 +11013,7 @@
         <v>39</v>
       </c>
       <c r="M177" s="38"/>
-      <c r="N177" s="3"/>
+      <c r="N177" s="53"/>
       <c r="O177" s="38"/>
       <c r="P177" s="38" t="s">
         <v>39</v>
@@ -10682,7 +11023,7 @@
       <c r="S177" s="39"/>
       <c r="T177" s="39"/>
     </row>
-    <row r="178" spans="1:20" x14ac:dyDescent="1.4">
+    <row r="178" spans="1:20" x14ac:dyDescent="1.1000000000000001">
       <c r="A178" s="8" t="s">
         <v>553</v>
       </c>
@@ -10710,7 +11051,7 @@
         <v>39</v>
       </c>
       <c r="M178" s="38"/>
-      <c r="N178" s="3"/>
+      <c r="N178" s="53"/>
       <c r="O178" s="38"/>
       <c r="P178" s="38" t="s">
         <v>39</v>
@@ -10720,7 +11061,7 @@
       <c r="S178" s="39"/>
       <c r="T178" s="39"/>
     </row>
-    <row r="179" spans="1:20" ht="91.5" x14ac:dyDescent="1.4">
+    <row r="179" spans="1:20" ht="92" x14ac:dyDescent="1.1000000000000001">
       <c r="A179" s="8" t="s">
         <v>556</v>
       </c>
@@ -10748,7 +11089,7 @@
         <v>39</v>
       </c>
       <c r="M179" s="38"/>
-      <c r="N179" s="3"/>
+      <c r="N179" s="53"/>
       <c r="O179" s="38"/>
       <c r="P179" s="38" t="s">
         <v>39</v>
@@ -10758,7 +11099,7 @@
       <c r="S179" s="39"/>
       <c r="T179" s="39"/>
     </row>
-    <row r="180" spans="1:20" x14ac:dyDescent="1.4">
+    <row r="180" spans="1:20" x14ac:dyDescent="1.1000000000000001">
       <c r="A180" s="8" t="s">
         <v>558</v>
       </c>
@@ -10786,7 +11127,7 @@
         <v>39</v>
       </c>
       <c r="M180" s="38"/>
-      <c r="N180" s="3"/>
+      <c r="N180" s="53"/>
       <c r="O180" s="38"/>
       <c r="P180" s="38" t="s">
         <v>39</v>
@@ -10796,7 +11137,7 @@
       <c r="S180" s="39"/>
       <c r="T180" s="39"/>
     </row>
-    <row r="181" spans="1:20" x14ac:dyDescent="1.4">
+    <row r="181" spans="1:20" x14ac:dyDescent="1.1000000000000001">
       <c r="A181" s="8" t="s">
         <v>560</v>
       </c>
@@ -10824,7 +11165,7 @@
         <v>39</v>
       </c>
       <c r="M181" s="38"/>
-      <c r="N181" s="3"/>
+      <c r="N181" s="53"/>
       <c r="O181" s="38"/>
       <c r="P181" s="38" t="s">
         <v>39</v>
@@ -10834,7 +11175,7 @@
       <c r="S181" s="39"/>
       <c r="T181" s="39"/>
     </row>
-    <row r="182" spans="1:20" x14ac:dyDescent="1.4">
+    <row r="182" spans="1:20" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A182" s="8" t="s">
         <v>562</v>
       </c>
@@ -10862,7 +11203,7 @@
         <v>39</v>
       </c>
       <c r="M182" s="38"/>
-      <c r="N182" s="3"/>
+      <c r="N182" s="53"/>
       <c r="O182" s="38"/>
       <c r="P182" s="38" t="s">
         <v>39</v>
@@ -10872,7 +11213,7 @@
       <c r="S182" s="39"/>
       <c r="T182" s="39"/>
     </row>
-    <row r="183" spans="1:20" x14ac:dyDescent="1.4">
+    <row r="183" spans="1:20" x14ac:dyDescent="1.1000000000000001">
       <c r="A183" s="8" t="s">
         <v>564</v>
       </c>
@@ -10900,7 +11241,7 @@
         <v>39</v>
       </c>
       <c r="M183" s="38"/>
-      <c r="N183" s="3"/>
+      <c r="N183" s="53"/>
       <c r="O183" s="38"/>
       <c r="P183" s="38" t="s">
         <v>39</v>
@@ -10910,7 +11251,7 @@
       <c r="S183" s="39"/>
       <c r="T183" s="39"/>
     </row>
-    <row r="184" spans="1:20" ht="92.65" x14ac:dyDescent="1.4">
+    <row r="184" spans="1:20" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A184" s="8" t="s">
         <v>566</v>
       </c>
@@ -10938,7 +11279,7 @@
         <v>39</v>
       </c>
       <c r="M184" s="38"/>
-      <c r="N184" s="3"/>
+      <c r="N184" s="53"/>
       <c r="O184" s="38"/>
       <c r="P184" s="38" t="s">
         <v>39</v>
@@ -10948,7 +11289,7 @@
       <c r="S184" s="39"/>
       <c r="T184" s="39"/>
     </row>
-    <row r="185" spans="1:20" ht="92.65" x14ac:dyDescent="1.4">
+    <row r="185" spans="1:20" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A185" s="8" t="s">
         <v>568</v>
       </c>
@@ -10976,7 +11317,7 @@
         <v>39</v>
       </c>
       <c r="M185" s="38"/>
-      <c r="N185" s="3"/>
+      <c r="N185" s="53"/>
       <c r="O185" s="38"/>
       <c r="P185" s="38" t="s">
         <v>39</v>
@@ -10986,7 +11327,7 @@
       <c r="S185" s="39"/>
       <c r="T185" s="39"/>
     </row>
-    <row r="186" spans="1:20" ht="92.65" x14ac:dyDescent="1.4">
+    <row r="186" spans="1:20" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A186" s="8" t="s">
         <v>571</v>
       </c>
@@ -11014,7 +11355,7 @@
         <v>39</v>
       </c>
       <c r="M186" s="38"/>
-      <c r="N186" s="3"/>
+      <c r="N186" s="53"/>
       <c r="O186" s="38"/>
       <c r="P186" s="38" t="s">
         <v>39</v>
@@ -11024,7 +11365,7 @@
       <c r="S186" s="39"/>
       <c r="T186" s="39"/>
     </row>
-    <row r="187" spans="1:20" ht="92.65" x14ac:dyDescent="1.4">
+    <row r="187" spans="1:20" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A187" s="8" t="s">
         <v>574</v>
       </c>
@@ -11052,7 +11393,7 @@
         <v>39</v>
       </c>
       <c r="M187" s="38"/>
-      <c r="N187" s="3"/>
+      <c r="N187" s="53"/>
       <c r="O187" s="38"/>
       <c r="P187" s="38" t="s">
         <v>39</v>
@@ -11062,7 +11403,7 @@
       <c r="S187" s="39"/>
       <c r="T187" s="39"/>
     </row>
-    <row r="188" spans="1:20" ht="92.65" x14ac:dyDescent="1.4">
+    <row r="188" spans="1:20" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A188" s="8" t="s">
         <v>577</v>
       </c>
@@ -11090,7 +11431,7 @@
         <v>39</v>
       </c>
       <c r="M188" s="38"/>
-      <c r="N188" s="3"/>
+      <c r="N188" s="53"/>
       <c r="O188" s="38"/>
       <c r="P188" s="38" t="s">
         <v>39</v>
@@ -11100,7 +11441,7 @@
       <c r="S188" s="39"/>
       <c r="T188" s="39"/>
     </row>
-    <row r="189" spans="1:20" ht="92.65" x14ac:dyDescent="1.4">
+    <row r="189" spans="1:20" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A189" s="8" t="s">
         <v>580</v>
       </c>
@@ -11128,7 +11469,7 @@
         <v>39</v>
       </c>
       <c r="M189" s="38"/>
-      <c r="N189" s="3"/>
+      <c r="N189" s="53"/>
       <c r="O189" s="38"/>
       <c r="P189" s="38" t="s">
         <v>39</v>
@@ -11138,7 +11479,7 @@
       <c r="S189" s="39"/>
       <c r="T189" s="39"/>
     </row>
-    <row r="190" spans="1:20" ht="92.65" x14ac:dyDescent="1.4">
+    <row r="190" spans="1:20" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A190" s="8" t="s">
         <v>583</v>
       </c>
@@ -11166,7 +11507,7 @@
         <v>39</v>
       </c>
       <c r="M190" s="38"/>
-      <c r="N190" s="3"/>
+      <c r="N190" s="53"/>
       <c r="O190" s="38"/>
       <c r="P190" s="38" t="s">
         <v>39</v>
@@ -11176,7 +11517,7 @@
       <c r="S190" s="39"/>
       <c r="T190" s="39"/>
     </row>
-    <row r="191" spans="1:20" ht="92.65" x14ac:dyDescent="1.4">
+    <row r="191" spans="1:20" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A191" s="8" t="s">
         <v>586</v>
       </c>
@@ -11204,7 +11545,7 @@
         <v>39</v>
       </c>
       <c r="M191" s="38"/>
-      <c r="N191" s="3"/>
+      <c r="N191" s="53"/>
       <c r="O191" s="38"/>
       <c r="P191" s="38" t="s">
         <v>39</v>
@@ -11214,7 +11555,7 @@
       <c r="S191" s="39"/>
       <c r="T191" s="39"/>
     </row>
-    <row r="192" spans="1:20" ht="92.65" x14ac:dyDescent="1.4">
+    <row r="192" spans="1:20" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A192" s="8" t="s">
         <v>589</v>
       </c>
@@ -11242,7 +11583,7 @@
         <v>39</v>
       </c>
       <c r="M192" s="38"/>
-      <c r="N192" s="3"/>
+      <c r="N192" s="53"/>
       <c r="O192" s="38"/>
       <c r="P192" s="38" t="s">
         <v>39</v>
@@ -11252,7 +11593,7 @@
       <c r="S192" s="39"/>
       <c r="T192" s="39"/>
     </row>
-    <row r="193" spans="1:20" ht="92.65" x14ac:dyDescent="1.4">
+    <row r="193" spans="1:20" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A193" s="8" t="s">
         <v>592</v>
       </c>
@@ -11280,7 +11621,7 @@
         <v>39</v>
       </c>
       <c r="M193" s="38"/>
-      <c r="N193" s="3"/>
+      <c r="N193" s="53"/>
       <c r="O193" s="38"/>
       <c r="P193" s="38" t="s">
         <v>39</v>
@@ -11290,7 +11631,7 @@
       <c r="S193" s="39"/>
       <c r="T193" s="39"/>
     </row>
-    <row r="194" spans="1:20" ht="92.65" x14ac:dyDescent="1.4">
+    <row r="194" spans="1:20" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A194" s="8" t="s">
         <v>595</v>
       </c>
@@ -11318,7 +11659,7 @@
         <v>39</v>
       </c>
       <c r="M194" s="38"/>
-      <c r="N194" s="3"/>
+      <c r="N194" s="53"/>
       <c r="O194" s="38"/>
       <c r="P194" s="38" t="s">
         <v>39</v>
@@ -11328,7 +11669,7 @@
       <c r="S194" s="39"/>
       <c r="T194" s="39"/>
     </row>
-    <row r="195" spans="1:20" ht="92.65" x14ac:dyDescent="1.4">
+    <row r="195" spans="1:20" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A195" s="8" t="s">
         <v>598</v>
       </c>
@@ -11356,7 +11697,7 @@
         <v>39</v>
       </c>
       <c r="M195" s="38"/>
-      <c r="N195" s="3"/>
+      <c r="N195" s="53"/>
       <c r="O195" s="38"/>
       <c r="P195" s="38" t="s">
         <v>39</v>
@@ -11366,7 +11707,7 @@
       <c r="S195" s="39"/>
       <c r="T195" s="39"/>
     </row>
-    <row r="196" spans="1:20" x14ac:dyDescent="1.4">
+    <row r="196" spans="1:20" x14ac:dyDescent="1.1000000000000001">
       <c r="A196" s="8" t="s">
         <v>601</v>
       </c>
@@ -11394,7 +11735,7 @@
         <v>39</v>
       </c>
       <c r="M196" s="38"/>
-      <c r="N196" s="3"/>
+      <c r="N196" s="53"/>
       <c r="O196" s="38"/>
       <c r="P196" s="38" t="s">
         <v>39</v>
@@ -11404,7 +11745,7 @@
       <c r="S196" s="39"/>
       <c r="T196" s="39"/>
     </row>
-    <row r="197" spans="1:20" ht="92.65" x14ac:dyDescent="1.4">
+    <row r="197" spans="1:20" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A197" s="8" t="s">
         <v>604</v>
       </c>
@@ -11432,7 +11773,7 @@
         <v>39</v>
       </c>
       <c r="M197" s="38"/>
-      <c r="N197" s="3"/>
+      <c r="N197" s="53"/>
       <c r="O197" s="38"/>
       <c r="P197" s="38" t="s">
         <v>39</v>
@@ -11442,7 +11783,7 @@
       <c r="S197" s="39"/>
       <c r="T197" s="39"/>
     </row>
-    <row r="198" spans="1:20" ht="92.65" x14ac:dyDescent="1.4">
+    <row r="198" spans="1:20" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A198" s="8" t="s">
         <v>607</v>
       </c>
@@ -11470,7 +11811,7 @@
         <v>39</v>
       </c>
       <c r="M198" s="38"/>
-      <c r="N198" s="3"/>
+      <c r="N198" s="53"/>
       <c r="O198" s="38"/>
       <c r="P198" s="38" t="s">
         <v>39</v>
@@ -11480,7 +11821,7 @@
       <c r="S198" s="39"/>
       <c r="T198" s="39"/>
     </row>
-    <row r="199" spans="1:20" ht="92.65" x14ac:dyDescent="1.4">
+    <row r="199" spans="1:20" ht="139.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A199" s="8" t="s">
         <v>610</v>
       </c>
@@ -11508,7 +11849,7 @@
         <v>39</v>
       </c>
       <c r="M199" s="38"/>
-      <c r="N199" s="3"/>
+      <c r="N199" s="53"/>
       <c r="O199" s="38"/>
       <c r="P199" s="38" t="s">
         <v>39</v>
@@ -11518,7 +11859,7 @@
       <c r="S199" s="39"/>
       <c r="T199" s="39"/>
     </row>
-    <row r="200" spans="1:20" ht="92.65" x14ac:dyDescent="1.4">
+    <row r="200" spans="1:20" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A200" s="8" t="s">
         <v>613</v>
       </c>
@@ -11546,7 +11887,7 @@
         <v>39</v>
       </c>
       <c r="M200" s="38"/>
-      <c r="N200" s="3"/>
+      <c r="N200" s="53"/>
       <c r="O200" s="38"/>
       <c r="P200" s="38" t="s">
         <v>39</v>
@@ -11556,7 +11897,7 @@
       <c r="S200" s="39"/>
       <c r="T200" s="39"/>
     </row>
-    <row r="201" spans="1:20" ht="92.65" x14ac:dyDescent="1.4">
+    <row r="201" spans="1:20" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A201" s="8" t="s">
         <v>616</v>
       </c>
@@ -11584,7 +11925,7 @@
         <v>39</v>
       </c>
       <c r="M201" s="38"/>
-      <c r="N201" s="3"/>
+      <c r="N201" s="53"/>
       <c r="O201" s="38"/>
       <c r="P201" s="38" t="s">
         <v>39</v>
@@ -11594,7 +11935,7 @@
       <c r="S201" s="39"/>
       <c r="T201" s="39"/>
     </row>
-    <row r="202" spans="1:20" ht="92.65" x14ac:dyDescent="1.4">
+    <row r="202" spans="1:20" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A202" s="8" t="s">
         <v>619</v>
       </c>
@@ -11622,7 +11963,7 @@
         <v>39</v>
       </c>
       <c r="M202" s="38"/>
-      <c r="N202" s="3"/>
+      <c r="N202" s="53"/>
       <c r="O202" s="38"/>
       <c r="P202" s="38" t="s">
         <v>39</v>
@@ -11632,7 +11973,7 @@
       <c r="S202" s="39"/>
       <c r="T202" s="39"/>
     </row>
-    <row r="203" spans="1:20" ht="92.65" x14ac:dyDescent="1.4">
+    <row r="203" spans="1:20" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A203" s="8" t="s">
         <v>622</v>
       </c>
@@ -11660,7 +12001,7 @@
         <v>39</v>
       </c>
       <c r="M203" s="38"/>
-      <c r="N203" s="3"/>
+      <c r="N203" s="53"/>
       <c r="O203" s="38"/>
       <c r="P203" s="38" t="s">
         <v>39</v>
@@ -11670,7 +12011,7 @@
       <c r="S203" s="39"/>
       <c r="T203" s="39"/>
     </row>
-    <row r="204" spans="1:20" ht="350.25" customHeight="1" x14ac:dyDescent="1.4">
+    <row r="204" spans="1:20" ht="350.25" customHeight="1" x14ac:dyDescent="1.1000000000000001">
       <c r="A204" s="8" t="s">
         <v>625</v>
       </c>
@@ -11697,7 +12038,7 @@
       <c r="K204" s="38"/>
       <c r="L204" s="3"/>
       <c r="M204" s="38"/>
-      <c r="N204" s="3"/>
+      <c r="N204" s="53"/>
       <c r="O204" s="38"/>
       <c r="P204" s="38"/>
       <c r="Q204" s="38"/>
@@ -11705,7 +12046,7 @@
       <c r="S204" s="39"/>
       <c r="T204" s="39"/>
     </row>
-    <row r="205" spans="1:20" ht="300" customHeight="1" x14ac:dyDescent="1.4">
+    <row r="205" spans="1:20" ht="300" customHeight="1" x14ac:dyDescent="1.1000000000000001">
       <c r="A205" s="8" t="s">
         <v>629</v>
       </c>
@@ -11736,7 +12077,7 @@
         <v>39</v>
       </c>
       <c r="M205" s="38"/>
-      <c r="N205" s="3"/>
+      <c r="N205" s="53"/>
       <c r="O205" s="38"/>
       <c r="P205" s="38" t="s">
         <v>39</v>
@@ -11746,7 +12087,7 @@
       <c r="S205" s="39"/>
       <c r="T205" s="39"/>
     </row>
-    <row r="206" spans="1:20" ht="300" customHeight="1" x14ac:dyDescent="1.4">
+    <row r="206" spans="1:20" ht="300" customHeight="1" x14ac:dyDescent="1.1000000000000001">
       <c r="A206" s="8" t="s">
         <v>632</v>
       </c>
@@ -11777,7 +12118,7 @@
         <v>39</v>
       </c>
       <c r="M206" s="38"/>
-      <c r="N206" s="3"/>
+      <c r="N206" s="53"/>
       <c r="O206" s="38"/>
       <c r="P206" s="38" t="s">
         <v>39</v>
@@ -11787,7 +12128,7 @@
       <c r="S206" s="39"/>
       <c r="T206" s="39"/>
     </row>
-    <row r="207" spans="1:20" ht="300" customHeight="1" x14ac:dyDescent="1.4">
+    <row r="207" spans="1:20" ht="300" customHeight="1" x14ac:dyDescent="1.1000000000000001">
       <c r="A207" s="8" t="s">
         <v>634</v>
       </c>
@@ -11814,7 +12155,7 @@
       <c r="K207" s="38"/>
       <c r="L207" s="3"/>
       <c r="M207" s="38"/>
-      <c r="N207" s="3"/>
+      <c r="N207" s="53"/>
       <c r="O207" s="38"/>
       <c r="P207" s="38"/>
       <c r="Q207" s="38"/>
@@ -11822,7 +12163,7 @@
       <c r="S207" s="39"/>
       <c r="T207" s="39"/>
     </row>
-    <row r="208" spans="1:20" ht="300" customHeight="1" x14ac:dyDescent="1.4">
+    <row r="208" spans="1:20" ht="300" customHeight="1" x14ac:dyDescent="1.1000000000000001">
       <c r="A208" s="8" t="s">
         <v>637</v>
       </c>
@@ -11853,7 +12194,7 @@
         <v>39</v>
       </c>
       <c r="M208" s="38"/>
-      <c r="N208" s="3"/>
+      <c r="N208" s="53"/>
       <c r="O208" s="38"/>
       <c r="P208" s="38" t="s">
         <v>39</v>
@@ -11863,7 +12204,7 @@
       <c r="S208" s="39"/>
       <c r="T208" s="39"/>
     </row>
-    <row r="209" spans="1:20" ht="300" customHeight="1" x14ac:dyDescent="1.4">
+    <row r="209" spans="1:20" ht="300" customHeight="1" x14ac:dyDescent="1.1000000000000001">
       <c r="A209" s="8" t="s">
         <v>639</v>
       </c>
@@ -11890,7 +12231,7 @@
       <c r="K209" s="38"/>
       <c r="L209" s="3"/>
       <c r="M209" s="38"/>
-      <c r="N209" s="3"/>
+      <c r="N209" s="53"/>
       <c r="O209" s="38"/>
       <c r="P209" s="38" t="s">
         <v>642</v>
@@ -11900,7 +12241,7 @@
       <c r="S209" s="39"/>
       <c r="T209" s="39"/>
     </row>
-    <row r="210" spans="1:20" ht="399.75" customHeight="1" x14ac:dyDescent="1.4">
+    <row r="210" spans="1:20" ht="399.75" customHeight="1" x14ac:dyDescent="1.1000000000000001">
       <c r="A210" s="8" t="s">
         <v>643</v>
       </c>
@@ -11927,7 +12268,7 @@
       <c r="K210" s="3"/>
       <c r="L210" s="3"/>
       <c r="M210" s="3"/>
-      <c r="N210" s="3"/>
+      <c r="N210" s="53"/>
       <c r="O210" s="3"/>
       <c r="P210" s="3" t="s">
         <v>645</v>
@@ -11935,7 +12276,7 @@
       <c r="Q210" s="3"/>
       <c r="R210" s="3"/>
     </row>
-    <row r="211" spans="1:20" ht="300" customHeight="1" x14ac:dyDescent="1.4">
+    <row r="211" spans="1:20" ht="300" customHeight="1" x14ac:dyDescent="1.1000000000000001">
       <c r="A211" s="8" t="s">
         <v>646</v>
       </c>
@@ -11962,13 +12303,13 @@
       <c r="K211" s="3"/>
       <c r="L211" s="3"/>
       <c r="M211" s="3"/>
-      <c r="N211" s="3"/>
+      <c r="N211" s="53"/>
       <c r="O211" s="3"/>
       <c r="P211" s="3"/>
       <c r="Q211" s="3"/>
       <c r="R211" s="3"/>
     </row>
-    <row r="212" spans="1:20" ht="300" customHeight="1" x14ac:dyDescent="1.4">
+    <row r="212" spans="1:20" ht="300" customHeight="1" x14ac:dyDescent="1.1000000000000001">
       <c r="A212" s="8" t="s">
         <v>648</v>
       </c>
@@ -11995,13 +12336,13 @@
       <c r="K212" s="3"/>
       <c r="L212" s="3"/>
       <c r="M212" s="3"/>
-      <c r="N212" s="3"/>
+      <c r="N212" s="53"/>
       <c r="O212" s="3"/>
       <c r="P212" s="3"/>
       <c r="Q212" s="3"/>
       <c r="R212" s="3"/>
     </row>
-    <row r="213" spans="1:20" ht="150" customHeight="1" x14ac:dyDescent="1.4">
+    <row r="213" spans="1:20" ht="150" customHeight="1" x14ac:dyDescent="1.1000000000000001">
       <c r="A213" s="8" t="s">
         <v>650</v>
       </c>
@@ -12028,13 +12369,13 @@
       <c r="K213" s="3"/>
       <c r="L213" s="3"/>
       <c r="M213" s="3"/>
-      <c r="N213" s="3"/>
+      <c r="N213" s="53"/>
       <c r="O213" s="3"/>
       <c r="P213" s="3"/>
       <c r="Q213" s="3"/>
       <c r="R213" s="3"/>
     </row>
-    <row r="214" spans="1:20" ht="93.75" x14ac:dyDescent="1.4">
+    <row r="214" spans="1:20" ht="95" x14ac:dyDescent="1.1000000000000001">
       <c r="A214" s="3" t="s">
         <v>652</v>
       </c>
@@ -12058,13 +12399,13 @@
       <c r="K214" s="3"/>
       <c r="L214" s="3"/>
       <c r="M214" s="3"/>
-      <c r="N214" s="3"/>
+      <c r="N214" s="53"/>
       <c r="O214" s="3"/>
       <c r="P214" s="3"/>
       <c r="Q214" s="3"/>
       <c r="R214" s="3"/>
     </row>
-    <row r="215" spans="1:20" x14ac:dyDescent="1.4">
+    <row r="215" spans="1:20" x14ac:dyDescent="1.1000000000000001">
       <c r="A215" s="3" t="s">
         <v>655</v>
       </c>
@@ -12088,13 +12429,13 @@
       <c r="K215" s="3"/>
       <c r="L215" s="3"/>
       <c r="M215" s="3"/>
-      <c r="N215" s="3"/>
+      <c r="N215" s="53"/>
       <c r="O215" s="3"/>
       <c r="P215" s="3"/>
       <c r="Q215" s="3"/>
       <c r="R215" s="3"/>
     </row>
-    <row r="216" spans="1:20" x14ac:dyDescent="1.4">
+    <row r="216" spans="1:20" ht="95" x14ac:dyDescent="1.1000000000000001">
       <c r="A216" s="3" t="s">
         <v>658</v>
       </c>
@@ -12118,13 +12459,13 @@
       <c r="K216" s="3"/>
       <c r="L216" s="3"/>
       <c r="M216" s="3"/>
-      <c r="N216" s="3"/>
+      <c r="N216" s="53"/>
       <c r="O216" s="3"/>
       <c r="P216" s="3"/>
       <c r="Q216" s="3"/>
       <c r="R216" s="3"/>
     </row>
-    <row r="217" spans="1:20" x14ac:dyDescent="1.4">
+    <row r="217" spans="1:20" x14ac:dyDescent="1.1000000000000001">
       <c r="A217" s="3" t="s">
         <v>661</v>
       </c>
@@ -12148,13 +12489,13 @@
       <c r="K217" s="3"/>
       <c r="L217" s="3"/>
       <c r="M217" s="3"/>
-      <c r="N217" s="3"/>
+      <c r="N217" s="53"/>
       <c r="O217" s="3"/>
       <c r="P217" s="3"/>
       <c r="Q217" s="3"/>
       <c r="R217" s="3"/>
     </row>
-    <row r="218" spans="1:20" x14ac:dyDescent="1.4">
+    <row r="218" spans="1:20" ht="95" x14ac:dyDescent="1.1000000000000001">
       <c r="A218" s="3" t="s">
         <v>664</v>
       </c>
@@ -12176,13 +12517,13 @@
       <c r="K218" s="3"/>
       <c r="L218" s="3"/>
       <c r="M218" s="3"/>
-      <c r="N218" s="3"/>
+      <c r="N218" s="53"/>
       <c r="O218" s="3"/>
       <c r="P218" s="3"/>
       <c r="Q218" s="3"/>
       <c r="R218" s="3"/>
     </row>
-    <row r="219" spans="1:20" x14ac:dyDescent="1.4">
+    <row r="219" spans="1:20" x14ac:dyDescent="1.1000000000000001">
       <c r="A219" s="3" t="s">
         <v>666</v>
       </c>
@@ -12204,13 +12545,13 @@
       <c r="K219" s="3"/>
       <c r="L219" s="3"/>
       <c r="M219" s="3"/>
-      <c r="N219" s="3"/>
+      <c r="N219" s="53"/>
       <c r="O219" s="3"/>
       <c r="P219" s="3"/>
       <c r="Q219" s="3"/>
       <c r="R219" s="3"/>
     </row>
-    <row r="220" spans="1:20" x14ac:dyDescent="1.4">
+    <row r="220" spans="1:20" x14ac:dyDescent="1.1000000000000001">
       <c r="A220" s="3" t="s">
         <v>668</v>
       </c>
@@ -12234,13 +12575,13 @@
       <c r="K220" s="3"/>
       <c r="L220" s="3"/>
       <c r="M220" s="3"/>
-      <c r="N220" s="3"/>
+      <c r="N220" s="53"/>
       <c r="O220" s="3"/>
       <c r="P220" s="3"/>
       <c r="Q220" s="3"/>
       <c r="R220" s="3"/>
     </row>
-    <row r="221" spans="1:20" ht="93.75" x14ac:dyDescent="1.4">
+    <row r="221" spans="1:20" ht="95" x14ac:dyDescent="1.1000000000000001">
       <c r="A221" s="3" t="s">
         <v>671</v>
       </c>
@@ -12264,13 +12605,13 @@
       <c r="K221" s="3"/>
       <c r="L221" s="3"/>
       <c r="M221" s="3"/>
-      <c r="N221" s="3"/>
+      <c r="N221" s="53"/>
       <c r="O221" s="3"/>
       <c r="P221" s="3"/>
       <c r="Q221" s="3"/>
       <c r="R221" s="3"/>
     </row>
-    <row r="222" spans="1:20" x14ac:dyDescent="1.4">
+    <row r="222" spans="1:20" x14ac:dyDescent="1.1000000000000001">
       <c r="A222" s="3" t="s">
         <v>674</v>
       </c>
@@ -12294,13 +12635,13 @@
       <c r="K222" s="3"/>
       <c r="L222" s="3"/>
       <c r="M222" s="3"/>
-      <c r="N222" s="3"/>
+      <c r="N222" s="53"/>
       <c r="O222" s="3"/>
       <c r="P222" s="3"/>
       <c r="Q222" s="3"/>
       <c r="R222" s="3"/>
     </row>
-    <row r="223" spans="1:20" ht="93.75" x14ac:dyDescent="1.4">
+    <row r="223" spans="1:20" ht="95" x14ac:dyDescent="1.1000000000000001">
       <c r="A223" s="3" t="s">
         <v>677</v>
       </c>
@@ -12326,13 +12667,13 @@
       <c r="K223" s="3"/>
       <c r="L223" s="3"/>
       <c r="M223" s="3"/>
-      <c r="N223" s="3"/>
+      <c r="N223" s="53"/>
       <c r="O223" s="3"/>
       <c r="P223" s="3"/>
       <c r="Q223" s="3"/>
       <c r="R223" s="3"/>
     </row>
-    <row r="224" spans="1:20" x14ac:dyDescent="1.4">
+    <row r="224" spans="1:20" x14ac:dyDescent="1.1000000000000001">
       <c r="A224" s="3" t="s">
         <v>681</v>
       </c>
@@ -12356,13 +12697,13 @@
       <c r="K224" s="3"/>
       <c r="L224" s="3"/>
       <c r="M224" s="3"/>
-      <c r="N224" s="3"/>
+      <c r="N224" s="53"/>
       <c r="O224" s="3"/>
       <c r="P224" s="3"/>
       <c r="Q224" s="3"/>
       <c r="R224" s="3"/>
     </row>
-    <row r="225" spans="1:18" x14ac:dyDescent="1.4">
+    <row r="225" spans="1:18" x14ac:dyDescent="1.1000000000000001">
       <c r="A225" s="3" t="s">
         <v>684</v>
       </c>
@@ -12386,13 +12727,13 @@
       <c r="K225" s="3"/>
       <c r="L225" s="3"/>
       <c r="M225" s="3"/>
-      <c r="N225" s="3"/>
+      <c r="N225" s="53"/>
       <c r="O225" s="3"/>
       <c r="P225" s="3"/>
       <c r="Q225" s="3"/>
       <c r="R225" s="3"/>
     </row>
-    <row r="226" spans="1:18" ht="93.75" x14ac:dyDescent="1.4">
+    <row r="226" spans="1:18" ht="95" x14ac:dyDescent="1.1000000000000001">
       <c r="A226" s="3" t="s">
         <v>688</v>
       </c>
@@ -12416,13 +12757,13 @@
       <c r="K226" s="3"/>
       <c r="L226" s="3"/>
       <c r="M226" s="3"/>
-      <c r="N226" s="3"/>
+      <c r="N226" s="53"/>
       <c r="O226" s="3"/>
       <c r="P226" s="3"/>
       <c r="Q226" s="3"/>
       <c r="R226" s="3"/>
     </row>
-    <row r="227" spans="1:18" ht="93.75" x14ac:dyDescent="1.4">
+    <row r="227" spans="1:18" ht="95" x14ac:dyDescent="1.1000000000000001">
       <c r="A227" s="3" t="s">
         <v>692</v>
       </c>
@@ -12446,13 +12787,13 @@
       <c r="K227" s="3"/>
       <c r="L227" s="3"/>
       <c r="M227" s="3"/>
-      <c r="N227" s="3"/>
+      <c r="N227" s="53"/>
       <c r="O227" s="3"/>
       <c r="P227" s="3"/>
       <c r="Q227" s="3"/>
       <c r="R227" s="3"/>
     </row>
-    <row r="228" spans="1:18" ht="93.75" x14ac:dyDescent="1.4">
+    <row r="228" spans="1:18" ht="95" x14ac:dyDescent="1.1000000000000001">
       <c r="A228" s="3" t="s">
         <v>695</v>
       </c>
@@ -12476,22 +12817,22 @@
       <c r="K228" s="3"/>
       <c r="L228" s="3"/>
       <c r="M228" s="3"/>
-      <c r="N228" s="3"/>
+      <c r="N228" s="53"/>
       <c r="O228" s="3"/>
       <c r="P228" s="3"/>
       <c r="Q228" s="3"/>
       <c r="R228" s="3"/>
     </row>
-    <row r="229" spans="1:18" x14ac:dyDescent="1.4">
+    <row r="229" spans="1:18" x14ac:dyDescent="1.1000000000000001">
       <c r="J229" s="3"/>
     </row>
-    <row r="230" spans="1:18" x14ac:dyDescent="1.4">
+    <row r="230" spans="1:18" x14ac:dyDescent="1.1000000000000001">
       <c r="J230" s="3"/>
     </row>
-    <row r="231" spans="1:18" x14ac:dyDescent="1.4">
+    <row r="231" spans="1:18" x14ac:dyDescent="1.1000000000000001">
       <c r="J231" s="3"/>
     </row>
-    <row r="232" spans="1:18" x14ac:dyDescent="1.4">
+    <row r="232" spans="1:18" x14ac:dyDescent="1.1000000000000001">
       <c r="J232" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added group 16 testing requirements spreadsheet
</commit_message>
<xml_diff>
--- a/FinalRequirements.xlsx
+++ b/FinalRequirements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\18173\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B12CE0B-41AC-4954-B735-8F932E0A9A56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3A24A5B-6B1D-47A7-9A11-D7010DD1A445}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -248,7 +248,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1262" uniqueCount="724">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1284" uniqueCount="724">
   <si>
     <t>Testing</t>
   </si>
@@ -5165,8 +5165,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:T232"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E127" zoomScale="10" zoomScaleNormal="20" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1:N1048576"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="17" zoomScaleNormal="20" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="47.5" x14ac:dyDescent="1.1000000000000001"/>
@@ -10727,7 +10727,9 @@
         <v>43</v>
       </c>
       <c r="M163" s="38"/>
-      <c r="N163" s="3"/>
+      <c r="N163" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="O163" s="38"/>
       <c r="P163" s="38" t="s">
         <v>43</v>
@@ -10765,7 +10767,9 @@
         <v>43</v>
       </c>
       <c r="M164" s="38"/>
-      <c r="N164" s="3"/>
+      <c r="N164" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="O164" s="38"/>
       <c r="P164" s="38" t="s">
         <v>43</v>
@@ -10803,7 +10807,9 @@
         <v>43</v>
       </c>
       <c r="M165" s="38"/>
-      <c r="N165" s="3"/>
+      <c r="N165" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="O165" s="38"/>
       <c r="P165" s="38" t="s">
         <v>43</v>
@@ -10841,7 +10847,9 @@
         <v>43</v>
       </c>
       <c r="M166" s="38"/>
-      <c r="N166" s="3"/>
+      <c r="N166" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="O166" s="38"/>
       <c r="P166" s="38" t="s">
         <v>43</v>
@@ -10879,7 +10887,9 @@
         <v>43</v>
       </c>
       <c r="M167" s="38"/>
-      <c r="N167" s="3"/>
+      <c r="N167" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="O167" s="38"/>
       <c r="P167" s="38" t="s">
         <v>43</v>
@@ -10917,7 +10927,9 @@
         <v>43</v>
       </c>
       <c r="M168" s="38"/>
-      <c r="N168" s="3"/>
+      <c r="N168" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="O168" s="38"/>
       <c r="P168" s="38"/>
       <c r="Q168" s="38"/>
@@ -10953,7 +10965,9 @@
         <v>43</v>
       </c>
       <c r="M169" s="38"/>
-      <c r="N169" s="3"/>
+      <c r="N169" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="O169" s="38"/>
       <c r="P169" s="38"/>
       <c r="Q169" s="38"/>
@@ -10989,7 +11003,9 @@
         <v>43</v>
       </c>
       <c r="M170" s="38"/>
-      <c r="N170" s="3"/>
+      <c r="N170" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="O170" s="38"/>
       <c r="P170" s="38"/>
       <c r="Q170" s="38"/>
@@ -11021,7 +11037,9 @@
       <c r="K171" s="38"/>
       <c r="L171" s="8"/>
       <c r="M171" s="38"/>
-      <c r="N171" s="3"/>
+      <c r="N171" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="O171" s="38"/>
       <c r="P171" s="38"/>
       <c r="Q171" s="38"/>
@@ -11057,7 +11075,9 @@
         <v>43</v>
       </c>
       <c r="M172" s="38"/>
-      <c r="N172" s="3"/>
+      <c r="N172" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="O172" s="38"/>
       <c r="P172" s="38"/>
       <c r="Q172" s="38"/>
@@ -11093,7 +11113,9 @@
         <v>43</v>
       </c>
       <c r="M173" s="38"/>
-      <c r="N173" s="3"/>
+      <c r="N173" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="O173" s="38"/>
       <c r="P173" s="38"/>
       <c r="Q173" s="38"/>
@@ -11129,7 +11151,9 @@
         <v>43</v>
       </c>
       <c r="M174" s="38"/>
-      <c r="N174" s="3"/>
+      <c r="N174" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="O174" s="38"/>
       <c r="P174" s="38" t="s">
         <v>43</v>
@@ -11167,7 +11191,9 @@
         <v>43</v>
       </c>
       <c r="M175" s="38"/>
-      <c r="N175" s="3"/>
+      <c r="N175" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="O175" s="38"/>
       <c r="P175" s="38" t="s">
         <v>43</v>
@@ -11205,7 +11231,9 @@
         <v>43</v>
       </c>
       <c r="M176" s="38"/>
-      <c r="N176" s="3"/>
+      <c r="N176" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="O176" s="38"/>
       <c r="P176" s="38" t="s">
         <v>43</v>
@@ -11243,7 +11271,9 @@
         <v>43</v>
       </c>
       <c r="M177" s="38"/>
-      <c r="N177" s="3"/>
+      <c r="N177" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="O177" s="38"/>
       <c r="P177" s="38" t="s">
         <v>43</v>
@@ -11281,7 +11311,9 @@
         <v>43</v>
       </c>
       <c r="M178" s="38"/>
-      <c r="N178" s="3"/>
+      <c r="N178" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="O178" s="38"/>
       <c r="P178" s="38" t="s">
         <v>43</v>
@@ -11319,7 +11351,9 @@
         <v>43</v>
       </c>
       <c r="M179" s="38"/>
-      <c r="N179" s="3"/>
+      <c r="N179" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="O179" s="38"/>
       <c r="P179" s="38" t="s">
         <v>43</v>
@@ -11357,7 +11391,9 @@
         <v>43</v>
       </c>
       <c r="M180" s="38"/>
-      <c r="N180" s="3"/>
+      <c r="N180" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="O180" s="38"/>
       <c r="P180" s="38" t="s">
         <v>43</v>
@@ -11395,7 +11431,9 @@
         <v>43</v>
       </c>
       <c r="M181" s="38"/>
-      <c r="N181" s="3"/>
+      <c r="N181" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="O181" s="38"/>
       <c r="P181" s="38" t="s">
         <v>43</v>
@@ -11433,7 +11471,9 @@
         <v>43</v>
       </c>
       <c r="M182" s="38"/>
-      <c r="N182" s="3"/>
+      <c r="N182" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="O182" s="38"/>
       <c r="P182" s="38" t="s">
         <v>43</v>
@@ -11471,7 +11511,9 @@
         <v>43</v>
       </c>
       <c r="M183" s="38"/>
-      <c r="N183" s="3"/>
+      <c r="N183" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="O183" s="38"/>
       <c r="P183" s="38" t="s">
         <v>43</v>
@@ -11509,7 +11551,9 @@
         <v>43</v>
       </c>
       <c r="M184" s="38"/>
-      <c r="N184" s="3"/>
+      <c r="N184" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="O184" s="38"/>
       <c r="P184" s="38" t="s">
         <v>43</v>

</xml_diff>

<commit_message>
added group 12,16 test cases
</commit_message>
<xml_diff>
--- a/FinalRequirements.xlsx
+++ b/FinalRequirements.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1325" uniqueCount="765">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1361" uniqueCount="772">
   <si>
     <t xml:space="preserve">Testing</t>
   </si>
@@ -1220,6 +1220,9 @@
   </si>
   <si>
     <t xml:space="preserve">If a bot is in game, a unique tag shall be displayed for them, replacing where the ranking would normally be displayed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FAIL, TC094</t>
   </si>
   <si>
     <t xml:space="preserve">R095</t>
@@ -2377,6 +2380,9 @@
     <t xml:space="preserve">cse3310/checkers/src/main/webapp/Leaderboard/leaderboard.html</t>
   </si>
   <si>
+    <t xml:space="preserve">FAIL, TC201</t>
+  </si>
+  <si>
     <t xml:space="preserve">cannot test, since login is not working and cannot play game</t>
   </si>
   <si>
@@ -2416,6 +2422,9 @@
     <t xml:space="preserve">The Summary UI section must be part of a single-page HTML interface.</t>
   </si>
   <si>
+    <t xml:space="preserve">FAIL, TC206</t>
+  </si>
+  <si>
     <t xml:space="preserve">cannot test, since signup and login is not working</t>
   </si>
   <si>
@@ -2428,6 +2437,9 @@
     <t xml:space="preserve">The Summary section's visibility is controlled using showContent() and hideContent() functions which toggle display via CSS.</t>
   </si>
   <si>
+    <t xml:space="preserve">FAIL, TC207</t>
+  </si>
+  <si>
     <t xml:space="preserve">not able to test login is not working</t>
   </si>
   <si>
@@ -2437,16 +2449,25 @@
     <t xml:space="preserve">Each Summary client must have a unique identifier.</t>
   </si>
   <si>
+    <t xml:space="preserve">FAIL, TC208</t>
+  </si>
+  <si>
     <t xml:space="preserve">R209</t>
   </si>
   <si>
     <t xml:space="preserve">The leaderboard must auto-update when new game results are available.</t>
   </si>
   <si>
+    <t xml:space="preserve">FAIL, TC209</t>
+  </si>
+  <si>
     <t xml:space="preserve">R210</t>
   </si>
   <si>
     <t xml:space="preserve">The leaderboard shall display player statistics such as number of wins and losses.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FAIL, TC210</t>
   </si>
   <si>
     <t xml:space="preserve">R211</t>
@@ -3143,13 +3164,13 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>37800</xdr:colOff>
+      <xdr:colOff>11160</xdr:colOff>
       <xdr:row>276</xdr:row>
       <xdr:rowOff>180720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>990360</xdr:colOff>
+      <xdr:colOff>963720</xdr:colOff>
       <xdr:row>279</xdr:row>
       <xdr:rowOff>132840</xdr:rowOff>
     </xdr:to>
@@ -3176,13 +3197,13 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
+      <xdr:colOff>201960</xdr:colOff>
       <xdr:row>276</xdr:row>
       <xdr:rowOff>371160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1180800</xdr:colOff>
+      <xdr:colOff>1154160</xdr:colOff>
       <xdr:row>280</xdr:row>
       <xdr:rowOff>123480</xdr:rowOff>
     </xdr:to>
@@ -3209,13 +3230,13 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>419040</xdr:colOff>
+      <xdr:colOff>392400</xdr:colOff>
       <xdr:row>276</xdr:row>
       <xdr:rowOff>561600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1371600</xdr:colOff>
+      <xdr:colOff>1344960</xdr:colOff>
       <xdr:row>281</xdr:row>
       <xdr:rowOff>113760</xdr:rowOff>
     </xdr:to>
@@ -3242,13 +3263,13 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>133200</xdr:colOff>
+      <xdr:colOff>106560</xdr:colOff>
       <xdr:row>276</xdr:row>
       <xdr:rowOff>180720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1085760</xdr:colOff>
+      <xdr:colOff>1059120</xdr:colOff>
       <xdr:row>279</xdr:row>
       <xdr:rowOff>132840</xdr:rowOff>
     </xdr:to>
@@ -3275,13 +3296,13 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>323640</xdr:colOff>
+      <xdr:colOff>297000</xdr:colOff>
       <xdr:row>276</xdr:row>
       <xdr:rowOff>371160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1276200</xdr:colOff>
+      <xdr:colOff>1249560</xdr:colOff>
       <xdr:row>280</xdr:row>
       <xdr:rowOff>123480</xdr:rowOff>
     </xdr:to>
@@ -3308,13 +3329,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>676080</xdr:colOff>
+      <xdr:colOff>649440</xdr:colOff>
       <xdr:row>163</xdr:row>
       <xdr:rowOff>99000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>4084560</xdr:colOff>
+      <xdr:colOff>4057920</xdr:colOff>
       <xdr:row>163</xdr:row>
       <xdr:rowOff>142920</xdr:rowOff>
     </xdr:to>
@@ -3366,7 +3387,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="97393320" y="246687120"/>
+          <a:off x="97419960" y="246687120"/>
           <a:ext cx="14632920" cy="3884400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3403,7 +3424,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="49087800" y="242314560"/>
+          <a:off x="49114440" y="242314560"/>
           <a:ext cx="4081320" cy="544320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3440,7 +3461,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="48750480" y="243524880"/>
+          <a:off x="48777120" y="243524880"/>
           <a:ext cx="4422240" cy="1380600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3477,7 +3498,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="49087800" y="242314560"/>
+          <a:off x="49114440" y="242314560"/>
           <a:ext cx="4081320" cy="544320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3514,7 +3535,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="48750480" y="243524880"/>
+          <a:off x="48777120" y="243524880"/>
           <a:ext cx="4422240" cy="1380600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3551,7 +3572,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="46013760" y="244671480"/>
+          <a:off x="46040400" y="244671480"/>
           <a:ext cx="3552120" cy="1902960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3588,7 +3609,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="45641160" y="246951000"/>
+          <a:off x="45667800" y="246951000"/>
           <a:ext cx="3533040" cy="844920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3625,7 +3646,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="45806760" y="247840920"/>
+          <a:off x="45833400" y="247840920"/>
           <a:ext cx="3552120" cy="818280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3662,7 +3683,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="49616640" y="247716720"/>
+          <a:off x="49643280" y="247716720"/>
           <a:ext cx="3476160" cy="894240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3699,7 +3720,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="45806760" y="248793480"/>
+          <a:off x="45833400" y="248793480"/>
           <a:ext cx="3647520" cy="780120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3736,7 +3757,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="49824000" y="248752080"/>
+          <a:off x="49850640" y="248752080"/>
           <a:ext cx="3533040" cy="999360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3773,7 +3794,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="45641160" y="249770160"/>
+          <a:off x="45667800" y="249770160"/>
           <a:ext cx="3552120" cy="895680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3810,7 +3831,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="45641160" y="250970400"/>
+          <a:off x="45667800" y="250970400"/>
           <a:ext cx="3637800" cy="732600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3847,7 +3868,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="45641160" y="252151560"/>
+          <a:off x="45667800" y="252151560"/>
           <a:ext cx="3628440" cy="732600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3884,7 +3905,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="45641160" y="253332720"/>
+          <a:off x="45667800" y="253332720"/>
           <a:ext cx="3714120" cy="757440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3921,7 +3942,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="45641160" y="255104280"/>
+          <a:off x="45667800" y="255104280"/>
           <a:ext cx="3513960" cy="1369440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3958,7 +3979,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="45682560" y="256823640"/>
+          <a:off x="45709200" y="256823640"/>
           <a:ext cx="3666600" cy="1955880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3995,7 +4016,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="45641160" y="258057000"/>
+          <a:off x="45667800" y="258057000"/>
           <a:ext cx="3609360" cy="732600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4032,7 +4053,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="45641160" y="259238160"/>
+          <a:off x="45667800" y="259238160"/>
           <a:ext cx="3666600" cy="1294560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4069,7 +4090,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="45889560" y="261040680"/>
+          <a:off x="45916200" y="261040680"/>
           <a:ext cx="3752280" cy="1448640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4106,7 +4127,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="46013760" y="267122160"/>
+          <a:off x="46040400" y="267122160"/>
           <a:ext cx="3580920" cy="995760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4143,7 +4164,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="46013760" y="269059680"/>
+          <a:off x="46040400" y="269059680"/>
           <a:ext cx="3542760" cy="2372400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4180,7 +4201,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="45641160" y="272230200"/>
+          <a:off x="45667800" y="272230200"/>
           <a:ext cx="3666600" cy="780120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4217,7 +4238,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="80776080" y="128837880"/>
+          <a:off x="80802720" y="128837880"/>
           <a:ext cx="8972640" cy="2456640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4254,7 +4275,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="81191880" y="134902440"/>
+          <a:off x="81218520" y="134902440"/>
           <a:ext cx="7145280" cy="5181120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4291,7 +4312,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="81215640" y="138931920"/>
+          <a:off x="81242280" y="138931920"/>
           <a:ext cx="5173560" cy="3538440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4328,7 +4349,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="81191880" y="142960680"/>
+          <a:off x="81218520" y="142960680"/>
           <a:ext cx="4070880" cy="3827880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4365,7 +4386,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="81453600" y="146413800"/>
+          <a:off x="81480240" y="146413800"/>
           <a:ext cx="8696520" cy="5628240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4402,7 +4423,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="80882280" y="153023760"/>
+          <a:off x="80908920" y="153023760"/>
           <a:ext cx="9372960" cy="6121800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4439,7 +4460,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="60096240" y="7493400"/>
+          <a:off x="60122880" y="7493400"/>
           <a:ext cx="3454200" cy="1958400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4476,7 +4497,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="59334480" y="28867320"/>
+          <a:off x="59361120" y="28867320"/>
           <a:ext cx="5070960" cy="1330560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4513,7 +4534,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="60096240" y="7493400"/>
+          <a:off x="60122880" y="7493400"/>
           <a:ext cx="3457080" cy="1958400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4550,7 +4571,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="59334480" y="28867320"/>
+          <a:off x="59361120" y="28867320"/>
           <a:ext cx="8028720" cy="1330560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4587,7 +4608,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="60096240" y="7550280"/>
+          <a:off x="60122880" y="7550280"/>
           <a:ext cx="3454560" cy="1958760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4624,7 +4645,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="59334480" y="28175760"/>
+          <a:off x="59361120" y="28175760"/>
           <a:ext cx="5071320" cy="1330920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4661,7 +4682,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="60096240" y="7550280"/>
+          <a:off x="60122880" y="7550280"/>
           <a:ext cx="3457440" cy="1958760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4698,7 +4719,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="59334480" y="28175760"/>
+          <a:off x="59361120" y="28175760"/>
           <a:ext cx="8029080" cy="1330920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4715,8 +4736,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A3:C202" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A3:C202"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A3:C228" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A3:C228"/>
   <tableColumns count="3">
     <tableColumn id="1" name="ID"/>
     <tableColumn id="2" name="Group"/>
@@ -4838,15 +4859,15 @@
   </sheetPr>
   <dimension ref="A2:T232"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="20" zoomScaleNormal="20" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G112" activeCellId="0" sqref="G112"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A70" colorId="64" zoomScale="20" zoomScaleNormal="20" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K95" activeCellId="0" sqref="K95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8203125" defaultRowHeight="47.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="161.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="161.79"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="4" min="4" style="1" width="250.37"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="5" min="5" style="1" width="210.64"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="6" min="6" style="2" width="164.36"/>
@@ -8163,7 +8184,9 @@
       <c r="F95" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="G95" s="13"/>
+      <c r="G95" s="13" t="s">
+        <v>43</v>
+      </c>
       <c r="H95" s="3"/>
       <c r="I95" s="3"/>
       <c r="J95" s="3" t="s">
@@ -8199,7 +8222,9 @@
       <c r="F96" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="G96" s="13"/>
+      <c r="G96" s="13" t="s">
+        <v>43</v>
+      </c>
       <c r="H96" s="3"/>
       <c r="I96" s="3"/>
       <c r="J96" s="3" t="s">
@@ -8233,7 +8258,9 @@
       </c>
       <c r="E97" s="11"/>
       <c r="F97" s="15"/>
-      <c r="G97" s="13"/>
+      <c r="G97" s="13" t="s">
+        <v>360</v>
+      </c>
       <c r="H97" s="3"/>
       <c r="I97" s="3"/>
       <c r="J97" s="3"/>
@@ -8248,20 +8275,22 @@
     </row>
     <row r="98" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="8" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="B98" s="8" t="n">
         <v>11</v>
       </c>
       <c r="C98" s="9" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="D98" s="9"/>
       <c r="E98" s="11"/>
       <c r="F98" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="G98" s="13"/>
+      <c r="G98" s="13" t="s">
+        <v>43</v>
+      </c>
       <c r="H98" s="3"/>
       <c r="I98" s="3"/>
       <c r="J98" s="3" t="s">
@@ -8280,13 +8309,13 @@
     </row>
     <row r="99" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="8" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="B99" s="8" t="n">
         <v>11</v>
       </c>
       <c r="C99" s="9" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="D99" s="9" t="s">
         <v>305</v>
@@ -8294,12 +8323,12 @@
       <c r="E99" s="11"/>
       <c r="F99" s="15"/>
       <c r="G99" s="32" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="H99" s="3"/>
       <c r="I99" s="3"/>
       <c r="J99" s="3" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="K99" s="3"/>
       <c r="L99" s="30" t="s">
@@ -8314,21 +8343,21 @@
     </row>
     <row r="100" customFormat="false" ht="159.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="8" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="B100" s="8" t="n">
         <v>11</v>
       </c>
       <c r="C100" s="9" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="D100" s="9" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="E100" s="11"/>
       <c r="F100" s="15"/>
       <c r="G100" s="13" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="H100" s="3"/>
       <c r="I100" s="3"/>
@@ -8346,21 +8375,21 @@
     </row>
     <row r="101" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="8" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="B101" s="8" t="n">
         <v>11</v>
       </c>
       <c r="C101" s="9" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="D101" s="9" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="E101" s="11"/>
       <c r="F101" s="15"/>
       <c r="G101" s="13" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="H101" s="3"/>
       <c r="I101" s="3"/>
@@ -8381,21 +8410,21 @@
     </row>
     <row r="102" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="8" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="B102" s="8" t="n">
         <v>11</v>
       </c>
       <c r="C102" s="9" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="D102" s="9" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="E102" s="11"/>
       <c r="F102" s="15"/>
       <c r="G102" s="13" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="H102" s="3"/>
       <c r="I102" s="3"/>
@@ -8416,19 +8445,19 @@
     </row>
     <row r="103" customFormat="false" ht="120.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="8" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="B103" s="8" t="n">
         <v>11</v>
       </c>
       <c r="C103" s="9" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="D103" s="9"/>
       <c r="E103" s="11"/>
       <c r="F103" s="15"/>
       <c r="G103" s="32" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="H103" s="3"/>
       <c r="I103" s="3"/>
@@ -8438,7 +8467,7 @@
         <v>230</v>
       </c>
       <c r="M103" s="3" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="N103" s="3"/>
       <c r="O103" s="3"/>
@@ -8448,21 +8477,21 @@
     </row>
     <row r="104" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="8" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="B104" s="8" t="n">
         <v>11</v>
       </c>
       <c r="C104" s="9" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="D104" s="9" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="E104" s="11"/>
       <c r="F104" s="15"/>
       <c r="G104" s="13" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="H104" s="3"/>
       <c r="I104" s="3"/>
@@ -8483,21 +8512,21 @@
     </row>
     <row r="105" customFormat="false" ht="120.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="8" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="B105" s="8" t="n">
         <v>11</v>
       </c>
       <c r="C105" s="9" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="D105" s="9" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="E105" s="11"/>
       <c r="F105" s="15"/>
       <c r="G105" s="13" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="H105" s="3"/>
       <c r="I105" s="3"/>
@@ -8515,21 +8544,21 @@
     </row>
     <row r="106" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="8" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="B106" s="8" t="n">
         <v>11</v>
       </c>
       <c r="C106" s="9" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="D106" s="9" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="E106" s="11"/>
       <c r="F106" s="15"/>
       <c r="G106" s="32" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="H106" s="3"/>
       <c r="I106" s="3"/>
@@ -8550,21 +8579,21 @@
     </row>
     <row r="107" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="8" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="B107" s="8" t="n">
         <v>11</v>
       </c>
       <c r="C107" s="9" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="D107" s="9" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="E107" s="11"/>
       <c r="F107" s="15"/>
       <c r="G107" s="13" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="H107" s="3"/>
       <c r="I107" s="3"/>
@@ -8582,21 +8611,21 @@
     </row>
     <row r="108" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="8" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B108" s="8" t="n">
         <v>11</v>
       </c>
       <c r="C108" s="9" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="D108" s="9" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="E108" s="11"/>
       <c r="F108" s="15"/>
       <c r="G108" s="13" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="H108" s="3"/>
       <c r="I108" s="3"/>
@@ -8614,21 +8643,21 @@
     </row>
     <row r="109" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="8" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B109" s="8" t="n">
         <v>11</v>
       </c>
       <c r="C109" s="9" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="D109" s="9" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="E109" s="11"/>
       <c r="F109" s="15"/>
       <c r="G109" s="32" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="H109" s="3"/>
       <c r="I109" s="3"/>
@@ -8649,21 +8678,21 @@
     </row>
     <row r="110" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="8" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B110" s="8" t="n">
         <v>11</v>
       </c>
       <c r="C110" s="9" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="D110" s="9" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="E110" s="11"/>
       <c r="F110" s="15"/>
       <c r="G110" s="13" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="H110" s="3"/>
       <c r="I110" s="3"/>
@@ -8681,20 +8710,20 @@
     </row>
     <row r="111" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="8" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="B111" s="8" t="n">
         <v>24</v>
       </c>
       <c r="C111" s="9" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="D111" s="8" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="E111" s="11"/>
       <c r="F111" s="15" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="G111" s="13"/>
       <c r="H111" s="3"/>
@@ -8716,20 +8745,20 @@
     </row>
     <row r="112" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="8" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="B112" s="8" t="n">
         <v>24</v>
       </c>
       <c r="C112" s="9" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="D112" s="8" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="E112" s="11"/>
       <c r="F112" s="15" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="G112" s="13"/>
       <c r="H112" s="3"/>
@@ -8748,16 +8777,16 @@
     </row>
     <row r="113" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="8" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="B113" s="8" t="n">
         <v>24</v>
       </c>
       <c r="C113" s="9" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="D113" s="8" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="E113" s="11"/>
       <c r="F113" s="15" t="s">
@@ -8780,16 +8809,16 @@
     </row>
     <row r="114" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="8" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="B114" s="8" t="n">
         <v>24</v>
       </c>
       <c r="C114" s="9" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="D114" s="8" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="E114" s="11"/>
       <c r="F114" s="15" t="s">
@@ -8812,20 +8841,20 @@
     </row>
     <row r="115" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="8" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="B115" s="8" t="n">
         <v>24</v>
       </c>
       <c r="C115" s="9" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="D115" s="8" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="E115" s="11"/>
       <c r="F115" s="15" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="G115" s="13"/>
       <c r="H115" s="3"/>
@@ -8844,20 +8873,20 @@
     </row>
     <row r="116" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="8" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="B116" s="8" t="n">
         <v>24</v>
       </c>
       <c r="C116" s="9" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="D116" s="8" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="E116" s="11"/>
       <c r="F116" s="15" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="G116" s="13"/>
       <c r="H116" s="3"/>
@@ -8879,16 +8908,16 @@
     </row>
     <row r="117" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="8" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="B117" s="8" t="n">
         <v>24</v>
       </c>
       <c r="C117" s="9" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="D117" s="8" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="E117" s="11"/>
       <c r="F117" s="15" t="s">
@@ -8911,20 +8940,20 @@
     </row>
     <row r="118" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="8" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="B118" s="8" t="n">
         <v>24</v>
       </c>
       <c r="C118" s="9" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="D118" s="8" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="E118" s="11"/>
       <c r="F118" s="15" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="G118" s="13"/>
       <c r="H118" s="3"/>
@@ -8946,16 +8975,16 @@
     </row>
     <row r="119" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="8" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="B119" s="8" t="n">
         <v>24</v>
       </c>
       <c r="C119" s="9" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="D119" s="8" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="E119" s="11"/>
       <c r="F119" s="15" t="s">
@@ -8978,20 +9007,20 @@
     </row>
     <row r="120" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="8" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="B120" s="8" t="n">
         <v>24</v>
       </c>
       <c r="C120" s="9" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="D120" s="8" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="E120" s="11"/>
       <c r="F120" s="15" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="G120" s="13"/>
       <c r="H120" s="3"/>
@@ -9013,16 +9042,16 @@
     </row>
     <row r="121" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="8" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="B121" s="8" t="n">
         <v>24</v>
       </c>
       <c r="C121" s="9" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="D121" s="8" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="E121" s="11"/>
       <c r="F121" s="15" t="s">
@@ -9045,16 +9074,16 @@
     </row>
     <row r="122" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="8" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="B122" s="8" t="n">
         <v>24</v>
       </c>
       <c r="C122" s="9" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="D122" s="8" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="E122" s="11"/>
       <c r="F122" s="15" t="s">
@@ -9077,20 +9106,20 @@
     </row>
     <row r="123" customFormat="false" ht="120.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="8" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="B123" s="8" t="n">
         <v>24</v>
       </c>
       <c r="C123" s="9" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="D123" s="8" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="E123" s="11"/>
       <c r="F123" s="15" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="G123" s="13"/>
       <c r="H123" s="3"/>
@@ -9112,20 +9141,20 @@
     </row>
     <row r="124" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="8" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="B124" s="8" t="n">
         <v>24</v>
       </c>
       <c r="C124" s="9" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="D124" s="8" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="E124" s="11"/>
       <c r="F124" s="15" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="G124" s="13"/>
       <c r="H124" s="3"/>
@@ -9145,20 +9174,20 @@
     </row>
     <row r="125" customFormat="false" ht="159.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="8" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="B125" s="8" t="n">
         <v>24</v>
       </c>
       <c r="C125" s="9" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="D125" s="8" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="E125" s="11"/>
       <c r="F125" s="15" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="G125" s="13"/>
       <c r="H125" s="3"/>
@@ -9180,20 +9209,20 @@
     </row>
     <row r="126" customFormat="false" ht="120.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="8" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="B126" s="8" t="n">
         <v>24</v>
       </c>
       <c r="C126" s="9" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="D126" s="8" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="E126" s="11"/>
       <c r="F126" s="15" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="G126" s="13"/>
       <c r="H126" s="3"/>
@@ -9212,21 +9241,21 @@
     </row>
     <row r="127" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="8" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="B127" s="8" t="n">
         <v>9</v>
       </c>
       <c r="C127" s="19" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="D127" s="33" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="E127" s="11"/>
       <c r="F127" s="15"/>
       <c r="G127" s="13" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="H127" s="3"/>
       <c r="I127" s="3"/>
@@ -9247,19 +9276,19 @@
     </row>
     <row r="128" s="41" customFormat="true" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="34" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="B128" s="34" t="n">
         <v>9</v>
       </c>
       <c r="C128" s="35" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="D128" s="36" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="E128" s="37" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="F128" s="15"/>
       <c r="G128" s="38"/>
@@ -9282,21 +9311,21 @@
     </row>
     <row r="129" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="8" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="B129" s="8" t="n">
         <v>9</v>
       </c>
       <c r="C129" s="19" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="D129" s="33" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="E129" s="11"/>
       <c r="F129" s="15"/>
       <c r="G129" s="13" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="H129" s="39"/>
       <c r="I129" s="39"/>
@@ -9317,21 +9346,21 @@
     </row>
     <row r="130" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="8" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="B130" s="8" t="n">
         <v>9</v>
       </c>
       <c r="C130" s="16" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="D130" s="33" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="E130" s="11"/>
       <c r="F130" s="15"/>
       <c r="G130" s="38" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="H130" s="39"/>
       <c r="I130" s="39"/>
@@ -9352,19 +9381,19 @@
     </row>
     <row r="131" s="41" customFormat="true" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="34" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="B131" s="34" t="n">
         <v>9</v>
       </c>
       <c r="C131" s="42" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="D131" s="36" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="E131" s="37" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="F131" s="15"/>
       <c r="G131" s="13"/>
@@ -9387,21 +9416,21 @@
     </row>
     <row r="132" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="8" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="B132" s="8" t="n">
         <v>9</v>
       </c>
       <c r="C132" s="16" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="D132" s="33" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="E132" s="11"/>
       <c r="F132" s="15"/>
       <c r="G132" s="38" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="H132" s="39"/>
       <c r="I132" s="39"/>
@@ -9422,21 +9451,21 @@
     </row>
     <row r="133" customFormat="false" ht="174.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A133" s="8" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="B133" s="8" t="n">
         <v>9</v>
       </c>
       <c r="C133" s="16" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="D133" s="33" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="E133" s="11"/>
       <c r="F133" s="15"/>
       <c r="G133" s="13" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="H133" s="39"/>
       <c r="I133" s="39"/>
@@ -9457,21 +9486,21 @@
     </row>
     <row r="134" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="8" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="B134" s="8" t="n">
         <v>9</v>
       </c>
       <c r="C134" s="16" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="D134" s="33" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="E134" s="11"/>
       <c r="F134" s="15"/>
       <c r="G134" s="38" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="H134" s="39"/>
       <c r="I134" s="39"/>
@@ -9492,21 +9521,21 @@
     </row>
     <row r="135" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="8" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="B135" s="8" t="n">
         <v>9</v>
       </c>
       <c r="C135" s="16" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="D135" s="33" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="E135" s="11"/>
       <c r="F135" s="15"/>
       <c r="G135" s="13" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="H135" s="39"/>
       <c r="I135" s="39"/>
@@ -9527,21 +9556,21 @@
     </row>
     <row r="136" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="8" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="B136" s="8" t="n">
         <v>9</v>
       </c>
       <c r="C136" s="16" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="D136" s="33" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="E136" s="11"/>
       <c r="F136" s="15"/>
       <c r="G136" s="38" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="H136" s="3"/>
       <c r="I136" s="3"/>
@@ -9560,21 +9589,21 @@
     </row>
     <row r="137" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="8" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="B137" s="8" t="n">
         <v>9</v>
       </c>
       <c r="C137" s="16" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="D137" s="33" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="E137" s="11"/>
       <c r="F137" s="15"/>
       <c r="G137" s="13" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="H137" s="3"/>
       <c r="I137" s="3"/>
@@ -9593,21 +9622,21 @@
     </row>
     <row r="138" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="8" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="B138" s="8" t="n">
         <v>9</v>
       </c>
       <c r="C138" s="16" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="D138" s="33" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="E138" s="11"/>
       <c r="F138" s="15"/>
       <c r="G138" s="38" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="H138" s="3"/>
       <c r="I138" s="3"/>
@@ -9626,21 +9655,21 @@
     </row>
     <row r="139" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="8" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="B139" s="8" t="n">
         <v>9</v>
       </c>
       <c r="C139" s="16" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="D139" s="33" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="E139" s="11"/>
       <c r="F139" s="15"/>
       <c r="G139" s="13" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="H139" s="3"/>
       <c r="I139" s="3"/>
@@ -9659,21 +9688,21 @@
     </row>
     <row r="140" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="8" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="B140" s="8" t="n">
         <v>9</v>
       </c>
       <c r="C140" s="16" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="D140" s="33" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="E140" s="11"/>
       <c r="F140" s="15"/>
       <c r="G140" s="38" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="H140" s="3"/>
       <c r="I140" s="3"/>
@@ -9692,21 +9721,21 @@
     </row>
     <row r="141" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="8" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="B141" s="8" t="n">
         <v>9</v>
       </c>
       <c r="C141" s="16" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="D141" s="33" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="E141" s="11"/>
       <c r="F141" s="15"/>
       <c r="G141" s="13" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="H141" s="3"/>
       <c r="I141" s="3"/>
@@ -9725,21 +9754,21 @@
     </row>
     <row r="142" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="8" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="B142" s="8" t="n">
         <v>9</v>
       </c>
       <c r="C142" s="16" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="D142" s="33" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="E142" s="11"/>
       <c r="F142" s="15"/>
       <c r="G142" s="38" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="H142" s="3"/>
       <c r="I142" s="3"/>
@@ -9758,21 +9787,21 @@
     </row>
     <row r="143" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="8" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="B143" s="8" t="n">
         <v>9</v>
       </c>
       <c r="C143" s="16" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="D143" s="33" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="E143" s="11"/>
       <c r="F143" s="15"/>
       <c r="G143" s="13" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="H143" s="3"/>
       <c r="I143" s="3"/>
@@ -9791,19 +9820,19 @@
     </row>
     <row r="144" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="43" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="B144" s="43" t="n">
         <v>9</v>
       </c>
       <c r="C144" s="44" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="D144" s="45" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="E144" s="46" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="F144" s="15"/>
       <c r="G144" s="38"/>
@@ -9823,21 +9852,21 @@
     </row>
     <row r="145" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="8" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="B145" s="8" t="n">
         <v>9</v>
       </c>
       <c r="C145" s="16" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="D145" s="33" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="E145" s="11"/>
       <c r="F145" s="15"/>
       <c r="G145" s="13" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="H145" s="39"/>
       <c r="I145" s="39"/>
@@ -9860,21 +9889,21 @@
     </row>
     <row r="146" customFormat="false" ht="120.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="8" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="B146" s="8" t="n">
         <v>9</v>
       </c>
       <c r="C146" s="16" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="D146" s="33" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="E146" s="11"/>
       <c r="F146" s="15"/>
       <c r="G146" s="38" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="H146" s="39"/>
       <c r="I146" s="39"/>
@@ -9897,21 +9926,21 @@
     </row>
     <row r="147" customFormat="false" ht="120.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="8" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="B147" s="8" t="n">
         <v>9</v>
       </c>
       <c r="C147" s="16" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="D147" s="33" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="E147" s="11"/>
       <c r="F147" s="15"/>
       <c r="G147" s="13" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="H147" s="39"/>
       <c r="I147" s="39"/>
@@ -9932,21 +9961,21 @@
     </row>
     <row r="148" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="8" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="B148" s="8" t="n">
         <v>9</v>
       </c>
       <c r="C148" s="16" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="D148" s="33" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="E148" s="11"/>
       <c r="F148" s="15"/>
       <c r="G148" s="38" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="H148" s="39"/>
       <c r="I148" s="39"/>
@@ -9967,19 +9996,19 @@
     </row>
     <row r="149" s="41" customFormat="true" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="34" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B149" s="34" t="n">
         <v>9</v>
       </c>
       <c r="C149" s="42" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="D149" s="36" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="E149" s="37" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="F149" s="15"/>
       <c r="G149" s="13"/>
@@ -9999,21 +10028,21 @@
     </row>
     <row r="150" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="8" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="B150" s="8" t="n">
         <v>9</v>
       </c>
       <c r="C150" s="16" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="D150" s="33" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="E150" s="11"/>
       <c r="F150" s="15"/>
       <c r="G150" s="38" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="H150" s="39"/>
       <c r="I150" s="39"/>
@@ -10034,16 +10063,16 @@
     </row>
     <row r="151" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="8" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="B151" s="8" t="n">
         <v>22</v>
       </c>
       <c r="C151" s="16" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="D151" s="33" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="E151" s="11"/>
       <c r="F151" s="15"/>
@@ -10066,16 +10095,16 @@
     </row>
     <row r="152" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="8" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="B152" s="8" t="n">
         <v>22</v>
       </c>
       <c r="C152" s="16" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="D152" s="33" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="E152" s="11"/>
       <c r="F152" s="15"/>
@@ -10098,16 +10127,16 @@
     </row>
     <row r="153" customFormat="false" ht="120.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="8" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="B153" s="8" t="n">
         <v>22</v>
       </c>
       <c r="C153" s="16" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="D153" s="33" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="E153" s="11"/>
       <c r="F153" s="15" t="s">
@@ -10136,16 +10165,16 @@
     </row>
     <row r="154" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="8" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="B154" s="8" t="n">
         <v>22</v>
       </c>
       <c r="C154" s="16" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="D154" s="33" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="E154" s="11"/>
       <c r="F154" s="15" t="s">
@@ -10174,16 +10203,16 @@
     </row>
     <row r="155" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="8" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="B155" s="8" t="n">
         <v>22</v>
       </c>
       <c r="C155" s="16" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="D155" s="33" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="E155" s="11"/>
       <c r="F155" s="15" t="s">
@@ -10212,16 +10241,16 @@
     </row>
     <row r="156" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="8" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="B156" s="8" t="n">
         <v>22</v>
       </c>
       <c r="C156" s="16" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="D156" s="33" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="E156" s="11"/>
       <c r="F156" s="15" t="s">
@@ -10250,16 +10279,16 @@
     </row>
     <row r="157" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="8" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="B157" s="8" t="n">
         <v>22</v>
       </c>
       <c r="C157" s="16" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="D157" s="33" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="E157" s="11"/>
       <c r="F157" s="15" t="s">
@@ -10288,16 +10317,16 @@
     </row>
     <row r="158" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="8" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="B158" s="8" t="n">
         <v>22</v>
       </c>
       <c r="C158" s="16" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="D158" s="33" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="E158" s="11"/>
       <c r="F158" s="15" t="s">
@@ -10326,16 +10355,16 @@
     </row>
     <row r="159" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="8" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="B159" s="8" t="n">
         <v>22</v>
       </c>
       <c r="C159" s="16" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="D159" s="33" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="E159" s="11"/>
       <c r="F159" s="15" t="s">
@@ -10364,16 +10393,16 @@
     </row>
     <row r="160" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="8" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="B160" s="8" t="n">
         <v>22</v>
       </c>
       <c r="C160" s="16" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="D160" s="33" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="E160" s="11"/>
       <c r="F160" s="15" t="s">
@@ -10402,16 +10431,16 @@
     </row>
     <row r="161" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="8" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="B161" s="8" t="n">
         <v>22</v>
       </c>
       <c r="C161" s="16" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="D161" s="33" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="E161" s="11"/>
       <c r="F161" s="15" t="s">
@@ -10440,16 +10469,16 @@
     </row>
     <row r="162" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="8" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="B162" s="8" t="n">
         <v>22</v>
       </c>
       <c r="C162" s="16" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="D162" s="33" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="E162" s="11"/>
       <c r="F162" s="15" t="s">
@@ -10478,22 +10507,24 @@
     </row>
     <row r="163" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="8" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="B163" s="8" t="n">
         <v>16</v>
       </c>
       <c r="C163" s="9" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="D163" s="8" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="E163" s="11"/>
       <c r="F163" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="G163" s="38"/>
+      <c r="G163" s="38" t="s">
+        <v>43</v>
+      </c>
       <c r="H163" s="39"/>
       <c r="I163" s="39"/>
       <c r="J163" s="39" t="s">
@@ -10518,22 +10549,24 @@
     </row>
     <row r="164" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="8" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="B164" s="8" t="n">
         <v>16</v>
       </c>
       <c r="C164" s="9" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="D164" s="8" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="E164" s="47"/>
       <c r="F164" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="G164" s="38"/>
+      <c r="G164" s="38" t="s">
+        <v>43</v>
+      </c>
       <c r="H164" s="39"/>
       <c r="I164" s="39"/>
       <c r="J164" s="39" t="s">
@@ -10558,22 +10591,24 @@
     </row>
     <row r="165" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="8" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="B165" s="8" t="n">
         <v>16</v>
       </c>
       <c r="C165" s="9" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="D165" s="8" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="E165" s="47"/>
       <c r="F165" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="G165" s="38"/>
+      <c r="G165" s="38" t="s">
+        <v>43</v>
+      </c>
       <c r="H165" s="39"/>
       <c r="I165" s="39"/>
       <c r="J165" s="39" t="s">
@@ -10598,22 +10633,24 @@
     </row>
     <row r="166" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="8" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="B166" s="8" t="n">
         <v>16</v>
       </c>
       <c r="C166" s="9" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D166" s="8" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="E166" s="47"/>
       <c r="F166" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="G166" s="38"/>
+      <c r="G166" s="38" t="s">
+        <v>43</v>
+      </c>
       <c r="H166" s="39"/>
       <c r="I166" s="39"/>
       <c r="J166" s="39" t="s">
@@ -10638,22 +10675,24 @@
     </row>
     <row r="167" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="8" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="B167" s="8" t="n">
         <v>16</v>
       </c>
       <c r="C167" s="9" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="D167" s="8" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="E167" s="47"/>
       <c r="F167" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="G167" s="38"/>
+      <c r="G167" s="38" t="s">
+        <v>43</v>
+      </c>
       <c r="H167" s="39"/>
       <c r="I167" s="39"/>
       <c r="J167" s="39" t="s">
@@ -10678,22 +10717,24 @@
     </row>
     <row r="168" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="8" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="B168" s="8" t="n">
         <v>16</v>
       </c>
       <c r="C168" s="9" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="D168" s="8" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="E168" s="47"/>
       <c r="F168" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="G168" s="38"/>
+      <c r="G168" s="38" t="s">
+        <v>43</v>
+      </c>
       <c r="H168" s="39"/>
       <c r="I168" s="39"/>
       <c r="J168" s="39" t="s">
@@ -10716,22 +10757,24 @@
     </row>
     <row r="169" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="8" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="B169" s="8" t="n">
         <v>16</v>
       </c>
       <c r="C169" s="9" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="D169" s="8" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="E169" s="47"/>
       <c r="F169" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="G169" s="38"/>
+      <c r="G169" s="38" t="s">
+        <v>43</v>
+      </c>
       <c r="H169" s="39"/>
       <c r="I169" s="39"/>
       <c r="J169" s="39" t="s">
@@ -10754,22 +10797,24 @@
     </row>
     <row r="170" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="8" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="B170" s="8" t="n">
         <v>16</v>
       </c>
       <c r="C170" s="9" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="D170" s="8" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="E170" s="47"/>
       <c r="F170" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="G170" s="38"/>
+      <c r="G170" s="38" t="s">
+        <v>43</v>
+      </c>
       <c r="H170" s="39"/>
       <c r="I170" s="39"/>
       <c r="J170" s="39" t="s">
@@ -10792,20 +10837,22 @@
     </row>
     <row r="171" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="8" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="B171" s="8" t="n">
         <v>16</v>
       </c>
       <c r="C171" s="9" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="D171" s="8" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="E171" s="47"/>
       <c r="F171" s="48"/>
-      <c r="G171" s="38"/>
+      <c r="G171" s="38" t="s">
+        <v>43</v>
+      </c>
       <c r="H171" s="39"/>
       <c r="I171" s="39"/>
       <c r="J171" s="39" t="s">
@@ -10826,22 +10873,24 @@
     </row>
     <row r="172" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="8" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="B172" s="8" t="n">
         <v>16</v>
       </c>
       <c r="C172" s="9" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="D172" s="8" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="E172" s="47"/>
       <c r="F172" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="G172" s="38"/>
+      <c r="G172" s="38" t="s">
+        <v>43</v>
+      </c>
       <c r="H172" s="39"/>
       <c r="I172" s="39"/>
       <c r="J172" s="39" t="s">
@@ -10864,22 +10913,24 @@
     </row>
     <row r="173" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="8" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="B173" s="8" t="n">
         <v>16</v>
       </c>
       <c r="C173" s="9" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="D173" s="8" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="E173" s="47"/>
       <c r="F173" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="G173" s="38"/>
+      <c r="G173" s="38" t="s">
+        <v>43</v>
+      </c>
       <c r="H173" s="39"/>
       <c r="I173" s="39"/>
       <c r="J173" s="39" t="s">
@@ -10902,22 +10953,24 @@
     </row>
     <row r="174" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="8" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="B174" s="8" t="n">
         <v>16</v>
       </c>
       <c r="C174" s="9" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="D174" s="8" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="E174" s="47"/>
       <c r="F174" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="G174" s="38"/>
+      <c r="G174" s="38" t="s">
+        <v>43</v>
+      </c>
       <c r="H174" s="39"/>
       <c r="I174" s="39"/>
       <c r="J174" s="39" t="s">
@@ -10942,22 +10995,24 @@
     </row>
     <row r="175" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="8" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="B175" s="8" t="n">
         <v>16</v>
       </c>
       <c r="C175" s="49" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="D175" s="8" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="E175" s="47"/>
       <c r="F175" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="G175" s="38"/>
+      <c r="G175" s="38" t="s">
+        <v>43</v>
+      </c>
       <c r="H175" s="39"/>
       <c r="I175" s="39"/>
       <c r="J175" s="39" t="s">
@@ -10982,22 +11037,24 @@
     </row>
     <row r="176" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="8" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="B176" s="8" t="n">
         <v>16</v>
       </c>
       <c r="C176" s="49" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="D176" s="8" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="E176" s="47"/>
       <c r="F176" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="G176" s="38"/>
+      <c r="G176" s="38" t="s">
+        <v>43</v>
+      </c>
       <c r="H176" s="39"/>
       <c r="I176" s="39"/>
       <c r="J176" s="39" t="s">
@@ -11022,22 +11079,24 @@
     </row>
     <row r="177" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="8" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="B177" s="8" t="n">
         <v>16</v>
       </c>
       <c r="C177" s="49" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="D177" s="8" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="E177" s="47"/>
       <c r="F177" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="G177" s="38"/>
+      <c r="G177" s="38" t="s">
+        <v>43</v>
+      </c>
       <c r="H177" s="39"/>
       <c r="I177" s="39"/>
       <c r="J177" s="39" t="s">
@@ -11062,22 +11121,24 @@
     </row>
     <row r="178" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="8" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="B178" s="8" t="n">
         <v>16</v>
       </c>
       <c r="C178" s="9" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="D178" s="8" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="E178" s="47"/>
       <c r="F178" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="G178" s="38"/>
+      <c r="G178" s="38" t="s">
+        <v>43</v>
+      </c>
       <c r="H178" s="39"/>
       <c r="I178" s="39"/>
       <c r="J178" s="39" t="s">
@@ -11102,22 +11163,24 @@
     </row>
     <row r="179" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="8" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="B179" s="8" t="n">
         <v>16</v>
       </c>
       <c r="C179" s="18" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="D179" s="8" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="E179" s="47"/>
       <c r="F179" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="G179" s="38"/>
+      <c r="G179" s="38" t="s">
+        <v>43</v>
+      </c>
       <c r="H179" s="39"/>
       <c r="I179" s="39"/>
       <c r="J179" s="39" t="s">
@@ -11142,22 +11205,24 @@
     </row>
     <row r="180" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="8" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="B180" s="8" t="n">
         <v>16</v>
       </c>
       <c r="C180" s="9" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="D180" s="8" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="E180" s="47"/>
       <c r="F180" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="G180" s="38"/>
+      <c r="G180" s="38" t="s">
+        <v>43</v>
+      </c>
       <c r="H180" s="39"/>
       <c r="I180" s="39"/>
       <c r="J180" s="39" t="s">
@@ -11182,22 +11247,24 @@
     </row>
     <row r="181" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="8" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="B181" s="8" t="n">
         <v>16</v>
       </c>
       <c r="C181" s="9" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="D181" s="8" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="E181" s="47"/>
       <c r="F181" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="G181" s="38"/>
+      <c r="G181" s="38" t="s">
+        <v>43</v>
+      </c>
       <c r="H181" s="39"/>
       <c r="I181" s="39"/>
       <c r="J181" s="39" t="s">
@@ -11222,22 +11289,24 @@
     </row>
     <row r="182" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="8" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="B182" s="8" t="n">
         <v>16</v>
       </c>
       <c r="C182" s="9" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="D182" s="8" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="E182" s="47"/>
       <c r="F182" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="G182" s="38"/>
+      <c r="G182" s="38" t="s">
+        <v>43</v>
+      </c>
       <c r="H182" s="39"/>
       <c r="I182" s="39"/>
       <c r="J182" s="39" t="s">
@@ -11262,22 +11331,24 @@
     </row>
     <row r="183" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="8" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="B183" s="8" t="n">
         <v>16</v>
       </c>
       <c r="C183" s="9" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="D183" s="8" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="E183" s="47"/>
       <c r="F183" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="G183" s="38"/>
+      <c r="G183" s="38" t="s">
+        <v>43</v>
+      </c>
       <c r="H183" s="39"/>
       <c r="I183" s="39"/>
       <c r="J183" s="39" t="s">
@@ -11302,22 +11373,24 @@
     </row>
     <row r="184" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="8" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="B184" s="8" t="n">
         <v>16</v>
       </c>
       <c r="C184" s="9" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="D184" s="8" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="E184" s="47"/>
       <c r="F184" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="G184" s="38"/>
+      <c r="G184" s="38" t="s">
+        <v>43</v>
+      </c>
       <c r="H184" s="39"/>
       <c r="I184" s="39"/>
       <c r="J184" s="39" t="s">
@@ -11342,16 +11415,16 @@
     </row>
     <row r="185" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="8" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="B185" s="8" t="n">
         <v>15</v>
       </c>
       <c r="C185" s="9" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="D185" s="50" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="E185" s="47"/>
       <c r="F185" s="15" t="s">
@@ -11380,16 +11453,16 @@
     </row>
     <row r="186" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="8" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="B186" s="8" t="n">
         <v>15</v>
       </c>
       <c r="C186" s="9" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="D186" s="50" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="E186" s="47"/>
       <c r="F186" s="48" t="s">
@@ -11418,16 +11491,16 @@
     </row>
     <row r="187" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="8" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="B187" s="8" t="n">
         <v>15</v>
       </c>
       <c r="C187" s="9" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="D187" s="50" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="E187" s="47"/>
       <c r="F187" s="48" t="s">
@@ -11456,16 +11529,16 @@
     </row>
     <row r="188" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="8" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="B188" s="8" t="n">
         <v>15</v>
       </c>
       <c r="C188" s="9" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="D188" s="50" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="E188" s="47"/>
       <c r="F188" s="48" t="s">
@@ -11494,16 +11567,16 @@
     </row>
     <row r="189" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="8" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="B189" s="8" t="n">
         <v>15</v>
       </c>
       <c r="C189" s="9" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="D189" s="50" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="E189" s="47"/>
       <c r="F189" s="48" t="s">
@@ -11532,16 +11605,16 @@
     </row>
     <row r="190" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="8" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="B190" s="8" t="n">
         <v>15</v>
       </c>
       <c r="C190" s="9" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="D190" s="50" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="E190" s="47"/>
       <c r="F190" s="48" t="s">
@@ -11570,16 +11643,16 @@
     </row>
     <row r="191" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="8" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="B191" s="8" t="n">
         <v>15</v>
       </c>
       <c r="C191" s="9" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="D191" s="50" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="E191" s="47"/>
       <c r="F191" s="48" t="s">
@@ -11608,16 +11681,16 @@
     </row>
     <row r="192" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="8" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="B192" s="8" t="n">
         <v>15</v>
       </c>
       <c r="C192" s="9" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="D192" s="50" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
       <c r="E192" s="47"/>
       <c r="F192" s="48" t="s">
@@ -11646,16 +11719,16 @@
     </row>
     <row r="193" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="8" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="B193" s="8" t="n">
         <v>15</v>
       </c>
       <c r="C193" s="9" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="D193" s="50" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="E193" s="47"/>
       <c r="F193" s="48" t="s">
@@ -11684,16 +11757,16 @@
     </row>
     <row r="194" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="8" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="B194" s="8" t="n">
         <v>15</v>
       </c>
       <c r="C194" s="9" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="D194" s="50" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="E194" s="47"/>
       <c r="F194" s="48" t="s">
@@ -11722,16 +11795,16 @@
     </row>
     <row r="195" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="8" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="B195" s="8" t="n">
         <v>15</v>
       </c>
       <c r="C195" s="9" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="D195" s="50" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
       <c r="E195" s="47"/>
       <c r="F195" s="48" t="s">
@@ -11760,16 +11833,16 @@
     </row>
     <row r="196" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="8" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="B196" s="8" t="n">
         <v>15</v>
       </c>
       <c r="C196" s="9" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="D196" s="50" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
       <c r="E196" s="47"/>
       <c r="F196" s="48" t="s">
@@ -11798,16 +11871,16 @@
     </row>
     <row r="197" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="8" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="B197" s="8" t="n">
         <v>15</v>
       </c>
       <c r="C197" s="9" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="D197" s="50" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="E197" s="47"/>
       <c r="F197" s="48" t="s">
@@ -11836,16 +11909,16 @@
     </row>
     <row r="198" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="8" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="B198" s="8" t="n">
         <v>15</v>
       </c>
       <c r="C198" s="9" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="D198" s="50" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="E198" s="47"/>
       <c r="F198" s="48" t="s">
@@ -11874,16 +11947,16 @@
     </row>
     <row r="199" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="8" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
       <c r="B199" s="8" t="n">
         <v>15</v>
       </c>
       <c r="C199" s="9" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
       <c r="D199" s="50" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="E199" s="47"/>
       <c r="F199" s="48" t="s">
@@ -11912,16 +11985,16 @@
     </row>
     <row r="200" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="8" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
       <c r="B200" s="8" t="n">
         <v>15</v>
       </c>
       <c r="C200" s="9" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="D200" s="50" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c r="E200" s="47"/>
       <c r="F200" s="48" t="s">
@@ -11950,16 +12023,16 @@
     </row>
     <row r="201" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="8" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
       <c r="B201" s="8" t="n">
         <v>15</v>
       </c>
       <c r="C201" s="9" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="D201" s="50" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="E201" s="47"/>
       <c r="F201" s="48" t="s">
@@ -11988,16 +12061,16 @@
     </row>
     <row r="202" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="8" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
       <c r="B202" s="8" t="n">
         <v>15</v>
       </c>
       <c r="C202" s="9" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="D202" s="50" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
       <c r="E202" s="47"/>
       <c r="F202" s="48" t="s">
@@ -12026,16 +12099,16 @@
     </row>
     <row r="203" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="8" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="B203" s="8" t="n">
         <v>15</v>
       </c>
       <c r="C203" s="9" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="D203" s="8" t="s">
-        <v>687</v>
+        <v>688</v>
       </c>
       <c r="E203" s="47"/>
       <c r="F203" s="48" t="s">
@@ -12064,27 +12137,29 @@
     </row>
     <row r="204" customFormat="false" ht="350.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A204" s="8" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="B204" s="3" t="n">
         <v>12</v>
       </c>
       <c r="C204" s="4" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
       <c r="D204" s="3" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="E204" s="5" t="e">
         <f aca="false">#VALUE!</f>
         <v>#VALUE!</v>
       </c>
       <c r="F204" s="51"/>
-      <c r="G204" s="38"/>
+      <c r="G204" s="38" t="s">
+        <v>692</v>
+      </c>
       <c r="H204" s="39"/>
       <c r="I204" s="39"/>
       <c r="J204" s="39" t="s">
-        <v>691</v>
+        <v>693</v>
       </c>
       <c r="K204" s="39"/>
       <c r="L204" s="3"/>
@@ -12099,16 +12174,16 @@
     </row>
     <row r="205" customFormat="false" ht="300" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A205" s="8" t="s">
-        <v>692</v>
+        <v>694</v>
       </c>
       <c r="B205" s="3" t="n">
         <v>12</v>
       </c>
       <c r="C205" s="4" t="s">
-        <v>693</v>
+        <v>695</v>
       </c>
       <c r="D205" s="3" t="s">
-        <v>694</v>
+        <v>696</v>
       </c>
       <c r="E205" s="5" t="e">
         <f aca="false">#VALUE!</f>
@@ -12117,7 +12192,9 @@
       <c r="F205" s="51" t="s">
         <v>43</v>
       </c>
-      <c r="G205" s="38"/>
+      <c r="G205" s="38" t="s">
+        <v>43</v>
+      </c>
       <c r="H205" s="39"/>
       <c r="I205" s="39"/>
       <c r="J205" s="39" t="s">
@@ -12140,16 +12217,16 @@
     </row>
     <row r="206" customFormat="false" ht="300" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A206" s="8" t="s">
-        <v>695</v>
+        <v>697</v>
       </c>
       <c r="B206" s="3" t="n">
         <v>12</v>
       </c>
       <c r="C206" s="4" t="s">
+        <v>698</v>
+      </c>
+      <c r="D206" s="3" t="s">
         <v>696</v>
-      </c>
-      <c r="D206" s="3" t="s">
-        <v>694</v>
       </c>
       <c r="E206" s="5" t="e">
         <f aca="false">#VALUE!</f>
@@ -12158,7 +12235,9 @@
       <c r="F206" s="51" t="s">
         <v>43</v>
       </c>
-      <c r="G206" s="38"/>
+      <c r="G206" s="38" t="s">
+        <v>43</v>
+      </c>
       <c r="H206" s="39"/>
       <c r="I206" s="39"/>
       <c r="J206" s="39" t="s">
@@ -12181,27 +12260,29 @@
     </row>
     <row r="207" customFormat="false" ht="300" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A207" s="8" t="s">
-        <v>697</v>
+        <v>699</v>
       </c>
       <c r="B207" s="3" t="n">
         <v>12</v>
       </c>
       <c r="C207" s="4" t="s">
-        <v>698</v>
+        <v>700</v>
       </c>
       <c r="D207" s="3" t="s">
-        <v>694</v>
+        <v>696</v>
       </c>
       <c r="E207" s="5" t="e">
         <f aca="false">#VALUE!</f>
         <v>#VALUE!</v>
       </c>
       <c r="F207" s="51"/>
-      <c r="G207" s="38"/>
+      <c r="G207" s="38" t="s">
+        <v>43</v>
+      </c>
       <c r="H207" s="39"/>
       <c r="I207" s="39"/>
       <c r="J207" s="39" t="s">
-        <v>699</v>
+        <v>701</v>
       </c>
       <c r="K207" s="39"/>
       <c r="L207" s="3"/>
@@ -12216,16 +12297,16 @@
     </row>
     <row r="208" customFormat="false" ht="300" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A208" s="8" t="s">
-        <v>700</v>
+        <v>702</v>
       </c>
       <c r="B208" s="3" t="n">
         <v>12</v>
       </c>
       <c r="C208" s="4" t="s">
-        <v>701</v>
+        <v>703</v>
       </c>
       <c r="D208" s="3" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="E208" s="5" t="e">
         <f aca="false">#VALUE!</f>
@@ -12234,7 +12315,9 @@
       <c r="F208" s="51" t="s">
         <v>43</v>
       </c>
-      <c r="G208" s="38"/>
+      <c r="G208" s="38" t="s">
+        <v>43</v>
+      </c>
       <c r="H208" s="39"/>
       <c r="I208" s="39"/>
       <c r="J208" s="39" t="s">
@@ -12257,27 +12340,29 @@
     </row>
     <row r="209" customFormat="false" ht="300" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A209" s="8" t="s">
-        <v>702</v>
+        <v>704</v>
       </c>
       <c r="B209" s="3" t="n">
         <v>12</v>
       </c>
       <c r="C209" s="4" t="s">
-        <v>703</v>
+        <v>705</v>
       </c>
       <c r="D209" s="3" t="s">
-        <v>694</v>
+        <v>696</v>
       </c>
       <c r="E209" s="5" t="e">
         <f aca="false">#VALUE!</f>
         <v>#VALUE!</v>
       </c>
       <c r="F209" s="51"/>
-      <c r="G209" s="38"/>
+      <c r="G209" s="38" t="s">
+        <v>706</v>
+      </c>
       <c r="H209" s="39"/>
       <c r="I209" s="39"/>
       <c r="J209" s="39" t="s">
-        <v>704</v>
+        <v>707</v>
       </c>
       <c r="K209" s="39"/>
       <c r="L209" s="3"/>
@@ -12285,7 +12370,7 @@
       <c r="N209" s="3"/>
       <c r="O209" s="39"/>
       <c r="P209" s="39" t="s">
-        <v>705</v>
+        <v>708</v>
       </c>
       <c r="Q209" s="39"/>
       <c r="R209" s="39"/>
@@ -12294,27 +12379,29 @@
     </row>
     <row r="210" customFormat="false" ht="399.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A210" s="8" t="s">
-        <v>706</v>
+        <v>709</v>
       </c>
       <c r="B210" s="3" t="n">
         <v>12</v>
       </c>
       <c r="C210" s="4" t="s">
-        <v>707</v>
+        <v>710</v>
       </c>
       <c r="D210" s="3" t="s">
-        <v>694</v>
+        <v>696</v>
       </c>
       <c r="E210" s="5" t="e">
         <f aca="false">#VALUE!</f>
         <v>#VALUE!</v>
       </c>
       <c r="F210" s="51"/>
-      <c r="G210" s="13"/>
+      <c r="G210" s="38" t="s">
+        <v>711</v>
+      </c>
       <c r="H210" s="3"/>
       <c r="I210" s="3"/>
       <c r="J210" s="39" t="s">
-        <v>704</v>
+        <v>707</v>
       </c>
       <c r="K210" s="3"/>
       <c r="L210" s="3"/>
@@ -12322,34 +12409,36 @@
       <c r="N210" s="3"/>
       <c r="O210" s="3"/>
       <c r="P210" s="3" t="s">
-        <v>708</v>
+        <v>712</v>
       </c>
       <c r="Q210" s="3"/>
       <c r="R210" s="3"/>
     </row>
     <row r="211" customFormat="false" ht="300" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A211" s="8" t="s">
-        <v>709</v>
+        <v>713</v>
       </c>
       <c r="B211" s="3" t="n">
         <v>12</v>
       </c>
       <c r="C211" s="4" t="s">
-        <v>710</v>
+        <v>714</v>
       </c>
       <c r="D211" s="3" t="s">
-        <v>694</v>
+        <v>696</v>
       </c>
       <c r="E211" s="5" t="e">
         <f aca="false">#VALUE!</f>
         <v>#VALUE!</v>
       </c>
       <c r="F211" s="51"/>
-      <c r="G211" s="13"/>
+      <c r="G211" s="38" t="s">
+        <v>715</v>
+      </c>
       <c r="H211" s="3"/>
       <c r="I211" s="3"/>
       <c r="J211" s="39" t="s">
-        <v>704</v>
+        <v>707</v>
       </c>
       <c r="K211" s="3"/>
       <c r="L211" s="3"/>
@@ -12362,27 +12451,29 @@
     </row>
     <row r="212" customFormat="false" ht="300" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A212" s="8" t="s">
-        <v>711</v>
+        <v>716</v>
       </c>
       <c r="B212" s="3" t="n">
         <v>12</v>
       </c>
       <c r="C212" s="4" t="s">
-        <v>712</v>
+        <v>717</v>
       </c>
       <c r="D212" s="3" t="s">
-        <v>694</v>
+        <v>696</v>
       </c>
       <c r="E212" s="5" t="e">
         <f aca="false">#VALUE!</f>
         <v>#VALUE!</v>
       </c>
       <c r="F212" s="51"/>
-      <c r="G212" s="13"/>
+      <c r="G212" s="38" t="s">
+        <v>718</v>
+      </c>
       <c r="H212" s="3"/>
       <c r="I212" s="3"/>
       <c r="J212" s="39" t="s">
-        <v>704</v>
+        <v>707</v>
       </c>
       <c r="K212" s="3"/>
       <c r="L212" s="3"/>
@@ -12395,27 +12486,29 @@
     </row>
     <row r="213" customFormat="false" ht="150" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A213" s="8" t="s">
-        <v>713</v>
+        <v>719</v>
       </c>
       <c r="B213" s="3" t="n">
         <v>12</v>
       </c>
       <c r="C213" s="4" t="s">
-        <v>714</v>
+        <v>720</v>
       </c>
       <c r="D213" s="3" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="E213" s="5" t="e">
         <f aca="false">#VALUE!</f>
         <v>#VALUE!</v>
       </c>
       <c r="F213" s="51"/>
-      <c r="G213" s="13"/>
+      <c r="G213" s="38" t="s">
+        <v>721</v>
+      </c>
       <c r="H213" s="3"/>
       <c r="I213" s="3"/>
       <c r="J213" s="39" t="s">
-        <v>704</v>
+        <v>707</v>
       </c>
       <c r="K213" s="3"/>
       <c r="L213" s="3"/>
@@ -12428,16 +12521,16 @@
     </row>
     <row r="214" customFormat="false" ht="98.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="3" t="s">
-        <v>715</v>
+        <v>722</v>
       </c>
       <c r="B214" s="3" t="n">
         <v>23</v>
       </c>
       <c r="C214" s="4" t="s">
-        <v>716</v>
+        <v>723</v>
       </c>
       <c r="D214" s="3" t="s">
-        <v>717</v>
+        <v>724</v>
       </c>
       <c r="E214" s="5"/>
       <c r="F214" s="51"/>
@@ -12458,16 +12551,16 @@
     </row>
     <row r="215" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="3" t="s">
-        <v>718</v>
+        <v>725</v>
       </c>
       <c r="B215" s="3" t="n">
         <v>23</v>
       </c>
       <c r="C215" s="4" t="s">
-        <v>719</v>
+        <v>726</v>
       </c>
       <c r="D215" s="3" t="s">
-        <v>720</v>
+        <v>727</v>
       </c>
       <c r="E215" s="5"/>
       <c r="F215" s="51"/>
@@ -12488,16 +12581,16 @@
     </row>
     <row r="216" customFormat="false" ht="49.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="3" t="s">
-        <v>721</v>
+        <v>728</v>
       </c>
       <c r="B216" s="3" t="n">
         <v>23</v>
       </c>
       <c r="C216" s="4" t="s">
-        <v>722</v>
+        <v>729</v>
       </c>
       <c r="D216" s="3" t="s">
-        <v>720</v>
+        <v>727</v>
       </c>
       <c r="E216" s="5"/>
       <c r="F216" s="51"/>
@@ -12505,7 +12598,7 @@
       <c r="H216" s="3"/>
       <c r="I216" s="3"/>
       <c r="J216" s="3" t="s">
-        <v>723</v>
+        <v>730</v>
       </c>
       <c r="K216" s="3"/>
       <c r="L216" s="3"/>
@@ -12518,16 +12611,16 @@
     </row>
     <row r="217" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="3" t="s">
-        <v>724</v>
+        <v>731</v>
       </c>
       <c r="B217" s="3" t="n">
         <v>23</v>
       </c>
       <c r="C217" s="4" t="s">
-        <v>725</v>
+        <v>732</v>
       </c>
       <c r="D217" s="3" t="s">
-        <v>720</v>
+        <v>727</v>
       </c>
       <c r="E217" s="5"/>
       <c r="F217" s="51"/>
@@ -12535,7 +12628,7 @@
       <c r="H217" s="3"/>
       <c r="I217" s="3"/>
       <c r="J217" s="3" t="s">
-        <v>726</v>
+        <v>733</v>
       </c>
       <c r="K217" s="3"/>
       <c r="L217" s="3"/>
@@ -12548,13 +12641,13 @@
     </row>
     <row r="218" customFormat="false" ht="98.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="3" t="s">
-        <v>727</v>
+        <v>734</v>
       </c>
       <c r="B218" s="3" t="n">
         <v>23</v>
       </c>
       <c r="C218" s="4" t="s">
-        <v>728</v>
+        <v>735</v>
       </c>
       <c r="D218" s="3"/>
       <c r="E218" s="5"/>
@@ -12563,7 +12656,7 @@
       <c r="H218" s="3"/>
       <c r="I218" s="3"/>
       <c r="J218" s="3" t="s">
-        <v>723</v>
+        <v>730</v>
       </c>
       <c r="K218" s="3"/>
       <c r="L218" s="3"/>
@@ -12576,13 +12669,13 @@
     </row>
     <row r="219" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="3" t="s">
-        <v>729</v>
+        <v>736</v>
       </c>
       <c r="B219" s="3" t="n">
         <v>23</v>
       </c>
       <c r="C219" s="4" t="s">
-        <v>730</v>
+        <v>737</v>
       </c>
       <c r="D219" s="3"/>
       <c r="E219" s="5"/>
@@ -12591,7 +12684,7 @@
       <c r="H219" s="3"/>
       <c r="I219" s="3"/>
       <c r="J219" s="3" t="s">
-        <v>723</v>
+        <v>730</v>
       </c>
       <c r="K219" s="3"/>
       <c r="L219" s="3"/>
@@ -12604,16 +12697,16 @@
     </row>
     <row r="220" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="3" t="s">
-        <v>731</v>
+        <v>738</v>
       </c>
       <c r="B220" s="3" t="n">
         <v>23</v>
       </c>
       <c r="C220" s="4" t="s">
-        <v>732</v>
+        <v>739</v>
       </c>
       <c r="D220" s="3" t="s">
-        <v>733</v>
+        <v>740</v>
       </c>
       <c r="E220" s="5"/>
       <c r="F220" s="51"/>
@@ -12621,7 +12714,7 @@
       <c r="H220" s="3"/>
       <c r="I220" s="3"/>
       <c r="J220" s="3" t="s">
-        <v>723</v>
+        <v>730</v>
       </c>
       <c r="K220" s="3"/>
       <c r="L220" s="3"/>
@@ -12634,16 +12727,16 @@
     </row>
     <row r="221" customFormat="false" ht="98.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="3" t="s">
-        <v>734</v>
+        <v>741</v>
       </c>
       <c r="B221" s="3" t="n">
         <v>23</v>
       </c>
       <c r="C221" s="4" t="s">
-        <v>735</v>
+        <v>742</v>
       </c>
       <c r="D221" s="3" t="s">
-        <v>736</v>
+        <v>743</v>
       </c>
       <c r="E221" s="5"/>
       <c r="F221" s="51"/>
@@ -12651,7 +12744,7 @@
       <c r="H221" s="3"/>
       <c r="I221" s="3"/>
       <c r="J221" s="3" t="s">
-        <v>723</v>
+        <v>730</v>
       </c>
       <c r="K221" s="3"/>
       <c r="L221" s="3"/>
@@ -12664,16 +12757,16 @@
     </row>
     <row r="222" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="3" t="s">
-        <v>737</v>
+        <v>744</v>
       </c>
       <c r="B222" s="3" t="n">
         <v>23</v>
       </c>
       <c r="C222" s="4" t="s">
-        <v>738</v>
+        <v>745</v>
       </c>
       <c r="D222" s="3" t="s">
-        <v>739</v>
+        <v>746</v>
       </c>
       <c r="E222" s="5"/>
       <c r="F222" s="51"/>
@@ -12681,7 +12774,7 @@
       <c r="H222" s="3"/>
       <c r="I222" s="3"/>
       <c r="J222" s="3" t="s">
-        <v>723</v>
+        <v>730</v>
       </c>
       <c r="K222" s="3"/>
       <c r="L222" s="3"/>
@@ -12694,26 +12787,26 @@
     </row>
     <row r="223" customFormat="false" ht="98.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="3" t="s">
-        <v>740</v>
+        <v>747</v>
       </c>
       <c r="B223" s="3" t="n">
         <v>23</v>
       </c>
       <c r="C223" s="4" t="s">
-        <v>741</v>
+        <v>748</v>
       </c>
       <c r="D223" s="3" t="s">
-        <v>742</v>
+        <v>749</v>
       </c>
       <c r="E223" s="5"/>
       <c r="F223" s="51"/>
       <c r="G223" s="13" t="s">
-        <v>743</v>
+        <v>750</v>
       </c>
       <c r="H223" s="3"/>
       <c r="I223" s="3"/>
       <c r="J223" s="3" t="s">
-        <v>723</v>
+        <v>730</v>
       </c>
       <c r="K223" s="3"/>
       <c r="L223" s="3"/>
@@ -12726,26 +12819,26 @@
     </row>
     <row r="224" customFormat="false" ht="49.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="3" t="s">
-        <v>744</v>
+        <v>751</v>
       </c>
       <c r="B224" s="3" t="n">
         <v>23</v>
       </c>
       <c r="C224" s="4" t="s">
-        <v>745</v>
+        <v>752</v>
       </c>
       <c r="D224" s="3" t="s">
-        <v>746</v>
+        <v>753</v>
       </c>
       <c r="E224" s="5"/>
       <c r="F224" s="51" t="s">
-        <v>747</v>
+        <v>754</v>
       </c>
       <c r="G224" s="13"/>
       <c r="H224" s="3"/>
       <c r="I224" s="3"/>
       <c r="J224" s="3" t="s">
-        <v>723</v>
+        <v>730</v>
       </c>
       <c r="K224" s="3"/>
       <c r="L224" s="3"/>
@@ -12758,26 +12851,26 @@
     </row>
     <row r="225" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="3" t="s">
-        <v>748</v>
+        <v>755</v>
       </c>
       <c r="B225" s="3" t="n">
         <v>23</v>
       </c>
       <c r="C225" s="4" t="s">
-        <v>749</v>
+        <v>756</v>
       </c>
       <c r="D225" s="3" t="s">
-        <v>750</v>
+        <v>757</v>
       </c>
       <c r="E225" s="5"/>
       <c r="F225" s="51" t="s">
-        <v>751</v>
+        <v>758</v>
       </c>
       <c r="G225" s="13"/>
       <c r="H225" s="3"/>
       <c r="I225" s="3"/>
       <c r="J225" s="3" t="s">
-        <v>752</v>
+        <v>759</v>
       </c>
       <c r="K225" s="3"/>
       <c r="L225" s="3"/>
@@ -12790,26 +12883,26 @@
     </row>
     <row r="226" customFormat="false" ht="98.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="3" t="s">
-        <v>753</v>
+        <v>760</v>
       </c>
       <c r="B226" s="3" t="n">
         <v>23</v>
       </c>
       <c r="C226" s="4" t="s">
-        <v>754</v>
+        <v>761</v>
       </c>
       <c r="D226" s="3" t="s">
-        <v>755</v>
+        <v>762</v>
       </c>
       <c r="E226" s="5"/>
       <c r="F226" s="51" t="s">
-        <v>756</v>
+        <v>763</v>
       </c>
       <c r="G226" s="13"/>
       <c r="H226" s="3"/>
       <c r="I226" s="3"/>
       <c r="J226" s="3" t="s">
-        <v>757</v>
+        <v>764</v>
       </c>
       <c r="K226" s="3"/>
       <c r="L226" s="3"/>
@@ -12822,26 +12915,26 @@
     </row>
     <row r="227" customFormat="false" ht="98.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="3" t="s">
-        <v>758</v>
+        <v>765</v>
       </c>
       <c r="B227" s="3" t="n">
         <v>23</v>
       </c>
       <c r="C227" s="4" t="s">
-        <v>759</v>
+        <v>766</v>
       </c>
       <c r="D227" s="3" t="s">
-        <v>760</v>
+        <v>767</v>
       </c>
       <c r="E227" s="5"/>
       <c r="F227" s="52" t="s">
-        <v>761</v>
+        <v>768</v>
       </c>
       <c r="G227" s="13"/>
       <c r="H227" s="3"/>
       <c r="I227" s="3"/>
       <c r="J227" s="3" t="s">
-        <v>757</v>
+        <v>764</v>
       </c>
       <c r="K227" s="3"/>
       <c r="L227" s="3"/>
@@ -12854,26 +12947,26 @@
     </row>
     <row r="228" customFormat="false" ht="98.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="3" t="s">
-        <v>762</v>
+        <v>769</v>
       </c>
       <c r="B228" s="3" t="n">
         <v>23</v>
       </c>
       <c r="C228" s="4" t="s">
-        <v>763</v>
+        <v>770</v>
       </c>
       <c r="D228" s="3" t="s">
-        <v>746</v>
+        <v>753</v>
       </c>
       <c r="E228" s="5"/>
       <c r="F228" s="53" t="s">
-        <v>747</v>
+        <v>754</v>
       </c>
       <c r="G228" s="13"/>
       <c r="H228" s="3"/>
       <c r="I228" s="3"/>
       <c r="J228" s="3" t="s">
-        <v>764</v>
+        <v>771</v>
       </c>
       <c r="K228" s="3"/>
       <c r="L228" s="3"/>

</xml_diff>

<commit_message>
updated FinalRequirements for group 13
</commit_message>
<xml_diff>
--- a/FinalRequirements.xlsx
+++ b/FinalRequirements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28816"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mavsuta-my.sharepoint.com/personal/mxn0591_mavs_uta_edu/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aadar\cse3310-sp25-003\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B0BDCD45-D981-4D39-8B9D-A874967DAC8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEDC84E6-4CBB-4C7B-8DE4-471B7A2BC0A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -91,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1232" uniqueCount="699">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1252" uniqueCount="719">
   <si>
     <t>Testing</t>
   </si>
@@ -2343,12 +2343,72 @@
   <si>
     <t>cannot join game, therefore cannot test it</t>
   </si>
+  <si>
+    <t>R226</t>
+  </si>
+  <si>
+    <t>The system must parse JSON data received from the Login Page and use it to star the user sessions.</t>
+  </si>
+  <si>
+    <t>R227</t>
+  </si>
+  <si>
+    <t>The system must receive and process game status from the Game Manager to update the frontend.</t>
+  </si>
+  <si>
+    <t>R228</t>
+  </si>
+  <si>
+    <t>The system must process user input from the Join Game Page to begin the pairing.</t>
+  </si>
+  <si>
+    <t>R229</t>
+  </si>
+  <si>
+    <t>The system must forward input from the Join Game Page to the Pair Up system to initiate game setup.</t>
+  </si>
+  <si>
+    <t>R230</t>
+  </si>
+  <si>
+    <t>The system must request and receive user profile data (including UserID, Wins, and Losses) from the database as a JSON object.</t>
+  </si>
+  <si>
+    <t>R231</t>
+  </si>
+  <si>
+    <t>The system must receive game move data from the Game Manager in object format for client-side.</t>
+  </si>
+  <si>
+    <t>R232</t>
+  </si>
+  <si>
+    <t>The system must receive and handle object data for the leaderboard from the database and render it to the UI.</t>
+  </si>
+  <si>
+    <t>R233</t>
+  </si>
+  <si>
+    <t>Page will transition between pages (Login, Join Game, Game View, Leaderboard) based on websocket events and internal state.</t>
+  </si>
+  <si>
+    <t>R234</t>
+  </si>
+  <si>
+    <t>All user interface updates will be handled in JavaScript/HTML/CSS and game logic on the java server side.</t>
+  </si>
+  <si>
+    <t>R235</t>
+  </si>
+  <si>
+    <t>Websockets will be used for communication between the Java backend, Database and JavaScript frontend.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2444,7 +2504,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -2560,11 +2620,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -2684,6 +2757,11 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4460,43 +4538,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:T228"/>
+  <dimension ref="A2:T240"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E209" zoomScale="21" zoomScaleNormal="28" workbookViewId="0">
-      <selection activeCell="J1660" sqref="J1660"/>
+    <sheetView tabSelected="1" topLeftCell="A221" zoomScale="21" zoomScaleNormal="28" workbookViewId="0">
+      <selection activeCell="E235" sqref="E235"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="46.5"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="47.4" x14ac:dyDescent="0.9"/>
   <cols>
     <col min="1" max="1" width="21" style="1" customWidth="1"/>
-    <col min="2" max="2" width="19.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="161.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="250.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="210.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="164.28515625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="104.28515625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="34.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="30.140625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="165.28515625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="34.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="161.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="250.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="210.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="164.33203125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="104.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="34.6640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="30.109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="165.33203125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="34.109375" style="1" customWidth="1"/>
     <col min="12" max="12" width="131" style="1" customWidth="1"/>
     <col min="13" max="13" width="33" style="1" customWidth="1"/>
-    <col min="14" max="14" width="46.42578125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="46.44140625" style="1" customWidth="1"/>
     <col min="15" max="15" width="33" style="1" customWidth="1"/>
     <col min="16" max="16" width="133" style="1" customWidth="1"/>
     <col min="17" max="17" width="158" style="1" customWidth="1"/>
-    <col min="18" max="18" width="40.140625" style="1" customWidth="1"/>
-    <col min="19" max="19" width="8.7109375" style="1"/>
-    <col min="20" max="20" width="153.140625" style="1" customWidth="1"/>
-    <col min="21" max="16384" width="8.7109375" style="1"/>
+    <col min="18" max="18" width="40.109375" style="1" customWidth="1"/>
+    <col min="19" max="19" width="8.6640625" style="1"/>
+    <col min="20" max="20" width="153.109375" style="1" customWidth="1"/>
+    <col min="21" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.9">
       <c r="L2" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.9">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -4552,7 +4630,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="139.5">
+    <row r="4" spans="1:20" ht="142.19999999999999" x14ac:dyDescent="0.9">
       <c r="A4" s="8" t="s">
         <v>19</v>
       </c>
@@ -4594,7 +4672,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="291" customHeight="1">
+    <row r="5" spans="1:20" ht="291" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A5" s="8" t="s">
         <v>25</v>
       </c>
@@ -4628,7 +4706,7 @@
       <c r="Q5" s="3"/>
       <c r="R5" s="3"/>
     </row>
-    <row r="6" spans="1:20" ht="285.75" customHeight="1">
+    <row r="6" spans="1:20" ht="285.75" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A6" s="8" t="s">
         <v>28</v>
       </c>
@@ -4662,7 +4740,7 @@
       <c r="Q6" s="3"/>
       <c r="R6" s="3"/>
     </row>
-    <row r="7" spans="1:20" ht="287.25" customHeight="1">
+    <row r="7" spans="1:20" ht="287.25" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A7" s="8" t="s">
         <v>31</v>
       </c>
@@ -4696,7 +4774,7 @@
       <c r="Q7" s="3"/>
       <c r="R7" s="3"/>
     </row>
-    <row r="8" spans="1:20" ht="329.25" customHeight="1">
+    <row r="8" spans="1:20" ht="329.25" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A8" s="8" t="s">
         <v>34</v>
       </c>
@@ -4730,7 +4808,7 @@
       <c r="Q8" s="3"/>
       <c r="R8" s="3"/>
     </row>
-    <row r="9" spans="1:20" ht="138">
+    <row r="9" spans="1:20" ht="139.80000000000001" x14ac:dyDescent="0.9">
       <c r="A9" s="8" t="s">
         <v>37</v>
       </c>
@@ -4766,7 +4844,7 @@
       <c r="Q9" s="3"/>
       <c r="R9" s="3"/>
     </row>
-    <row r="10" spans="1:20" ht="318" customHeight="1">
+    <row r="10" spans="1:20" ht="318" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A10" s="8" t="s">
         <v>40</v>
       </c>
@@ -4803,7 +4881,7 @@
       <c r="Q10" s="3"/>
       <c r="R10" s="3"/>
     </row>
-    <row r="11" spans="1:20" ht="318" customHeight="1">
+    <row r="11" spans="1:20" ht="318" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A11" s="8" t="s">
         <v>44</v>
       </c>
@@ -4842,7 +4920,7 @@
       <c r="Q11" s="3"/>
       <c r="R11" s="3"/>
     </row>
-    <row r="12" spans="1:20" ht="334.5" customHeight="1">
+    <row r="12" spans="1:20" ht="334.5" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A12" s="8" t="s">
         <v>50</v>
       </c>
@@ -4880,7 +4958,7 @@
       <c r="Q12" s="3"/>
       <c r="R12" s="3"/>
     </row>
-    <row r="13" spans="1:20" ht="313.5" customHeight="1">
+    <row r="13" spans="1:20" ht="313.5" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A13" s="8" t="s">
         <v>55</v>
       </c>
@@ -4917,7 +4995,7 @@
       <c r="Q13" s="3"/>
       <c r="R13" s="3"/>
     </row>
-    <row r="14" spans="1:20" ht="249.75" customHeight="1">
+    <row r="14" spans="1:20" ht="249.75" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A14" s="8" t="s">
         <v>60</v>
       </c>
@@ -4954,7 +5032,7 @@
       <c r="Q14" s="3"/>
       <c r="R14" s="3"/>
     </row>
-    <row r="15" spans="1:20" ht="399.75" customHeight="1">
+    <row r="15" spans="1:20" ht="399.75" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A15" s="8" t="s">
         <v>65</v>
       </c>
@@ -4993,7 +5071,7 @@
       <c r="Q15" s="3"/>
       <c r="R15" s="3"/>
     </row>
-    <row r="16" spans="1:20" ht="183.75">
+    <row r="16" spans="1:20" ht="186" x14ac:dyDescent="0.9">
       <c r="A16" s="8" t="s">
         <v>71</v>
       </c>
@@ -5027,7 +5105,7 @@
       <c r="Q16" s="3"/>
       <c r="R16" s="3"/>
     </row>
-    <row r="17" spans="1:18" ht="249.75" customHeight="1">
+    <row r="17" spans="1:18" ht="249.75" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A17" s="8" t="s">
         <v>76</v>
       </c>
@@ -5062,7 +5140,7 @@
       <c r="Q17" s="3"/>
       <c r="R17" s="3"/>
     </row>
-    <row r="18" spans="1:18" ht="249.75" customHeight="1">
+    <row r="18" spans="1:18" ht="249.75" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A18" s="8" t="s">
         <v>81</v>
       </c>
@@ -5095,7 +5173,7 @@
       <c r="Q18" s="3"/>
       <c r="R18" s="3"/>
     </row>
-    <row r="19" spans="1:18" ht="92.25">
+    <row r="19" spans="1:18" ht="93.6" x14ac:dyDescent="0.9">
       <c r="A19" s="8" t="s">
         <v>84</v>
       </c>
@@ -5127,7 +5205,7 @@
       <c r="Q19" s="3"/>
       <c r="R19" s="3"/>
     </row>
-    <row r="20" spans="1:18" ht="249.75" customHeight="1">
+    <row r="20" spans="1:18" ht="249.75" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A20" s="8" t="s">
         <v>87</v>
       </c>
@@ -5162,7 +5240,7 @@
       <c r="Q20" s="3"/>
       <c r="R20" s="3"/>
     </row>
-    <row r="21" spans="1:18" ht="199.5" customHeight="1">
+    <row r="21" spans="1:18" ht="199.5" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A21" s="8" t="s">
         <v>91</v>
       </c>
@@ -5197,7 +5275,7 @@
       <c r="Q21" s="3"/>
       <c r="R21" s="3"/>
     </row>
-    <row r="22" spans="1:18" ht="349.5" customHeight="1">
+    <row r="22" spans="1:18" ht="349.5" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A22" s="8" t="s">
         <v>95</v>
       </c>
@@ -5230,7 +5308,7 @@
       <c r="Q22" s="3"/>
       <c r="R22" s="3"/>
     </row>
-    <row r="23" spans="1:18" ht="300" customHeight="1">
+    <row r="23" spans="1:18" ht="300" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A23" s="8" t="s">
         <v>98</v>
       </c>
@@ -5263,7 +5341,7 @@
       <c r="Q23" s="3"/>
       <c r="R23" s="3"/>
     </row>
-    <row r="24" spans="1:18" ht="349.5" customHeight="1">
+    <row r="24" spans="1:18" ht="349.5" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A24" s="8" t="s">
         <v>101</v>
       </c>
@@ -5296,7 +5374,7 @@
       <c r="Q24" s="3"/>
       <c r="R24" s="3"/>
     </row>
-    <row r="25" spans="1:18" ht="349.5" customHeight="1">
+    <row r="25" spans="1:18" ht="349.5" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A25" s="8" t="s">
         <v>104</v>
       </c>
@@ -5329,7 +5407,7 @@
       <c r="Q25" s="3"/>
       <c r="R25" s="3"/>
     </row>
-    <row r="26" spans="1:18" ht="349.5" customHeight="1">
+    <row r="26" spans="1:18" ht="349.5" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A26" s="8" t="s">
         <v>107</v>
       </c>
@@ -5362,7 +5440,7 @@
       <c r="Q26" s="3"/>
       <c r="R26" s="3"/>
     </row>
-    <row r="27" spans="1:18" ht="399.75" customHeight="1">
+    <row r="27" spans="1:18" ht="399.75" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A27" s="8" t="s">
         <v>110</v>
       </c>
@@ -5395,7 +5473,7 @@
       <c r="Q27" s="3"/>
       <c r="R27" s="3"/>
     </row>
-    <row r="28" spans="1:18" ht="300" customHeight="1">
+    <row r="28" spans="1:18" ht="300" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A28" s="10" t="s">
         <v>113</v>
       </c>
@@ -5428,7 +5506,7 @@
       <c r="Q28" s="3"/>
       <c r="R28" s="3"/>
     </row>
-    <row r="29" spans="1:18" ht="94.5" customHeight="1">
+    <row r="29" spans="1:18" ht="94.5" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A29" s="10" t="s">
         <v>116</v>
       </c>
@@ -5467,7 +5545,7 @@
       </c>
       <c r="R29" s="3"/>
     </row>
-    <row r="30" spans="1:18" ht="349.5" customHeight="1">
+    <row r="30" spans="1:18" ht="349.5" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A30" s="10" t="s">
         <v>119</v>
       </c>
@@ -5504,7 +5582,7 @@
       </c>
       <c r="R30" s="3"/>
     </row>
-    <row r="31" spans="1:18" ht="349.5" customHeight="1">
+    <row r="31" spans="1:18" ht="349.5" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A31" s="8" t="s">
         <v>122</v>
       </c>
@@ -5541,7 +5619,7 @@
       </c>
       <c r="R31" s="3"/>
     </row>
-    <row r="32" spans="1:18" ht="92.25">
+    <row r="32" spans="1:18" ht="93.6" x14ac:dyDescent="0.9">
       <c r="A32" s="8" t="s">
         <v>125</v>
       </c>
@@ -5579,7 +5657,7 @@
       </c>
       <c r="R32" s="3"/>
     </row>
-    <row r="33" spans="1:18" ht="138">
+    <row r="33" spans="1:18" ht="139.80000000000001" x14ac:dyDescent="0.9">
       <c r="A33" s="8" t="s">
         <v>128</v>
       </c>
@@ -5617,7 +5695,7 @@
       </c>
       <c r="R33" s="3"/>
     </row>
-    <row r="34" spans="1:18" ht="92.25" customHeight="1">
+    <row r="34" spans="1:18" ht="92.25" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A34" s="8" t="s">
         <v>131</v>
       </c>
@@ -5655,7 +5733,7 @@
       </c>
       <c r="R34" s="3"/>
     </row>
-    <row r="35" spans="1:18" ht="99" customHeight="1">
+    <row r="35" spans="1:18" ht="99" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A35" s="8" t="s">
         <v>134</v>
       </c>
@@ -5693,7 +5771,7 @@
       </c>
       <c r="R35" s="3"/>
     </row>
-    <row r="36" spans="1:18" ht="93">
+    <row r="36" spans="1:18" ht="94.8" x14ac:dyDescent="0.9">
       <c r="A36" s="8" t="s">
         <v>136</v>
       </c>
@@ -5727,7 +5805,7 @@
       </c>
       <c r="R36" s="3"/>
     </row>
-    <row r="37" spans="1:18" ht="138">
+    <row r="37" spans="1:18" ht="139.80000000000001" x14ac:dyDescent="0.9">
       <c r="A37" s="8" t="s">
         <v>139</v>
       </c>
@@ -5761,7 +5839,7 @@
       </c>
       <c r="R37" s="3"/>
     </row>
-    <row r="38" spans="1:18" ht="138">
+    <row r="38" spans="1:18" ht="139.80000000000001" x14ac:dyDescent="0.9">
       <c r="A38" s="8" t="s">
         <v>141</v>
       </c>
@@ -5795,7 +5873,7 @@
       </c>
       <c r="R38" s="3"/>
     </row>
-    <row r="39" spans="1:18" ht="138">
+    <row r="39" spans="1:18" ht="139.80000000000001" x14ac:dyDescent="0.9">
       <c r="A39" s="8" t="s">
         <v>144</v>
       </c>
@@ -5829,7 +5907,7 @@
       </c>
       <c r="R39" s="3"/>
     </row>
-    <row r="40" spans="1:18" ht="93">
+    <row r="40" spans="1:18" ht="94.8" x14ac:dyDescent="0.9">
       <c r="A40" s="8" t="s">
         <v>147</v>
       </c>
@@ -5867,7 +5945,7 @@
       </c>
       <c r="R40" s="3"/>
     </row>
-    <row r="41" spans="1:18" ht="93">
+    <row r="41" spans="1:18" ht="94.8" x14ac:dyDescent="0.9">
       <c r="A41" s="8" t="s">
         <v>150</v>
       </c>
@@ -5905,7 +5983,7 @@
       </c>
       <c r="R41" s="3"/>
     </row>
-    <row r="42" spans="1:18" ht="138">
+    <row r="42" spans="1:18" ht="139.80000000000001" x14ac:dyDescent="0.9">
       <c r="A42" s="8" t="s">
         <v>153</v>
       </c>
@@ -5943,7 +6021,7 @@
       </c>
       <c r="R42" s="3"/>
     </row>
-    <row r="43" spans="1:18" ht="93">
+    <row r="43" spans="1:18" ht="94.8" x14ac:dyDescent="0.9">
       <c r="A43" s="8" t="s">
         <v>156</v>
       </c>
@@ -5977,7 +6055,7 @@
       </c>
       <c r="R43" s="3"/>
     </row>
-    <row r="44" spans="1:18" ht="93">
+    <row r="44" spans="1:18" ht="94.8" x14ac:dyDescent="0.9">
       <c r="A44" s="8" t="s">
         <v>159</v>
       </c>
@@ -6011,7 +6089,7 @@
       </c>
       <c r="R44" s="3"/>
     </row>
-    <row r="45" spans="1:18" ht="93">
+    <row r="45" spans="1:18" ht="94.8" x14ac:dyDescent="0.9">
       <c r="A45" s="8" t="s">
         <v>161</v>
       </c>
@@ -6045,7 +6123,7 @@
       </c>
       <c r="R45" s="3"/>
     </row>
-    <row r="46" spans="1:18" ht="93">
+    <row r="46" spans="1:18" ht="94.8" x14ac:dyDescent="0.9">
       <c r="A46" s="8" t="s">
         <v>164</v>
       </c>
@@ -6079,7 +6157,7 @@
       </c>
       <c r="R46" s="3"/>
     </row>
-    <row r="47" spans="1:18" ht="138">
+    <row r="47" spans="1:18" ht="139.80000000000001" x14ac:dyDescent="0.9">
       <c r="A47" s="8" t="s">
         <v>166</v>
       </c>
@@ -6113,7 +6191,7 @@
       </c>
       <c r="R47" s="3"/>
     </row>
-    <row r="48" spans="1:18" ht="93">
+    <row r="48" spans="1:18" ht="94.8" x14ac:dyDescent="0.9">
       <c r="A48" s="8" t="s">
         <v>168</v>
       </c>
@@ -6147,7 +6225,7 @@
       </c>
       <c r="R48" s="3"/>
     </row>
-    <row r="49" spans="1:18" ht="92.25">
+    <row r="49" spans="1:18" ht="93.6" x14ac:dyDescent="0.9">
       <c r="A49" s="8" t="s">
         <v>170</v>
       </c>
@@ -6185,7 +6263,7 @@
       </c>
       <c r="R49" s="3"/>
     </row>
-    <row r="50" spans="1:18" ht="183.75">
+    <row r="50" spans="1:18" ht="186" x14ac:dyDescent="0.9">
       <c r="A50" s="8" t="s">
         <v>172</v>
       </c>
@@ -6223,7 +6301,7 @@
       </c>
       <c r="R50" s="3"/>
     </row>
-    <row r="51" spans="1:18" ht="234.75" customHeight="1">
+    <row r="51" spans="1:18" ht="234.75" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A51" s="8" t="s">
         <v>174</v>
       </c>
@@ -6255,7 +6333,7 @@
       <c r="Q51" s="3"/>
       <c r="R51" s="3"/>
     </row>
-    <row r="52" spans="1:18" ht="92.25">
+    <row r="52" spans="1:18" ht="93.6" x14ac:dyDescent="0.9">
       <c r="A52" s="8" t="s">
         <v>178</v>
       </c>
@@ -6289,7 +6367,7 @@
       </c>
       <c r="R52" s="3"/>
     </row>
-    <row r="53" spans="1:18" ht="92.25">
+    <row r="53" spans="1:18" ht="93.6" x14ac:dyDescent="0.9">
       <c r="A53" s="23" t="s">
         <v>180</v>
       </c>
@@ -6319,7 +6397,7 @@
       <c r="Q53" s="3"/>
       <c r="R53" s="3"/>
     </row>
-    <row r="54" spans="1:18" ht="92.25">
+    <row r="54" spans="1:18" ht="93.6" x14ac:dyDescent="0.9">
       <c r="A54" s="23" t="s">
         <v>183</v>
       </c>
@@ -6349,7 +6427,7 @@
       <c r="Q54" s="3"/>
       <c r="R54" s="3"/>
     </row>
-    <row r="55" spans="1:18" ht="275.25">
+    <row r="55" spans="1:18" ht="278.39999999999998" x14ac:dyDescent="0.9">
       <c r="A55" s="8" t="s">
         <v>186</v>
       </c>
@@ -6382,7 +6460,7 @@
       <c r="Q55" s="3"/>
       <c r="R55" s="3"/>
     </row>
-    <row r="56" spans="1:18">
+    <row r="56" spans="1:18" x14ac:dyDescent="0.9">
       <c r="A56" s="23" t="s">
         <v>190</v>
       </c>
@@ -6416,7 +6494,7 @@
       </c>
       <c r="R56" s="3"/>
     </row>
-    <row r="57" spans="1:18" ht="275.25">
+    <row r="57" spans="1:18" ht="278.39999999999998" x14ac:dyDescent="0.9">
       <c r="A57" s="8" t="s">
         <v>193</v>
       </c>
@@ -6449,7 +6527,7 @@
       <c r="Q57" s="3"/>
       <c r="R57" s="3"/>
     </row>
-    <row r="58" spans="1:18">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.9">
       <c r="A58" s="8" t="s">
         <v>197</v>
       </c>
@@ -6483,7 +6561,7 @@
       </c>
       <c r="R58" s="3"/>
     </row>
-    <row r="59" spans="1:18" ht="275.25">
+    <row r="59" spans="1:18" ht="278.39999999999998" x14ac:dyDescent="0.9">
       <c r="A59" s="8" t="s">
         <v>200</v>
       </c>
@@ -6516,7 +6594,7 @@
       <c r="Q59" s="3"/>
       <c r="R59" s="3"/>
     </row>
-    <row r="60" spans="1:18" ht="408.75" customHeight="1">
+    <row r="60" spans="1:18" ht="408.75" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A60" s="8" t="s">
         <v>203</v>
       </c>
@@ -6548,7 +6626,7 @@
       <c r="Q60" s="3"/>
       <c r="R60" s="3"/>
     </row>
-    <row r="61" spans="1:18" ht="92.25">
+    <row r="61" spans="1:18" ht="93.6" x14ac:dyDescent="0.9">
       <c r="A61" s="23" t="s">
         <v>208</v>
       </c>
@@ -6582,7 +6660,7 @@
       </c>
       <c r="R61" s="3"/>
     </row>
-    <row r="62" spans="1:18" ht="408.75" customHeight="1">
+    <row r="62" spans="1:18" ht="408.75" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A62" s="8" t="s">
         <v>210</v>
       </c>
@@ -6614,7 +6692,7 @@
       <c r="Q62" s="3"/>
       <c r="R62" s="3"/>
     </row>
-    <row r="63" spans="1:18">
+    <row r="63" spans="1:18" x14ac:dyDescent="0.9">
       <c r="A63" s="23" t="s">
         <v>214</v>
       </c>
@@ -6644,7 +6722,7 @@
       <c r="Q63" s="3"/>
       <c r="R63" s="3"/>
     </row>
-    <row r="64" spans="1:18" ht="92.25">
+    <row r="64" spans="1:18" ht="93.6" x14ac:dyDescent="0.9">
       <c r="A64" s="23" t="s">
         <v>216</v>
       </c>
@@ -6674,7 +6752,7 @@
       <c r="Q64" s="3"/>
       <c r="R64" s="3"/>
     </row>
-    <row r="65" spans="1:18" ht="92.25">
+    <row r="65" spans="1:18" ht="93.6" x14ac:dyDescent="0.9">
       <c r="A65" s="8" t="s">
         <v>219</v>
       </c>
@@ -6708,7 +6786,7 @@
       </c>
       <c r="R65" s="3"/>
     </row>
-    <row r="66" spans="1:18">
+    <row r="66" spans="1:18" x14ac:dyDescent="0.9">
       <c r="A66" s="8" t="s">
         <v>222</v>
       </c>
@@ -6742,7 +6820,7 @@
       </c>
       <c r="R66" s="3"/>
     </row>
-    <row r="67" spans="1:18" ht="91.5">
+    <row r="67" spans="1:18" ht="92.4" x14ac:dyDescent="0.9">
       <c r="A67" s="8" t="s">
         <v>225</v>
       </c>
@@ -6775,7 +6853,7 @@
       <c r="Q67" s="3"/>
       <c r="R67" s="3"/>
     </row>
-    <row r="68" spans="1:18" ht="91.5">
+    <row r="68" spans="1:18" ht="92.4" x14ac:dyDescent="0.9">
       <c r="A68" s="8" t="s">
         <v>227</v>
       </c>
@@ -6808,7 +6886,7 @@
       <c r="Q68" s="3"/>
       <c r="R68" s="3"/>
     </row>
-    <row r="69" spans="1:18" ht="92.25">
+    <row r="69" spans="1:18" ht="93.6" x14ac:dyDescent="0.9">
       <c r="A69" s="8" t="s">
         <v>230</v>
       </c>
@@ -6841,7 +6919,7 @@
       <c r="Q69" s="3"/>
       <c r="R69" s="3"/>
     </row>
-    <row r="70" spans="1:18" ht="92.25">
+    <row r="70" spans="1:18" ht="93.6" x14ac:dyDescent="0.9">
       <c r="A70" s="8" t="s">
         <v>233</v>
       </c>
@@ -6873,7 +6951,7 @@
       <c r="Q70" s="3"/>
       <c r="R70" s="3"/>
     </row>
-    <row r="71" spans="1:18" ht="92.25">
+    <row r="71" spans="1:18" ht="93.6" x14ac:dyDescent="0.9">
       <c r="A71" s="8" t="s">
         <v>237</v>
       </c>
@@ -6905,7 +6983,7 @@
       <c r="Q71" s="3"/>
       <c r="R71" s="3"/>
     </row>
-    <row r="72" spans="1:18" ht="92.25">
+    <row r="72" spans="1:18" ht="93.6" x14ac:dyDescent="0.9">
       <c r="A72" s="8" t="s">
         <v>241</v>
       </c>
@@ -6937,7 +7015,7 @@
       <c r="Q72" s="3"/>
       <c r="R72" s="3"/>
     </row>
-    <row r="73" spans="1:18" ht="92.25">
+    <row r="73" spans="1:18" ht="93.6" x14ac:dyDescent="0.9">
       <c r="A73" s="8" t="s">
         <v>244</v>
       </c>
@@ -6968,7 +7046,7 @@
       <c r="Q73" s="3"/>
       <c r="R73" s="3"/>
     </row>
-    <row r="74" spans="1:18" ht="138">
+    <row r="74" spans="1:18" ht="139.80000000000001" x14ac:dyDescent="0.9">
       <c r="A74" s="8" t="s">
         <v>246</v>
       </c>
@@ -6996,7 +7074,7 @@
       <c r="Q74" s="3"/>
       <c r="R74" s="3"/>
     </row>
-    <row r="75" spans="1:18" ht="92.25">
+    <row r="75" spans="1:18" ht="93.6" x14ac:dyDescent="0.9">
       <c r="A75" s="8" t="s">
         <v>248</v>
       </c>
@@ -7026,7 +7104,7 @@
       <c r="Q75" s="3"/>
       <c r="R75" s="3"/>
     </row>
-    <row r="76" spans="1:18" ht="92.25">
+    <row r="76" spans="1:18" ht="93.6" x14ac:dyDescent="0.9">
       <c r="A76" s="8" t="s">
         <v>251</v>
       </c>
@@ -7058,7 +7136,7 @@
       <c r="Q76" s="3"/>
       <c r="R76" s="3"/>
     </row>
-    <row r="77" spans="1:18" ht="92.25">
+    <row r="77" spans="1:18" ht="93.6" x14ac:dyDescent="0.9">
       <c r="A77" s="8" t="s">
         <v>255</v>
       </c>
@@ -7090,7 +7168,7 @@
       <c r="Q77" s="3"/>
       <c r="R77" s="3"/>
     </row>
-    <row r="78" spans="1:18" ht="92.25">
+    <row r="78" spans="1:18" ht="93.6" x14ac:dyDescent="0.9">
       <c r="A78" s="8" t="s">
         <v>258</v>
       </c>
@@ -7120,7 +7198,7 @@
       <c r="Q78" s="3"/>
       <c r="R78" s="3"/>
     </row>
-    <row r="79" spans="1:18" ht="92.25">
+    <row r="79" spans="1:18" ht="93.6" x14ac:dyDescent="0.9">
       <c r="A79" s="8" t="s">
         <v>260</v>
       </c>
@@ -7152,7 +7230,7 @@
       <c r="Q79" s="3"/>
       <c r="R79" s="3"/>
     </row>
-    <row r="80" spans="1:18" ht="92.25">
+    <row r="80" spans="1:18" ht="93.6" x14ac:dyDescent="0.9">
       <c r="A80" s="8" t="s">
         <v>263</v>
       </c>
@@ -7184,7 +7262,7 @@
       <c r="Q80" s="3"/>
       <c r="R80" s="3"/>
     </row>
-    <row r="81" spans="1:18" ht="92.25">
+    <row r="81" spans="1:18" ht="93.6" x14ac:dyDescent="0.9">
       <c r="A81" s="8" t="s">
         <v>266</v>
       </c>
@@ -7216,7 +7294,7 @@
       <c r="Q81" s="3"/>
       <c r="R81" s="3"/>
     </row>
-    <row r="82" spans="1:18">
+    <row r="82" spans="1:18" x14ac:dyDescent="0.9">
       <c r="A82" s="8" t="s">
         <v>270</v>
       </c>
@@ -7248,7 +7326,7 @@
       <c r="Q82" s="3"/>
       <c r="R82" s="3"/>
     </row>
-    <row r="83" spans="1:18" ht="92.25">
+    <row r="83" spans="1:18" ht="93.6" x14ac:dyDescent="0.9">
       <c r="A83" s="8" t="s">
         <v>273</v>
       </c>
@@ -7280,7 +7358,7 @@
       <c r="Q83" s="3"/>
       <c r="R83" s="3"/>
     </row>
-    <row r="84" spans="1:18" ht="92.25">
+    <row r="84" spans="1:18" ht="93.6" x14ac:dyDescent="0.9">
       <c r="A84" s="8" t="s">
         <v>275</v>
       </c>
@@ -7312,7 +7390,7 @@
       <c r="Q84" s="3"/>
       <c r="R84" s="3"/>
     </row>
-    <row r="85" spans="1:18" ht="92.25">
+    <row r="85" spans="1:18" ht="93.6" x14ac:dyDescent="0.9">
       <c r="A85" s="8" t="s">
         <v>277</v>
       </c>
@@ -7344,7 +7422,7 @@
       <c r="Q85" s="3"/>
       <c r="R85" s="3"/>
     </row>
-    <row r="86" spans="1:18">
+    <row r="86" spans="1:18" x14ac:dyDescent="0.9">
       <c r="A86" s="8" t="s">
         <v>281</v>
       </c>
@@ -7374,7 +7452,7 @@
       <c r="Q86" s="3"/>
       <c r="R86" s="3"/>
     </row>
-    <row r="87" spans="1:18" ht="92.25">
+    <row r="87" spans="1:18" ht="93.6" x14ac:dyDescent="0.9">
       <c r="A87" s="8" t="s">
         <v>283</v>
       </c>
@@ -7404,7 +7482,7 @@
       <c r="Q87" s="3"/>
       <c r="R87" s="3"/>
     </row>
-    <row r="88" spans="1:18">
+    <row r="88" spans="1:18" x14ac:dyDescent="0.9">
       <c r="A88" s="8" t="s">
         <v>286</v>
       </c>
@@ -7434,7 +7512,7 @@
       <c r="Q88" s="3"/>
       <c r="R88" s="3"/>
     </row>
-    <row r="89" spans="1:18">
+    <row r="89" spans="1:18" x14ac:dyDescent="0.9">
       <c r="A89" s="8" t="s">
         <v>289</v>
       </c>
@@ -7466,7 +7544,7 @@
       <c r="Q89" s="3"/>
       <c r="R89" s="3"/>
     </row>
-    <row r="90" spans="1:18">
+    <row r="90" spans="1:18" x14ac:dyDescent="0.9">
       <c r="A90" s="8" t="s">
         <v>291</v>
       </c>
@@ -7498,7 +7576,7 @@
       <c r="Q90" s="3"/>
       <c r="R90" s="3"/>
     </row>
-    <row r="91" spans="1:18" ht="92.25">
+    <row r="91" spans="1:18" ht="93.6" x14ac:dyDescent="0.9">
       <c r="A91" s="8" t="s">
         <v>293</v>
       </c>
@@ -7530,7 +7608,7 @@
       <c r="Q91" s="3"/>
       <c r="R91" s="3"/>
     </row>
-    <row r="92" spans="1:18" ht="92.25">
+    <row r="92" spans="1:18" ht="93.6" x14ac:dyDescent="0.9">
       <c r="A92" s="8" t="s">
         <v>295</v>
       </c>
@@ -7562,7 +7640,7 @@
       <c r="Q92" s="3"/>
       <c r="R92" s="3"/>
     </row>
-    <row r="93" spans="1:18" ht="275.25">
+    <row r="93" spans="1:18" ht="278.39999999999998" x14ac:dyDescent="0.9">
       <c r="A93" s="8" t="s">
         <v>298</v>
       </c>
@@ -7590,7 +7668,7 @@
       <c r="Q93" s="3"/>
       <c r="R93" s="3"/>
     </row>
-    <row r="94" spans="1:18" ht="92.25">
+    <row r="94" spans="1:18" ht="93.6" x14ac:dyDescent="0.9">
       <c r="A94" s="8" t="s">
         <v>300</v>
       </c>
@@ -7618,7 +7696,7 @@
       <c r="Q94" s="3"/>
       <c r="R94" s="3"/>
     </row>
-    <row r="95" spans="1:18" ht="183.75">
+    <row r="95" spans="1:18" ht="186" x14ac:dyDescent="0.9">
       <c r="A95" s="8" t="s">
         <v>302</v>
       </c>
@@ -7654,7 +7732,7 @@
       <c r="Q95" s="3"/>
       <c r="R95" s="3"/>
     </row>
-    <row r="96" spans="1:18" ht="92.25">
+    <row r="96" spans="1:18" ht="93.6" x14ac:dyDescent="0.9">
       <c r="A96" s="8" t="s">
         <v>305</v>
       </c>
@@ -7690,7 +7768,7 @@
       <c r="Q96" s="3"/>
       <c r="R96" s="3"/>
     </row>
-    <row r="97" spans="1:18" ht="138">
+    <row r="97" spans="1:18" ht="139.80000000000001" x14ac:dyDescent="0.9">
       <c r="A97" s="8" t="s">
         <v>307</v>
       </c>
@@ -7718,7 +7796,7 @@
       <c r="Q97" s="3"/>
       <c r="R97" s="3"/>
     </row>
-    <row r="98" spans="1:18" ht="92.25">
+    <row r="98" spans="1:18" ht="93.6" x14ac:dyDescent="0.9">
       <c r="A98" s="8" t="s">
         <v>309</v>
       </c>
@@ -7750,7 +7828,7 @@
       <c r="Q98" s="3"/>
       <c r="R98" s="3"/>
     </row>
-    <row r="99" spans="1:18" ht="138">
+    <row r="99" spans="1:18" ht="139.80000000000001" x14ac:dyDescent="0.9">
       <c r="A99" s="8" t="s">
         <v>311</v>
       </c>
@@ -7782,7 +7860,7 @@
       <c r="Q99" s="3"/>
       <c r="R99" s="3"/>
     </row>
-    <row r="100" spans="1:18" ht="229.5">
+    <row r="100" spans="1:18" ht="232.2" x14ac:dyDescent="0.9">
       <c r="A100" s="8" t="s">
         <v>314</v>
       </c>
@@ -7812,7 +7890,7 @@
       <c r="Q100" s="3"/>
       <c r="R100" s="3"/>
     </row>
-    <row r="101" spans="1:18" ht="92.25">
+    <row r="101" spans="1:18" ht="93.6" x14ac:dyDescent="0.9">
       <c r="A101" s="8" t="s">
         <v>317</v>
       </c>
@@ -7845,7 +7923,7 @@
       <c r="Q101" s="3"/>
       <c r="R101" s="3"/>
     </row>
-    <row r="102" spans="1:18" ht="92.25">
+    <row r="102" spans="1:18" ht="93.6" x14ac:dyDescent="0.9">
       <c r="A102" s="8" t="s">
         <v>320</v>
       </c>
@@ -7878,7 +7956,7 @@
       <c r="Q102" s="3"/>
       <c r="R102" s="3"/>
     </row>
-    <row r="103" spans="1:18" ht="183.75">
+    <row r="103" spans="1:18" ht="186" x14ac:dyDescent="0.9">
       <c r="A103" s="8" t="s">
         <v>322</v>
       </c>
@@ -7908,7 +7986,7 @@
       <c r="Q103" s="3"/>
       <c r="R103" s="3"/>
     </row>
-    <row r="104" spans="1:18" ht="92.25">
+    <row r="104" spans="1:18" ht="93.6" x14ac:dyDescent="0.9">
       <c r="A104" s="8" t="s">
         <v>325</v>
       </c>
@@ -7941,7 +8019,7 @@
       <c r="Q104" s="3"/>
       <c r="R104" s="3"/>
     </row>
-    <row r="105" spans="1:18" ht="138">
+    <row r="105" spans="1:18" ht="139.80000000000001" x14ac:dyDescent="0.9">
       <c r="A105" s="8" t="s">
         <v>328</v>
       </c>
@@ -7971,7 +8049,7 @@
       <c r="Q105" s="3"/>
       <c r="R105" s="3"/>
     </row>
-    <row r="106" spans="1:18" ht="92.25">
+    <row r="106" spans="1:18" ht="93.6" x14ac:dyDescent="0.9">
       <c r="A106" s="8" t="s">
         <v>330</v>
       </c>
@@ -8004,7 +8082,7 @@
       <c r="Q106" s="3"/>
       <c r="R106" s="3"/>
     </row>
-    <row r="107" spans="1:18" ht="92.25">
+    <row r="107" spans="1:18" ht="93.6" x14ac:dyDescent="0.9">
       <c r="A107" s="8" t="s">
         <v>332</v>
       </c>
@@ -8034,7 +8112,7 @@
       <c r="Q107" s="3"/>
       <c r="R107" s="3"/>
     </row>
-    <row r="108" spans="1:18" ht="92.25">
+    <row r="108" spans="1:18" ht="93.6" x14ac:dyDescent="0.9">
       <c r="A108" s="8" t="s">
         <v>334</v>
       </c>
@@ -8064,7 +8142,7 @@
       <c r="Q108" s="3"/>
       <c r="R108" s="3"/>
     </row>
-    <row r="109" spans="1:18" ht="138">
+    <row r="109" spans="1:18" ht="139.80000000000001" x14ac:dyDescent="0.9">
       <c r="A109" s="8" t="s">
         <v>336</v>
       </c>
@@ -8097,7 +8175,7 @@
       <c r="Q109" s="3"/>
       <c r="R109" s="3"/>
     </row>
-    <row r="110" spans="1:18" ht="92.25">
+    <row r="110" spans="1:18" ht="93.6" x14ac:dyDescent="0.9">
       <c r="A110" s="8" t="s">
         <v>338</v>
       </c>
@@ -8127,7 +8205,7 @@
       <c r="Q110" s="3"/>
       <c r="R110" s="3"/>
     </row>
-    <row r="111" spans="1:18">
+    <row r="111" spans="1:18" x14ac:dyDescent="0.9">
       <c r="A111" s="8" t="s">
         <v>340</v>
       </c>
@@ -8162,7 +8240,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="112" spans="1:18" ht="92.25">
+    <row r="112" spans="1:18" ht="93.6" x14ac:dyDescent="0.9">
       <c r="A112" s="8" t="s">
         <v>344</v>
       </c>
@@ -8194,7 +8272,7 @@
       <c r="Q112" s="3"/>
       <c r="R112" s="3"/>
     </row>
-    <row r="113" spans="1:20" ht="92.25">
+    <row r="113" spans="1:20" ht="93.6" x14ac:dyDescent="0.9">
       <c r="A113" s="8" t="s">
         <v>348</v>
       </c>
@@ -8226,7 +8304,7 @@
       <c r="Q113" s="3"/>
       <c r="R113" s="3"/>
     </row>
-    <row r="114" spans="1:20" ht="92.25">
+    <row r="114" spans="1:20" ht="93.6" x14ac:dyDescent="0.9">
       <c r="A114" s="8" t="s">
         <v>350</v>
       </c>
@@ -8258,7 +8336,7 @@
       <c r="Q114" s="3"/>
       <c r="R114" s="3"/>
     </row>
-    <row r="115" spans="1:20" ht="92.25">
+    <row r="115" spans="1:20" ht="93.6" x14ac:dyDescent="0.9">
       <c r="A115" s="8" t="s">
         <v>352</v>
       </c>
@@ -8290,7 +8368,7 @@
       <c r="Q115" s="3"/>
       <c r="R115" s="3"/>
     </row>
-    <row r="116" spans="1:20" ht="92.25">
+    <row r="116" spans="1:20" ht="93.6" x14ac:dyDescent="0.9">
       <c r="A116" s="8" t="s">
         <v>356</v>
       </c>
@@ -8325,7 +8403,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="117" spans="1:20" ht="92.25">
+    <row r="117" spans="1:20" ht="93.6" x14ac:dyDescent="0.9">
       <c r="A117" s="8" t="s">
         <v>359</v>
       </c>
@@ -8357,7 +8435,7 @@
       <c r="Q117" s="3"/>
       <c r="R117" s="3"/>
     </row>
-    <row r="118" spans="1:20" ht="92.25">
+    <row r="118" spans="1:20" ht="93.6" x14ac:dyDescent="0.9">
       <c r="A118" s="8" t="s">
         <v>362</v>
       </c>
@@ -8392,7 +8470,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="119" spans="1:20" ht="92.25">
+    <row r="119" spans="1:20" ht="93.6" x14ac:dyDescent="0.9">
       <c r="A119" s="8" t="s">
         <v>366</v>
       </c>
@@ -8424,7 +8502,7 @@
       <c r="Q119" s="3"/>
       <c r="R119" s="3"/>
     </row>
-    <row r="120" spans="1:20" ht="138">
+    <row r="120" spans="1:20" ht="139.80000000000001" x14ac:dyDescent="0.9">
       <c r="A120" s="8" t="s">
         <v>368</v>
       </c>
@@ -8459,7 +8537,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="121" spans="1:20" ht="138">
+    <row r="121" spans="1:20" ht="139.80000000000001" x14ac:dyDescent="0.9">
       <c r="A121" s="8" t="s">
         <v>372</v>
       </c>
@@ -8491,7 +8569,7 @@
       <c r="Q121" s="3"/>
       <c r="R121" s="3"/>
     </row>
-    <row r="122" spans="1:20" ht="138">
+    <row r="122" spans="1:20" ht="139.80000000000001" x14ac:dyDescent="0.9">
       <c r="A122" s="8" t="s">
         <v>374</v>
       </c>
@@ -8523,7 +8601,7 @@
       <c r="Q122" s="3"/>
       <c r="R122" s="3"/>
     </row>
-    <row r="123" spans="1:20" ht="183.75">
+    <row r="123" spans="1:20" ht="186" x14ac:dyDescent="0.9">
       <c r="A123" s="8" t="s">
         <v>376</v>
       </c>
@@ -8558,7 +8636,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="124" spans="1:20">
+    <row r="124" spans="1:20" x14ac:dyDescent="0.9">
       <c r="A124" s="8" t="s">
         <v>379</v>
       </c>
@@ -8591,7 +8669,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="125" spans="1:20" ht="275.25">
+    <row r="125" spans="1:20" ht="278.39999999999998" x14ac:dyDescent="0.9">
       <c r="A125" s="8" t="s">
         <v>381</v>
       </c>
@@ -8626,7 +8704,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="126" spans="1:20" ht="183.75">
+    <row r="126" spans="1:20" ht="186" x14ac:dyDescent="0.9">
       <c r="A126" s="8" t="s">
         <v>383</v>
       </c>
@@ -8658,7 +8736,7 @@
       <c r="Q126" s="3"/>
       <c r="R126" s="3"/>
     </row>
-    <row r="127" spans="1:20" ht="137.25">
+    <row r="127" spans="1:20" ht="138.6" x14ac:dyDescent="0.9">
       <c r="A127" s="8" t="s">
         <v>385</v>
       </c>
@@ -8693,7 +8771,7 @@
       <c r="Q127" s="3"/>
       <c r="R127" s="3"/>
     </row>
-    <row r="128" spans="1:20" s="40" customFormat="1" ht="91.5">
+    <row r="128" spans="1:20" s="40" customFormat="1" ht="92.4" x14ac:dyDescent="0.9">
       <c r="A128" s="33" t="s">
         <v>389</v>
       </c>
@@ -8728,7 +8806,7 @@
       <c r="S128" s="39"/>
       <c r="T128" s="39"/>
     </row>
-    <row r="129" spans="1:20" ht="91.5">
+    <row r="129" spans="1:20" ht="92.4" x14ac:dyDescent="0.9">
       <c r="A129" s="8" t="s">
         <v>393</v>
       </c>
@@ -8765,7 +8843,7 @@
       <c r="S129" s="39"/>
       <c r="T129" s="39"/>
     </row>
-    <row r="130" spans="1:20" ht="92.25">
+    <row r="130" spans="1:20" ht="93.6" x14ac:dyDescent="0.9">
       <c r="A130" s="8" t="s">
         <v>397</v>
       </c>
@@ -8802,7 +8880,7 @@
       <c r="S130" s="39"/>
       <c r="T130" s="39"/>
     </row>
-    <row r="131" spans="1:20" s="40" customFormat="1" ht="92.25">
+    <row r="131" spans="1:20" s="40" customFormat="1" ht="93.6" x14ac:dyDescent="0.9">
       <c r="A131" s="33" t="s">
         <v>400</v>
       </c>
@@ -8837,7 +8915,7 @@
       <c r="S131" s="39"/>
       <c r="T131" s="39"/>
     </row>
-    <row r="132" spans="1:20">
+    <row r="132" spans="1:20" x14ac:dyDescent="0.9">
       <c r="A132" s="8" t="s">
         <v>403</v>
       </c>
@@ -8872,7 +8950,7 @@
       <c r="S132" s="39"/>
       <c r="T132" s="39"/>
     </row>
-    <row r="133" spans="1:20" ht="174.75" customHeight="1">
+    <row r="133" spans="1:20" ht="174.75" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A133" s="8" t="s">
         <v>407</v>
       </c>
@@ -8909,7 +8987,7 @@
       <c r="S133" s="39"/>
       <c r="T133" s="39"/>
     </row>
-    <row r="134" spans="1:20">
+    <row r="134" spans="1:20" x14ac:dyDescent="0.9">
       <c r="A134" s="8" t="s">
         <v>411</v>
       </c>
@@ -8946,7 +9024,7 @@
       <c r="S134" s="39"/>
       <c r="T134" s="39"/>
     </row>
-    <row r="135" spans="1:20">
+    <row r="135" spans="1:20" x14ac:dyDescent="0.9">
       <c r="A135" s="8" t="s">
         <v>415</v>
       </c>
@@ -8981,7 +9059,7 @@
       <c r="S135" s="39"/>
       <c r="T135" s="39"/>
     </row>
-    <row r="136" spans="1:20" ht="92.25">
+    <row r="136" spans="1:20" ht="93.6" x14ac:dyDescent="0.9">
       <c r="A136" s="8" t="s">
         <v>419</v>
       </c>
@@ -9014,7 +9092,7 @@
       <c r="Q136" s="3"/>
       <c r="R136" s="3"/>
     </row>
-    <row r="137" spans="1:20" ht="92.25">
+    <row r="137" spans="1:20" ht="93.6" x14ac:dyDescent="0.9">
       <c r="A137" s="8" t="s">
         <v>423</v>
       </c>
@@ -9047,7 +9125,7 @@
       <c r="Q137" s="3"/>
       <c r="R137" s="3"/>
     </row>
-    <row r="138" spans="1:20" ht="138">
+    <row r="138" spans="1:20" ht="139.80000000000001" x14ac:dyDescent="0.9">
       <c r="A138" s="8" t="s">
         <v>426</v>
       </c>
@@ -9080,7 +9158,7 @@
       <c r="Q138" s="3"/>
       <c r="R138" s="3"/>
     </row>
-    <row r="139" spans="1:20" ht="92.25">
+    <row r="139" spans="1:20" ht="93.6" x14ac:dyDescent="0.9">
       <c r="A139" s="8" t="s">
         <v>430</v>
       </c>
@@ -9113,7 +9191,7 @@
       <c r="Q139" s="3"/>
       <c r="R139" s="3"/>
     </row>
-    <row r="140" spans="1:20" ht="138">
+    <row r="140" spans="1:20" ht="139.80000000000001" x14ac:dyDescent="0.9">
       <c r="A140" s="8" t="s">
         <v>433</v>
       </c>
@@ -9146,7 +9224,7 @@
       <c r="Q140" s="3"/>
       <c r="R140" s="3"/>
     </row>
-    <row r="141" spans="1:20" ht="138">
+    <row r="141" spans="1:20" ht="93.6" x14ac:dyDescent="0.9">
       <c r="A141" s="8" t="s">
         <v>437</v>
       </c>
@@ -9179,7 +9257,7 @@
       <c r="Q141" s="3"/>
       <c r="R141" s="3"/>
     </row>
-    <row r="142" spans="1:20" ht="92.25">
+    <row r="142" spans="1:20" ht="93.6" x14ac:dyDescent="0.9">
       <c r="A142" s="8" t="s">
         <v>440</v>
       </c>
@@ -9212,7 +9290,7 @@
       <c r="Q142" s="3"/>
       <c r="R142" s="3"/>
     </row>
-    <row r="143" spans="1:20" ht="138">
+    <row r="143" spans="1:20" ht="139.80000000000001" x14ac:dyDescent="0.9">
       <c r="A143" s="8" t="s">
         <v>443</v>
       </c>
@@ -9245,7 +9323,7 @@
       <c r="Q143" s="3"/>
       <c r="R143" s="3"/>
     </row>
-    <row r="144" spans="1:20" ht="138">
+    <row r="144" spans="1:20" ht="139.80000000000001" x14ac:dyDescent="0.9">
       <c r="A144" s="42" t="s">
         <v>446</v>
       </c>
@@ -9277,7 +9355,7 @@
       <c r="S144" s="39"/>
       <c r="T144" s="39"/>
     </row>
-    <row r="145" spans="1:20" ht="138">
+    <row r="145" spans="1:20" ht="139.80000000000001" x14ac:dyDescent="0.9">
       <c r="A145" s="8" t="s">
         <v>450</v>
       </c>
@@ -9314,7 +9392,7 @@
       <c r="S145" s="39"/>
       <c r="T145" s="39"/>
     </row>
-    <row r="146" spans="1:20" ht="138">
+    <row r="146" spans="1:20" ht="139.80000000000001" x14ac:dyDescent="0.9">
       <c r="A146" s="8" t="s">
         <v>454</v>
       </c>
@@ -9351,7 +9429,7 @@
       <c r="S146" s="39"/>
       <c r="T146" s="39"/>
     </row>
-    <row r="147" spans="1:20" ht="138">
+    <row r="147" spans="1:20" ht="139.80000000000001" x14ac:dyDescent="0.9">
       <c r="A147" s="8" t="s">
         <v>458</v>
       </c>
@@ -9386,7 +9464,7 @@
       <c r="S147" s="39"/>
       <c r="T147" s="39"/>
     </row>
-    <row r="148" spans="1:20" ht="138">
+    <row r="148" spans="1:20" ht="139.80000000000001" x14ac:dyDescent="0.9">
       <c r="A148" s="8" t="s">
         <v>462</v>
       </c>
@@ -9421,7 +9499,7 @@
       <c r="S148" s="39"/>
       <c r="T148" s="39"/>
     </row>
-    <row r="149" spans="1:20" s="40" customFormat="1" ht="138">
+    <row r="149" spans="1:20" s="40" customFormat="1" ht="139.80000000000001" x14ac:dyDescent="0.9">
       <c r="A149" s="33" t="s">
         <v>466</v>
       </c>
@@ -9453,7 +9531,7 @@
       <c r="S149" s="39"/>
       <c r="T149" s="39"/>
     </row>
-    <row r="150" spans="1:20" ht="138">
+    <row r="150" spans="1:20" ht="139.80000000000001" x14ac:dyDescent="0.9">
       <c r="A150" s="8" t="s">
         <v>470</v>
       </c>
@@ -9488,7 +9566,7 @@
       <c r="S150" s="39"/>
       <c r="T150" s="39"/>
     </row>
-    <row r="151" spans="1:20" ht="138">
+    <row r="151" spans="1:20" ht="139.80000000000001" x14ac:dyDescent="0.9">
       <c r="A151" s="8" t="s">
         <v>474</v>
       </c>
@@ -9520,7 +9598,7 @@
       <c r="S151" s="39"/>
       <c r="T151" s="39"/>
     </row>
-    <row r="152" spans="1:20" ht="92.25">
+    <row r="152" spans="1:20" ht="93.6" x14ac:dyDescent="0.9">
       <c r="A152" s="8" t="s">
         <v>477</v>
       </c>
@@ -9552,7 +9630,7 @@
       <c r="S152" s="39"/>
       <c r="T152" s="39"/>
     </row>
-    <row r="153" spans="1:20" ht="138">
+    <row r="153" spans="1:20" ht="139.80000000000001" x14ac:dyDescent="0.9">
       <c r="A153" s="8" t="s">
         <v>480</v>
       </c>
@@ -9590,7 +9668,7 @@
       <c r="S153" s="39"/>
       <c r="T153" s="39"/>
     </row>
-    <row r="154" spans="1:20" ht="138">
+    <row r="154" spans="1:20" ht="139.80000000000001" x14ac:dyDescent="0.9">
       <c r="A154" s="8" t="s">
         <v>483</v>
       </c>
@@ -9628,7 +9706,7 @@
       <c r="S154" s="39"/>
       <c r="T154" s="39"/>
     </row>
-    <row r="155" spans="1:20" ht="92.25">
+    <row r="155" spans="1:20" ht="93.6" x14ac:dyDescent="0.9">
       <c r="A155" s="8" t="s">
         <v>486</v>
       </c>
@@ -9666,7 +9744,7 @@
       <c r="S155" s="39"/>
       <c r="T155" s="39"/>
     </row>
-    <row r="156" spans="1:20" ht="138">
+    <row r="156" spans="1:20" ht="139.80000000000001" x14ac:dyDescent="0.9">
       <c r="A156" s="8" t="s">
         <v>489</v>
       </c>
@@ -9704,7 +9782,7 @@
       <c r="S156" s="39"/>
       <c r="T156" s="39"/>
     </row>
-    <row r="157" spans="1:20" ht="92.25">
+    <row r="157" spans="1:20" ht="93.6" x14ac:dyDescent="0.9">
       <c r="A157" s="8" t="s">
         <v>491</v>
       </c>
@@ -9742,7 +9820,7 @@
       <c r="S157" s="39"/>
       <c r="T157" s="39"/>
     </row>
-    <row r="158" spans="1:20" ht="138">
+    <row r="158" spans="1:20" ht="139.80000000000001" x14ac:dyDescent="0.9">
       <c r="A158" s="8" t="s">
         <v>493</v>
       </c>
@@ -9780,7 +9858,7 @@
       <c r="S158" s="39"/>
       <c r="T158" s="39"/>
     </row>
-    <row r="159" spans="1:20" ht="92.25">
+    <row r="159" spans="1:20" ht="93.6" x14ac:dyDescent="0.9">
       <c r="A159" s="8" t="s">
         <v>496</v>
       </c>
@@ -9818,7 +9896,7 @@
       <c r="S159" s="39"/>
       <c r="T159" s="39"/>
     </row>
-    <row r="160" spans="1:20" ht="92.25">
+    <row r="160" spans="1:20" ht="93.6" x14ac:dyDescent="0.9">
       <c r="A160" s="8" t="s">
         <v>499</v>
       </c>
@@ -9856,7 +9934,7 @@
       <c r="S160" s="39"/>
       <c r="T160" s="39"/>
     </row>
-    <row r="161" spans="1:20" ht="92.25">
+    <row r="161" spans="1:20" ht="93.6" x14ac:dyDescent="0.9">
       <c r="A161" s="8" t="s">
         <v>502</v>
       </c>
@@ -9894,7 +9972,7 @@
       <c r="S161" s="39"/>
       <c r="T161" s="39"/>
     </row>
-    <row r="162" spans="1:20">
+    <row r="162" spans="1:20" x14ac:dyDescent="0.9">
       <c r="A162" s="8" t="s">
         <v>505</v>
       </c>
@@ -9932,7 +10010,7 @@
       <c r="S162" s="39"/>
       <c r="T162" s="39"/>
     </row>
-    <row r="163" spans="1:20" ht="92.25">
+    <row r="163" spans="1:20" x14ac:dyDescent="0.9">
       <c r="A163" s="8" t="s">
         <v>508</v>
       </c>
@@ -9970,7 +10048,7 @@
       <c r="S163" s="39"/>
       <c r="T163" s="39"/>
     </row>
-    <row r="164" spans="1:20">
+    <row r="164" spans="1:20" x14ac:dyDescent="0.9">
       <c r="A164" s="8" t="s">
         <v>511</v>
       </c>
@@ -10008,7 +10086,7 @@
       <c r="S164" s="39"/>
       <c r="T164" s="39"/>
     </row>
-    <row r="165" spans="1:20">
+    <row r="165" spans="1:20" x14ac:dyDescent="0.9">
       <c r="A165" s="8" t="s">
         <v>514</v>
       </c>
@@ -10046,7 +10124,7 @@
       <c r="S165" s="39"/>
       <c r="T165" s="39"/>
     </row>
-    <row r="166" spans="1:20">
+    <row r="166" spans="1:20" x14ac:dyDescent="0.9">
       <c r="A166" s="8" t="s">
         <v>517</v>
       </c>
@@ -10084,7 +10162,7 @@
       <c r="S166" s="39"/>
       <c r="T166" s="39"/>
     </row>
-    <row r="167" spans="1:20">
+    <row r="167" spans="1:20" x14ac:dyDescent="0.9">
       <c r="A167" s="8" t="s">
         <v>520</v>
       </c>
@@ -10122,7 +10200,7 @@
       <c r="S167" s="39"/>
       <c r="T167" s="39"/>
     </row>
-    <row r="168" spans="1:20" ht="92.25">
+    <row r="168" spans="1:20" ht="93.6" x14ac:dyDescent="0.9">
       <c r="A168" s="8" t="s">
         <v>523</v>
       </c>
@@ -10158,7 +10236,7 @@
       <c r="S168" s="39"/>
       <c r="T168" s="39"/>
     </row>
-    <row r="169" spans="1:20">
+    <row r="169" spans="1:20" x14ac:dyDescent="0.9">
       <c r="A169" s="8" t="s">
         <v>526</v>
       </c>
@@ -10194,7 +10272,7 @@
       <c r="S169" s="39"/>
       <c r="T169" s="39"/>
     </row>
-    <row r="170" spans="1:20">
+    <row r="170" spans="1:20" x14ac:dyDescent="0.9">
       <c r="A170" s="8" t="s">
         <v>529</v>
       </c>
@@ -10230,7 +10308,7 @@
       <c r="S170" s="39"/>
       <c r="T170" s="39"/>
     </row>
-    <row r="171" spans="1:20">
+    <row r="171" spans="1:20" x14ac:dyDescent="0.9">
       <c r="A171" s="8" t="s">
         <v>532</v>
       </c>
@@ -10262,7 +10340,7 @@
       <c r="S171" s="39"/>
       <c r="T171" s="39"/>
     </row>
-    <row r="172" spans="1:20" ht="92.25">
+    <row r="172" spans="1:20" ht="93.6" x14ac:dyDescent="0.9">
       <c r="A172" s="8" t="s">
         <v>535</v>
       </c>
@@ -10298,7 +10376,7 @@
       <c r="S172" s="39"/>
       <c r="T172" s="39"/>
     </row>
-    <row r="173" spans="1:20">
+    <row r="173" spans="1:20" x14ac:dyDescent="0.9">
       <c r="A173" s="8" t="s">
         <v>538</v>
       </c>
@@ -10334,7 +10412,7 @@
       <c r="S173" s="39"/>
       <c r="T173" s="39"/>
     </row>
-    <row r="174" spans="1:20" ht="92.25">
+    <row r="174" spans="1:20" ht="93.6" x14ac:dyDescent="0.9">
       <c r="A174" s="8" t="s">
         <v>541</v>
       </c>
@@ -10372,7 +10450,7 @@
       <c r="S174" s="39"/>
       <c r="T174" s="39"/>
     </row>
-    <row r="175" spans="1:20">
+    <row r="175" spans="1:20" x14ac:dyDescent="0.9">
       <c r="A175" s="8" t="s">
         <v>544</v>
       </c>
@@ -10410,7 +10488,7 @@
       <c r="S175" s="39"/>
       <c r="T175" s="39"/>
     </row>
-    <row r="176" spans="1:20">
+    <row r="176" spans="1:20" x14ac:dyDescent="0.9">
       <c r="A176" s="8" t="s">
         <v>547</v>
       </c>
@@ -10448,7 +10526,7 @@
       <c r="S176" s="39"/>
       <c r="T176" s="39"/>
     </row>
-    <row r="177" spans="1:20">
+    <row r="177" spans="1:20" x14ac:dyDescent="0.9">
       <c r="A177" s="8" t="s">
         <v>550</v>
       </c>
@@ -10486,7 +10564,7 @@
       <c r="S177" s="39"/>
       <c r="T177" s="39"/>
     </row>
-    <row r="178" spans="1:20" ht="92.25">
+    <row r="178" spans="1:20" ht="93.6" x14ac:dyDescent="0.9">
       <c r="A178" s="8" t="s">
         <v>553</v>
       </c>
@@ -10524,7 +10602,7 @@
       <c r="S178" s="39"/>
       <c r="T178" s="39"/>
     </row>
-    <row r="179" spans="1:20" ht="91.5">
+    <row r="179" spans="1:20" ht="92.4" x14ac:dyDescent="0.9">
       <c r="A179" s="8" t="s">
         <v>556</v>
       </c>
@@ -10562,7 +10640,7 @@
       <c r="S179" s="39"/>
       <c r="T179" s="39"/>
     </row>
-    <row r="180" spans="1:20">
+    <row r="180" spans="1:20" x14ac:dyDescent="0.9">
       <c r="A180" s="8" t="s">
         <v>558</v>
       </c>
@@ -10600,7 +10678,7 @@
       <c r="S180" s="39"/>
       <c r="T180" s="39"/>
     </row>
-    <row r="181" spans="1:20">
+    <row r="181" spans="1:20" x14ac:dyDescent="0.9">
       <c r="A181" s="8" t="s">
         <v>560</v>
       </c>
@@ -10638,7 +10716,7 @@
       <c r="S181" s="39"/>
       <c r="T181" s="39"/>
     </row>
-    <row r="182" spans="1:20" ht="92.25">
+    <row r="182" spans="1:20" ht="93.6" x14ac:dyDescent="0.9">
       <c r="A182" s="8" t="s">
         <v>562</v>
       </c>
@@ -10676,7 +10754,7 @@
       <c r="S182" s="39"/>
       <c r="T182" s="39"/>
     </row>
-    <row r="183" spans="1:20">
+    <row r="183" spans="1:20" x14ac:dyDescent="0.9">
       <c r="A183" s="8" t="s">
         <v>564</v>
       </c>
@@ -10714,7 +10792,7 @@
       <c r="S183" s="39"/>
       <c r="T183" s="39"/>
     </row>
-    <row r="184" spans="1:20" ht="92.25">
+    <row r="184" spans="1:20" ht="93.6" x14ac:dyDescent="0.9">
       <c r="A184" s="8" t="s">
         <v>566</v>
       </c>
@@ -10752,7 +10830,7 @@
       <c r="S184" s="39"/>
       <c r="T184" s="39"/>
     </row>
-    <row r="185" spans="1:20" ht="92.25">
+    <row r="185" spans="1:20" ht="93.6" x14ac:dyDescent="0.9">
       <c r="A185" s="8" t="s">
         <v>568</v>
       </c>
@@ -10790,7 +10868,7 @@
       <c r="S185" s="39"/>
       <c r="T185" s="39"/>
     </row>
-    <row r="186" spans="1:20" ht="92.25">
+    <row r="186" spans="1:20" ht="93.6" x14ac:dyDescent="0.9">
       <c r="A186" s="8" t="s">
         <v>571</v>
       </c>
@@ -10828,7 +10906,7 @@
       <c r="S186" s="39"/>
       <c r="T186" s="39"/>
     </row>
-    <row r="187" spans="1:20" ht="92.25">
+    <row r="187" spans="1:20" ht="93.6" x14ac:dyDescent="0.9">
       <c r="A187" s="8" t="s">
         <v>574</v>
       </c>
@@ -10866,7 +10944,7 @@
       <c r="S187" s="39"/>
       <c r="T187" s="39"/>
     </row>
-    <row r="188" spans="1:20" ht="92.25">
+    <row r="188" spans="1:20" ht="93.6" x14ac:dyDescent="0.9">
       <c r="A188" s="8" t="s">
         <v>577</v>
       </c>
@@ -10904,7 +10982,7 @@
       <c r="S188" s="39"/>
       <c r="T188" s="39"/>
     </row>
-    <row r="189" spans="1:20" ht="92.25">
+    <row r="189" spans="1:20" ht="93.6" x14ac:dyDescent="0.9">
       <c r="A189" s="8" t="s">
         <v>580</v>
       </c>
@@ -10942,7 +11020,7 @@
       <c r="S189" s="39"/>
       <c r="T189" s="39"/>
     </row>
-    <row r="190" spans="1:20" ht="92.25">
+    <row r="190" spans="1:20" ht="93.6" x14ac:dyDescent="0.9">
       <c r="A190" s="8" t="s">
         <v>583</v>
       </c>
@@ -10980,7 +11058,7 @@
       <c r="S190" s="39"/>
       <c r="T190" s="39"/>
     </row>
-    <row r="191" spans="1:20" ht="92.25">
+    <row r="191" spans="1:20" ht="93.6" x14ac:dyDescent="0.9">
       <c r="A191" s="8" t="s">
         <v>586</v>
       </c>
@@ -11018,7 +11096,7 @@
       <c r="S191" s="39"/>
       <c r="T191" s="39"/>
     </row>
-    <row r="192" spans="1:20" ht="92.25">
+    <row r="192" spans="1:20" ht="93.6" x14ac:dyDescent="0.9">
       <c r="A192" s="8" t="s">
         <v>589</v>
       </c>
@@ -11056,7 +11134,7 @@
       <c r="S192" s="39"/>
       <c r="T192" s="39"/>
     </row>
-    <row r="193" spans="1:20" ht="92.25">
+    <row r="193" spans="1:20" ht="93.6" x14ac:dyDescent="0.9">
       <c r="A193" s="8" t="s">
         <v>592</v>
       </c>
@@ -11094,7 +11172,7 @@
       <c r="S193" s="39"/>
       <c r="T193" s="39"/>
     </row>
-    <row r="194" spans="1:20" ht="92.25">
+    <row r="194" spans="1:20" ht="93.6" x14ac:dyDescent="0.9">
       <c r="A194" s="8" t="s">
         <v>595</v>
       </c>
@@ -11132,7 +11210,7 @@
       <c r="S194" s="39"/>
       <c r="T194" s="39"/>
     </row>
-    <row r="195" spans="1:20" ht="92.25">
+    <row r="195" spans="1:20" ht="93.6" x14ac:dyDescent="0.9">
       <c r="A195" s="8" t="s">
         <v>598</v>
       </c>
@@ -11170,7 +11248,7 @@
       <c r="S195" s="39"/>
       <c r="T195" s="39"/>
     </row>
-    <row r="196" spans="1:20" ht="92.25">
+    <row r="196" spans="1:20" x14ac:dyDescent="0.9">
       <c r="A196" s="8" t="s">
         <v>601</v>
       </c>
@@ -11208,7 +11286,7 @@
       <c r="S196" s="39"/>
       <c r="T196" s="39"/>
     </row>
-    <row r="197" spans="1:20" ht="92.25">
+    <row r="197" spans="1:20" ht="93.6" x14ac:dyDescent="0.9">
       <c r="A197" s="8" t="s">
         <v>604</v>
       </c>
@@ -11246,7 +11324,7 @@
       <c r="S197" s="39"/>
       <c r="T197" s="39"/>
     </row>
-    <row r="198" spans="1:20" ht="92.25">
+    <row r="198" spans="1:20" ht="93.6" x14ac:dyDescent="0.9">
       <c r="A198" s="8" t="s">
         <v>607</v>
       </c>
@@ -11284,7 +11362,7 @@
       <c r="S198" s="39"/>
       <c r="T198" s="39"/>
     </row>
-    <row r="199" spans="1:20" ht="138">
+    <row r="199" spans="1:20" ht="139.80000000000001" x14ac:dyDescent="0.9">
       <c r="A199" s="8" t="s">
         <v>610</v>
       </c>
@@ -11322,7 +11400,7 @@
       <c r="S199" s="39"/>
       <c r="T199" s="39"/>
     </row>
-    <row r="200" spans="1:20" ht="92.25">
+    <row r="200" spans="1:20" ht="93.6" x14ac:dyDescent="0.9">
       <c r="A200" s="8" t="s">
         <v>613</v>
       </c>
@@ -11360,7 +11438,7 @@
       <c r="S200" s="39"/>
       <c r="T200" s="39"/>
     </row>
-    <row r="201" spans="1:20" ht="92.25">
+    <row r="201" spans="1:20" ht="93.6" x14ac:dyDescent="0.9">
       <c r="A201" s="8" t="s">
         <v>616</v>
       </c>
@@ -11398,7 +11476,7 @@
       <c r="S201" s="39"/>
       <c r="T201" s="39"/>
     </row>
-    <row r="202" spans="1:20" ht="92.25">
+    <row r="202" spans="1:20" ht="93.6" x14ac:dyDescent="0.9">
       <c r="A202" s="8" t="s">
         <v>619</v>
       </c>
@@ -11436,7 +11514,7 @@
       <c r="S202" s="39"/>
       <c r="T202" s="39"/>
     </row>
-    <row r="203" spans="1:20" ht="92.25">
+    <row r="203" spans="1:20" ht="93.6" x14ac:dyDescent="0.9">
       <c r="A203" s="8" t="s">
         <v>622</v>
       </c>
@@ -11474,7 +11552,7 @@
       <c r="S203" s="39"/>
       <c r="T203" s="39"/>
     </row>
-    <row r="204" spans="1:20" ht="350.25" customHeight="1">
+    <row r="204" spans="1:20" ht="350.25" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A204" s="8" t="s">
         <v>625</v>
       </c>
@@ -11511,7 +11589,7 @@
       <c r="S204" s="39"/>
       <c r="T204" s="39"/>
     </row>
-    <row r="205" spans="1:20" ht="300" customHeight="1">
+    <row r="205" spans="1:20" ht="300" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A205" s="8" t="s">
         <v>630</v>
       </c>
@@ -11552,7 +11630,7 @@
       <c r="S205" s="39"/>
       <c r="T205" s="39"/>
     </row>
-    <row r="206" spans="1:20" ht="300" customHeight="1">
+    <row r="206" spans="1:20" ht="300" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A206" s="8" t="s">
         <v>633</v>
       </c>
@@ -11593,7 +11671,7 @@
       <c r="S206" s="39"/>
       <c r="T206" s="39"/>
     </row>
-    <row r="207" spans="1:20" ht="300" customHeight="1">
+    <row r="207" spans="1:20" ht="300" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A207" s="8" t="s">
         <v>635</v>
       </c>
@@ -11630,7 +11708,7 @@
       <c r="S207" s="39"/>
       <c r="T207" s="39"/>
     </row>
-    <row r="208" spans="1:20" ht="300" customHeight="1">
+    <row r="208" spans="1:20" ht="300" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A208" s="8" t="s">
         <v>638</v>
       </c>
@@ -11671,7 +11749,7 @@
       <c r="S208" s="39"/>
       <c r="T208" s="39"/>
     </row>
-    <row r="209" spans="1:20" ht="300" customHeight="1">
+    <row r="209" spans="1:20" ht="300" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A209" s="8" t="s">
         <v>640</v>
       </c>
@@ -11710,7 +11788,7 @@
       <c r="S209" s="39"/>
       <c r="T209" s="39"/>
     </row>
-    <row r="210" spans="1:20" ht="399.75" customHeight="1">
+    <row r="210" spans="1:20" ht="399.75" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A210" s="8" t="s">
         <v>644</v>
       </c>
@@ -11747,7 +11825,7 @@
       <c r="Q210" s="3"/>
       <c r="R210" s="3"/>
     </row>
-    <row r="211" spans="1:20" ht="300" customHeight="1">
+    <row r="211" spans="1:20" ht="300" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A211" s="8" t="s">
         <v>647</v>
       </c>
@@ -11782,7 +11860,7 @@
       <c r="Q211" s="3"/>
       <c r="R211" s="3"/>
     </row>
-    <row r="212" spans="1:20" ht="300" customHeight="1">
+    <row r="212" spans="1:20" ht="300" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A212" s="8" t="s">
         <v>649</v>
       </c>
@@ -11817,7 +11895,7 @@
       <c r="Q212" s="3"/>
       <c r="R212" s="3"/>
     </row>
-    <row r="213" spans="1:20" ht="150" customHeight="1">
+    <row r="213" spans="1:20" ht="150" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A213" s="8" t="s">
         <v>651</v>
       </c>
@@ -11852,7 +11930,7 @@
       <c r="Q213" s="3"/>
       <c r="R213" s="3"/>
     </row>
-    <row r="214" spans="1:20" ht="93">
+    <row r="214" spans="1:20" ht="94.8" x14ac:dyDescent="0.9">
       <c r="A214" s="3" t="s">
         <v>653</v>
       </c>
@@ -11884,7 +11962,7 @@
       <c r="Q214" s="3"/>
       <c r="R214" s="3"/>
     </row>
-    <row r="215" spans="1:20">
+    <row r="215" spans="1:20" x14ac:dyDescent="0.9">
       <c r="A215" s="3" t="s">
         <v>656</v>
       </c>
@@ -11916,7 +11994,7 @@
       <c r="Q215" s="3"/>
       <c r="R215" s="3"/>
     </row>
-    <row r="216" spans="1:20" ht="93">
+    <row r="216" spans="1:20" ht="94.8" x14ac:dyDescent="0.9">
       <c r="A216" s="3" t="s">
         <v>659</v>
       </c>
@@ -11948,7 +12026,7 @@
       <c r="Q216" s="3"/>
       <c r="R216" s="3"/>
     </row>
-    <row r="217" spans="1:20">
+    <row r="217" spans="1:20" x14ac:dyDescent="0.9">
       <c r="A217" s="3" t="s">
         <v>662</v>
       </c>
@@ -11980,7 +12058,7 @@
       <c r="Q217" s="3"/>
       <c r="R217" s="3"/>
     </row>
-    <row r="218" spans="1:20" ht="93">
+    <row r="218" spans="1:20" ht="94.8" x14ac:dyDescent="0.9">
       <c r="A218" s="3" t="s">
         <v>665</v>
       </c>
@@ -12010,7 +12088,7 @@
       <c r="Q218" s="3"/>
       <c r="R218" s="3"/>
     </row>
-    <row r="219" spans="1:20">
+    <row r="219" spans="1:20" x14ac:dyDescent="0.9">
       <c r="A219" s="3" t="s">
         <v>667</v>
       </c>
@@ -12040,7 +12118,7 @@
       <c r="Q219" s="3"/>
       <c r="R219" s="3"/>
     </row>
-    <row r="220" spans="1:20">
+    <row r="220" spans="1:20" x14ac:dyDescent="0.9">
       <c r="A220" s="3" t="s">
         <v>669</v>
       </c>
@@ -12072,7 +12150,7 @@
       <c r="Q220" s="3"/>
       <c r="R220" s="3"/>
     </row>
-    <row r="221" spans="1:20" ht="93">
+    <row r="221" spans="1:20" ht="94.8" x14ac:dyDescent="0.9">
       <c r="A221" s="3" t="s">
         <v>672</v>
       </c>
@@ -12104,7 +12182,7 @@
       <c r="Q221" s="3"/>
       <c r="R221" s="3"/>
     </row>
-    <row r="222" spans="1:20">
+    <row r="222" spans="1:20" x14ac:dyDescent="0.9">
       <c r="A222" s="3" t="s">
         <v>675</v>
       </c>
@@ -12136,7 +12214,7 @@
       <c r="Q222" s="3"/>
       <c r="R222" s="3"/>
     </row>
-    <row r="223" spans="1:20" ht="93">
+    <row r="223" spans="1:20" ht="94.8" x14ac:dyDescent="0.9">
       <c r="A223" s="3" t="s">
         <v>678</v>
       </c>
@@ -12170,7 +12248,7 @@
       <c r="Q223" s="3"/>
       <c r="R223" s="3"/>
     </row>
-    <row r="224" spans="1:20" ht="93">
+    <row r="224" spans="1:20" x14ac:dyDescent="0.9">
       <c r="A224" s="3" t="s">
         <v>682</v>
       </c>
@@ -12202,7 +12280,7 @@
       <c r="Q224" s="3"/>
       <c r="R224" s="3"/>
     </row>
-    <row r="225" spans="1:18">
+    <row r="225" spans="1:18" x14ac:dyDescent="0.9">
       <c r="A225" s="3" t="s">
         <v>685</v>
       </c>
@@ -12234,7 +12312,7 @@
       <c r="Q225" s="3"/>
       <c r="R225" s="3"/>
     </row>
-    <row r="226" spans="1:18" ht="93">
+    <row r="226" spans="1:18" ht="94.8" x14ac:dyDescent="0.9">
       <c r="A226" s="3" t="s">
         <v>689</v>
       </c>
@@ -12266,7 +12344,7 @@
       <c r="Q226" s="3"/>
       <c r="R226" s="3"/>
     </row>
-    <row r="227" spans="1:18" ht="93">
+    <row r="227" spans="1:18" ht="94.8" x14ac:dyDescent="0.9">
       <c r="A227" s="3" t="s">
         <v>693</v>
       </c>
@@ -12298,7 +12376,7 @@
       <c r="Q227" s="3"/>
       <c r="R227" s="3"/>
     </row>
-    <row r="228" spans="1:18" ht="93">
+    <row r="228" spans="1:18" ht="94.8" x14ac:dyDescent="0.9">
       <c r="A228" s="3" t="s">
         <v>696</v>
       </c>
@@ -12329,6 +12407,306 @@
       <c r="P228" s="3"/>
       <c r="Q228" s="3"/>
       <c r="R228" s="3"/>
+    </row>
+    <row r="229" spans="1:18" ht="94.8" x14ac:dyDescent="0.9">
+      <c r="A229" s="53" t="s">
+        <v>699</v>
+      </c>
+      <c r="B229" s="53">
+        <v>13</v>
+      </c>
+      <c r="C229" s="54" t="s">
+        <v>700</v>
+      </c>
+      <c r="D229" s="3"/>
+      <c r="E229" s="3"/>
+      <c r="F229" s="55"/>
+      <c r="G229" s="3"/>
+      <c r="H229" s="3"/>
+      <c r="I229" s="3"/>
+      <c r="J229" s="3"/>
+      <c r="K229" s="3"/>
+      <c r="L229" s="3"/>
+      <c r="M229" s="3"/>
+      <c r="N229" s="3"/>
+      <c r="O229" s="3"/>
+      <c r="P229" s="3"/>
+      <c r="Q229" s="3"/>
+      <c r="R229" s="3"/>
+    </row>
+    <row r="230" spans="1:18" ht="94.8" x14ac:dyDescent="0.9">
+      <c r="A230" s="53" t="s">
+        <v>701</v>
+      </c>
+      <c r="B230" s="53">
+        <v>13</v>
+      </c>
+      <c r="C230" s="54" t="s">
+        <v>702</v>
+      </c>
+      <c r="D230" s="3"/>
+      <c r="E230" s="3"/>
+      <c r="F230" s="55"/>
+      <c r="G230" s="3"/>
+      <c r="H230" s="3"/>
+      <c r="I230" s="3"/>
+      <c r="J230" s="3"/>
+      <c r="K230" s="3"/>
+      <c r="L230" s="3"/>
+      <c r="M230" s="3"/>
+      <c r="N230" s="3"/>
+      <c r="O230" s="3"/>
+      <c r="P230" s="3"/>
+      <c r="Q230" s="3"/>
+      <c r="R230" s="3"/>
+    </row>
+    <row r="231" spans="1:18" ht="94.8" x14ac:dyDescent="0.9">
+      <c r="A231" s="53" t="s">
+        <v>703</v>
+      </c>
+      <c r="B231" s="53">
+        <v>13</v>
+      </c>
+      <c r="C231" s="54" t="s">
+        <v>704</v>
+      </c>
+      <c r="D231" s="3"/>
+      <c r="E231" s="3"/>
+      <c r="F231" s="55"/>
+      <c r="G231" s="3"/>
+      <c r="H231" s="3"/>
+      <c r="I231" s="3"/>
+      <c r="J231" s="3"/>
+      <c r="K231" s="3"/>
+      <c r="L231" s="3"/>
+      <c r="M231" s="3"/>
+      <c r="N231" s="3"/>
+      <c r="O231" s="3"/>
+      <c r="P231" s="3"/>
+      <c r="Q231" s="3"/>
+      <c r="R231" s="3"/>
+    </row>
+    <row r="232" spans="1:18" ht="94.8" x14ac:dyDescent="0.9">
+      <c r="A232" s="53" t="s">
+        <v>705</v>
+      </c>
+      <c r="B232" s="53">
+        <v>13</v>
+      </c>
+      <c r="C232" s="54" t="s">
+        <v>706</v>
+      </c>
+      <c r="D232" s="3"/>
+      <c r="E232" s="3"/>
+      <c r="F232" s="55"/>
+      <c r="G232" s="3"/>
+      <c r="H232" s="3"/>
+      <c r="I232" s="3"/>
+      <c r="J232" s="3"/>
+      <c r="K232" s="3"/>
+      <c r="L232" s="3"/>
+      <c r="M232" s="3"/>
+      <c r="N232" s="3"/>
+      <c r="O232" s="3"/>
+      <c r="P232" s="3"/>
+      <c r="Q232" s="3"/>
+      <c r="R232" s="3"/>
+    </row>
+    <row r="233" spans="1:18" ht="142.19999999999999" x14ac:dyDescent="0.9">
+      <c r="A233" s="53" t="s">
+        <v>707</v>
+      </c>
+      <c r="B233" s="53">
+        <v>13</v>
+      </c>
+      <c r="C233" s="54" t="s">
+        <v>708</v>
+      </c>
+      <c r="D233" s="3"/>
+      <c r="E233" s="3"/>
+      <c r="F233" s="55"/>
+      <c r="G233" s="3"/>
+      <c r="H233" s="3"/>
+      <c r="I233" s="3"/>
+      <c r="J233" s="3"/>
+      <c r="K233" s="3"/>
+      <c r="L233" s="3"/>
+      <c r="M233" s="3"/>
+      <c r="N233" s="3"/>
+      <c r="O233" s="3"/>
+      <c r="P233" s="3"/>
+      <c r="Q233" s="3"/>
+      <c r="R233" s="3"/>
+    </row>
+    <row r="234" spans="1:18" ht="94.8" x14ac:dyDescent="0.9">
+      <c r="A234" s="53" t="s">
+        <v>709</v>
+      </c>
+      <c r="B234" s="53">
+        <v>13</v>
+      </c>
+      <c r="C234" s="54" t="s">
+        <v>710</v>
+      </c>
+      <c r="D234" s="3"/>
+      <c r="E234" s="3"/>
+      <c r="F234" s="55"/>
+      <c r="G234" s="3"/>
+      <c r="H234" s="3"/>
+      <c r="I234" s="3"/>
+      <c r="J234" s="3"/>
+      <c r="K234" s="3"/>
+      <c r="L234" s="3"/>
+      <c r="M234" s="3"/>
+      <c r="N234" s="3"/>
+      <c r="O234" s="3"/>
+      <c r="P234" s="3"/>
+      <c r="Q234" s="3"/>
+      <c r="R234" s="3"/>
+    </row>
+    <row r="235" spans="1:18" ht="142.19999999999999" x14ac:dyDescent="0.9">
+      <c r="A235" s="53" t="s">
+        <v>711</v>
+      </c>
+      <c r="B235" s="53">
+        <v>13</v>
+      </c>
+      <c r="C235" s="54" t="s">
+        <v>712</v>
+      </c>
+      <c r="D235" s="3"/>
+      <c r="E235" s="3"/>
+      <c r="F235" s="55"/>
+      <c r="G235" s="3"/>
+      <c r="H235" s="3"/>
+      <c r="I235" s="3"/>
+      <c r="J235" s="3"/>
+      <c r="K235" s="3"/>
+      <c r="L235" s="3"/>
+      <c r="M235" s="3"/>
+      <c r="N235" s="3"/>
+      <c r="O235" s="3"/>
+      <c r="P235" s="3"/>
+      <c r="Q235" s="3"/>
+      <c r="R235" s="3"/>
+    </row>
+    <row r="236" spans="1:18" ht="142.19999999999999" x14ac:dyDescent="0.9">
+      <c r="A236" s="53" t="s">
+        <v>713</v>
+      </c>
+      <c r="B236" s="53">
+        <v>13</v>
+      </c>
+      <c r="C236" s="54" t="s">
+        <v>714</v>
+      </c>
+      <c r="D236" s="3"/>
+      <c r="E236" s="3"/>
+      <c r="F236" s="55"/>
+      <c r="G236" s="3"/>
+      <c r="H236" s="3"/>
+      <c r="I236" s="3"/>
+      <c r="J236" s="3"/>
+      <c r="K236" s="3"/>
+      <c r="L236" s="3"/>
+      <c r="M236" s="3"/>
+      <c r="N236" s="3"/>
+      <c r="O236" s="3"/>
+      <c r="P236" s="3"/>
+      <c r="Q236" s="3"/>
+      <c r="R236" s="3"/>
+    </row>
+    <row r="237" spans="1:18" ht="142.19999999999999" x14ac:dyDescent="0.9">
+      <c r="A237" s="53" t="s">
+        <v>715</v>
+      </c>
+      <c r="B237" s="53">
+        <v>13</v>
+      </c>
+      <c r="C237" s="54" t="s">
+        <v>716</v>
+      </c>
+      <c r="D237" s="3"/>
+      <c r="E237" s="3"/>
+      <c r="F237" s="55"/>
+      <c r="G237" s="3"/>
+      <c r="H237" s="3"/>
+      <c r="I237" s="3"/>
+      <c r="J237" s="3"/>
+      <c r="K237" s="3"/>
+      <c r="L237" s="3"/>
+      <c r="M237" s="3"/>
+      <c r="N237" s="3"/>
+      <c r="O237" s="3"/>
+      <c r="P237" s="3"/>
+      <c r="Q237" s="3"/>
+      <c r="R237" s="3"/>
+    </row>
+    <row r="238" spans="1:18" ht="94.8" x14ac:dyDescent="0.9">
+      <c r="A238" s="53" t="s">
+        <v>717</v>
+      </c>
+      <c r="B238" s="53">
+        <v>13</v>
+      </c>
+      <c r="C238" s="54" t="s">
+        <v>718</v>
+      </c>
+      <c r="D238" s="3"/>
+      <c r="E238" s="3"/>
+      <c r="F238" s="55"/>
+      <c r="G238" s="3"/>
+      <c r="H238" s="3"/>
+      <c r="I238" s="3"/>
+      <c r="J238" s="3"/>
+      <c r="K238" s="3"/>
+      <c r="L238" s="3"/>
+      <c r="M238" s="3"/>
+      <c r="N238" s="3"/>
+      <c r="O238" s="3"/>
+      <c r="P238" s="3"/>
+      <c r="Q238" s="3"/>
+      <c r="R238" s="3"/>
+    </row>
+    <row r="239" spans="1:18" x14ac:dyDescent="0.9">
+      <c r="A239" s="3"/>
+      <c r="B239" s="3"/>
+      <c r="C239" s="4"/>
+      <c r="D239" s="3"/>
+      <c r="E239" s="3"/>
+      <c r="F239" s="55"/>
+      <c r="G239" s="3"/>
+      <c r="H239" s="3"/>
+      <c r="I239" s="3"/>
+      <c r="J239" s="3"/>
+      <c r="K239" s="3"/>
+      <c r="L239" s="3"/>
+      <c r="M239" s="3"/>
+      <c r="N239" s="3"/>
+      <c r="O239" s="3"/>
+      <c r="P239" s="3"/>
+      <c r="Q239" s="3"/>
+      <c r="R239" s="3"/>
+    </row>
+    <row r="240" spans="1:18" x14ac:dyDescent="0.9">
+      <c r="A240" s="3"/>
+      <c r="B240" s="3"/>
+      <c r="C240" s="4"/>
+      <c r="D240" s="3"/>
+      <c r="E240" s="3"/>
+      <c r="F240" s="55"/>
+      <c r="G240" s="3"/>
+      <c r="H240" s="3"/>
+      <c r="I240" s="3"/>
+      <c r="J240" s="3"/>
+      <c r="K240" s="3"/>
+      <c r="L240" s="3"/>
+      <c r="M240" s="3"/>
+      <c r="N240" s="3"/>
+      <c r="O240" s="3"/>
+      <c r="P240" s="3"/>
+      <c r="Q240" s="3"/>
+      <c r="R240" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -12349,15 +12727,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000470215BC4A30A4187D23D62A4EC96F3" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0276ec8e258d46ff7cd3f9c3f2a1b5d7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="687acdf3-ad85-4bdb-a62b-77fce9e2a613" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fc2a4560534904d2742450f63d0b5b2b" ns3:_="">
     <xsd:import namespace="687acdf3-ad85-4bdb-a62b-77fce9e2a613"/>
@@ -12513,14 +12882,47 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{348A41D9-E042-4893-9C37-7D13B167F5BD}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{348A41D9-E042-4893-9C37-7D13B167F5BD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="687acdf3-ad85-4bdb-a62b-77fce9e2a613"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F79A7D57-BF41-4B12-9712-226D862B76C0}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{12CE1AE3-5F37-4838-9901-BD8B31E4F67F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="687acdf3-ad85-4bdb-a62b-77fce9e2a613"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{12CE1AE3-5F37-4838-9901-BD8B31E4F67F}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F79A7D57-BF41-4B12-9712-226D862B76C0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added testing for group 15 and 14
</commit_message>
<xml_diff>
--- a/FinalRequirements.xlsx
+++ b/FinalRequirements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mavsuta-my.sharepoint.com/personal/axr0602_mavs_uta_edu/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\18173\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1060BA44-E407-4F4A-9FCA-34447C6BB144}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA080D1D-5EB5-44B9-B54A-3705885527F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="23260" windowHeight="13900" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
   <metadataTypes count="1">
     <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
-  <futureMetadata name="XLRICHVALUE" count="4">
+  <futureMetadata name="XLRICHVALUE" count="24">
     <bk>
       <extLst>
         <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
@@ -72,8 +72,148 @@
         </ext>
       </extLst>
     </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="4"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="5"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="6"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="7"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="8"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="9"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="10"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="11"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="12"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="13"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="14"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="15"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="16"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="17"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="18"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="19"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="20"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="21"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="22"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="23"/>
+        </ext>
+      </extLst>
+    </bk>
   </futureMetadata>
-  <valueMetadata count="4">
+  <valueMetadata count="24">
     <bk>
       <rc t="1" v="0"/>
     </bk>
@@ -86,12 +226,72 @@
     <bk>
       <rc t="1" v="3"/>
     </bk>
+    <bk>
+      <rc t="1" v="4"/>
+    </bk>
+    <bk>
+      <rc t="1" v="5"/>
+    </bk>
+    <bk>
+      <rc t="1" v="6"/>
+    </bk>
+    <bk>
+      <rc t="1" v="7"/>
+    </bk>
+    <bk>
+      <rc t="1" v="8"/>
+    </bk>
+    <bk>
+      <rc t="1" v="9"/>
+    </bk>
+    <bk>
+      <rc t="1" v="10"/>
+    </bk>
+    <bk>
+      <rc t="1" v="11"/>
+    </bk>
+    <bk>
+      <rc t="1" v="12"/>
+    </bk>
+    <bk>
+      <rc t="1" v="13"/>
+    </bk>
+    <bk>
+      <rc t="1" v="14"/>
+    </bk>
+    <bk>
+      <rc t="1" v="15"/>
+    </bk>
+    <bk>
+      <rc t="1" v="16"/>
+    </bk>
+    <bk>
+      <rc t="1" v="17"/>
+    </bk>
+    <bk>
+      <rc t="1" v="18"/>
+    </bk>
+    <bk>
+      <rc t="1" v="19"/>
+    </bk>
+    <bk>
+      <rc t="1" v="20"/>
+    </bk>
+    <bk>
+      <rc t="1" v="21"/>
+    </bk>
+    <bk>
+      <rc t="1" v="22"/>
+    </bk>
+    <bk>
+      <rc t="1" v="23"/>
+    </bk>
   </valueMetadata>
 </metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1269" uniqueCount="719">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1371" uniqueCount="750">
   <si>
     <t>Testing</t>
   </si>
@@ -2403,12 +2603,117 @@
   <si>
     <t>Websockets will be used for communication between the Java backend, Database and JavaScript frontend.</t>
   </si>
+  <si>
+    <t>The page is not showing 
+the username of the player
+who joined, it is just showing 
+Player 1 or player 2</t>
+  </si>
+  <si>
+    <t>Yes the page shows the 
+2 bots are in the lobby</t>
+  </si>
+  <si>
+    <t>Yes the page shows the 
+10 lobbies that users can join</t>
+  </si>
+  <si>
+    <t>Yes the page shows the 
+back button but it is not functioning , i.e nothing happens.</t>
+  </si>
+  <si>
+    <t>Yes the page shows the 
+list of available lobbies</t>
+  </si>
+  <si>
+    <t>Single user is not able to join the lobby, if 2 players/Bot is there then directly enter the game but can't wait in lobby</t>
+  </si>
+  <si>
+    <t>No the page does not show the current status of the lobby.</t>
+  </si>
+  <si>
+    <t>Page does not shows the number of players in the lobby</t>
+  </si>
+  <si>
+    <t>Since there is no any interface for lobby, user cannot leave the lobby</t>
+  </si>
+  <si>
+    <t>Does not have "Start Game" button</t>
+  </si>
+  <si>
+    <t>No any error message</t>
+  </si>
+  <si>
+    <t>Color of the button
+changes but button has no function</t>
+  </si>
+  <si>
+    <t>User can add the 
+Bot I/BotII</t>
+  </si>
+  <si>
+    <t>No any waiting message
+was displayed</t>
+  </si>
+  <si>
+    <t>Since there is no any interface for lobby, user cannot see which lobby they are in</t>
+  </si>
+  <si>
+    <t>User are able to leave the game but it goes to create account/login page</t>
+  </si>
+  <si>
+    <t>Since there is no any interface for lobby, user cannot see any progress</t>
+  </si>
+  <si>
+    <t>Page is not showing any 
+users</t>
+  </si>
+  <si>
+    <t>Bot is not responding</t>
+  </si>
+  <si>
+    <t>Bot is not showing any legal moves</t>
+  </si>
+  <si>
+    <t>not testable since every piece has 
+been moving illegally</t>
+  </si>
+  <si>
+    <t>Not testable</t>
+  </si>
+  <si>
+    <t>invalid move</t>
+  </si>
+  <si>
+    <t>Move a regular piece to the opponent’s last row</t>
+  </si>
+  <si>
+    <t>Move a red regular piece backward</t>
+  </si>
+  <si>
+    <t>Move a king piece backward</t>
+  </si>
+  <si>
+    <t>Move to a light square</t>
+  </si>
+  <si>
+    <t>show current board</t>
+  </si>
+  <si>
+    <t>lobby will show 1 player</t>
+  </si>
+  <si>
+    <t>Lobby created with human and bot,</t>
+  </si>
+  <si>
+    <t>show open lobbies</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2465,6 +2770,12 @@
       <family val="1"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="36"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -2504,7 +2815,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -2633,11 +2944,71 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -2762,6 +3133,19 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4334,6 +4718,244 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>571680</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>945720</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>9890243</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>2276640</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="38" name="Picture 37">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E364C7C3-2D8B-400F-9927-00125C994529}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId29"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="95554980" y="29558820"/>
+          <a:ext cx="5071320" cy="1330920"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>571680</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>945720</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>11759093</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>2276640</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="40" name="Picture 39">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D61B4D5A-ECBA-4280-B095-BF16C16B5551}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId29"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="95554980" y="29558820"/>
+          <a:ext cx="6940170" cy="1330920"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>253999</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>9890387</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>1585450</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="42" name="Picture 41">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0EC8D694-F111-436D-B559-3FA732E73DF5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId29">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="95554800" y="28867099"/>
+          <a:ext cx="5071644" cy="1331451"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>1333501</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>187502</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>6319763</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>2146475</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="43" name="Picture 42">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C54E22C8-CDA3-4492-A6DA-7FB33A784281}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId30">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="96371834" y="7505121"/>
+          <a:ext cx="4986262" cy="1958973"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>253999</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>11759293</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>1585450</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="44" name="Picture 43">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{179288C1-2A7A-407D-91E1-C76CFD82E1F3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId29">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="95554800" y="28867099"/>
+          <a:ext cx="6940550" cy="1331451"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4378,7 +5000,7 @@
 </file>
 
 <file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
-<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="4">
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="24">
   <rv s="0">
     <v>0</v>
     <v>5</v>
@@ -4393,6 +5015,86 @@
   </rv>
   <rv s="0">
     <v>3</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>4</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>5</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>6</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>7</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>8</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>9</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>10</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>11</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>12</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>13</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>14</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>15</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>16</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>17</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>18</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>19</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>20</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>21</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>22</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>23</v>
     <v>5</v>
   </rv>
 </rvData>
@@ -4413,6 +5115,26 @@
   <rel r:id="rId2"/>
   <rel r:id="rId3"/>
   <rel r:id="rId4"/>
+  <rel r:id="rId5"/>
+  <rel r:id="rId6"/>
+  <rel r:id="rId7"/>
+  <rel r:id="rId8"/>
+  <rel r:id="rId9"/>
+  <rel r:id="rId10"/>
+  <rel r:id="rId11"/>
+  <rel r:id="rId12"/>
+  <rel r:id="rId13"/>
+  <rel r:id="rId14"/>
+  <rel r:id="rId15"/>
+  <rel r:id="rId16"/>
+  <rel r:id="rId17"/>
+  <rel r:id="rId18"/>
+  <rel r:id="rId19"/>
+  <rel r:id="rId20"/>
+  <rel r:id="rId21"/>
+  <rel r:id="rId22"/>
+  <rel r:id="rId23"/>
+  <rel r:id="rId24"/>
 </richValueRels>
 </file>
 
@@ -4540,41 +5262,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:T240"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I211" zoomScale="21" zoomScaleNormal="28" workbookViewId="0">
-      <selection activeCell="P217" sqref="P217"/>
+    <sheetView tabSelected="1" topLeftCell="H9" zoomScale="21" zoomScaleNormal="28" workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="47"/>
+  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="47.5" x14ac:dyDescent="1.1000000000000001"/>
   <cols>
     <col min="1" max="1" width="21" style="1" customWidth="1"/>
-    <col min="2" max="2" width="19.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="161.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="250.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="210.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="164.33203125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="104.33203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="34.6640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="30.1640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="165.33203125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="34.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.453125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="161.453125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="250.36328125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="210.6328125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="164.36328125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="104.36328125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="34.6328125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="30.1796875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="165.36328125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="34.1796875" style="1" customWidth="1"/>
     <col min="12" max="12" width="131" style="1" customWidth="1"/>
     <col min="13" max="13" width="33" style="1" customWidth="1"/>
-    <col min="14" max="14" width="46.5" style="1" customWidth="1"/>
+    <col min="14" max="14" width="187.6328125" style="1" customWidth="1"/>
     <col min="15" max="15" width="33" style="1" customWidth="1"/>
     <col min="16" max="16" width="133" style="1" customWidth="1"/>
     <col min="17" max="17" width="158" style="1" customWidth="1"/>
-    <col min="18" max="18" width="40.1640625" style="1" customWidth="1"/>
-    <col min="19" max="19" width="8.6640625" style="1"/>
-    <col min="20" max="20" width="153.1640625" style="1" customWidth="1"/>
-    <col min="21" max="16384" width="8.6640625" style="1"/>
+    <col min="18" max="18" width="40.1796875" style="1" customWidth="1"/>
+    <col min="19" max="19" width="8.6328125" style="1"/>
+    <col min="20" max="20" width="153.1796875" style="1" customWidth="1"/>
+    <col min="21" max="16384" width="8.6328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:20" ht="48" thickBot="1" x14ac:dyDescent="1.1499999999999999">
       <c r="L2" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="48">
+    <row r="3" spans="1:20" ht="48" thickBot="1" x14ac:dyDescent="1.1499999999999999">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -4614,7 +5336,7 @@
       <c r="M3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="N3" s="56" t="s">
         <v>14</v>
       </c>
       <c r="O3" s="3" t="s">
@@ -4630,7 +5352,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="144">
+    <row r="4" spans="1:20" ht="142.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A4" s="8" t="s">
         <v>19</v>
       </c>
@@ -4661,7 +5383,9 @@
       <c r="M4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="N4" s="3"/>
+      <c r="N4" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="O4" s="3"/>
       <c r="P4" s="3" t="s">
         <v>22</v>
@@ -4672,7 +5396,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="291" customHeight="1">
+    <row r="5" spans="1:20" ht="291" customHeight="1" x14ac:dyDescent="1.1000000000000001">
       <c r="A5" s="8" t="s">
         <v>25</v>
       </c>
@@ -4700,13 +5424,15 @@
         <v>#VALUE!</v>
       </c>
       <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
+      <c r="N5" s="4" t="s">
+        <v>719</v>
+      </c>
       <c r="O5" s="3"/>
       <c r="P5" s="3"/>
       <c r="Q5" s="3"/>
       <c r="R5" s="3"/>
     </row>
-    <row r="6" spans="1:20" ht="285.75" customHeight="1">
+    <row r="6" spans="1:20" ht="285.75" customHeight="1" x14ac:dyDescent="1.1000000000000001">
       <c r="A6" s="8" t="s">
         <v>28</v>
       </c>
@@ -4734,13 +5460,15 @@
         <v>#VALUE!</v>
       </c>
       <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
+      <c r="N6" s="4" t="s">
+        <v>720</v>
+      </c>
       <c r="O6" s="3"/>
       <c r="P6" s="3"/>
       <c r="Q6" s="3"/>
       <c r="R6" s="3"/>
     </row>
-    <row r="7" spans="1:20" ht="287.25" customHeight="1">
+    <row r="7" spans="1:20" ht="287.25" customHeight="1" x14ac:dyDescent="1.1000000000000001">
       <c r="A7" s="8" t="s">
         <v>31</v>
       </c>
@@ -4768,13 +5496,15 @@
         <v>#VALUE!</v>
       </c>
       <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
+      <c r="N7" s="4" t="s">
+        <v>721</v>
+      </c>
       <c r="O7" s="3"/>
       <c r="P7" s="3"/>
       <c r="Q7" s="3"/>
       <c r="R7" s="3"/>
     </row>
-    <row r="8" spans="1:20" ht="329.25" customHeight="1">
+    <row r="8" spans="1:20" ht="329.25" customHeight="1" x14ac:dyDescent="1.1000000000000001">
       <c r="A8" s="8" t="s">
         <v>34</v>
       </c>
@@ -4802,13 +5532,15 @@
         <v>#VALUE!</v>
       </c>
       <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
+      <c r="N8" s="4" t="s">
+        <v>722</v>
+      </c>
       <c r="O8" s="3"/>
       <c r="P8" s="3"/>
       <c r="Q8" s="3"/>
       <c r="R8" s="3"/>
     </row>
-    <row r="9" spans="1:20" ht="140">
+    <row r="9" spans="1:20" ht="139.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A9" s="8" t="s">
         <v>37</v>
       </c>
@@ -4836,7 +5568,9 @@
         <v>39</v>
       </c>
       <c r="M9" s="3"/>
-      <c r="N9" s="3"/>
+      <c r="N9" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="O9" s="3"/>
       <c r="P9" s="3" t="s">
         <v>39</v>
@@ -4844,7 +5578,7 @@
       <c r="Q9" s="3"/>
       <c r="R9" s="3"/>
     </row>
-    <row r="10" spans="1:20" ht="318" customHeight="1">
+    <row r="10" spans="1:20" ht="318" customHeight="1" x14ac:dyDescent="1.1000000000000001">
       <c r="A10" s="8" t="s">
         <v>40</v>
       </c>
@@ -4875,13 +5609,15 @@
       <c r="M10" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="N10" s="3"/>
+      <c r="N10" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="O10" s="3"/>
       <c r="P10" s="3"/>
       <c r="Q10" s="3"/>
       <c r="R10" s="3"/>
     </row>
-    <row r="11" spans="1:20" ht="318" customHeight="1">
+    <row r="11" spans="1:20" ht="318" customHeight="1" x14ac:dyDescent="1.1000000000000001">
       <c r="A11" s="8" t="s">
         <v>44</v>
       </c>
@@ -4912,7 +5648,9 @@
       <c r="M11" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="N11" s="3"/>
+      <c r="N11" s="4" t="s">
+        <v>723</v>
+      </c>
       <c r="O11" s="3"/>
       <c r="P11" s="3" t="s">
         <v>49</v>
@@ -4920,7 +5658,7 @@
       <c r="Q11" s="3"/>
       <c r="R11" s="3"/>
     </row>
-    <row r="12" spans="1:20" ht="334.5" customHeight="1">
+    <row r="12" spans="1:20" ht="334.5" customHeight="1" x14ac:dyDescent="1.1000000000000001">
       <c r="A12" s="8" t="s">
         <v>50</v>
       </c>
@@ -4950,7 +5688,9 @@
         <v>#VALUE!</v>
       </c>
       <c r="M12" s="3"/>
-      <c r="N12" s="3"/>
+      <c r="N12" s="4" t="s">
+        <v>724</v>
+      </c>
       <c r="O12" s="3"/>
       <c r="P12" s="3" t="s">
         <v>54</v>
@@ -4958,7 +5698,7 @@
       <c r="Q12" s="3"/>
       <c r="R12" s="3"/>
     </row>
-    <row r="13" spans="1:20" ht="313.5" customHeight="1">
+    <row r="13" spans="1:20" ht="313.5" customHeight="1" x14ac:dyDescent="1.1000000000000001">
       <c r="A13" s="8" t="s">
         <v>55</v>
       </c>
@@ -4989,13 +5729,15 @@
       <c r="M13" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="N13" s="3"/>
+      <c r="N13" s="4" t="s">
+        <v>725</v>
+      </c>
       <c r="O13" s="3"/>
       <c r="P13" s="3"/>
       <c r="Q13" s="3"/>
       <c r="R13" s="3"/>
     </row>
-    <row r="14" spans="1:20" ht="249.75" customHeight="1">
+    <row r="14" spans="1:20" ht="249.75" customHeight="1" x14ac:dyDescent="1.1000000000000001">
       <c r="A14" s="8" t="s">
         <v>60</v>
       </c>
@@ -5026,13 +5768,15 @@
       <c r="M14" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="N14" s="3"/>
+      <c r="N14" s="4" t="s">
+        <v>726</v>
+      </c>
       <c r="O14" s="3"/>
       <c r="P14" s="3"/>
       <c r="Q14" s="3"/>
       <c r="R14" s="3"/>
     </row>
-    <row r="15" spans="1:20" ht="399.75" customHeight="1">
+    <row r="15" spans="1:20" ht="399.75" customHeight="1" x14ac:dyDescent="1.1000000000000001">
       <c r="A15" s="8" t="s">
         <v>65</v>
       </c>
@@ -5063,7 +5807,9 @@
       <c r="M15" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="N15" s="3"/>
+      <c r="N15" s="4" t="s">
+        <v>727</v>
+      </c>
       <c r="O15" s="3"/>
       <c r="P15" s="3" t="s">
         <v>70</v>
@@ -5071,7 +5817,7 @@
       <c r="Q15" s="3"/>
       <c r="R15" s="3"/>
     </row>
-    <row r="16" spans="1:20" ht="186">
+    <row r="16" spans="1:20" ht="185.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A16" s="8" t="s">
         <v>71</v>
       </c>
@@ -5099,13 +5845,15 @@
       <c r="M16" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="N16" s="3"/>
+      <c r="N16" s="4" t="s">
+        <v>728</v>
+      </c>
       <c r="O16" s="3"/>
       <c r="P16" s="3"/>
       <c r="Q16" s="3"/>
       <c r="R16" s="3"/>
     </row>
-    <row r="17" spans="1:18" ht="249.75" customHeight="1">
+    <row r="17" spans="1:18" ht="249.75" customHeight="1" x14ac:dyDescent="1.1000000000000001">
       <c r="A17" s="8" t="s">
         <v>76</v>
       </c>
@@ -5134,13 +5882,15 @@
       <c r="M17" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="N17" s="3"/>
+      <c r="N17" s="3" t="s">
+        <v>729</v>
+      </c>
       <c r="O17" s="3"/>
       <c r="P17" s="3"/>
       <c r="Q17" s="3"/>
       <c r="R17" s="3"/>
     </row>
-    <row r="18" spans="1:18" ht="249.75" customHeight="1">
+    <row r="18" spans="1:18" ht="249.75" customHeight="1" x14ac:dyDescent="1.1000000000000001">
       <c r="A18" s="8" t="s">
         <v>81</v>
       </c>
@@ -5167,13 +5917,15 @@
         <v>23</v>
       </c>
       <c r="M18" s="10"/>
-      <c r="N18" s="3"/>
+      <c r="N18" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="O18" s="3"/>
       <c r="P18" s="3"/>
       <c r="Q18" s="3"/>
       <c r="R18" s="3"/>
     </row>
-    <row r="19" spans="1:18" ht="94">
+    <row r="19" spans="1:18" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A19" s="8" t="s">
         <v>84</v>
       </c>
@@ -5199,13 +5951,15 @@
       <c r="M19" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="N19" s="3"/>
+      <c r="N19" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="O19" s="3"/>
       <c r="P19" s="3"/>
       <c r="Q19" s="3"/>
       <c r="R19" s="3"/>
     </row>
-    <row r="20" spans="1:18" ht="249.75" customHeight="1">
+    <row r="20" spans="1:18" ht="249.75" customHeight="1" x14ac:dyDescent="1.1000000000000001">
       <c r="A20" s="8" t="s">
         <v>87</v>
       </c>
@@ -5234,13 +5988,15 @@
       <c r="M20" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="N20" s="3"/>
+      <c r="N20" s="4" t="s">
+        <v>730</v>
+      </c>
       <c r="O20" s="3"/>
       <c r="P20" s="3"/>
       <c r="Q20" s="3"/>
       <c r="R20" s="3"/>
     </row>
-    <row r="21" spans="1:18" ht="199.5" customHeight="1">
+    <row r="21" spans="1:18" ht="199.5" customHeight="1" x14ac:dyDescent="1.1000000000000001">
       <c r="A21" s="8" t="s">
         <v>91</v>
       </c>
@@ -5269,13 +6025,15 @@
       <c r="M21" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="N21" s="3"/>
+      <c r="N21" s="4" t="s">
+        <v>731</v>
+      </c>
       <c r="O21" s="3"/>
       <c r="P21" s="3"/>
       <c r="Q21" s="3"/>
       <c r="R21" s="3"/>
     </row>
-    <row r="22" spans="1:18" ht="349.5" customHeight="1">
+    <row r="22" spans="1:18" ht="349.5" customHeight="1" x14ac:dyDescent="1.1000000000000001">
       <c r="A22" s="8" t="s">
         <v>95</v>
       </c>
@@ -5302,13 +6060,15 @@
         <v>23</v>
       </c>
       <c r="M22" s="10"/>
-      <c r="N22" s="3"/>
+      <c r="N22" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="O22" s="3"/>
       <c r="P22" s="3"/>
       <c r="Q22" s="3"/>
       <c r="R22" s="3"/>
     </row>
-    <row r="23" spans="1:18" ht="300" customHeight="1">
+    <row r="23" spans="1:18" ht="300" customHeight="1" x14ac:dyDescent="1.1000000000000001">
       <c r="A23" s="8" t="s">
         <v>98</v>
       </c>
@@ -5335,13 +6095,15 @@
         <v>23</v>
       </c>
       <c r="M23" s="10"/>
-      <c r="N23" s="3"/>
+      <c r="N23" s="4" t="s">
+        <v>732</v>
+      </c>
       <c r="O23" s="3"/>
       <c r="P23" s="3"/>
       <c r="Q23" s="3"/>
       <c r="R23" s="3"/>
     </row>
-    <row r="24" spans="1:18" ht="349.5" customHeight="1">
+    <row r="24" spans="1:18" ht="349.5" customHeight="1" x14ac:dyDescent="1.1000000000000001">
       <c r="A24" s="8" t="s">
         <v>101</v>
       </c>
@@ -5368,13 +6130,15 @@
         <v>23</v>
       </c>
       <c r="M24" s="10"/>
-      <c r="N24" s="3"/>
+      <c r="N24" s="4" t="s">
+        <v>733</v>
+      </c>
       <c r="O24" s="3"/>
       <c r="P24" s="3"/>
       <c r="Q24" s="3"/>
       <c r="R24" s="3"/>
     </row>
-    <row r="25" spans="1:18" ht="349.5" customHeight="1">
+    <row r="25" spans="1:18" ht="349.5" customHeight="1" x14ac:dyDescent="1.1000000000000001">
       <c r="A25" s="8" t="s">
         <v>104</v>
       </c>
@@ -5401,13 +6165,15 @@
         <v>23</v>
       </c>
       <c r="M25" s="10"/>
-      <c r="N25" s="3"/>
+      <c r="N25" s="4" t="s">
+        <v>734</v>
+      </c>
       <c r="O25" s="3"/>
       <c r="P25" s="3"/>
       <c r="Q25" s="3"/>
       <c r="R25" s="3"/>
     </row>
-    <row r="26" spans="1:18" ht="349.5" customHeight="1">
+    <row r="26" spans="1:18" ht="349.5" customHeight="1" x14ac:dyDescent="1.1000000000000001">
       <c r="A26" s="8" t="s">
         <v>107</v>
       </c>
@@ -5434,13 +6200,15 @@
         <v>23</v>
       </c>
       <c r="M26" s="10"/>
-      <c r="N26" s="3"/>
+      <c r="N26" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="O26" s="3"/>
       <c r="P26" s="3"/>
       <c r="Q26" s="3"/>
       <c r="R26" s="3"/>
     </row>
-    <row r="27" spans="1:18" ht="399.75" customHeight="1">
+    <row r="27" spans="1:18" ht="399.75" customHeight="1" x14ac:dyDescent="1.1000000000000001">
       <c r="A27" s="8" t="s">
         <v>110</v>
       </c>
@@ -5467,13 +6235,15 @@
         <v>23</v>
       </c>
       <c r="M27" s="10"/>
-      <c r="N27" s="3"/>
+      <c r="N27" s="4" t="s">
+        <v>735</v>
+      </c>
       <c r="O27" s="3"/>
       <c r="P27" s="3"/>
       <c r="Q27" s="3"/>
       <c r="R27" s="3"/>
     </row>
-    <row r="28" spans="1:18" ht="300" customHeight="1">
+    <row r="28" spans="1:18" ht="300" customHeight="1" x14ac:dyDescent="1.1000000000000001">
       <c r="A28" s="10" t="s">
         <v>113</v>
       </c>
@@ -5500,13 +6270,15 @@
         <v>23</v>
       </c>
       <c r="M28" s="10"/>
-      <c r="N28" s="3"/>
+      <c r="N28" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="O28" s="3"/>
       <c r="P28" s="3"/>
       <c r="Q28" s="3"/>
       <c r="R28" s="3"/>
     </row>
-    <row r="29" spans="1:18" ht="94.5" customHeight="1">
+    <row r="29" spans="1:18" ht="94.5" customHeight="1" x14ac:dyDescent="1.1000000000000001">
       <c r="A29" s="10" t="s">
         <v>116</v>
       </c>
@@ -5535,7 +6307,9 @@
         <v>39</v>
       </c>
       <c r="M29" s="10"/>
-      <c r="N29" s="3"/>
+      <c r="N29" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="O29" s="3"/>
       <c r="P29" s="3" t="s">
         <v>39</v>
@@ -5545,7 +6319,7 @@
       </c>
       <c r="R29" s="3"/>
     </row>
-    <row r="30" spans="1:18" ht="349.5" customHeight="1">
+    <row r="30" spans="1:18" ht="349.5" customHeight="1" x14ac:dyDescent="1.1000000000000001">
       <c r="A30" s="10" t="s">
         <v>119</v>
       </c>
@@ -5572,7 +6346,9 @@
         <v>23</v>
       </c>
       <c r="M30" s="10"/>
-      <c r="N30" s="3"/>
+      <c r="N30" s="4" t="s">
+        <v>736</v>
+      </c>
       <c r="O30" s="3"/>
       <c r="P30" s="3" t="s">
         <v>39</v>
@@ -5582,7 +6358,7 @@
       </c>
       <c r="R30" s="3"/>
     </row>
-    <row r="31" spans="1:18" ht="349.5" customHeight="1">
+    <row r="31" spans="1:18" ht="349.5" customHeight="1" x14ac:dyDescent="1.1000000000000001">
       <c r="A31" s="8" t="s">
         <v>122</v>
       </c>
@@ -5609,7 +6385,9 @@
         <v>23</v>
       </c>
       <c r="M31" s="10"/>
-      <c r="N31" s="3"/>
+      <c r="N31" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="O31" s="3"/>
       <c r="P31" s="3" t="s">
         <v>39</v>
@@ -5619,7 +6397,7 @@
       </c>
       <c r="R31" s="3"/>
     </row>
-    <row r="32" spans="1:18" ht="94">
+    <row r="32" spans="1:18" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A32" s="8" t="s">
         <v>125</v>
       </c>
@@ -5647,7 +6425,9 @@
         <v>39</v>
       </c>
       <c r="M32" s="20"/>
-      <c r="N32" s="3"/>
+      <c r="N32" s="20" t="s">
+        <v>39</v>
+      </c>
       <c r="O32" s="3"/>
       <c r="P32" s="3" t="s">
         <v>39</v>
@@ -5657,7 +6437,7 @@
       </c>
       <c r="R32" s="3"/>
     </row>
-    <row r="33" spans="1:18" ht="140">
+    <row r="33" spans="1:18" ht="139.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A33" s="8" t="s">
         <v>128</v>
       </c>
@@ -5685,7 +6465,9 @@
         <v>130</v>
       </c>
       <c r="M33" s="10"/>
-      <c r="N33" s="3"/>
+      <c r="N33" s="10" t="s">
+        <v>130</v>
+      </c>
       <c r="O33" s="3"/>
       <c r="P33" s="3" t="s">
         <v>39</v>
@@ -5695,7 +6477,7 @@
       </c>
       <c r="R33" s="3"/>
     </row>
-    <row r="34" spans="1:18" ht="92.25" customHeight="1">
+    <row r="34" spans="1:18" ht="92.25" customHeight="1" x14ac:dyDescent="1.1000000000000001">
       <c r="A34" s="8" t="s">
         <v>131</v>
       </c>
@@ -5723,7 +6505,9 @@
         <v>39</v>
       </c>
       <c r="M34" s="10"/>
-      <c r="N34" s="3"/>
+      <c r="N34" s="10" t="s">
+        <v>39</v>
+      </c>
       <c r="O34" s="3"/>
       <c r="P34" s="3" t="s">
         <v>39</v>
@@ -5733,7 +6517,7 @@
       </c>
       <c r="R34" s="3"/>
     </row>
-    <row r="35" spans="1:18" ht="99" customHeight="1">
+    <row r="35" spans="1:18" ht="99" customHeight="1" x14ac:dyDescent="1.1000000000000001">
       <c r="A35" s="8" t="s">
         <v>134</v>
       </c>
@@ -5761,7 +6545,9 @@
         <v>39</v>
       </c>
       <c r="M35" s="10"/>
-      <c r="N35" s="3"/>
+      <c r="N35" s="10" t="s">
+        <v>39</v>
+      </c>
       <c r="O35" s="3"/>
       <c r="P35" s="3" t="s">
         <v>39</v>
@@ -5771,7 +6557,7 @@
       </c>
       <c r="R35" s="3"/>
     </row>
-    <row r="36" spans="1:18" ht="96">
+    <row r="36" spans="1:18" ht="95" x14ac:dyDescent="1.1000000000000001">
       <c r="A36" s="8" t="s">
         <v>136</v>
       </c>
@@ -5795,7 +6581,9 @@
         <v>138</v>
       </c>
       <c r="M36" s="4"/>
-      <c r="N36" s="3"/>
+      <c r="N36" s="10" t="s">
+        <v>39</v>
+      </c>
       <c r="O36" s="3"/>
       <c r="P36" s="3" t="s">
         <v>39</v>
@@ -5805,7 +6593,7 @@
       </c>
       <c r="R36" s="3"/>
     </row>
-    <row r="37" spans="1:18" ht="140">
+    <row r="37" spans="1:18" ht="139.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A37" s="8" t="s">
         <v>139</v>
       </c>
@@ -5829,7 +6617,9 @@
         <v>138</v>
       </c>
       <c r="M37" s="4"/>
-      <c r="N37" s="3"/>
+      <c r="N37" s="3" t="s">
+        <v>737</v>
+      </c>
       <c r="O37" s="3"/>
       <c r="P37" s="3" t="s">
         <v>39</v>
@@ -5839,7 +6629,7 @@
       </c>
       <c r="R37" s="3"/>
     </row>
-    <row r="38" spans="1:18" ht="140">
+    <row r="38" spans="1:18" ht="139.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A38" s="8" t="s">
         <v>141</v>
       </c>
@@ -5863,7 +6653,9 @@
         <v>138</v>
       </c>
       <c r="M38" s="4"/>
-      <c r="N38" s="3"/>
+      <c r="N38" s="3" t="s">
+        <v>738</v>
+      </c>
       <c r="O38" s="3"/>
       <c r="P38" s="3" t="s">
         <v>39</v>
@@ -5873,7 +6665,7 @@
       </c>
       <c r="R38" s="3"/>
     </row>
-    <row r="39" spans="1:18" ht="140">
+    <row r="39" spans="1:18" ht="139.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A39" s="8" t="s">
         <v>144</v>
       </c>
@@ -5897,7 +6689,9 @@
         <v>138</v>
       </c>
       <c r="M39" s="4"/>
-      <c r="N39" s="3"/>
+      <c r="N39" s="3" t="s">
+        <v>738</v>
+      </c>
       <c r="O39" s="3"/>
       <c r="P39" s="3" t="s">
         <v>39</v>
@@ -5907,7 +6701,7 @@
       </c>
       <c r="R39" s="3"/>
     </row>
-    <row r="40" spans="1:18" ht="96">
+    <row r="40" spans="1:18" ht="95" x14ac:dyDescent="1.1000000000000001">
       <c r="A40" s="8" t="s">
         <v>147</v>
       </c>
@@ -5935,7 +6729,9 @@
         <v>138</v>
       </c>
       <c r="M40" s="4"/>
-      <c r="N40" s="3"/>
+      <c r="N40" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="O40" s="3"/>
       <c r="P40" s="3" t="s">
         <v>39</v>
@@ -5945,7 +6741,7 @@
       </c>
       <c r="R40" s="3"/>
     </row>
-    <row r="41" spans="1:18" ht="96">
+    <row r="41" spans="1:18" ht="95" x14ac:dyDescent="1.1000000000000001">
       <c r="A41" s="8" t="s">
         <v>150</v>
       </c>
@@ -5973,7 +6769,9 @@
         <v>138</v>
       </c>
       <c r="M41" s="4"/>
-      <c r="N41" s="3"/>
+      <c r="N41" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="O41" s="3"/>
       <c r="P41" s="3" t="s">
         <v>39</v>
@@ -5983,7 +6781,7 @@
       </c>
       <c r="R41" s="3"/>
     </row>
-    <row r="42" spans="1:18" ht="140">
+    <row r="42" spans="1:18" ht="139.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A42" s="8" t="s">
         <v>153</v>
       </c>
@@ -6011,7 +6809,9 @@
         <v>138</v>
       </c>
       <c r="M42" s="4"/>
-      <c r="N42" s="3"/>
+      <c r="N42" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="O42" s="3"/>
       <c r="P42" s="3" t="s">
         <v>39</v>
@@ -6021,7 +6821,7 @@
       </c>
       <c r="R42" s="3"/>
     </row>
-    <row r="43" spans="1:18" ht="96">
+    <row r="43" spans="1:18" ht="95" x14ac:dyDescent="1.1000000000000001">
       <c r="A43" s="8" t="s">
         <v>156</v>
       </c>
@@ -6045,7 +6845,9 @@
         <v>138</v>
       </c>
       <c r="M43" s="4"/>
-      <c r="N43" s="3"/>
+      <c r="N43" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="O43" s="3"/>
       <c r="P43" s="3" t="s">
         <v>39</v>
@@ -6055,7 +6857,7 @@
       </c>
       <c r="R43" s="3"/>
     </row>
-    <row r="44" spans="1:18" ht="96">
+    <row r="44" spans="1:18" ht="95" x14ac:dyDescent="1.1000000000000001">
       <c r="A44" s="8" t="s">
         <v>159</v>
       </c>
@@ -6079,7 +6881,9 @@
         <v>138</v>
       </c>
       <c r="M44" s="4"/>
-      <c r="N44" s="3"/>
+      <c r="N44" s="4" t="s">
+        <v>739</v>
+      </c>
       <c r="O44" s="3"/>
       <c r="P44" s="3" t="s">
         <v>39</v>
@@ -6089,7 +6893,7 @@
       </c>
       <c r="R44" s="3"/>
     </row>
-    <row r="45" spans="1:18" ht="96">
+    <row r="45" spans="1:18" ht="95" x14ac:dyDescent="1.1000000000000001">
       <c r="A45" s="8" t="s">
         <v>161</v>
       </c>
@@ -6113,7 +6917,9 @@
         <v>138</v>
       </c>
       <c r="M45" s="4"/>
-      <c r="N45" s="3"/>
+      <c r="N45" s="3" t="s">
+        <v>740</v>
+      </c>
       <c r="O45" s="3"/>
       <c r="P45" s="3" t="s">
         <v>39</v>
@@ -6123,7 +6929,7 @@
       </c>
       <c r="R45" s="3"/>
     </row>
-    <row r="46" spans="1:18" ht="96">
+    <row r="46" spans="1:18" ht="95" x14ac:dyDescent="1.1000000000000001">
       <c r="A46" s="8" t="s">
         <v>164</v>
       </c>
@@ -6147,7 +6953,9 @@
         <v>138</v>
       </c>
       <c r="M46" s="4"/>
-      <c r="N46" s="3"/>
+      <c r="N46" s="4" t="s">
+        <v>739</v>
+      </c>
       <c r="O46" s="3"/>
       <c r="P46" s="3" t="s">
         <v>39</v>
@@ -6157,7 +6965,7 @@
       </c>
       <c r="R46" s="3"/>
     </row>
-    <row r="47" spans="1:18" ht="140">
+    <row r="47" spans="1:18" ht="139.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A47" s="8" t="s">
         <v>166</v>
       </c>
@@ -6181,7 +6989,9 @@
         <v>138</v>
       </c>
       <c r="M47" s="4"/>
-      <c r="N47" s="3"/>
+      <c r="N47" s="3" t="s">
+        <v>254</v>
+      </c>
       <c r="O47" s="3"/>
       <c r="P47" s="3" t="s">
         <v>39</v>
@@ -6191,7 +7001,7 @@
       </c>
       <c r="R47" s="3"/>
     </row>
-    <row r="48" spans="1:18" ht="96">
+    <row r="48" spans="1:18" ht="95" x14ac:dyDescent="1.1000000000000001">
       <c r="A48" s="8" t="s">
         <v>168</v>
       </c>
@@ -6215,7 +7025,9 @@
         <v>138</v>
       </c>
       <c r="M48" s="4"/>
-      <c r="N48" s="3"/>
+      <c r="N48" s="3" t="s">
+        <v>254</v>
+      </c>
       <c r="O48" s="3"/>
       <c r="P48" s="3" t="s">
         <v>39</v>
@@ -6225,7 +7037,7 @@
       </c>
       <c r="R48" s="3"/>
     </row>
-    <row r="49" spans="1:18" ht="94">
+    <row r="49" spans="1:18" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A49" s="8" t="s">
         <v>170</v>
       </c>
@@ -6253,7 +7065,9 @@
         <v>39</v>
       </c>
       <c r="M49" s="10"/>
-      <c r="N49" s="3"/>
+      <c r="N49" s="10" t="s">
+        <v>39</v>
+      </c>
       <c r="O49" s="3"/>
       <c r="P49" s="3" t="s">
         <v>39</v>
@@ -6263,7 +7077,7 @@
       </c>
       <c r="R49" s="3"/>
     </row>
-    <row r="50" spans="1:18" ht="186">
+    <row r="50" spans="1:18" ht="186" thickBot="1" x14ac:dyDescent="1.1499999999999999">
       <c r="A50" s="8" t="s">
         <v>172</v>
       </c>
@@ -6291,7 +7105,9 @@
         <v>39</v>
       </c>
       <c r="M50" s="10"/>
-      <c r="N50" s="3"/>
+      <c r="N50" s="10" t="s">
+        <v>39</v>
+      </c>
       <c r="O50" s="3"/>
       <c r="P50" s="3" t="s">
         <v>39</v>
@@ -6301,7 +7117,7 @@
       </c>
       <c r="R50" s="3"/>
     </row>
-    <row r="51" spans="1:18" ht="234.75" customHeight="1">
+    <row r="51" spans="1:18" ht="234.75" customHeight="1" thickBot="1" x14ac:dyDescent="1.1499999999999999">
       <c r="A51" s="8" t="s">
         <v>174</v>
       </c>
@@ -6333,7 +7149,7 @@
       <c r="Q51" s="3"/>
       <c r="R51" s="3"/>
     </row>
-    <row r="52" spans="1:18" ht="94">
+    <row r="52" spans="1:18" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A52" s="8" t="s">
         <v>178</v>
       </c>
@@ -6367,7 +7183,7 @@
       </c>
       <c r="R52" s="3"/>
     </row>
-    <row r="53" spans="1:18" ht="48">
+    <row r="53" spans="1:18" x14ac:dyDescent="1.1000000000000001">
       <c r="A53" s="23" t="s">
         <v>180</v>
       </c>
@@ -6397,7 +7213,7 @@
       <c r="Q53" s="3"/>
       <c r="R53" s="3"/>
     </row>
-    <row r="54" spans="1:18" ht="48">
+    <row r="54" spans="1:18" x14ac:dyDescent="1.1000000000000001">
       <c r="A54" s="23" t="s">
         <v>183</v>
       </c>
@@ -6427,7 +7243,7 @@
       <c r="Q54" s="3"/>
       <c r="R54" s="3"/>
     </row>
-    <row r="55" spans="1:18" ht="278">
+    <row r="55" spans="1:18" ht="277.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A55" s="8" t="s">
         <v>186</v>
       </c>
@@ -6460,7 +7276,7 @@
       <c r="Q55" s="3"/>
       <c r="R55" s="3"/>
     </row>
-    <row r="56" spans="1:18" ht="48">
+    <row r="56" spans="1:18" x14ac:dyDescent="1.1000000000000001">
       <c r="A56" s="23" t="s">
         <v>190</v>
       </c>
@@ -6494,7 +7310,7 @@
       </c>
       <c r="R56" s="3"/>
     </row>
-    <row r="57" spans="1:18" ht="278">
+    <row r="57" spans="1:18" ht="277.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A57" s="8" t="s">
         <v>193</v>
       </c>
@@ -6527,7 +7343,7 @@
       <c r="Q57" s="3"/>
       <c r="R57" s="3"/>
     </row>
-    <row r="58" spans="1:18" ht="48">
+    <row r="58" spans="1:18" x14ac:dyDescent="1.1000000000000001">
       <c r="A58" s="8" t="s">
         <v>197</v>
       </c>
@@ -6561,7 +7377,7 @@
       </c>
       <c r="R58" s="3"/>
     </row>
-    <row r="59" spans="1:18" ht="278">
+    <row r="59" spans="1:18" ht="277.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A59" s="8" t="s">
         <v>200</v>
       </c>
@@ -6594,7 +7410,7 @@
       <c r="Q59" s="3"/>
       <c r="R59" s="3"/>
     </row>
-    <row r="60" spans="1:18" ht="408.75" customHeight="1">
+    <row r="60" spans="1:18" ht="408.75" customHeight="1" x14ac:dyDescent="1.1000000000000001">
       <c r="A60" s="8" t="s">
         <v>203</v>
       </c>
@@ -6626,7 +7442,7 @@
       <c r="Q60" s="3"/>
       <c r="R60" s="3"/>
     </row>
-    <row r="61" spans="1:18" ht="94">
+    <row r="61" spans="1:18" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A61" s="23" t="s">
         <v>208</v>
       </c>
@@ -6660,7 +7476,7 @@
       </c>
       <c r="R61" s="3"/>
     </row>
-    <row r="62" spans="1:18" ht="408.75" customHeight="1">
+    <row r="62" spans="1:18" ht="408.75" customHeight="1" x14ac:dyDescent="1.1000000000000001">
       <c r="A62" s="8" t="s">
         <v>210</v>
       </c>
@@ -6692,7 +7508,7 @@
       <c r="Q62" s="3"/>
       <c r="R62" s="3"/>
     </row>
-    <row r="63" spans="1:18" ht="48">
+    <row r="63" spans="1:18" x14ac:dyDescent="1.1000000000000001">
       <c r="A63" s="23" t="s">
         <v>214</v>
       </c>
@@ -6722,7 +7538,7 @@
       <c r="Q63" s="3"/>
       <c r="R63" s="3"/>
     </row>
-    <row r="64" spans="1:18" ht="94">
+    <row r="64" spans="1:18" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A64" s="23" t="s">
         <v>216</v>
       </c>
@@ -6752,7 +7568,7 @@
       <c r="Q64" s="3"/>
       <c r="R64" s="3"/>
     </row>
-    <row r="65" spans="1:18" ht="94">
+    <row r="65" spans="1:18" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A65" s="8" t="s">
         <v>219</v>
       </c>
@@ -6786,7 +7602,7 @@
       </c>
       <c r="R65" s="3"/>
     </row>
-    <row r="66" spans="1:18" ht="48">
+    <row r="66" spans="1:18" x14ac:dyDescent="1.1000000000000001">
       <c r="A66" s="8" t="s">
         <v>222</v>
       </c>
@@ -6820,7 +7636,7 @@
       </c>
       <c r="R66" s="3"/>
     </row>
-    <row r="67" spans="1:18" ht="92">
+    <row r="67" spans="1:18" ht="92" x14ac:dyDescent="1.1000000000000001">
       <c r="A67" s="8" t="s">
         <v>225</v>
       </c>
@@ -6853,7 +7669,7 @@
       <c r="Q67" s="3"/>
       <c r="R67" s="3"/>
     </row>
-    <row r="68" spans="1:18" ht="92">
+    <row r="68" spans="1:18" ht="92" x14ac:dyDescent="1.1000000000000001">
       <c r="A68" s="8" t="s">
         <v>227</v>
       </c>
@@ -6886,7 +7702,7 @@
       <c r="Q68" s="3"/>
       <c r="R68" s="3"/>
     </row>
-    <row r="69" spans="1:18" ht="94">
+    <row r="69" spans="1:18" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A69" s="8" t="s">
         <v>230</v>
       </c>
@@ -6919,7 +7735,7 @@
       <c r="Q69" s="3"/>
       <c r="R69" s="3"/>
     </row>
-    <row r="70" spans="1:18" ht="94">
+    <row r="70" spans="1:18" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A70" s="8" t="s">
         <v>233</v>
       </c>
@@ -6951,7 +7767,7 @@
       <c r="Q70" s="3"/>
       <c r="R70" s="3"/>
     </row>
-    <row r="71" spans="1:18" ht="94">
+    <row r="71" spans="1:18" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A71" s="8" t="s">
         <v>237</v>
       </c>
@@ -6983,7 +7799,7 @@
       <c r="Q71" s="3"/>
       <c r="R71" s="3"/>
     </row>
-    <row r="72" spans="1:18" ht="94">
+    <row r="72" spans="1:18" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A72" s="8" t="s">
         <v>241</v>
       </c>
@@ -7015,7 +7831,7 @@
       <c r="Q72" s="3"/>
       <c r="R72" s="3"/>
     </row>
-    <row r="73" spans="1:18" ht="94">
+    <row r="73" spans="1:18" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A73" s="8" t="s">
         <v>244</v>
       </c>
@@ -7046,7 +7862,7 @@
       <c r="Q73" s="3"/>
       <c r="R73" s="3"/>
     </row>
-    <row r="74" spans="1:18" ht="140">
+    <row r="74" spans="1:18" ht="139.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A74" s="8" t="s">
         <v>246</v>
       </c>
@@ -7074,7 +7890,7 @@
       <c r="Q74" s="3"/>
       <c r="R74" s="3"/>
     </row>
-    <row r="75" spans="1:18" ht="94">
+    <row r="75" spans="1:18" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A75" s="8" t="s">
         <v>248</v>
       </c>
@@ -7104,7 +7920,7 @@
       <c r="Q75" s="3"/>
       <c r="R75" s="3"/>
     </row>
-    <row r="76" spans="1:18" ht="48">
+    <row r="76" spans="1:18" x14ac:dyDescent="1.1000000000000001">
       <c r="A76" s="8" t="s">
         <v>251</v>
       </c>
@@ -7136,7 +7952,7 @@
       <c r="Q76" s="3"/>
       <c r="R76" s="3"/>
     </row>
-    <row r="77" spans="1:18" ht="94">
+    <row r="77" spans="1:18" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A77" s="8" t="s">
         <v>255</v>
       </c>
@@ -7168,7 +7984,7 @@
       <c r="Q77" s="3"/>
       <c r="R77" s="3"/>
     </row>
-    <row r="78" spans="1:18" ht="94">
+    <row r="78" spans="1:18" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A78" s="8" t="s">
         <v>258</v>
       </c>
@@ -7198,7 +8014,7 @@
       <c r="Q78" s="3"/>
       <c r="R78" s="3"/>
     </row>
-    <row r="79" spans="1:18" ht="94">
+    <row r="79" spans="1:18" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A79" s="8" t="s">
         <v>260</v>
       </c>
@@ -7230,7 +8046,7 @@
       <c r="Q79" s="3"/>
       <c r="R79" s="3"/>
     </row>
-    <row r="80" spans="1:18" ht="94">
+    <row r="80" spans="1:18" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A80" s="8" t="s">
         <v>263</v>
       </c>
@@ -7262,7 +8078,7 @@
       <c r="Q80" s="3"/>
       <c r="R80" s="3"/>
     </row>
-    <row r="81" spans="1:18" ht="94">
+    <row r="81" spans="1:18" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A81" s="8" t="s">
         <v>266</v>
       </c>
@@ -7294,7 +8110,7 @@
       <c r="Q81" s="3"/>
       <c r="R81" s="3"/>
     </row>
-    <row r="82" spans="1:18" ht="48">
+    <row r="82" spans="1:18" x14ac:dyDescent="1.1000000000000001">
       <c r="A82" s="8" t="s">
         <v>270</v>
       </c>
@@ -7326,7 +8142,7 @@
       <c r="Q82" s="3"/>
       <c r="R82" s="3"/>
     </row>
-    <row r="83" spans="1:18" ht="94">
+    <row r="83" spans="1:18" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A83" s="8" t="s">
         <v>273</v>
       </c>
@@ -7358,7 +8174,7 @@
       <c r="Q83" s="3"/>
       <c r="R83" s="3"/>
     </row>
-    <row r="84" spans="1:18" ht="94">
+    <row r="84" spans="1:18" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A84" s="8" t="s">
         <v>275</v>
       </c>
@@ -7390,7 +8206,7 @@
       <c r="Q84" s="3"/>
       <c r="R84" s="3"/>
     </row>
-    <row r="85" spans="1:18" ht="94">
+    <row r="85" spans="1:18" x14ac:dyDescent="1.1000000000000001">
       <c r="A85" s="8" t="s">
         <v>277</v>
       </c>
@@ -7422,7 +8238,7 @@
       <c r="Q85" s="3"/>
       <c r="R85" s="3"/>
     </row>
-    <row r="86" spans="1:18" ht="48">
+    <row r="86" spans="1:18" x14ac:dyDescent="1.1000000000000001">
       <c r="A86" s="8" t="s">
         <v>281</v>
       </c>
@@ -7452,7 +8268,7 @@
       <c r="Q86" s="3"/>
       <c r="R86" s="3"/>
     </row>
-    <row r="87" spans="1:18" ht="48">
+    <row r="87" spans="1:18" x14ac:dyDescent="1.1000000000000001">
       <c r="A87" s="8" t="s">
         <v>283</v>
       </c>
@@ -7482,7 +8298,7 @@
       <c r="Q87" s="3"/>
       <c r="R87" s="3"/>
     </row>
-    <row r="88" spans="1:18" ht="48">
+    <row r="88" spans="1:18" x14ac:dyDescent="1.1000000000000001">
       <c r="A88" s="8" t="s">
         <v>286</v>
       </c>
@@ -7512,7 +8328,7 @@
       <c r="Q88" s="3"/>
       <c r="R88" s="3"/>
     </row>
-    <row r="89" spans="1:18" ht="48">
+    <row r="89" spans="1:18" x14ac:dyDescent="1.1000000000000001">
       <c r="A89" s="8" t="s">
         <v>289</v>
       </c>
@@ -7544,7 +8360,7 @@
       <c r="Q89" s="3"/>
       <c r="R89" s="3"/>
     </row>
-    <row r="90" spans="1:18" ht="48">
+    <row r="90" spans="1:18" x14ac:dyDescent="1.1000000000000001">
       <c r="A90" s="8" t="s">
         <v>291</v>
       </c>
@@ -7576,7 +8392,7 @@
       <c r="Q90" s="3"/>
       <c r="R90" s="3"/>
     </row>
-    <row r="91" spans="1:18" ht="94">
+    <row r="91" spans="1:18" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A91" s="8" t="s">
         <v>293</v>
       </c>
@@ -7608,7 +8424,7 @@
       <c r="Q91" s="3"/>
       <c r="R91" s="3"/>
     </row>
-    <row r="92" spans="1:18" ht="94">
+    <row r="92" spans="1:18" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A92" s="8" t="s">
         <v>295</v>
       </c>
@@ -7640,7 +8456,7 @@
       <c r="Q92" s="3"/>
       <c r="R92" s="3"/>
     </row>
-    <row r="93" spans="1:18" ht="232">
+    <row r="93" spans="1:18" ht="231.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A93" s="8" t="s">
         <v>298</v>
       </c>
@@ -7668,7 +8484,7 @@
       <c r="Q93" s="3"/>
       <c r="R93" s="3"/>
     </row>
-    <row r="94" spans="1:18" ht="94">
+    <row r="94" spans="1:18" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A94" s="8" t="s">
         <v>300</v>
       </c>
@@ -7696,7 +8512,7 @@
       <c r="Q94" s="3"/>
       <c r="R94" s="3"/>
     </row>
-    <row r="95" spans="1:18" ht="186">
+    <row r="95" spans="1:18" ht="139.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A95" s="8" t="s">
         <v>302</v>
       </c>
@@ -7732,7 +8548,7 @@
       <c r="Q95" s="3"/>
       <c r="R95" s="3"/>
     </row>
-    <row r="96" spans="1:18" ht="94">
+    <row r="96" spans="1:18" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A96" s="8" t="s">
         <v>305</v>
       </c>
@@ -7768,7 +8584,7 @@
       <c r="Q96" s="3"/>
       <c r="R96" s="3"/>
     </row>
-    <row r="97" spans="1:18" ht="140">
+    <row r="97" spans="1:18" ht="139.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A97" s="8" t="s">
         <v>307</v>
       </c>
@@ -7796,7 +8612,7 @@
       <c r="Q97" s="3"/>
       <c r="R97" s="3"/>
     </row>
-    <row r="98" spans="1:18" ht="94">
+    <row r="98" spans="1:18" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A98" s="8" t="s">
         <v>309</v>
       </c>
@@ -7828,7 +8644,7 @@
       <c r="Q98" s="3"/>
       <c r="R98" s="3"/>
     </row>
-    <row r="99" spans="1:18" ht="140">
+    <row r="99" spans="1:18" ht="139.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A99" s="8" t="s">
         <v>311</v>
       </c>
@@ -7860,7 +8676,7 @@
       <c r="Q99" s="3"/>
       <c r="R99" s="3"/>
     </row>
-    <row r="100" spans="1:18" ht="232">
+    <row r="100" spans="1:18" ht="231.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A100" s="8" t="s">
         <v>314</v>
       </c>
@@ -7890,7 +8706,7 @@
       <c r="Q100" s="3"/>
       <c r="R100" s="3"/>
     </row>
-    <row r="101" spans="1:18" ht="94">
+    <row r="101" spans="1:18" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A101" s="8" t="s">
         <v>317</v>
       </c>
@@ -7923,7 +8739,7 @@
       <c r="Q101" s="3"/>
       <c r="R101" s="3"/>
     </row>
-    <row r="102" spans="1:18" ht="94">
+    <row r="102" spans="1:18" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A102" s="8" t="s">
         <v>320</v>
       </c>
@@ -7956,7 +8772,7 @@
       <c r="Q102" s="3"/>
       <c r="R102" s="3"/>
     </row>
-    <row r="103" spans="1:18" ht="140">
+    <row r="103" spans="1:18" ht="139.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A103" s="8" t="s">
         <v>322</v>
       </c>
@@ -7986,7 +8802,7 @@
       <c r="Q103" s="3"/>
       <c r="R103" s="3"/>
     </row>
-    <row r="104" spans="1:18" ht="94">
+    <row r="104" spans="1:18" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A104" s="8" t="s">
         <v>325</v>
       </c>
@@ -8019,7 +8835,7 @@
       <c r="Q104" s="3"/>
       <c r="R104" s="3"/>
     </row>
-    <row r="105" spans="1:18" ht="140">
+    <row r="105" spans="1:18" ht="139.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A105" s="8" t="s">
         <v>328</v>
       </c>
@@ -8049,7 +8865,7 @@
       <c r="Q105" s="3"/>
       <c r="R105" s="3"/>
     </row>
-    <row r="106" spans="1:18" ht="94">
+    <row r="106" spans="1:18" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A106" s="8" t="s">
         <v>330</v>
       </c>
@@ -8082,7 +8898,7 @@
       <c r="Q106" s="3"/>
       <c r="R106" s="3"/>
     </row>
-    <row r="107" spans="1:18" ht="94">
+    <row r="107" spans="1:18" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A107" s="8" t="s">
         <v>332</v>
       </c>
@@ -8112,7 +8928,7 @@
       <c r="Q107" s="3"/>
       <c r="R107" s="3"/>
     </row>
-    <row r="108" spans="1:18" ht="94">
+    <row r="108" spans="1:18" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A108" s="8" t="s">
         <v>334</v>
       </c>
@@ -8142,7 +8958,7 @@
       <c r="Q108" s="3"/>
       <c r="R108" s="3"/>
     </row>
-    <row r="109" spans="1:18" ht="94">
+    <row r="109" spans="1:18" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A109" s="8" t="s">
         <v>336</v>
       </c>
@@ -8175,7 +8991,7 @@
       <c r="Q109" s="3"/>
       <c r="R109" s="3"/>
     </row>
-    <row r="110" spans="1:18" ht="94">
+    <row r="110" spans="1:18" ht="48" thickBot="1" x14ac:dyDescent="1.1499999999999999">
       <c r="A110" s="8" t="s">
         <v>338</v>
       </c>
@@ -8205,7 +9021,7 @@
       <c r="Q110" s="3"/>
       <c r="R110" s="3"/>
     </row>
-    <row r="111" spans="1:18" ht="48">
+    <row r="111" spans="1:18" ht="48" thickBot="1" x14ac:dyDescent="1.1499999999999999">
       <c r="A111" s="8" t="s">
         <v>340</v>
       </c>
@@ -8231,7 +9047,9 @@
         <v>207</v>
       </c>
       <c r="M111" s="3"/>
-      <c r="N111" s="3"/>
+      <c r="N111" s="57" t="s">
+        <v>741</v>
+      </c>
       <c r="O111" s="3"/>
       <c r="P111" s="3"/>
       <c r="Q111" s="3"/>
@@ -8240,7 +9058,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="112" spans="1:18" ht="94">
+    <row r="112" spans="1:18" ht="94" thickBot="1" x14ac:dyDescent="1.1499999999999999">
       <c r="A112" s="8" t="s">
         <v>344</v>
       </c>
@@ -8266,13 +9084,15 @@
         <v>207</v>
       </c>
       <c r="M112" s="3"/>
-      <c r="N112" s="3"/>
+      <c r="N112" s="57" t="s">
+        <v>742</v>
+      </c>
       <c r="O112" s="3"/>
       <c r="P112" s="3"/>
       <c r="Q112" s="3"/>
       <c r="R112" s="3"/>
     </row>
-    <row r="113" spans="1:20" ht="48">
+    <row r="113" spans="1:20" ht="48" thickBot="1" x14ac:dyDescent="1.1499999999999999">
       <c r="A113" s="8" t="s">
         <v>348</v>
       </c>
@@ -8298,13 +9118,15 @@
         <v>207</v>
       </c>
       <c r="M113" s="3"/>
-      <c r="N113" s="3"/>
+      <c r="N113" s="57" t="s">
+        <v>743</v>
+      </c>
       <c r="O113" s="3"/>
       <c r="P113" s="3"/>
       <c r="Q113" s="3"/>
       <c r="R113" s="3"/>
     </row>
-    <row r="114" spans="1:20" ht="94">
+    <row r="114" spans="1:20" ht="94" thickBot="1" x14ac:dyDescent="1.1499999999999999">
       <c r="A114" s="8" t="s">
         <v>350</v>
       </c>
@@ -8330,13 +9152,15 @@
         <v>207</v>
       </c>
       <c r="M114" s="3"/>
-      <c r="N114" s="3"/>
+      <c r="N114" s="57" t="s">
+        <v>744</v>
+      </c>
       <c r="O114" s="3"/>
       <c r="P114" s="3"/>
       <c r="Q114" s="3"/>
       <c r="R114" s="3"/>
     </row>
-    <row r="115" spans="1:20" ht="94">
+    <row r="115" spans="1:20" ht="94" thickBot="1" x14ac:dyDescent="1.1499999999999999">
       <c r="A115" s="8" t="s">
         <v>352</v>
       </c>
@@ -8362,13 +9186,15 @@
         <v>207</v>
       </c>
       <c r="M115" s="3"/>
-      <c r="N115" s="3"/>
+      <c r="N115" s="58" t="s">
+        <v>745</v>
+      </c>
       <c r="O115" s="3"/>
       <c r="P115" s="3"/>
       <c r="Q115" s="3"/>
       <c r="R115" s="3"/>
     </row>
-    <row r="116" spans="1:20" ht="94">
+    <row r="116" spans="1:20" ht="94" thickBot="1" x14ac:dyDescent="1.1499999999999999">
       <c r="A116" s="8" t="s">
         <v>356</v>
       </c>
@@ -8394,7 +9220,9 @@
         <v>207</v>
       </c>
       <c r="M116" s="3"/>
-      <c r="N116" s="3"/>
+      <c r="N116" s="59" t="s">
+        <v>39</v>
+      </c>
       <c r="O116" s="3"/>
       <c r="P116" s="3"/>
       <c r="Q116" s="3"/>
@@ -8403,7 +9231,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="117" spans="1:20" ht="94">
+    <row r="117" spans="1:20" ht="94" thickBot="1" x14ac:dyDescent="1.1499999999999999">
       <c r="A117" s="8" t="s">
         <v>359</v>
       </c>
@@ -8429,13 +9257,15 @@
         <v>39</v>
       </c>
       <c r="M117" s="3"/>
-      <c r="N117" s="3"/>
+      <c r="N117" s="59" t="s">
+        <v>39</v>
+      </c>
       <c r="O117" s="3"/>
       <c r="P117" s="3"/>
       <c r="Q117" s="3"/>
       <c r="R117" s="3"/>
     </row>
-    <row r="118" spans="1:20" ht="94">
+    <row r="118" spans="1:20" ht="94" thickBot="1" x14ac:dyDescent="1.1499999999999999">
       <c r="A118" s="8" t="s">
         <v>362</v>
       </c>
@@ -8461,7 +9291,9 @@
         <v>39</v>
       </c>
       <c r="M118" s="3"/>
-      <c r="N118" s="3"/>
+      <c r="N118" s="59" t="s">
+        <v>39</v>
+      </c>
       <c r="O118" s="3"/>
       <c r="P118" s="3"/>
       <c r="Q118" s="3"/>
@@ -8470,7 +9302,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="119" spans="1:20" ht="94">
+    <row r="119" spans="1:20" ht="94" thickBot="1" x14ac:dyDescent="1.1499999999999999">
       <c r="A119" s="8" t="s">
         <v>366</v>
       </c>
@@ -8496,13 +9328,15 @@
         <v>207</v>
       </c>
       <c r="M119" s="3"/>
-      <c r="N119" s="3"/>
+      <c r="N119" s="59" t="s">
+        <v>746</v>
+      </c>
       <c r="O119" s="3"/>
       <c r="P119" s="3"/>
       <c r="Q119" s="3"/>
       <c r="R119" s="3"/>
     </row>
-    <row r="120" spans="1:20" ht="140">
+    <row r="120" spans="1:20" ht="140" thickBot="1" x14ac:dyDescent="1.1499999999999999">
       <c r="A120" s="8" t="s">
         <v>368</v>
       </c>
@@ -8528,7 +9362,9 @@
         <v>207</v>
       </c>
       <c r="M120" s="3"/>
-      <c r="N120" s="3"/>
+      <c r="N120" s="59" t="s">
+        <v>746</v>
+      </c>
       <c r="O120" s="3"/>
       <c r="P120" s="3"/>
       <c r="Q120" s="3"/>
@@ -8537,7 +9373,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="121" spans="1:20" ht="94">
+    <row r="121" spans="1:20" ht="94" thickBot="1" x14ac:dyDescent="1.1499999999999999">
       <c r="A121" s="8" t="s">
         <v>372</v>
       </c>
@@ -8563,13 +9399,15 @@
         <v>39</v>
       </c>
       <c r="M121" s="3"/>
-      <c r="N121" s="3"/>
+      <c r="N121" s="59" t="s">
+        <v>746</v>
+      </c>
       <c r="O121" s="3"/>
       <c r="P121" s="3"/>
       <c r="Q121" s="3"/>
       <c r="R121" s="3"/>
     </row>
-    <row r="122" spans="1:20" ht="140">
+    <row r="122" spans="1:20" ht="140" thickBot="1" x14ac:dyDescent="1.1499999999999999">
       <c r="A122" s="8" t="s">
         <v>374</v>
       </c>
@@ -8595,13 +9433,15 @@
         <v>39</v>
       </c>
       <c r="M122" s="3"/>
-      <c r="N122" s="3"/>
+      <c r="N122" s="59" t="s">
+        <v>746</v>
+      </c>
       <c r="O122" s="3"/>
       <c r="P122" s="3"/>
       <c r="Q122" s="3"/>
       <c r="R122" s="3"/>
     </row>
-    <row r="123" spans="1:20" ht="140">
+    <row r="123" spans="1:20" ht="140" thickBot="1" x14ac:dyDescent="1.1499999999999999">
       <c r="A123" s="8" t="s">
         <v>376</v>
       </c>
@@ -8627,7 +9467,9 @@
         <v>39</v>
       </c>
       <c r="M123" s="3"/>
-      <c r="N123" s="3"/>
+      <c r="N123" s="59" t="s">
+        <v>39</v>
+      </c>
       <c r="O123" s="3"/>
       <c r="P123" s="3"/>
       <c r="Q123" s="3"/>
@@ -8636,7 +9478,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="124" spans="1:20" ht="48">
+    <row r="124" spans="1:20" ht="48" thickBot="1" x14ac:dyDescent="1.1499999999999999">
       <c r="A124" s="8" t="s">
         <v>379</v>
       </c>
@@ -8660,7 +9502,9 @@
       <c r="K124" s="3"/>
       <c r="L124" s="10"/>
       <c r="M124" s="3"/>
-      <c r="N124" s="3"/>
+      <c r="N124" s="59" t="s">
+        <v>39</v>
+      </c>
       <c r="O124" s="3"/>
       <c r="P124" s="3"/>
       <c r="Q124" s="3"/>
@@ -8669,7 +9513,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="125" spans="1:20" ht="232">
+    <row r="125" spans="1:20" ht="232" thickBot="1" x14ac:dyDescent="1.1499999999999999">
       <c r="A125" s="8" t="s">
         <v>381</v>
       </c>
@@ -8695,7 +9539,9 @@
         <v>39</v>
       </c>
       <c r="M125" s="3"/>
-      <c r="N125" s="3"/>
+      <c r="N125" s="59" t="s">
+        <v>39</v>
+      </c>
       <c r="O125" s="3"/>
       <c r="P125" s="3"/>
       <c r="Q125" s="3"/>
@@ -8704,7 +9550,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="126" spans="1:20" ht="186">
+    <row r="126" spans="1:20" ht="186" thickBot="1" x14ac:dyDescent="1.1499999999999999">
       <c r="A126" s="8" t="s">
         <v>383</v>
       </c>
@@ -8730,13 +9576,15 @@
         <v>39</v>
       </c>
       <c r="M126" s="3"/>
-      <c r="N126" s="3"/>
+      <c r="N126" s="59" t="s">
+        <v>39</v>
+      </c>
       <c r="O126" s="3"/>
       <c r="P126" s="3"/>
       <c r="Q126" s="3"/>
       <c r="R126" s="3"/>
     </row>
-    <row r="127" spans="1:20" ht="138">
+    <row r="127" spans="1:20" ht="92" x14ac:dyDescent="1.1000000000000001">
       <c r="A127" s="8" t="s">
         <v>385</v>
       </c>
@@ -8762,8 +9610,7 @@
         <v>207</v>
       </c>
       <c r="M127" s="3"/>
-      <c r="N127" s="3" t="e">
-        <f>#VALUE!</f>
+      <c r="N127" s="3" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
       <c r="O127" s="3"/>
@@ -8771,7 +9618,7 @@
       <c r="Q127" s="3"/>
       <c r="R127" s="3"/>
     </row>
-    <row r="128" spans="1:20" s="40" customFormat="1" ht="92">
+    <row r="128" spans="1:20" s="40" customFormat="1" ht="92" x14ac:dyDescent="1.1000000000000001">
       <c r="A128" s="33" t="s">
         <v>389</v>
       </c>
@@ -8795,8 +9642,7 @@
       <c r="K128" s="38"/>
       <c r="L128" s="10"/>
       <c r="M128" s="38"/>
-      <c r="N128" s="3" t="e">
-        <f>#VALUE!</f>
+      <c r="N128" s="3" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
       <c r="O128" s="38"/>
@@ -8806,7 +9652,7 @@
       <c r="S128" s="39"/>
       <c r="T128" s="39"/>
     </row>
-    <row r="129" spans="1:20" ht="92">
+    <row r="129" spans="1:20" ht="92" x14ac:dyDescent="1.1000000000000001">
       <c r="A129" s="8" t="s">
         <v>393</v>
       </c>
@@ -8830,20 +9676,19 @@
       <c r="K129" s="38"/>
       <c r="L129" s="10"/>
       <c r="M129" s="38"/>
-      <c r="N129" s="3" t="e">
-        <f>#VALUE!</f>
+      <c r="N129" s="3" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
       <c r="O129" s="38"/>
       <c r="P129" s="38"/>
-      <c r="Q129" s="38" t="e" vm="1">
+      <c r="Q129" s="38" t="e" vm="3">
         <v>#VALUE!</v>
       </c>
       <c r="R129" s="38"/>
       <c r="S129" s="39"/>
       <c r="T129" s="39"/>
     </row>
-    <row r="130" spans="1:20" ht="94">
+    <row r="130" spans="1:20" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A130" s="8" t="s">
         <v>397</v>
       </c>
@@ -8867,20 +9712,19 @@
       <c r="K130" s="38"/>
       <c r="L130" s="10"/>
       <c r="M130" s="38"/>
-      <c r="N130" s="3" t="e">
-        <f>#VALUE!</f>
+      <c r="N130" s="3" t="e" vm="4">
         <v>#VALUE!</v>
       </c>
       <c r="O130" s="38"/>
       <c r="P130" s="38"/>
-      <c r="Q130" s="38" t="e" vm="2">
+      <c r="Q130" s="38" t="e" vm="5">
         <v>#VALUE!</v>
       </c>
       <c r="R130" s="38"/>
       <c r="S130" s="39"/>
       <c r="T130" s="39"/>
     </row>
-    <row r="131" spans="1:20" s="40" customFormat="1" ht="94">
+    <row r="131" spans="1:20" s="40" customFormat="1" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A131" s="33" t="s">
         <v>400</v>
       </c>
@@ -8904,8 +9748,7 @@
       <c r="K131" s="38"/>
       <c r="L131" s="10"/>
       <c r="M131" s="38"/>
-      <c r="N131" s="3" t="e">
-        <f>#VALUE!</f>
+      <c r="N131" s="3" t="e" vm="4">
         <v>#VALUE!</v>
       </c>
       <c r="O131" s="38"/>
@@ -8915,7 +9758,7 @@
       <c r="S131" s="39"/>
       <c r="T131" s="39"/>
     </row>
-    <row r="132" spans="1:20" ht="48">
+    <row r="132" spans="1:20" x14ac:dyDescent="1.1000000000000001">
       <c r="A132" s="8" t="s">
         <v>403</v>
       </c>
@@ -8939,8 +9782,7 @@
       <c r="K132" s="38"/>
       <c r="L132" s="10"/>
       <c r="M132" s="38"/>
-      <c r="N132" s="3" t="e">
-        <f>#VALUE!</f>
+      <c r="N132" s="3" t="e" vm="6">
         <v>#VALUE!</v>
       </c>
       <c r="O132" s="38"/>
@@ -8950,7 +9792,7 @@
       <c r="S132" s="39"/>
       <c r="T132" s="39"/>
     </row>
-    <row r="133" spans="1:20" ht="174.75" customHeight="1">
+    <row r="133" spans="1:20" ht="174.75" customHeight="1" x14ac:dyDescent="1.1000000000000001">
       <c r="A133" s="8" t="s">
         <v>407</v>
       </c>
@@ -8974,20 +9816,19 @@
       <c r="K133" s="38"/>
       <c r="L133" s="10"/>
       <c r="M133" s="38"/>
-      <c r="N133" s="3" t="e">
-        <f>#VALUE!</f>
+      <c r="N133" s="3" t="e" vm="7">
         <v>#VALUE!</v>
       </c>
       <c r="O133" s="38"/>
       <c r="P133" s="38"/>
-      <c r="Q133" s="38" t="e" vm="3">
+      <c r="Q133" s="38" t="e" vm="8">
         <v>#VALUE!</v>
       </c>
       <c r="R133" s="38"/>
       <c r="S133" s="39"/>
       <c r="T133" s="39"/>
     </row>
-    <row r="134" spans="1:20" ht="48">
+    <row r="134" spans="1:20" x14ac:dyDescent="1.1000000000000001">
       <c r="A134" s="8" t="s">
         <v>411</v>
       </c>
@@ -9011,20 +9852,19 @@
       <c r="K134" s="38"/>
       <c r="L134" s="10"/>
       <c r="M134" s="38"/>
-      <c r="N134" s="3" t="e">
-        <f>#VALUE!</f>
+      <c r="N134" s="3" t="e" vm="9">
         <v>#VALUE!</v>
       </c>
       <c r="O134" s="38"/>
       <c r="P134" s="38"/>
-      <c r="Q134" s="38" t="e" vm="4">
+      <c r="Q134" s="38" t="e" vm="10">
         <v>#VALUE!</v>
       </c>
       <c r="R134" s="38"/>
       <c r="S134" s="39"/>
       <c r="T134" s="39"/>
     </row>
-    <row r="135" spans="1:20" ht="48">
+    <row r="135" spans="1:20" x14ac:dyDescent="1.1000000000000001">
       <c r="A135" s="8" t="s">
         <v>415</v>
       </c>
@@ -9048,8 +9888,7 @@
       <c r="K135" s="38"/>
       <c r="L135" s="10"/>
       <c r="M135" s="38"/>
-      <c r="N135" s="3" t="e">
-        <f>#VALUE!</f>
+      <c r="N135" s="3" t="e" vm="11">
         <v>#VALUE!</v>
       </c>
       <c r="O135" s="38"/>
@@ -9059,7 +9898,7 @@
       <c r="S135" s="39"/>
       <c r="T135" s="39"/>
     </row>
-    <row r="136" spans="1:20" ht="94">
+    <row r="136" spans="1:20" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A136" s="8" t="s">
         <v>419</v>
       </c>
@@ -9083,8 +9922,7 @@
       <c r="K136" s="3"/>
       <c r="L136" s="10"/>
       <c r="M136" s="3"/>
-      <c r="N136" s="3" t="e">
-        <f>#VALUE!</f>
+      <c r="N136" s="3" t="e" vm="12">
         <v>#VALUE!</v>
       </c>
       <c r="O136" s="3"/>
@@ -9092,7 +9930,7 @@
       <c r="Q136" s="3"/>
       <c r="R136" s="3"/>
     </row>
-    <row r="137" spans="1:20" ht="94">
+    <row r="137" spans="1:20" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A137" s="8" t="s">
         <v>423</v>
       </c>
@@ -9116,8 +9954,7 @@
       <c r="K137" s="3"/>
       <c r="L137" s="10"/>
       <c r="M137" s="3"/>
-      <c r="N137" s="3" t="e">
-        <f>#VALUE!</f>
+      <c r="N137" s="3" t="e" vm="13">
         <v>#VALUE!</v>
       </c>
       <c r="O137" s="3"/>
@@ -9125,7 +9962,7 @@
       <c r="Q137" s="3"/>
       <c r="R137" s="3"/>
     </row>
-    <row r="138" spans="1:20" ht="140">
+    <row r="138" spans="1:20" ht="139.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A138" s="8" t="s">
         <v>426</v>
       </c>
@@ -9149,8 +9986,7 @@
       <c r="K138" s="3"/>
       <c r="L138" s="10"/>
       <c r="M138" s="3"/>
-      <c r="N138" s="3" t="e">
-        <f>#VALUE!</f>
+      <c r="N138" s="3" t="e" vm="14">
         <v>#VALUE!</v>
       </c>
       <c r="O138" s="3"/>
@@ -9158,7 +9994,7 @@
       <c r="Q138" s="3"/>
       <c r="R138" s="3"/>
     </row>
-    <row r="139" spans="1:20" ht="94">
+    <row r="139" spans="1:20" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A139" s="8" t="s">
         <v>430</v>
       </c>
@@ -9182,8 +10018,7 @@
       <c r="K139" s="3"/>
       <c r="L139" s="10"/>
       <c r="M139" s="3"/>
-      <c r="N139" s="3" t="e">
-        <f>#VALUE!</f>
+      <c r="N139" s="3" t="e" vm="15">
         <v>#VALUE!</v>
       </c>
       <c r="O139" s="3"/>
@@ -9191,7 +10026,7 @@
       <c r="Q139" s="3"/>
       <c r="R139" s="3"/>
     </row>
-    <row r="140" spans="1:20" ht="140">
+    <row r="140" spans="1:20" ht="139.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A140" s="8" t="s">
         <v>433</v>
       </c>
@@ -9215,8 +10050,7 @@
       <c r="K140" s="3"/>
       <c r="L140" s="10"/>
       <c r="M140" s="3"/>
-      <c r="N140" s="3" t="e">
-        <f>#VALUE!</f>
+      <c r="N140" s="3" t="e" vm="16">
         <v>#VALUE!</v>
       </c>
       <c r="O140" s="3"/>
@@ -9224,7 +10058,7 @@
       <c r="Q140" s="3"/>
       <c r="R140" s="3"/>
     </row>
-    <row r="141" spans="1:20" ht="94">
+    <row r="141" spans="1:20" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A141" s="8" t="s">
         <v>437</v>
       </c>
@@ -9248,8 +10082,7 @@
       <c r="K141" s="3"/>
       <c r="L141" s="10"/>
       <c r="M141" s="3"/>
-      <c r="N141" s="3" t="e">
-        <f>#VALUE!</f>
+      <c r="N141" s="3" t="e" vm="17">
         <v>#VALUE!</v>
       </c>
       <c r="O141" s="3"/>
@@ -9257,7 +10090,7 @@
       <c r="Q141" s="3"/>
       <c r="R141" s="3"/>
     </row>
-    <row r="142" spans="1:20" ht="94">
+    <row r="142" spans="1:20" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A142" s="8" t="s">
         <v>440</v>
       </c>
@@ -9281,8 +10114,7 @@
       <c r="K142" s="3"/>
       <c r="L142" s="10"/>
       <c r="M142" s="3"/>
-      <c r="N142" s="3" t="e">
-        <f>#VALUE!</f>
+      <c r="N142" s="3" t="e" vm="18">
         <v>#VALUE!</v>
       </c>
       <c r="O142" s="3"/>
@@ -9290,7 +10122,7 @@
       <c r="Q142" s="3"/>
       <c r="R142" s="3"/>
     </row>
-    <row r="143" spans="1:20" ht="140">
+    <row r="143" spans="1:20" ht="139.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A143" s="8" t="s">
         <v>443</v>
       </c>
@@ -9314,8 +10146,7 @@
       <c r="K143" s="3"/>
       <c r="L143" s="10"/>
       <c r="M143" s="3"/>
-      <c r="N143" s="3" t="e">
-        <f>#VALUE!</f>
+      <c r="N143" s="3" t="e" vm="19">
         <v>#VALUE!</v>
       </c>
       <c r="O143" s="3"/>
@@ -9323,7 +10154,7 @@
       <c r="Q143" s="3"/>
       <c r="R143" s="3"/>
     </row>
-    <row r="144" spans="1:20" ht="140">
+    <row r="144" spans="1:20" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A144" s="42" t="s">
         <v>446</v>
       </c>
@@ -9355,7 +10186,7 @@
       <c r="S144" s="39"/>
       <c r="T144" s="39"/>
     </row>
-    <row r="145" spans="1:20" ht="94">
+    <row r="145" spans="1:20" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A145" s="8" t="s">
         <v>450</v>
       </c>
@@ -9381,8 +10212,7 @@
         <v>207</v>
       </c>
       <c r="M145" s="38"/>
-      <c r="N145" s="3" t="e">
-        <f>#VALUE!</f>
+      <c r="N145" s="3" t="e" vm="20">
         <v>#VALUE!</v>
       </c>
       <c r="O145" s="38"/>
@@ -9392,7 +10222,7 @@
       <c r="S145" s="39"/>
       <c r="T145" s="39"/>
     </row>
-    <row r="146" spans="1:20" ht="140">
+    <row r="146" spans="1:20" ht="139.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A146" s="8" t="s">
         <v>454</v>
       </c>
@@ -9418,8 +10248,7 @@
         <v>207</v>
       </c>
       <c r="M146" s="38"/>
-      <c r="N146" s="3" t="e">
-        <f>#VALUE!</f>
+      <c r="N146" s="3" t="e" vm="21">
         <v>#VALUE!</v>
       </c>
       <c r="O146" s="38"/>
@@ -9429,7 +10258,7 @@
       <c r="S146" s="39"/>
       <c r="T146" s="39"/>
     </row>
-    <row r="147" spans="1:20" ht="140">
+    <row r="147" spans="1:20" ht="139.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A147" s="8" t="s">
         <v>458</v>
       </c>
@@ -9453,8 +10282,7 @@
       <c r="K147" s="38"/>
       <c r="L147" s="10"/>
       <c r="M147" s="38"/>
-      <c r="N147" s="3" t="e">
-        <f>#VALUE!</f>
+      <c r="N147" s="3" t="e" vm="22">
         <v>#VALUE!</v>
       </c>
       <c r="O147" s="38"/>
@@ -9464,7 +10292,7 @@
       <c r="S147" s="39"/>
       <c r="T147" s="39"/>
     </row>
-    <row r="148" spans="1:20" ht="140">
+    <row r="148" spans="1:20" ht="139.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A148" s="8" t="s">
         <v>462</v>
       </c>
@@ -9488,8 +10316,7 @@
       <c r="K148" s="38"/>
       <c r="L148" s="10"/>
       <c r="M148" s="38"/>
-      <c r="N148" s="3" t="e">
-        <f>#VALUE!</f>
+      <c r="N148" s="3" t="e" vm="23">
         <v>#VALUE!</v>
       </c>
       <c r="O148" s="38"/>
@@ -9499,7 +10326,7 @@
       <c r="S148" s="39"/>
       <c r="T148" s="39"/>
     </row>
-    <row r="149" spans="1:20" s="40" customFormat="1" ht="140">
+    <row r="149" spans="1:20" s="40" customFormat="1" ht="139.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A149" s="33" t="s">
         <v>466</v>
       </c>
@@ -9531,7 +10358,7 @@
       <c r="S149" s="39"/>
       <c r="T149" s="39"/>
     </row>
-    <row r="150" spans="1:20" ht="140">
+    <row r="150" spans="1:20" ht="139.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A150" s="8" t="s">
         <v>470</v>
       </c>
@@ -9555,8 +10382,7 @@
       <c r="K150" s="38"/>
       <c r="L150" s="10"/>
       <c r="M150" s="38"/>
-      <c r="N150" s="3" t="e">
-        <f>#VALUE!</f>
+      <c r="N150" s="3" t="e" vm="24">
         <v>#VALUE!</v>
       </c>
       <c r="O150" s="38"/>
@@ -9566,7 +10392,7 @@
       <c r="S150" s="39"/>
       <c r="T150" s="39"/>
     </row>
-    <row r="151" spans="1:20" ht="140">
+    <row r="151" spans="1:20" ht="139.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A151" s="8" t="s">
         <v>474</v>
       </c>
@@ -9598,7 +10424,7 @@
       <c r="S151" s="39"/>
       <c r="T151" s="39"/>
     </row>
-    <row r="152" spans="1:20" ht="94">
+    <row r="152" spans="1:20" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A152" s="8" t="s">
         <v>477</v>
       </c>
@@ -9630,7 +10456,7 @@
       <c r="S152" s="39"/>
       <c r="T152" s="39"/>
     </row>
-    <row r="153" spans="1:20" ht="140">
+    <row r="153" spans="1:20" ht="139.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A153" s="8" t="s">
         <v>480</v>
       </c>
@@ -9668,7 +10494,7 @@
       <c r="S153" s="39"/>
       <c r="T153" s="39"/>
     </row>
-    <row r="154" spans="1:20" ht="140">
+    <row r="154" spans="1:20" ht="139.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A154" s="8" t="s">
         <v>483</v>
       </c>
@@ -9706,7 +10532,7 @@
       <c r="S154" s="39"/>
       <c r="T154" s="39"/>
     </row>
-    <row r="155" spans="1:20" ht="94">
+    <row r="155" spans="1:20" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A155" s="8" t="s">
         <v>486</v>
       </c>
@@ -9744,7 +10570,7 @@
       <c r="S155" s="39"/>
       <c r="T155" s="39"/>
     </row>
-    <row r="156" spans="1:20" ht="140">
+    <row r="156" spans="1:20" ht="139.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A156" s="8" t="s">
         <v>489</v>
       </c>
@@ -9782,7 +10608,7 @@
       <c r="S156" s="39"/>
       <c r="T156" s="39"/>
     </row>
-    <row r="157" spans="1:20" ht="94">
+    <row r="157" spans="1:20" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A157" s="8" t="s">
         <v>491</v>
       </c>
@@ -9820,7 +10646,7 @@
       <c r="S157" s="39"/>
       <c r="T157" s="39"/>
     </row>
-    <row r="158" spans="1:20" ht="94">
+    <row r="158" spans="1:20" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A158" s="8" t="s">
         <v>493</v>
       </c>
@@ -9858,7 +10684,7 @@
       <c r="S158" s="39"/>
       <c r="T158" s="39"/>
     </row>
-    <row r="159" spans="1:20" ht="94">
+    <row r="159" spans="1:20" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A159" s="8" t="s">
         <v>496</v>
       </c>
@@ -9896,7 +10722,7 @@
       <c r="S159" s="39"/>
       <c r="T159" s="39"/>
     </row>
-    <row r="160" spans="1:20" ht="94">
+    <row r="160" spans="1:20" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A160" s="8" t="s">
         <v>499</v>
       </c>
@@ -9934,7 +10760,7 @@
       <c r="S160" s="39"/>
       <c r="T160" s="39"/>
     </row>
-    <row r="161" spans="1:20" ht="94">
+    <row r="161" spans="1:20" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A161" s="8" t="s">
         <v>502</v>
       </c>
@@ -9972,7 +10798,7 @@
       <c r="S161" s="39"/>
       <c r="T161" s="39"/>
     </row>
-    <row r="162" spans="1:20" ht="48">
+    <row r="162" spans="1:20" x14ac:dyDescent="1.1000000000000001">
       <c r="A162" s="8" t="s">
         <v>505</v>
       </c>
@@ -10010,7 +10836,7 @@
       <c r="S162" s="39"/>
       <c r="T162" s="39"/>
     </row>
-    <row r="163" spans="1:20" ht="48">
+    <row r="163" spans="1:20" x14ac:dyDescent="1.1000000000000001">
       <c r="A163" s="8" t="s">
         <v>508</v>
       </c>
@@ -10038,7 +10864,9 @@
         <v>39</v>
       </c>
       <c r="M163" s="38"/>
-      <c r="N163" s="3"/>
+      <c r="N163" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="O163" s="38"/>
       <c r="P163" s="38" t="s">
         <v>39</v>
@@ -10048,7 +10876,7 @@
       <c r="S163" s="39"/>
       <c r="T163" s="39"/>
     </row>
-    <row r="164" spans="1:20" ht="48">
+    <row r="164" spans="1:20" x14ac:dyDescent="1.1000000000000001">
       <c r="A164" s="8" t="s">
         <v>511</v>
       </c>
@@ -10076,7 +10904,9 @@
         <v>39</v>
       </c>
       <c r="M164" s="38"/>
-      <c r="N164" s="3"/>
+      <c r="N164" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="O164" s="38"/>
       <c r="P164" s="38" t="s">
         <v>39</v>
@@ -10086,7 +10916,7 @@
       <c r="S164" s="39"/>
       <c r="T164" s="39"/>
     </row>
-    <row r="165" spans="1:20" ht="48">
+    <row r="165" spans="1:20" x14ac:dyDescent="1.1000000000000001">
       <c r="A165" s="8" t="s">
         <v>514</v>
       </c>
@@ -10114,7 +10944,9 @@
         <v>39</v>
       </c>
       <c r="M165" s="38"/>
-      <c r="N165" s="3"/>
+      <c r="N165" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="O165" s="38"/>
       <c r="P165" s="38" t="s">
         <v>39</v>
@@ -10124,7 +10956,7 @@
       <c r="S165" s="39"/>
       <c r="T165" s="39"/>
     </row>
-    <row r="166" spans="1:20" ht="48">
+    <row r="166" spans="1:20" x14ac:dyDescent="1.1000000000000001">
       <c r="A166" s="8" t="s">
         <v>517</v>
       </c>
@@ -10152,7 +10984,9 @@
         <v>39</v>
       </c>
       <c r="M166" s="38"/>
-      <c r="N166" s="3"/>
+      <c r="N166" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="O166" s="38"/>
       <c r="P166" s="38" t="s">
         <v>39</v>
@@ -10162,7 +10996,7 @@
       <c r="S166" s="39"/>
       <c r="T166" s="39"/>
     </row>
-    <row r="167" spans="1:20" ht="48">
+    <row r="167" spans="1:20" x14ac:dyDescent="1.1000000000000001">
       <c r="A167" s="8" t="s">
         <v>520</v>
       </c>
@@ -10190,7 +11024,9 @@
         <v>39</v>
       </c>
       <c r="M167" s="38"/>
-      <c r="N167" s="3"/>
+      <c r="N167" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="O167" s="38"/>
       <c r="P167" s="38" t="s">
         <v>39</v>
@@ -10200,7 +11036,7 @@
       <c r="S167" s="39"/>
       <c r="T167" s="39"/>
     </row>
-    <row r="168" spans="1:20" ht="94">
+    <row r="168" spans="1:20" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A168" s="8" t="s">
         <v>523</v>
       </c>
@@ -10228,7 +11064,9 @@
         <v>39</v>
       </c>
       <c r="M168" s="38"/>
-      <c r="N168" s="3"/>
+      <c r="N168" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="O168" s="38"/>
       <c r="P168" s="38"/>
       <c r="Q168" s="38"/>
@@ -10236,7 +11074,7 @@
       <c r="S168" s="39"/>
       <c r="T168" s="39"/>
     </row>
-    <row r="169" spans="1:20" ht="48">
+    <row r="169" spans="1:20" x14ac:dyDescent="1.1000000000000001">
       <c r="A169" s="8" t="s">
         <v>526</v>
       </c>
@@ -10264,7 +11102,9 @@
         <v>39</v>
       </c>
       <c r="M169" s="38"/>
-      <c r="N169" s="3"/>
+      <c r="N169" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="O169" s="38"/>
       <c r="P169" s="38"/>
       <c r="Q169" s="38"/>
@@ -10272,7 +11112,7 @@
       <c r="S169" s="39"/>
       <c r="T169" s="39"/>
     </row>
-    <row r="170" spans="1:20" ht="48">
+    <row r="170" spans="1:20" x14ac:dyDescent="1.1000000000000001">
       <c r="A170" s="8" t="s">
         <v>529</v>
       </c>
@@ -10300,7 +11140,9 @@
         <v>39</v>
       </c>
       <c r="M170" s="38"/>
-      <c r="N170" s="3"/>
+      <c r="N170" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="O170" s="38"/>
       <c r="P170" s="38"/>
       <c r="Q170" s="38"/>
@@ -10308,7 +11150,7 @@
       <c r="S170" s="39"/>
       <c r="T170" s="39"/>
     </row>
-    <row r="171" spans="1:20" ht="48">
+    <row r="171" spans="1:20" x14ac:dyDescent="1.1000000000000001">
       <c r="A171" s="8" t="s">
         <v>532</v>
       </c>
@@ -10332,7 +11174,9 @@
       <c r="K171" s="38"/>
       <c r="L171" s="8"/>
       <c r="M171" s="38"/>
-      <c r="N171" s="3"/>
+      <c r="N171" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="O171" s="38"/>
       <c r="P171" s="38"/>
       <c r="Q171" s="38"/>
@@ -10340,7 +11184,7 @@
       <c r="S171" s="39"/>
       <c r="T171" s="39"/>
     </row>
-    <row r="172" spans="1:20" ht="94">
+    <row r="172" spans="1:20" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A172" s="8" t="s">
         <v>535</v>
       </c>
@@ -10368,7 +11212,9 @@
         <v>39</v>
       </c>
       <c r="M172" s="38"/>
-      <c r="N172" s="3"/>
+      <c r="N172" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="O172" s="38"/>
       <c r="P172" s="38"/>
       <c r="Q172" s="38"/>
@@ -10376,7 +11222,7 @@
       <c r="S172" s="39"/>
       <c r="T172" s="39"/>
     </row>
-    <row r="173" spans="1:20" ht="48">
+    <row r="173" spans="1:20" x14ac:dyDescent="1.1000000000000001">
       <c r="A173" s="8" t="s">
         <v>538</v>
       </c>
@@ -10404,7 +11250,9 @@
         <v>39</v>
       </c>
       <c r="M173" s="38"/>
-      <c r="N173" s="3"/>
+      <c r="N173" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="O173" s="38"/>
       <c r="P173" s="38"/>
       <c r="Q173" s="38"/>
@@ -10412,7 +11260,7 @@
       <c r="S173" s="39"/>
       <c r="T173" s="39"/>
     </row>
-    <row r="174" spans="1:20" ht="94">
+    <row r="174" spans="1:20" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A174" s="8" t="s">
         <v>541</v>
       </c>
@@ -10440,7 +11288,9 @@
         <v>39</v>
       </c>
       <c r="M174" s="38"/>
-      <c r="N174" s="3"/>
+      <c r="N174" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="O174" s="38"/>
       <c r="P174" s="38" t="s">
         <v>39</v>
@@ -10450,7 +11300,7 @@
       <c r="S174" s="39"/>
       <c r="T174" s="39"/>
     </row>
-    <row r="175" spans="1:20">
+    <row r="175" spans="1:20" x14ac:dyDescent="1.1000000000000001">
       <c r="A175" s="8" t="s">
         <v>544</v>
       </c>
@@ -10478,7 +11328,9 @@
         <v>39</v>
       </c>
       <c r="M175" s="38"/>
-      <c r="N175" s="3"/>
+      <c r="N175" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="O175" s="38"/>
       <c r="P175" s="38" t="s">
         <v>39</v>
@@ -10488,7 +11340,7 @@
       <c r="S175" s="39"/>
       <c r="T175" s="39"/>
     </row>
-    <row r="176" spans="1:20">
+    <row r="176" spans="1:20" x14ac:dyDescent="1.1000000000000001">
       <c r="A176" s="8" t="s">
         <v>547</v>
       </c>
@@ -10516,7 +11368,9 @@
         <v>39</v>
       </c>
       <c r="M176" s="38"/>
-      <c r="N176" s="3"/>
+      <c r="N176" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="O176" s="38"/>
       <c r="P176" s="38" t="s">
         <v>39</v>
@@ -10526,7 +11380,7 @@
       <c r="S176" s="39"/>
       <c r="T176" s="39"/>
     </row>
-    <row r="177" spans="1:20">
+    <row r="177" spans="1:20" x14ac:dyDescent="1.1000000000000001">
       <c r="A177" s="8" t="s">
         <v>550</v>
       </c>
@@ -10554,7 +11408,9 @@
         <v>39</v>
       </c>
       <c r="M177" s="38"/>
-      <c r="N177" s="3"/>
+      <c r="N177" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="O177" s="38"/>
       <c r="P177" s="38" t="s">
         <v>39</v>
@@ -10564,7 +11420,7 @@
       <c r="S177" s="39"/>
       <c r="T177" s="39"/>
     </row>
-    <row r="178" spans="1:20" ht="48">
+    <row r="178" spans="1:20" x14ac:dyDescent="1.1000000000000001">
       <c r="A178" s="8" t="s">
         <v>553</v>
       </c>
@@ -10592,7 +11448,9 @@
         <v>39</v>
       </c>
       <c r="M178" s="38"/>
-      <c r="N178" s="3"/>
+      <c r="N178" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="O178" s="38"/>
       <c r="P178" s="38" t="s">
         <v>39</v>
@@ -10602,7 +11460,7 @@
       <c r="S178" s="39"/>
       <c r="T178" s="39"/>
     </row>
-    <row r="179" spans="1:20" ht="92">
+    <row r="179" spans="1:20" ht="92" x14ac:dyDescent="1.1000000000000001">
       <c r="A179" s="8" t="s">
         <v>556</v>
       </c>
@@ -10630,7 +11488,9 @@
         <v>39</v>
       </c>
       <c r="M179" s="38"/>
-      <c r="N179" s="3"/>
+      <c r="N179" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="O179" s="38"/>
       <c r="P179" s="38" t="s">
         <v>39</v>
@@ -10640,7 +11500,7 @@
       <c r="S179" s="39"/>
       <c r="T179" s="39"/>
     </row>
-    <row r="180" spans="1:20" ht="48">
+    <row r="180" spans="1:20" x14ac:dyDescent="1.1000000000000001">
       <c r="A180" s="8" t="s">
         <v>558</v>
       </c>
@@ -10668,7 +11528,9 @@
         <v>39</v>
       </c>
       <c r="M180" s="38"/>
-      <c r="N180" s="3"/>
+      <c r="N180" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="O180" s="38"/>
       <c r="P180" s="38" t="s">
         <v>39</v>
@@ -10678,7 +11540,7 @@
       <c r="S180" s="39"/>
       <c r="T180" s="39"/>
     </row>
-    <row r="181" spans="1:20" ht="48">
+    <row r="181" spans="1:20" x14ac:dyDescent="1.1000000000000001">
       <c r="A181" s="8" t="s">
         <v>560</v>
       </c>
@@ -10706,7 +11568,9 @@
         <v>39</v>
       </c>
       <c r="M181" s="38"/>
-      <c r="N181" s="3"/>
+      <c r="N181" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="O181" s="38"/>
       <c r="P181" s="38" t="s">
         <v>39</v>
@@ -10716,7 +11580,7 @@
       <c r="S181" s="39"/>
       <c r="T181" s="39"/>
     </row>
-    <row r="182" spans="1:20" ht="94">
+    <row r="182" spans="1:20" x14ac:dyDescent="1.1000000000000001">
       <c r="A182" s="8" t="s">
         <v>562</v>
       </c>
@@ -10744,7 +11608,9 @@
         <v>39</v>
       </c>
       <c r="M182" s="38"/>
-      <c r="N182" s="3"/>
+      <c r="N182" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="O182" s="38"/>
       <c r="P182" s="38" t="s">
         <v>39</v>
@@ -10754,7 +11620,7 @@
       <c r="S182" s="39"/>
       <c r="T182" s="39"/>
     </row>
-    <row r="183" spans="1:20" ht="48">
+    <row r="183" spans="1:20" x14ac:dyDescent="1.1000000000000001">
       <c r="A183" s="8" t="s">
         <v>564</v>
       </c>
@@ -10782,7 +11648,9 @@
         <v>39</v>
       </c>
       <c r="M183" s="38"/>
-      <c r="N183" s="3"/>
+      <c r="N183" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="O183" s="38"/>
       <c r="P183" s="38" t="s">
         <v>39</v>
@@ -10792,7 +11660,7 @@
       <c r="S183" s="39"/>
       <c r="T183" s="39"/>
     </row>
-    <row r="184" spans="1:20" ht="94">
+    <row r="184" spans="1:20" ht="94" thickBot="1" x14ac:dyDescent="1.1499999999999999">
       <c r="A184" s="8" t="s">
         <v>566</v>
       </c>
@@ -10820,7 +11688,9 @@
         <v>39</v>
       </c>
       <c r="M184" s="38"/>
-      <c r="N184" s="3"/>
+      <c r="N184" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="O184" s="38"/>
       <c r="P184" s="38" t="s">
         <v>39</v>
@@ -10830,7 +11700,7 @@
       <c r="S184" s="39"/>
       <c r="T184" s="39"/>
     </row>
-    <row r="185" spans="1:20" ht="94">
+    <row r="185" spans="1:20" ht="94" thickBot="1" x14ac:dyDescent="1.1499999999999999">
       <c r="A185" s="8" t="s">
         <v>568</v>
       </c>
@@ -10858,7 +11728,9 @@
         <v>39</v>
       </c>
       <c r="M185" s="38"/>
-      <c r="N185" s="3"/>
+      <c r="N185" s="60" t="s">
+        <v>747</v>
+      </c>
       <c r="O185" s="38"/>
       <c r="P185" s="38" t="s">
         <v>39</v>
@@ -10868,7 +11740,7 @@
       <c r="S185" s="39"/>
       <c r="T185" s="39"/>
     </row>
-    <row r="186" spans="1:20" ht="94">
+    <row r="186" spans="1:20" ht="94" thickBot="1" x14ac:dyDescent="1.1499999999999999">
       <c r="A186" s="8" t="s">
         <v>571</v>
       </c>
@@ -10896,7 +11768,9 @@
         <v>39</v>
       </c>
       <c r="M186" s="38"/>
-      <c r="N186" s="3"/>
+      <c r="N186" s="58" t="s">
+        <v>747</v>
+      </c>
       <c r="O186" s="38"/>
       <c r="P186" s="38" t="s">
         <v>39</v>
@@ -10906,7 +11780,7 @@
       <c r="S186" s="39"/>
       <c r="T186" s="39"/>
     </row>
-    <row r="187" spans="1:20" ht="94">
+    <row r="187" spans="1:20" ht="94" thickBot="1" x14ac:dyDescent="1.1499999999999999">
       <c r="A187" s="8" t="s">
         <v>574</v>
       </c>
@@ -10934,7 +11808,9 @@
         <v>39</v>
       </c>
       <c r="M187" s="38"/>
-      <c r="N187" s="3"/>
+      <c r="N187" s="59" t="s">
+        <v>39</v>
+      </c>
       <c r="O187" s="38"/>
       <c r="P187" s="38" t="s">
         <v>39</v>
@@ -10944,7 +11820,7 @@
       <c r="S187" s="39"/>
       <c r="T187" s="39"/>
     </row>
-    <row r="188" spans="1:20" ht="94">
+    <row r="188" spans="1:20" ht="94" thickBot="1" x14ac:dyDescent="1.1499999999999999">
       <c r="A188" s="8" t="s">
         <v>577</v>
       </c>
@@ -10972,7 +11848,9 @@
         <v>39</v>
       </c>
       <c r="M188" s="38"/>
-      <c r="N188" s="3"/>
+      <c r="N188" s="59" t="s">
+        <v>39</v>
+      </c>
       <c r="O188" s="38"/>
       <c r="P188" s="38" t="s">
         <v>39</v>
@@ -10982,7 +11860,7 @@
       <c r="S188" s="39"/>
       <c r="T188" s="39"/>
     </row>
-    <row r="189" spans="1:20" ht="94">
+    <row r="189" spans="1:20" ht="94" thickBot="1" x14ac:dyDescent="1.1499999999999999">
       <c r="A189" s="8" t="s">
         <v>580</v>
       </c>
@@ -11010,7 +11888,9 @@
         <v>39</v>
       </c>
       <c r="M189" s="38"/>
-      <c r="N189" s="3"/>
+      <c r="N189" s="58" t="s">
+        <v>748</v>
+      </c>
       <c r="O189" s="38"/>
       <c r="P189" s="38" t="s">
         <v>39</v>
@@ -11020,7 +11900,7 @@
       <c r="S189" s="39"/>
       <c r="T189" s="39"/>
     </row>
-    <row r="190" spans="1:20" ht="94">
+    <row r="190" spans="1:20" ht="94" thickBot="1" x14ac:dyDescent="1.1499999999999999">
       <c r="A190" s="8" t="s">
         <v>583</v>
       </c>
@@ -11048,7 +11928,9 @@
         <v>39</v>
       </c>
       <c r="M190" s="38"/>
-      <c r="N190" s="3"/>
+      <c r="N190" s="59" t="s">
+        <v>39</v>
+      </c>
       <c r="O190" s="38"/>
       <c r="P190" s="38" t="s">
         <v>39</v>
@@ -11058,7 +11940,7 @@
       <c r="S190" s="39"/>
       <c r="T190" s="39"/>
     </row>
-    <row r="191" spans="1:20" ht="94">
+    <row r="191" spans="1:20" ht="94" thickBot="1" x14ac:dyDescent="1.1499999999999999">
       <c r="A191" s="8" t="s">
         <v>586</v>
       </c>
@@ -11086,7 +11968,9 @@
         <v>39</v>
       </c>
       <c r="M191" s="38"/>
-      <c r="N191" s="3"/>
+      <c r="N191" s="59" t="s">
+        <v>39</v>
+      </c>
       <c r="O191" s="38"/>
       <c r="P191" s="38" t="s">
         <v>39</v>
@@ -11096,7 +11980,7 @@
       <c r="S191" s="39"/>
       <c r="T191" s="39"/>
     </row>
-    <row r="192" spans="1:20" ht="94">
+    <row r="192" spans="1:20" ht="94" thickBot="1" x14ac:dyDescent="1.1499999999999999">
       <c r="A192" s="8" t="s">
         <v>589</v>
       </c>
@@ -11124,7 +12008,9 @@
         <v>39</v>
       </c>
       <c r="M192" s="38"/>
-      <c r="N192" s="3"/>
+      <c r="N192" s="58" t="s">
+        <v>749</v>
+      </c>
       <c r="O192" s="38"/>
       <c r="P192" s="38" t="s">
         <v>39</v>
@@ -11134,7 +12020,7 @@
       <c r="S192" s="39"/>
       <c r="T192" s="39"/>
     </row>
-    <row r="193" spans="1:20" ht="94">
+    <row r="193" spans="1:20" ht="94" thickBot="1" x14ac:dyDescent="1.1499999999999999">
       <c r="A193" s="8" t="s">
         <v>592</v>
       </c>
@@ -11162,7 +12048,9 @@
         <v>39</v>
       </c>
       <c r="M193" s="38"/>
-      <c r="N193" s="3"/>
+      <c r="N193" s="59" t="s">
+        <v>39</v>
+      </c>
       <c r="O193" s="38"/>
       <c r="P193" s="38" t="s">
         <v>39</v>
@@ -11172,7 +12060,7 @@
       <c r="S193" s="39"/>
       <c r="T193" s="39"/>
     </row>
-    <row r="194" spans="1:20" ht="94">
+    <row r="194" spans="1:20" ht="94" thickBot="1" x14ac:dyDescent="1.1499999999999999">
       <c r="A194" s="8" t="s">
         <v>595</v>
       </c>
@@ -11200,7 +12088,9 @@
         <v>39</v>
       </c>
       <c r="M194" s="38"/>
-      <c r="N194" s="3"/>
+      <c r="N194" s="59" t="s">
+        <v>39</v>
+      </c>
       <c r="O194" s="38"/>
       <c r="P194" s="38" t="s">
         <v>39</v>
@@ -11210,7 +12100,7 @@
       <c r="S194" s="39"/>
       <c r="T194" s="39"/>
     </row>
-    <row r="195" spans="1:20" ht="94">
+    <row r="195" spans="1:20" ht="94" thickBot="1" x14ac:dyDescent="1.1499999999999999">
       <c r="A195" s="8" t="s">
         <v>598</v>
       </c>
@@ -11238,7 +12128,9 @@
         <v>39</v>
       </c>
       <c r="M195" s="38"/>
-      <c r="N195" s="3"/>
+      <c r="N195" s="59" t="s">
+        <v>39</v>
+      </c>
       <c r="O195" s="38"/>
       <c r="P195" s="38" t="s">
         <v>39</v>
@@ -11248,7 +12140,7 @@
       <c r="S195" s="39"/>
       <c r="T195" s="39"/>
     </row>
-    <row r="196" spans="1:20" ht="48">
+    <row r="196" spans="1:20" ht="48" thickBot="1" x14ac:dyDescent="1.1499999999999999">
       <c r="A196" s="8" t="s">
         <v>601</v>
       </c>
@@ -11276,7 +12168,9 @@
         <v>39</v>
       </c>
       <c r="M196" s="38"/>
-      <c r="N196" s="3"/>
+      <c r="N196" s="59" t="s">
+        <v>39</v>
+      </c>
       <c r="O196" s="38"/>
       <c r="P196" s="38" t="s">
         <v>39</v>
@@ -11286,7 +12180,7 @@
       <c r="S196" s="39"/>
       <c r="T196" s="39"/>
     </row>
-    <row r="197" spans="1:20" ht="94">
+    <row r="197" spans="1:20" ht="94" thickBot="1" x14ac:dyDescent="1.1499999999999999">
       <c r="A197" s="8" t="s">
         <v>604</v>
       </c>
@@ -11314,7 +12208,9 @@
         <v>39</v>
       </c>
       <c r="M197" s="38"/>
-      <c r="N197" s="3"/>
+      <c r="N197" s="59" t="s">
+        <v>39</v>
+      </c>
       <c r="O197" s="38"/>
       <c r="P197" s="38" t="s">
         <v>39</v>
@@ -11324,7 +12220,7 @@
       <c r="S197" s="39"/>
       <c r="T197" s="39"/>
     </row>
-    <row r="198" spans="1:20" ht="94">
+    <row r="198" spans="1:20" ht="94" thickBot="1" x14ac:dyDescent="1.1499999999999999">
       <c r="A198" s="8" t="s">
         <v>607</v>
       </c>
@@ -11352,7 +12248,9 @@
         <v>39</v>
       </c>
       <c r="M198" s="38"/>
-      <c r="N198" s="3"/>
+      <c r="N198" s="59" t="s">
+        <v>39</v>
+      </c>
       <c r="O198" s="38"/>
       <c r="P198" s="38" t="s">
         <v>39</v>
@@ -11362,7 +12260,7 @@
       <c r="S198" s="39"/>
       <c r="T198" s="39"/>
     </row>
-    <row r="199" spans="1:20" ht="140">
+    <row r="199" spans="1:20" ht="94" thickBot="1" x14ac:dyDescent="1.1499999999999999">
       <c r="A199" s="8" t="s">
         <v>610</v>
       </c>
@@ -11390,7 +12288,9 @@
         <v>39</v>
       </c>
       <c r="M199" s="38"/>
-      <c r="N199" s="3"/>
+      <c r="N199" s="59" t="s">
+        <v>39</v>
+      </c>
       <c r="O199" s="38"/>
       <c r="P199" s="38" t="s">
         <v>39</v>
@@ -11400,7 +12300,7 @@
       <c r="S199" s="39"/>
       <c r="T199" s="39"/>
     </row>
-    <row r="200" spans="1:20" ht="94">
+    <row r="200" spans="1:20" ht="94" thickBot="1" x14ac:dyDescent="1.1499999999999999">
       <c r="A200" s="8" t="s">
         <v>613</v>
       </c>
@@ -11428,7 +12328,9 @@
         <v>39</v>
       </c>
       <c r="M200" s="38"/>
-      <c r="N200" s="3"/>
+      <c r="N200" s="59" t="s">
+        <v>39</v>
+      </c>
       <c r="O200" s="38"/>
       <c r="P200" s="38" t="s">
         <v>39</v>
@@ -11438,7 +12340,7 @@
       <c r="S200" s="39"/>
       <c r="T200" s="39"/>
     </row>
-    <row r="201" spans="1:20" ht="94">
+    <row r="201" spans="1:20" ht="94" thickBot="1" x14ac:dyDescent="1.1499999999999999">
       <c r="A201" s="8" t="s">
         <v>616</v>
       </c>
@@ -11466,7 +12368,9 @@
         <v>39</v>
       </c>
       <c r="M201" s="38"/>
-      <c r="N201" s="3"/>
+      <c r="N201" s="59" t="s">
+        <v>39</v>
+      </c>
       <c r="O201" s="38"/>
       <c r="P201" s="38" t="s">
         <v>39</v>
@@ -11476,7 +12380,7 @@
       <c r="S201" s="39"/>
       <c r="T201" s="39"/>
     </row>
-    <row r="202" spans="1:20" ht="94">
+    <row r="202" spans="1:20" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A202" s="8" t="s">
         <v>619</v>
       </c>
@@ -11514,7 +12418,7 @@
       <c r="S202" s="39"/>
       <c r="T202" s="39"/>
     </row>
-    <row r="203" spans="1:20" ht="94">
+    <row r="203" spans="1:20" ht="93.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A203" s="8" t="s">
         <v>622</v>
       </c>
@@ -11552,7 +12456,7 @@
       <c r="S203" s="39"/>
       <c r="T203" s="39"/>
     </row>
-    <row r="204" spans="1:20" ht="350.25" customHeight="1">
+    <row r="204" spans="1:20" ht="350.25" customHeight="1" x14ac:dyDescent="1.1000000000000001">
       <c r="A204" s="8" t="s">
         <v>625</v>
       </c>
@@ -11589,7 +12493,7 @@
       <c r="S204" s="39"/>
       <c r="T204" s="39"/>
     </row>
-    <row r="205" spans="1:20" ht="300" customHeight="1">
+    <row r="205" spans="1:20" ht="300" customHeight="1" x14ac:dyDescent="1.1000000000000001">
       <c r="A205" s="8" t="s">
         <v>630</v>
       </c>
@@ -11630,7 +12534,7 @@
       <c r="S205" s="39"/>
       <c r="T205" s="39"/>
     </row>
-    <row r="206" spans="1:20" ht="300" customHeight="1">
+    <row r="206" spans="1:20" ht="300" customHeight="1" x14ac:dyDescent="1.1000000000000001">
       <c r="A206" s="8" t="s">
         <v>633</v>
       </c>
@@ -11671,7 +12575,7 @@
       <c r="S206" s="39"/>
       <c r="T206" s="39"/>
     </row>
-    <row r="207" spans="1:20" ht="300" customHeight="1">
+    <row r="207" spans="1:20" ht="300" customHeight="1" x14ac:dyDescent="1.1000000000000001">
       <c r="A207" s="8" t="s">
         <v>635</v>
       </c>
@@ -11708,7 +12612,7 @@
       <c r="S207" s="39"/>
       <c r="T207" s="39"/>
     </row>
-    <row r="208" spans="1:20" ht="300" customHeight="1">
+    <row r="208" spans="1:20" ht="300" customHeight="1" x14ac:dyDescent="1.1000000000000001">
       <c r="A208" s="8" t="s">
         <v>638</v>
       </c>
@@ -11749,7 +12653,7 @@
       <c r="S208" s="39"/>
       <c r="T208" s="39"/>
     </row>
-    <row r="209" spans="1:20" ht="300" customHeight="1">
+    <row r="209" spans="1:20" ht="300" customHeight="1" x14ac:dyDescent="1.1000000000000001">
       <c r="A209" s="8" t="s">
         <v>640</v>
       </c>
@@ -11788,7 +12692,7 @@
       <c r="S209" s="39"/>
       <c r="T209" s="39"/>
     </row>
-    <row r="210" spans="1:20" ht="399.75" customHeight="1">
+    <row r="210" spans="1:20" ht="399.75" customHeight="1" x14ac:dyDescent="1.1000000000000001">
       <c r="A210" s="8" t="s">
         <v>644</v>
       </c>
@@ -11825,7 +12729,7 @@
       <c r="Q210" s="3"/>
       <c r="R210" s="3"/>
     </row>
-    <row r="211" spans="1:20" ht="300" customHeight="1">
+    <row r="211" spans="1:20" ht="300" customHeight="1" x14ac:dyDescent="1.1000000000000001">
       <c r="A211" s="8" t="s">
         <v>647</v>
       </c>
@@ -11860,7 +12764,7 @@
       <c r="Q211" s="3"/>
       <c r="R211" s="3"/>
     </row>
-    <row r="212" spans="1:20" ht="300" customHeight="1">
+    <row r="212" spans="1:20" ht="300" customHeight="1" x14ac:dyDescent="1.1000000000000001">
       <c r="A212" s="8" t="s">
         <v>649</v>
       </c>
@@ -11897,7 +12801,7 @@
       <c r="Q212" s="3"/>
       <c r="R212" s="3"/>
     </row>
-    <row r="213" spans="1:20" ht="150" customHeight="1">
+    <row r="213" spans="1:20" ht="150" customHeight="1" x14ac:dyDescent="1.1000000000000001">
       <c r="A213" s="8" t="s">
         <v>651</v>
       </c>
@@ -11934,7 +12838,7 @@
       <c r="Q213" s="3"/>
       <c r="R213" s="3"/>
     </row>
-    <row r="214" spans="1:20" ht="96">
+    <row r="214" spans="1:20" ht="95" x14ac:dyDescent="1.1000000000000001">
       <c r="A214" s="3" t="s">
         <v>653</v>
       </c>
@@ -11968,7 +12872,7 @@
       <c r="Q214" s="3"/>
       <c r="R214" s="3"/>
     </row>
-    <row r="215" spans="1:20" ht="48">
+    <row r="215" spans="1:20" x14ac:dyDescent="1.1000000000000001">
       <c r="A215" s="3" t="s">
         <v>656</v>
       </c>
@@ -12002,7 +12906,7 @@
       <c r="Q215" s="3"/>
       <c r="R215" s="3"/>
     </row>
-    <row r="216" spans="1:20" ht="48">
+    <row r="216" spans="1:20" x14ac:dyDescent="1.1000000000000001">
       <c r="A216" s="3" t="s">
         <v>659</v>
       </c>
@@ -12036,7 +12940,7 @@
       <c r="Q216" s="3"/>
       <c r="R216" s="3"/>
     </row>
-    <row r="217" spans="1:20" ht="48">
+    <row r="217" spans="1:20" x14ac:dyDescent="1.1000000000000001">
       <c r="A217" s="3" t="s">
         <v>662</v>
       </c>
@@ -12070,7 +12974,7 @@
       <c r="Q217" s="3"/>
       <c r="R217" s="3"/>
     </row>
-    <row r="218" spans="1:20" ht="96">
+    <row r="218" spans="1:20" ht="95" x14ac:dyDescent="1.1000000000000001">
       <c r="A218" s="3" t="s">
         <v>665</v>
       </c>
@@ -12102,7 +13006,7 @@
       <c r="Q218" s="3"/>
       <c r="R218" s="3"/>
     </row>
-    <row r="219" spans="1:20" ht="48">
+    <row r="219" spans="1:20" x14ac:dyDescent="1.1000000000000001">
       <c r="A219" s="3" t="s">
         <v>667</v>
       </c>
@@ -12134,7 +13038,7 @@
       <c r="Q219" s="3"/>
       <c r="R219" s="3"/>
     </row>
-    <row r="220" spans="1:20" ht="48">
+    <row r="220" spans="1:20" x14ac:dyDescent="1.1000000000000001">
       <c r="A220" s="3" t="s">
         <v>669</v>
       </c>
@@ -12168,7 +13072,7 @@
       <c r="Q220" s="3"/>
       <c r="R220" s="3"/>
     </row>
-    <row r="221" spans="1:20" ht="96">
+    <row r="221" spans="1:20" ht="95" x14ac:dyDescent="1.1000000000000001">
       <c r="A221" s="3" t="s">
         <v>672</v>
       </c>
@@ -12202,7 +13106,7 @@
       <c r="Q221" s="3"/>
       <c r="R221" s="3"/>
     </row>
-    <row r="222" spans="1:20" ht="48">
+    <row r="222" spans="1:20" x14ac:dyDescent="1.1000000000000001">
       <c r="A222" s="3" t="s">
         <v>675</v>
       </c>
@@ -12236,7 +13140,7 @@
       <c r="Q222" s="3"/>
       <c r="R222" s="3"/>
     </row>
-    <row r="223" spans="1:20" ht="96">
+    <row r="223" spans="1:20" ht="95" x14ac:dyDescent="1.1000000000000001">
       <c r="A223" s="3" t="s">
         <v>678</v>
       </c>
@@ -12272,7 +13176,7 @@
       <c r="Q223" s="3"/>
       <c r="R223" s="3"/>
     </row>
-    <row r="224" spans="1:20" ht="48">
+    <row r="224" spans="1:20" x14ac:dyDescent="1.1000000000000001">
       <c r="A224" s="3" t="s">
         <v>682</v>
       </c>
@@ -12306,7 +13210,7 @@
       <c r="Q224" s="3"/>
       <c r="R224" s="3"/>
     </row>
-    <row r="225" spans="1:18" ht="48">
+    <row r="225" spans="1:18" x14ac:dyDescent="1.1000000000000001">
       <c r="A225" s="3" t="s">
         <v>685</v>
       </c>
@@ -12340,7 +13244,7 @@
       <c r="Q225" s="3"/>
       <c r="R225" s="3"/>
     </row>
-    <row r="226" spans="1:18" ht="96">
+    <row r="226" spans="1:18" ht="95" x14ac:dyDescent="1.1000000000000001">
       <c r="A226" s="3" t="s">
         <v>689</v>
       </c>
@@ -12374,7 +13278,7 @@
       <c r="Q226" s="3"/>
       <c r="R226" s="3"/>
     </row>
-    <row r="227" spans="1:18" ht="96">
+    <row r="227" spans="1:18" ht="95.5" thickBot="1" x14ac:dyDescent="1.1499999999999999">
       <c r="A227" s="3" t="s">
         <v>693</v>
       </c>
@@ -12408,7 +13312,7 @@
       <c r="Q227" s="3"/>
       <c r="R227" s="3"/>
     </row>
-    <row r="228" spans="1:18" ht="96">
+    <row r="228" spans="1:18" ht="95.5" thickBot="1" x14ac:dyDescent="1.1499999999999999">
       <c r="A228" s="3" t="s">
         <v>696</v>
       </c>
@@ -12442,7 +13346,7 @@
       <c r="Q228" s="3"/>
       <c r="R228" s="3"/>
     </row>
-    <row r="229" spans="1:18" ht="96">
+    <row r="229" spans="1:18" ht="95" x14ac:dyDescent="1.1000000000000001">
       <c r="A229" s="53" t="s">
         <v>699</v>
       </c>
@@ -12462,13 +13366,12 @@
       <c r="K229" s="3"/>
       <c r="L229" s="3"/>
       <c r="M229" s="3"/>
-      <c r="N229" s="3"/>
       <c r="O229" s="3"/>
       <c r="P229" s="3"/>
       <c r="Q229" s="3"/>
       <c r="R229" s="3"/>
     </row>
-    <row r="230" spans="1:18" ht="96">
+    <row r="230" spans="1:18" ht="95" x14ac:dyDescent="1.1000000000000001">
       <c r="A230" s="53" t="s">
         <v>701</v>
       </c>
@@ -12488,13 +13391,12 @@
       <c r="K230" s="3"/>
       <c r="L230" s="3"/>
       <c r="M230" s="3"/>
-      <c r="N230" s="3"/>
       <c r="O230" s="3"/>
       <c r="P230" s="3"/>
       <c r="Q230" s="3"/>
       <c r="R230" s="3"/>
     </row>
-    <row r="231" spans="1:18" ht="96">
+    <row r="231" spans="1:18" ht="95" x14ac:dyDescent="1.1000000000000001">
       <c r="A231" s="53" t="s">
         <v>703</v>
       </c>
@@ -12514,13 +13416,12 @@
       <c r="K231" s="3"/>
       <c r="L231" s="3"/>
       <c r="M231" s="3"/>
-      <c r="N231" s="3"/>
       <c r="O231" s="3"/>
       <c r="P231" s="3"/>
       <c r="Q231" s="3"/>
       <c r="R231" s="3"/>
     </row>
-    <row r="232" spans="1:18" ht="96">
+    <row r="232" spans="1:18" ht="95" x14ac:dyDescent="1.1000000000000001">
       <c r="A232" s="53" t="s">
         <v>705</v>
       </c>
@@ -12540,13 +13441,12 @@
       <c r="K232" s="3"/>
       <c r="L232" s="3"/>
       <c r="M232" s="3"/>
-      <c r="N232" s="3"/>
       <c r="O232" s="3"/>
       <c r="P232" s="3"/>
       <c r="Q232" s="3"/>
       <c r="R232" s="3"/>
     </row>
-    <row r="233" spans="1:18" ht="144">
+    <row r="233" spans="1:18" ht="142.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A233" s="53" t="s">
         <v>707</v>
       </c>
@@ -12566,13 +13466,12 @@
       <c r="K233" s="3"/>
       <c r="L233" s="3"/>
       <c r="M233" s="3"/>
-      <c r="N233" s="3"/>
       <c r="O233" s="3"/>
       <c r="P233" s="3"/>
       <c r="Q233" s="3"/>
       <c r="R233" s="3"/>
     </row>
-    <row r="234" spans="1:18" ht="96">
+    <row r="234" spans="1:18" ht="95" x14ac:dyDescent="1.1000000000000001">
       <c r="A234" s="53" t="s">
         <v>709</v>
       </c>
@@ -12592,13 +13491,12 @@
       <c r="K234" s="3"/>
       <c r="L234" s="3"/>
       <c r="M234" s="3"/>
-      <c r="N234" s="3"/>
       <c r="O234" s="3"/>
       <c r="P234" s="3"/>
       <c r="Q234" s="3"/>
       <c r="R234" s="3"/>
     </row>
-    <row r="235" spans="1:18" ht="96">
+    <row r="235" spans="1:18" ht="95" x14ac:dyDescent="1.1000000000000001">
       <c r="A235" s="53" t="s">
         <v>711</v>
       </c>
@@ -12618,13 +13516,12 @@
       <c r="K235" s="3"/>
       <c r="L235" s="3"/>
       <c r="M235" s="3"/>
-      <c r="N235" s="3"/>
       <c r="O235" s="3"/>
       <c r="P235" s="3"/>
       <c r="Q235" s="3"/>
       <c r="R235" s="3"/>
     </row>
-    <row r="236" spans="1:18" ht="144">
+    <row r="236" spans="1:18" ht="142.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A236" s="53" t="s">
         <v>713</v>
       </c>
@@ -12644,13 +13541,12 @@
       <c r="K236" s="3"/>
       <c r="L236" s="3"/>
       <c r="M236" s="3"/>
-      <c r="N236" s="3"/>
       <c r="O236" s="3"/>
       <c r="P236" s="3"/>
       <c r="Q236" s="3"/>
       <c r="R236" s="3"/>
     </row>
-    <row r="237" spans="1:18" ht="144">
+    <row r="237" spans="1:18" ht="142.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A237" s="53" t="s">
         <v>715</v>
       </c>
@@ -12670,13 +13566,12 @@
       <c r="K237" s="3"/>
       <c r="L237" s="3"/>
       <c r="M237" s="3"/>
-      <c r="N237" s="3"/>
       <c r="O237" s="3"/>
       <c r="P237" s="3"/>
       <c r="Q237" s="3"/>
       <c r="R237" s="3"/>
     </row>
-    <row r="238" spans="1:18" ht="96">
+    <row r="238" spans="1:18" ht="95" x14ac:dyDescent="1.1000000000000001">
       <c r="A238" s="53" t="s">
         <v>717</v>
       </c>
@@ -12696,13 +13591,12 @@
       <c r="K238" s="3"/>
       <c r="L238" s="3"/>
       <c r="M238" s="3"/>
-      <c r="N238" s="3"/>
       <c r="O238" s="3"/>
       <c r="P238" s="3"/>
       <c r="Q238" s="3"/>
       <c r="R238" s="3"/>
     </row>
-    <row r="239" spans="1:18">
+    <row r="239" spans="1:18" x14ac:dyDescent="1.1000000000000001">
       <c r="A239" s="3"/>
       <c r="B239" s="3"/>
       <c r="C239" s="4"/>
@@ -12716,13 +13610,12 @@
       <c r="K239" s="3"/>
       <c r="L239" s="3"/>
       <c r="M239" s="3"/>
-      <c r="N239" s="3"/>
       <c r="O239" s="3"/>
       <c r="P239" s="3"/>
       <c r="Q239" s="3"/>
       <c r="R239" s="3"/>
     </row>
-    <row r="240" spans="1:18">
+    <row r="240" spans="1:18" x14ac:dyDescent="1.1000000000000001">
       <c r="A240" s="3"/>
       <c r="B240" s="3"/>
       <c r="C240" s="4"/>
@@ -12736,7 +13629,6 @@
       <c r="K240" s="3"/>
       <c r="L240" s="3"/>
       <c r="M240" s="3"/>
-      <c r="N240" s="3"/>
       <c r="O240" s="3"/>
       <c r="P240" s="3"/>
       <c r="Q240" s="3"/>
@@ -12753,23 +13645,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="687acdf3-ad85-4bdb-a62b-77fce9e2a613" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000470215BC4A30A4187D23D62A4EC96F3" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0276ec8e258d46ff7cd3f9c3f2a1b5d7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="687acdf3-ad85-4bdb-a62b-77fce9e2a613" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fc2a4560534904d2742450f63d0b5b2b" ns3:_="">
     <xsd:import namespace="687acdf3-ad85-4bdb-a62b-77fce9e2a613"/>
@@ -12925,25 +13800,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{348A41D9-E042-4893-9C37-7D13B167F5BD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="687acdf3-ad85-4bdb-a62b-77fce9e2a613"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F79A7D57-BF41-4B12-9712-226D862B76C0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="687acdf3-ad85-4bdb-a62b-77fce9e2a613" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{12CE1AE3-5F37-4838-9901-BD8B31E4F67F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -12959,4 +13833,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F79A7D57-BF41-4B12-9712-226D862B76C0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{348A41D9-E042-4893-9C37-7D13B167F5BD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="687acdf3-ad85-4bdb-a62b-77fce9e2a613"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>